<commit_message>
Week 21. Latest data
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlsmith/Desktop/Home Desktop – Carl’s iMac /Football/Season 2024 Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEE4CDE-E658-3C4E-9B9C-BCB1342BDFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBFC9E6A-BA8A-4A46-95C4-116ED451BF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="560" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="League Table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Board Room'!$A$1:$F$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Captains!$A$1:$G$34</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'League Table'!$A$3:$BJ$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'League Table'!$A$3:$BJ$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="192">
   <si>
     <t>WK 1</t>
   </si>
@@ -604,6 +604,18 @@
   </si>
   <si>
     <t>Lost 1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9-1</t>
+  </si>
+  <si>
+    <t>Dogger</t>
+  </si>
+  <si>
+    <t>Lost 1-9</t>
   </si>
 </sst>
 </file>
@@ -862,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1000,6 +1012,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,13 +1424,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BJ72"/>
+  <dimension ref="A1:BJ73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY43" sqref="AY43"/>
+      <selection pane="bottomRight" activeCell="BA5" sqref="BA5:BA38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1911,7 +1924,9 @@
       <c r="U5" s="18">
         <v>4</v>
       </c>
-      <c r="V5" s="18"/>
+      <c r="V5" s="18">
+        <v>-8</v>
+      </c>
       <c r="W5" s="18"/>
       <c r="X5" s="18"/>
       <c r="Y5" s="18"/>
@@ -1948,7 +1963,7 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8">
         <f>COUNT(B5:AY5)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BD5" s="8">
         <f>COUNTIF($B5:$AY5, "&gt;=1")</f>
@@ -1960,7 +1975,7 @@
       </c>
       <c r="BF5" s="8">
         <f>COUNTIF($B5:$AY5, "&lt;0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BG5" s="8">
         <f>SUM(BD5*3)+BE5</f>
@@ -1968,11 +1983,11 @@
       </c>
       <c r="BH5" s="8">
         <f>SUM(B5:AY5)</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="BI5" s="10">
         <f>SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.70588235294117652</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BJ5" s="10"/>
     </row>
@@ -2101,51 +2116,61 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="58"/>
+        <v>21</v>
+      </c>
+      <c r="B7" s="7">
+        <v>-1</v>
+      </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
-        <v>9</v>
-      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7">
+      <c r="F7" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="48">
         <v>0</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="7">
-        <v>7</v>
-      </c>
-      <c r="J7" s="48">
+        <v>-7</v>
+      </c>
+      <c r="J7" s="7">
         <v>8</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
       <c r="L7" s="7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="M7" s="7">
         <v>-1</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
+        <v>-1</v>
+      </c>
       <c r="P7" s="7">
         <v>2</v>
       </c>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="7">
+        <v>3</v>
+      </c>
       <c r="R7" s="53"/>
-      <c r="S7" s="48">
+      <c r="S7" s="7">
         <v>-2</v>
       </c>
       <c r="T7" s="7">
         <v>1</v>
       </c>
-      <c r="U7" s="7">
-        <v>4</v>
-      </c>
-      <c r="V7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7">
+        <v>8</v>
+      </c>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
@@ -2167,7 +2192,7 @@
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
-      <c r="AR7" s="58"/>
+      <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
@@ -2180,7 +2205,7 @@
       </c>
       <c r="BC7" s="8">
         <f>COUNT(B7:AY7)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="BD7" s="8">
         <f>COUNTIF($B7:$AY7, "&gt;=1")</f>
@@ -2188,29 +2213,29 @@
       </c>
       <c r="BE7" s="8">
         <f>COUNTIF($B7:$AY7, "0")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF7" s="8">
         <f>COUNTIF($B7:$AY7, "&lt;0")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BG7" s="8">
         <f>SUM(BD7*3)+BE7</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BH7" s="8">
         <f>SUM(B7:AY7)</f>
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="BI7" s="10">
         <f>SUM(BD7*3+BE7*1)/SUM(BC7*3)</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="BJ7" s="10"/>
     </row>
     <row r="8" spans="1:62" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B8" s="18">
         <v>-1</v>
@@ -2218,29 +2243,33 @@
       <c r="C8" s="18">
         <v>1</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="18">
+        <v>9</v>
+      </c>
+      <c r="E8" s="18">
+        <v>-1</v>
+      </c>
       <c r="F8" s="18">
-        <v>-1</v>
-      </c>
-      <c r="G8" s="49">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18">
         <v>0</v>
       </c>
       <c r="H8" s="51"/>
-      <c r="I8" s="18">
+      <c r="I8" s="49">
         <v>-7</v>
       </c>
       <c r="J8" s="18">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="K8" s="18">
         <v>0</v>
       </c>
       <c r="L8" s="18">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M8" s="18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N8" s="18">
         <v>0</v>
@@ -2248,21 +2277,19 @@
       <c r="O8" s="18">
         <v>-1</v>
       </c>
-      <c r="P8" s="18">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>3</v>
-      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
       <c r="R8" s="51"/>
-      <c r="S8" s="18">
-        <v>-2</v>
-      </c>
+      <c r="S8" s="18"/>
       <c r="T8" s="18">
         <v>1</v>
       </c>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
+      <c r="U8" s="18">
+        <v>4</v>
+      </c>
+      <c r="V8" s="18">
+        <v>8</v>
+      </c>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -2297,11 +2324,11 @@
       </c>
       <c r="BC8" s="8">
         <f>COUNT(B8:AY8)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BD8" s="8">
         <f>COUNTIF($B8:$AY8, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE8" s="8">
         <f>COUNTIF($B8:$AY8, "0")</f>
@@ -2313,26 +2340,26 @@
       </c>
       <c r="BG8" s="8">
         <f>SUM(BD8*3)+BE8</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="BH8" s="8">
         <f>SUM(B8:AY8)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BI8" s="10">
         <f>SUM(BD8*3+BE8*1)/SUM(BC8*3)</f>
-        <v>0.46666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="BJ8" s="10"/>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B9" s="16">
-        <v>-1</v>
-      </c>
-      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="50">
         <v>1</v>
       </c>
       <c r="D9" s="16">
@@ -2342,44 +2369,50 @@
         <v>-1</v>
       </c>
       <c r="F9" s="16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G9" s="16">
         <v>0</v>
       </c>
       <c r="H9" s="54"/>
-      <c r="I9" s="50">
+      <c r="I9" s="16">
         <v>-7</v>
       </c>
       <c r="J9" s="16">
-        <v>-8</v>
-      </c>
-      <c r="K9" s="16">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="K9" s="16"/>
       <c r="L9" s="16">
         <v>-2</v>
       </c>
       <c r="M9" s="16">
-        <v>1</v>
-      </c>
-      <c r="N9" s="16">
+        <v>-1</v>
+      </c>
+      <c r="N9" s="50">
         <v>0</v>
       </c>
       <c r="O9" s="16">
+        <v>1</v>
+      </c>
+      <c r="P9" s="16">
+        <v>-2</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>-3</v>
+      </c>
+      <c r="R9" s="54"/>
+      <c r="S9" s="16">
+        <v>2</v>
+      </c>
+      <c r="T9" s="16">
         <v>-1</v>
       </c>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16">
-        <v>1</v>
-      </c>
       <c r="U9" s="16">
-        <v>4</v>
-      </c>
-      <c r="V9" s="16"/>
+        <v>-4</v>
+      </c>
+      <c r="V9" s="16">
+        <v>8</v>
+      </c>
       <c r="W9" s="16"/>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
@@ -2414,49 +2447,49 @@
       </c>
       <c r="BC9" s="8">
         <f>COUNT(B9:AY9)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="BD9" s="8">
         <f>COUNTIF($B9:$AY9, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE9" s="8">
         <f>COUNTIF($B9:$AY9, "0")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BF9" s="8">
         <f>COUNTIF($B9:$AY9, "&lt;0")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BG9" s="8">
         <f>SUM(BD9*3)+BE9</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="BH9" s="8">
         <f>SUM(B9:AY9)</f>
-        <v>-3</v>
+        <v>8</v>
       </c>
       <c r="BI9" s="10">
         <f>SUM(BD9*3+BE9*1)/SUM(BC9*3)</f>
-        <v>0.46666666666666667</v>
+        <v>0.42592592592592593</v>
       </c>
       <c r="BJ9" s="10"/>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="16">
-        <v>1</v>
-      </c>
-      <c r="C10" s="50">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="B10" s="50">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="16">
+        <v>-1</v>
       </c>
       <c r="D10" s="16">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="E10" s="16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F10" s="16">
         <v>-1</v>
@@ -2465,42 +2498,40 @@
         <v>0</v>
       </c>
       <c r="H10" s="54"/>
-      <c r="I10" s="16">
-        <v>-7</v>
-      </c>
-      <c r="J10" s="16">
-        <v>8</v>
-      </c>
-      <c r="K10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16">
+        <v>0</v>
+      </c>
       <c r="L10" s="16">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="M10" s="16">
         <v>-1</v>
       </c>
-      <c r="N10" s="48">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7">
+      <c r="N10" s="7"/>
+      <c r="O10" s="48">
         <v>1</v>
       </c>
       <c r="P10" s="7">
         <v>-2</v>
       </c>
       <c r="Q10" s="7">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R10" s="54"/>
       <c r="S10" s="16">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="T10" s="16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U10" s="16">
-        <v>-4</v>
-      </c>
-      <c r="V10" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="V10" s="16">
+        <v>8</v>
+      </c>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
@@ -2535,11 +2566,11 @@
       </c>
       <c r="BC10" s="8">
         <f>COUNT(B10:AY10)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="BD10" s="8">
         <f>COUNTIF($B10:$AY10, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE10" s="8">
         <f>COUNTIF($B10:$AY10, "0")</f>
@@ -2547,68 +2578,60 @@
       </c>
       <c r="BF10" s="8">
         <f>COUNTIF($B10:$AY10, "&lt;0")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BG10" s="8">
         <f>SUM(BD10*3)+BE10</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="BH10" s="8">
         <f>SUM(B10:AY10)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI10" s="10">
         <f>SUM(BD10*3+BE10*1)/SUM(BC10*3)</f>
-        <v>0.39215686274509803</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="BJ10" s="10"/>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="48">
-        <v>-1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B11" s="58"/>
       <c r="C11" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D11" s="7">
-        <v>-9</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7">
-        <v>-1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="7">
         <v>0</v>
       </c>
       <c r="H11" s="53"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
+      <c r="I11" s="7">
+        <v>7</v>
+      </c>
+      <c r="J11" s="48">
+        <v>8</v>
+      </c>
+      <c r="K11" s="7"/>
       <c r="L11" s="7">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M11" s="7">
         <v>-1</v>
       </c>
       <c r="N11" s="7"/>
-      <c r="O11" s="48">
-        <v>1</v>
-      </c>
+      <c r="O11" s="7"/>
       <c r="P11" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="7"/>
       <c r="R11" s="53"/>
-      <c r="S11" s="7">
+      <c r="S11" s="48">
         <v>-2</v>
       </c>
       <c r="T11" s="7">
@@ -2639,7 +2662,7 @@
       <c r="AO11" s="7"/>
       <c r="AP11" s="7"/>
       <c r="AQ11" s="7"/>
-      <c r="AR11" s="7"/>
+      <c r="AR11" s="58"/>
       <c r="AS11" s="7"/>
       <c r="AT11" s="7"/>
       <c r="AU11" s="7"/>
@@ -2652,31 +2675,31 @@
       </c>
       <c r="BC11" s="8">
         <f>COUNT(B11:AY11)</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BD11" s="8">
         <f>COUNTIF($B11:$AY11, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE11" s="8">
         <f>COUNTIF($B11:$AY11, "0")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF11" s="8">
         <f>COUNTIF($B11:$AY11, "&lt;0")</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BG11" s="8">
         <f>SUM(BD11*3)+BE11</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BH11" s="8">
         <f>SUM(B11:AY11)</f>
-        <v>-5</v>
+        <v>27</v>
       </c>
       <c r="BI11" s="10">
         <f>SUM(BD11*3+BE11*1)/SUM(BC11*3)</f>
-        <v>0.44444444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BJ11" s="10"/>
     </row>
@@ -2720,7 +2743,9 @@
         <v>1</v>
       </c>
       <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
+      <c r="V12" s="48">
+        <v>8</v>
+      </c>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
@@ -2755,11 +2780,11 @@
       </c>
       <c r="BC12" s="8">
         <f>COUNT(B12:AY12)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD12" s="8">
         <f>COUNTIF($B12:$AY12, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE12" s="8">
         <f>COUNTIF($B12:$AY12, "0")</f>
@@ -2771,21 +2796,21 @@
       </c>
       <c r="BG12" s="8">
         <f>SUM(BD12*3)+BE12</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="BH12" s="8">
         <f>SUM(B12:AY12)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="BI12" s="10">
         <f>SUM(BD12*3+BE12*1)/SUM(BC12*3)</f>
-        <v>0.79166666666666663</v>
+        <v>0.81481481481481477</v>
       </c>
       <c r="BJ12" s="10"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="B13" s="7">
         <v>-1</v>
@@ -2793,9 +2818,11 @@
       <c r="C13" s="7">
         <v>-1</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7">
+        <v>-9</v>
+      </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="7">
+      <c r="F13" s="48">
         <v>-1</v>
       </c>
       <c r="G13" s="7">
@@ -2806,36 +2833,42 @@
         <v>7</v>
       </c>
       <c r="J13" s="7">
-        <v>8</v>
-      </c>
-      <c r="K13" s="48">
+        <v>-8</v>
+      </c>
+      <c r="K13" s="7">
         <v>0</v>
       </c>
       <c r="L13" s="7">
+        <v>2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>1</v>
+      </c>
+      <c r="P13" s="48">
         <v>-2</v>
       </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q13" s="7"/>
+      <c r="Q13" s="7">
+        <v>-3</v>
+      </c>
       <c r="R13" s="53"/>
       <c r="S13" s="7">
         <v>2</v>
       </c>
-      <c r="T13" s="48">
+      <c r="T13" s="7">
         <v>-1</v>
       </c>
       <c r="U13" s="7">
-        <v>4</v>
-      </c>
-      <c r="V13" s="7"/>
+        <v>-4</v>
+      </c>
+      <c r="V13" s="7">
+        <v>8</v>
+      </c>
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
@@ -2870,11 +2903,11 @@
       </c>
       <c r="BC13" s="8">
         <f>COUNT(B13:AY13)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="BD13" s="8">
         <f>COUNTIF($B13:$AY13, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE13" s="8">
         <f>COUNTIF($B13:$AY13, "0")</f>
@@ -2882,56 +2915,50 @@
       </c>
       <c r="BF13" s="8">
         <f>COUNTIF($B13:$AY13, "&lt;0")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BG13" s="8">
         <f>SUM(BD13*3)+BE13</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="BH13" s="8">
         <f>SUM(B13:AY13)</f>
-        <v>14</v>
+        <v>-9</v>
       </c>
       <c r="BI13" s="10">
         <f>SUM(BD13*3+BE13*1)/SUM(BC13*3)</f>
-        <v>0.42857142857142855</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="BJ13" s="10"/>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B14" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C14" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D14" s="7">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7">
-        <v>-1</v>
-      </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="7">
         <v>0</v>
       </c>
       <c r="H14" s="53"/>
-      <c r="I14" s="48">
-        <v>7</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="I14" s="7"/>
+      <c r="J14" s="48">
         <v>-8</v>
       </c>
-      <c r="K14" s="7">
-        <v>0</v>
-      </c>
-      <c r="L14" s="7">
-        <v>-2</v>
-      </c>
-      <c r="M14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
       <c r="N14" s="7">
         <v>0</v>
       </c>
@@ -2943,10 +2970,16 @@
         <v>3</v>
       </c>
       <c r="R14" s="53"/>
-      <c r="S14" s="7"/>
+      <c r="S14" s="7">
+        <v>-2</v>
+      </c>
       <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
+      <c r="U14" s="48">
+        <v>4</v>
+      </c>
+      <c r="V14" s="7">
+        <v>8</v>
+      </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
@@ -2985,11 +3018,11 @@
       </c>
       <c r="BD14" s="8">
         <f>COUNTIF($B14:$AY14, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE14" s="8">
         <f>COUNTIF($B14:$AY14, "0")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BF14" s="8">
         <f>COUNTIF($B14:$AY14, "&lt;0")</f>
@@ -2997,40 +3030,40 @@
       </c>
       <c r="BG14" s="8">
         <f>SUM(BD14*3)+BE14</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="BH14" s="8">
         <f>SUM(B14:AY14)</f>
-        <v>9</v>
+        <v>-2</v>
       </c>
       <c r="BI14" s="10">
         <f>SUM(BD14*3+BE14*1)/SUM(BC14*3)</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="BJ14" s="10"/>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B15" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7">
         <v>-1</v>
       </c>
       <c r="D15" s="7">
-        <v>-9</v>
+        <v>9</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="48">
+      <c r="F15" s="7">
         <v>-1</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
       </c>
       <c r="H15" s="53"/>
-      <c r="I15" s="7">
+      <c r="I15" s="48">
         <v>7</v>
       </c>
       <c r="J15" s="7">
@@ -3040,33 +3073,23 @@
         <v>0</v>
       </c>
       <c r="L15" s="7">
-        <v>2</v>
-      </c>
-      <c r="M15" s="7">
-        <v>1</v>
-      </c>
+        <v>-2</v>
+      </c>
+      <c r="M15" s="7"/>
       <c r="N15" s="7">
         <v>0</v>
       </c>
       <c r="O15" s="7">
         <v>1</v>
       </c>
-      <c r="P15" s="48">
-        <v>-2</v>
-      </c>
+      <c r="P15" s="7"/>
       <c r="Q15" s="7">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R15" s="53"/>
-      <c r="S15" s="7">
-        <v>2</v>
-      </c>
-      <c r="T15" s="7">
-        <v>-1</v>
-      </c>
-      <c r="U15" s="7">
-        <v>-4</v>
-      </c>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
@@ -3102,7 +3125,7 @@
       </c>
       <c r="BC15" s="8">
         <f>COUNT(B15:AY15)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="BD15" s="8">
         <f>COUNTIF($B15:$AY15, "&gt;=1")</f>
@@ -3114,7 +3137,7 @@
       </c>
       <c r="BF15" s="8">
         <f>COUNTIF($B15:$AY15, "&lt;0")</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BG15" s="8">
         <f>SUM(BD15*3)+BE15</f>
@@ -3122,19 +3145,21 @@
       </c>
       <c r="BH15" s="8">
         <f>SUM(B15:AY15)</f>
-        <v>-17</v>
+        <v>9</v>
       </c>
       <c r="BI15" s="10">
         <f>SUM(BD15*3+BE15*1)/SUM(BC15*3)</f>
-        <v>0.35294117647058826</v>
+        <v>0.5</v>
       </c>
       <c r="BJ15" s="10"/>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="7"/>
+        <v>107</v>
+      </c>
+      <c r="B16" s="7">
+        <v>-1</v>
+      </c>
       <c r="C16" s="7">
         <v>-1</v>
       </c>
@@ -3147,36 +3172,42 @@
         <v>0</v>
       </c>
       <c r="H16" s="53"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7">
+        <v>7</v>
+      </c>
       <c r="J16" s="7">
         <v>8</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="48">
+      <c r="K16" s="48">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>-2</v>
+      </c>
+      <c r="M16" s="7">
         <v>1</v>
       </c>
       <c r="N16" s="7">
         <v>0</v>
       </c>
-      <c r="O16" s="7">
-        <v>1</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7">
-        <v>-3</v>
-      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7">
+        <v>-2</v>
+      </c>
+      <c r="Q16" s="7"/>
       <c r="R16" s="53"/>
       <c r="S16" s="7">
         <v>2</v>
       </c>
-      <c r="T16" s="7">
-        <v>1</v>
+      <c r="T16" s="48">
+        <v>-1</v>
       </c>
       <c r="U16" s="7">
-        <v>-4</v>
-      </c>
-      <c r="V16" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="V16" s="7">
+        <v>-8</v>
+      </c>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
@@ -3211,7 +3242,7 @@
       </c>
       <c r="BC16" s="8">
         <f>COUNT(B16:AY16)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="BD16" s="8">
         <f>COUNTIF($B16:$AY16, "&gt;=1")</f>
@@ -3219,52 +3250,50 @@
       </c>
       <c r="BE16" s="8">
         <f>COUNTIF($B16:$AY16, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF16" s="8">
         <f>COUNTIF($B16:$AY16, "&lt;0")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BG16" s="8">
         <f>SUM(BD16*3)+BE16</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BH16" s="8">
         <f>SUM(B16:AY16)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BI16" s="10">
         <f>SUM(BD16*3+BE16*1)/SUM(BC16*3)</f>
-        <v>0.51515151515151514</v>
+        <v>0.4</v>
       </c>
       <c r="BJ16" s="10"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="7">
+        <v>79</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7">
         <v>-1</v>
       </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7">
-        <v>-9</v>
-      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>-1</v>
+      </c>
       <c r="G17" s="7">
         <v>0</v>
       </c>
       <c r="H17" s="53"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="48">
-        <v>-8</v>
+      <c r="J17" s="7">
+        <v>8</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="7">
+      <c r="M17" s="48">
         <v>1</v>
       </c>
       <c r="N17" s="7">
@@ -3275,17 +3304,21 @@
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R17" s="53"/>
       <c r="S17" s="7">
-        <v>-2</v>
-      </c>
-      <c r="T17" s="7"/>
-      <c r="U17" s="48">
-        <v>4</v>
-      </c>
-      <c r="V17" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7">
+        <v>-4</v>
+      </c>
+      <c r="V17" s="7">
+        <v>-8</v>
+      </c>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
       <c r="Y17" s="7"/>
@@ -3320,7 +3353,7 @@
       </c>
       <c r="BC17" s="8">
         <f>COUNT(B17:AY17)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BD17" s="8">
         <f>COUNTIF($B17:$AY17, "&gt;=1")</f>
@@ -3332,7 +3365,7 @@
       </c>
       <c r="BF17" s="8">
         <f>COUNTIF($B17:$AY17, "&lt;0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG17" s="8">
         <f>SUM(BD17*3)+BE17</f>
@@ -3340,44 +3373,46 @@
       </c>
       <c r="BH17" s="8">
         <f>SUM(B17:AY17)</f>
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="BI17" s="10">
         <f>SUM(BD17*3+BE17*1)/SUM(BC17*3)</f>
-        <v>0.51515151515151514</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="BJ17" s="10"/>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7">
         <v>1</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="48">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7"/>
+      <c r="E18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
       <c r="H18" s="53"/>
-      <c r="I18" s="7">
-        <v>-7</v>
-      </c>
+      <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="M18" s="7">
+        <v>1</v>
+      </c>
       <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q18" s="7"/>
+      <c r="O18" s="48">
+        <v>-1</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7">
+        <v>-3</v>
+      </c>
       <c r="R18" s="53"/>
       <c r="S18" s="7">
         <v>2</v>
@@ -3385,8 +3420,12 @@
       <c r="T18" s="7">
         <v>1</v>
       </c>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
+      <c r="U18" s="7">
+        <v>-4</v>
+      </c>
+      <c r="V18" s="7">
+        <v>8</v>
+      </c>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
@@ -3421,7 +3460,7 @@
       </c>
       <c r="BC18" s="8">
         <f>COUNT(B18:AY18)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="BD18" s="8">
         <f>COUNTIF($B18:$AY18, "&gt;=1")</f>
@@ -3429,76 +3468,64 @@
       </c>
       <c r="BE18" s="8">
         <f>COUNTIF($B18:$AY18, "0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF18" s="8">
         <f>COUNTIF($B18:$AY18, "&lt;0")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BG18" s="8">
         <f>SUM(BD18*3)+BE18</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BH18" s="8">
         <f>SUM(B18:AY18)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="BI18" s="10">
         <f>SUM(BD18*3+BE18*1)/SUM(BC18*3)</f>
-        <v>0.7142857142857143</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="BJ18" s="10"/>
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="7">
-        <v>-1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7">
+      <c r="E19" s="48">
         <v>1</v>
       </c>
       <c r="F19" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="53"/>
       <c r="I19" s="7">
         <v>-7</v>
       </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="7">
-        <v>0</v>
-      </c>
-      <c r="L19" s="48">
-        <v>2</v>
-      </c>
-      <c r="M19" s="7">
-        <v>1</v>
-      </c>
-      <c r="N19" s="7">
-        <v>0</v>
-      </c>
-      <c r="O19" s="7">
-        <v>-1</v>
-      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
       <c r="P19" s="7">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="53"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="48">
-        <v>-4</v>
-      </c>
+      <c r="S19" s="7">
+        <v>2</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
@@ -3534,19 +3561,19 @@
       </c>
       <c r="BC19" s="8">
         <f>COUNT(B19:AY19)</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BD19" s="8">
         <f>COUNTIF($B19:$AY19, "&gt;=1")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BE19" s="8">
         <f>COUNTIF($B19:$AY19, "0")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BF19" s="8">
         <f>COUNTIF($B19:$AY19, "&lt;0")</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="BG19" s="8">
         <f>SUM(BD19*3)+BE19</f>
@@ -3554,57 +3581,67 @@
       </c>
       <c r="BH19" s="8">
         <f>SUM(B19:AY19)</f>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="BI19" s="10">
         <f>SUM(BD19*3+BE19*1)/SUM(BC19*3)</f>
-        <v>0.38461538461538464</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="BJ19" s="10"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="B20" s="7">
+        <v>-1</v>
+      </c>
       <c r="C20" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
         <v>-1</v>
       </c>
-      <c r="F20" s="7"/>
       <c r="G20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="53"/>
-      <c r="I20" s="7"/>
+      <c r="I20" s="7">
+        <v>-7</v>
+      </c>
       <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="48">
+        <v>2</v>
+      </c>
       <c r="M20" s="7">
         <v>1</v>
       </c>
-      <c r="N20" s="7"/>
-      <c r="O20" s="48">
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7">
         <v>-1</v>
       </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7">
-        <v>-3</v>
-      </c>
+      <c r="P20" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="7"/>
       <c r="R20" s="53"/>
-      <c r="S20" s="7">
-        <v>2</v>
-      </c>
-      <c r="T20" s="7">
-        <v>1</v>
-      </c>
-      <c r="U20" s="7">
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="48">
         <v>-4</v>
       </c>
-      <c r="V20" s="7"/>
+      <c r="V20" s="7">
+        <v>-8</v>
+      </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
@@ -3639,7 +3676,7 @@
       </c>
       <c r="BC20" s="8">
         <f>COUNT(B20:AY20)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="BD20" s="8">
         <f>COUNTIF($B20:$AY20, "&gt;=1")</f>
@@ -3647,23 +3684,23 @@
       </c>
       <c r="BE20" s="8">
         <f>COUNTIF($B20:$AY20, "0")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF20" s="8">
         <f>COUNTIF($B20:$AY20, "&lt;0")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BG20" s="8">
         <f>SUM(BD20*3)+BE20</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BH20" s="8">
         <f>SUM(B20:AY20)</f>
-        <v>-4</v>
+        <v>-17</v>
       </c>
       <c r="BI20" s="10">
         <f>SUM(BD20*3+BE20*1)/SUM(BC20*3)</f>
-        <v>0.48148148148148145</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="BJ20" s="10"/>
     </row>
@@ -4223,7 +4260,9 @@
       <c r="U26" s="7">
         <v>-4</v>
       </c>
-      <c r="V26" s="7"/>
+      <c r="V26" s="7">
+        <v>-8</v>
+      </c>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -4258,7 +4297,7 @@
       </c>
       <c r="BC26" s="8">
         <f>COUNT(B26:AY26)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BD26" s="8">
         <f>COUNTIF($B26:$AY26, "&gt;=1")</f>
@@ -4270,7 +4309,7 @@
       </c>
       <c r="BF26" s="8">
         <f>COUNTIF($B26:$AY26, "&lt;0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BG26" s="8">
         <f>SUM(BD26*3)+BE26</f>
@@ -4278,11 +4317,11 @@
       </c>
       <c r="BH26" s="8">
         <f>SUM(B26:AY26)</f>
-        <v>-7</v>
+        <v>-15</v>
       </c>
       <c r="BI26" s="10">
         <f>SUM(BD26*3+BE26*1)/SUM(BC26*3)</f>
-        <v>0.25925925925925924</v>
+        <v>0.23333333333333334</v>
       </c>
       <c r="BJ26" s="10"/>
     </row>
@@ -4379,7 +4418,7 @@
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -4390,26 +4429,24 @@
       <c r="H28" s="53"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="7">
-        <v>0</v>
-      </c>
-      <c r="L28" s="48">
-        <v>-2</v>
-      </c>
-      <c r="M28" s="7">
-        <v>-1</v>
-      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
-      <c r="Q28" s="7">
-        <v>3</v>
-      </c>
+      <c r="Q28" s="7"/>
       <c r="R28" s="53"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
+      <c r="S28" s="7">
+        <v>2</v>
+      </c>
+      <c r="T28" s="7">
+        <v>-1</v>
+      </c>
       <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
+      <c r="V28" s="7">
+        <v>8</v>
+      </c>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
@@ -4444,31 +4481,31 @@
       </c>
       <c r="BC28" s="8">
         <f>COUNT(B28:AY28)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BD28" s="8">
         <f>COUNTIF($B28:$AY28, "&gt;=1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE28" s="8">
         <f>COUNTIF($B28:$AY28, "0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF28" s="8">
         <f>COUNTIF($B28:$AY28, "&lt;0")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG28" s="8">
         <f>SUM(BD28*3)+BE28</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BH28" s="8">
         <f>SUM(B28:AY28)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BI28" s="10">
         <f>SUM(BD28*3+BE28*1)/SUM(BC28*3)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BJ28" s="10"/>
     </row>
@@ -4567,7 +4604,7 @@
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>185</v>
+        <v>87</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -4578,20 +4615,28 @@
       <c r="H30" s="53"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="K30" s="7">
+        <v>0</v>
+      </c>
+      <c r="L30" s="48">
+        <v>-2</v>
+      </c>
+      <c r="M30" s="7">
+        <v>-1</v>
+      </c>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
+      <c r="Q30" s="7">
+        <v>3</v>
+      </c>
       <c r="R30" s="53"/>
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
-      <c r="U30" s="7">
-        <v>4</v>
-      </c>
-      <c r="V30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7">
+        <v>-8</v>
+      </c>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
@@ -4626,7 +4671,7 @@
       </c>
       <c r="BC30" s="8">
         <f>COUNT(B30:AY30)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BD30" s="8">
         <f>COUNTIF($B30:$AY30, "&gt;=1")</f>
@@ -4634,33 +4679,31 @@
       </c>
       <c r="BE30" s="8">
         <f>COUNTIF($B30:$AY30, "0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF30" s="8">
         <f>COUNTIF($B30:$AY30, "&lt;0")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG30" s="8">
         <f>SUM(BD30*3)+BE30</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BH30" s="8">
         <f>SUM(B30:AY30)</f>
-        <v>4</v>
+        <v>-8</v>
       </c>
       <c r="BI30" s="10">
         <f>SUM(BD30*3+BE30*1)/SUM(BC30*3)</f>
-        <v>1</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="BJ30" s="10"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -4679,7 +4722,9 @@
       <c r="R31" s="53"/>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
+      <c r="U31" s="7">
+        <v>4</v>
+      </c>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
@@ -4735,7 +4780,7 @@
       </c>
       <c r="BH31" s="8">
         <f>SUM(B31:AY31)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BI31" s="10">
         <f>SUM(BD31*3+BE31*1)/SUM(BC31*3)</f>
@@ -4745,9 +4790,11 @@
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -4764,14 +4811,12 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="53"/>
-      <c r="S32" s="7">
-        <v>2</v>
-      </c>
-      <c r="T32" s="7">
-        <v>-1</v>
-      </c>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
       <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
+      <c r="V32" s="7">
+        <v>-8</v>
+      </c>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
@@ -4826,7 +4871,7 @@
       </c>
       <c r="BH32" s="8">
         <f>SUM(B32:AY32)</f>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="BI32" s="10">
         <f>SUM(BD32*3+BE32*1)/SUM(BC32*3)</f>
@@ -5103,7 +5148,7 @@
     </row>
     <row r="36" spans="1:62" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -5120,16 +5165,14 @@
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="7">
-        <v>-3</v>
-      </c>
+      <c r="Q36" s="7"/>
       <c r="R36" s="53"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
-      <c r="U36" s="7">
-        <v>-4</v>
-      </c>
-      <c r="V36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="48">
+        <v>-8</v>
+      </c>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
@@ -5164,7 +5207,7 @@
       </c>
       <c r="BC36" s="8">
         <f>COUNT(B36:AY36)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BD36" s="8">
         <f>COUNTIF($B36:$AY36, "&gt;=1")</f>
@@ -5176,7 +5219,7 @@
       </c>
       <c r="BF36" s="8">
         <f>COUNTIF($B36:$AY36, "&lt;0")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG36" s="8">
         <f>SUM(BD36*3)+BE36</f>
@@ -5184,7 +5227,7 @@
       </c>
       <c r="BH36" s="8">
         <f>SUM(B36:AY36)</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="BI36" s="10">
         <f>SUM(BD36*3+BE36*1)/SUM(BC36*3)</f>
@@ -5281,306 +5324,303 @@
       </c>
       <c r="BJ37" s="10"/>
     </row>
-    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="27" t="s">
+    <row r="38" spans="1:62" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7">
+        <v>-3</v>
+      </c>
+      <c r="R38" s="53"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7">
+        <v>-4</v>
+      </c>
+      <c r="V38" s="7">
+        <v>-8</v>
+      </c>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
+      <c r="AN38" s="7"/>
+      <c r="AO38" s="7"/>
+      <c r="AP38" s="7"/>
+      <c r="AQ38" s="7"/>
+      <c r="AR38" s="7"/>
+      <c r="AS38" s="7"/>
+      <c r="AT38" s="7"/>
+      <c r="AU38" s="7"/>
+      <c r="AV38" s="7"/>
+      <c r="AW38" s="7"/>
+      <c r="AX38" s="7"/>
+      <c r="AY38" s="7"/>
+      <c r="BA38" s="34">
+        <v>34</v>
+      </c>
+      <c r="BC38" s="8">
+        <f>COUNT(B38:AY38)</f>
+        <v>3</v>
+      </c>
+      <c r="BD38" s="8">
+        <f>COUNTIF($B38:$AY38, "&gt;=1")</f>
+        <v>0</v>
+      </c>
+      <c r="BE38" s="8">
+        <f>COUNTIF($B38:$AY38, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="BF38" s="8">
+        <f>COUNTIF($B38:$AY38, "&lt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="BG38" s="8">
+        <f>SUM(BD38*3)+BE38</f>
+        <v>0</v>
+      </c>
+      <c r="BH38" s="8">
+        <f>SUM(B38:AY38)</f>
+        <v>-15</v>
+      </c>
+      <c r="BI38" s="10">
+        <f>SUM(BD38*3+BE38*1)/SUM(BC38*3)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ38" s="10"/>
+    </row>
+    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="28">
-        <f t="shared" ref="B38:AD38" si="0">COUNT(B5:B37)</f>
+      <c r="B39" s="28">
+        <f t="shared" ref="B39:AD39" si="0">COUNT(B5:B38)</f>
         <v>16</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C39" s="28">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D39" s="28">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E38" s="28">
+      <c r="E39" s="28">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F39" s="28">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G38" s="28">
+      <c r="G39" s="28">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H38" s="28">
+      <c r="H39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="28">
+      <c r="I39" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J38" s="28">
+      <c r="J39" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="K38" s="28">
+      <c r="K39" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L38" s="28">
+      <c r="L39" s="28">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="M38" s="28">
+      <c r="M39" s="28">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="N38" s="28">
+      <c r="N39" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O38" s="28">
+      <c r="O39" s="28">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="P38" s="28">
+      <c r="P39" s="28">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q38" s="28">
+      <c r="Q39" s="28">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="R38" s="28">
+      <c r="R39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S38" s="28">
+      <c r="S39" s="28">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="T38" s="28">
+      <c r="T39" s="28">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="U38" s="28">
+      <c r="U39" s="28">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="V38" s="28">
+      <c r="V39" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W38" s="28">
+        <v>18</v>
+      </c>
+      <c r="W39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X38" s="28">
+      <c r="X39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y38" s="28">
+      <c r="Y39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z38" s="28">
+      <c r="Z39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA38" s="28">
+      <c r="AA39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB38" s="28">
+      <c r="AB39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC38" s="28">
+      <c r="AC39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD38" s="28">
+      <c r="AD39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE38" s="28">
-        <f t="shared" ref="AE38:AY38" si="1">COUNT(AE5:AE37)</f>
-        <v>0</v>
-      </c>
-      <c r="AF38" s="28">
+      <c r="AE39" s="28">
+        <f t="shared" ref="AE39:AY39" si="1">COUNT(AE5:AE38)</f>
+        <v>0</v>
+      </c>
+      <c r="AF39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG38" s="28">
+      <c r="AG39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH38" s="28">
+      <c r="AH39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI38" s="28">
+      <c r="AI39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ38" s="28">
+      <c r="AJ39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK38" s="28">
+      <c r="AK39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AL38" s="28">
+      <c r="AL39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AM38" s="28">
+      <c r="AM39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN38" s="28">
+      <c r="AN39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AO38" s="28">
+      <c r="AO39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AP38" s="28">
+      <c r="AP39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AQ38" s="28">
+      <c r="AQ39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AR38" s="28">
+      <c r="AR39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AS38" s="28">
+      <c r="AS39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AT38" s="28">
+      <c r="AT39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AU38" s="28">
+      <c r="AU39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AV38" s="28">
+      <c r="AV39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AW38" s="28">
+      <c r="AW39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AX38" s="28">
+      <c r="AX39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AY38" s="28">
+      <c r="AY39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BC38" s="8"/>
-      <c r="BD38" s="8"/>
-      <c r="BE38" s="8"/>
-      <c r="BF38" s="8"/>
-      <c r="BG38" s="8"/>
-      <c r="BH38" s="8"/>
-      <c r="BI38" s="10"/>
-      <c r="BJ38" s="10"/>
-    </row>
-    <row r="39" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="J39" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="M39" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="N39" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="O39" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="P39" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q39" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="R39" s="8"/>
-      <c r="S39" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="T39" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="U39" s="13"/>
-      <c r="V39" s="13"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="40"/>
-      <c r="AA39" s="13"/>
-      <c r="AB39" s="13"/>
-      <c r="AC39" s="8"/>
-      <c r="AD39" s="13"/>
-      <c r="AE39" s="13"/>
-      <c r="AF39" s="13"/>
-      <c r="AG39" s="8"/>
-      <c r="AH39" s="13"/>
-      <c r="AI39" s="8"/>
-      <c r="AJ39" s="8"/>
-      <c r="AK39" s="8"/>
-      <c r="AL39" s="8"/>
-      <c r="AM39" s="8"/>
-      <c r="AN39" s="8"/>
-      <c r="AO39" s="8"/>
-      <c r="AP39" s="8"/>
-      <c r="AQ39" s="8"/>
-      <c r="AR39" s="8"/>
-      <c r="AS39" s="8"/>
-      <c r="AT39" s="8"/>
-      <c r="AU39" s="8"/>
-      <c r="AV39" s="8"/>
-      <c r="AW39" s="8"/>
-      <c r="AX39" s="8"/>
-      <c r="AY39" s="8"/>
       <c r="BC39" s="8"/>
       <c r="BD39" s="8"/>
       <c r="BE39" s="8"/>
@@ -5591,39 +5631,79 @@
       <c r="BJ39" s="10"/>
     </row>
     <row r="40" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
+      <c r="A40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="N40" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="O40" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q40" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
+      <c r="S40" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="T40" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="U40" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="V40" s="13" t="s">
+        <v>189</v>
+      </c>
       <c r="X40" s="8"/>
       <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
-      <c r="AB40" s="8"/>
+      <c r="Z40" s="40"/>
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="13"/>
       <c r="AC40" s="8"/>
-      <c r="AD40" s="8"/>
-      <c r="AE40" s="8"/>
-      <c r="AF40" s="8"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="13"/>
+      <c r="AF40" s="13"/>
       <c r="AG40" s="8"/>
-      <c r="AH40" s="8"/>
+      <c r="AH40" s="13"/>
       <c r="AI40" s="8"/>
       <c r="AJ40" s="8"/>
       <c r="AK40" s="8"/>
@@ -5651,21 +5731,37 @@
       <c r="BJ40" s="10"/>
     </row>
     <row r="41" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="8"/>
+      <c r="AB41" s="8"/>
       <c r="AC41" s="8"/>
+      <c r="AD41" s="8"/>
+      <c r="AE41" s="8"/>
+      <c r="AF41" s="8"/>
       <c r="AG41" s="8"/>
       <c r="AH41" s="8"/>
       <c r="AI41" s="8"/>
@@ -5695,14 +5791,40 @@
       <c r="BJ41" s="10"/>
     </row>
     <row r="42" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A42" s="41"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
       <c r="Q42" s="8"/>
+      <c r="AC42" s="8"/>
+      <c r="AG42" s="8"/>
+      <c r="AH42" s="8"/>
+      <c r="AI42" s="8"/>
+      <c r="AJ42" s="8"/>
+      <c r="AK42" s="8"/>
+      <c r="AL42" s="8"/>
+      <c r="AM42" s="8"/>
+      <c r="AN42" s="8"/>
+      <c r="AO42" s="8"/>
+      <c r="AP42" s="8"/>
+      <c r="AQ42" s="8"/>
+      <c r="AR42" s="8"/>
+      <c r="AS42" s="8"/>
+      <c r="AT42" s="8"/>
+      <c r="AU42" s="8"/>
+      <c r="AV42" s="8"/>
+      <c r="AW42" s="8"/>
+      <c r="AX42" s="8"/>
+      <c r="AY42" s="8"/>
       <c r="BC42" s="8"/>
       <c r="BD42" s="8"/>
       <c r="BE42" s="8"/>
@@ -5713,30 +5835,38 @@
       <c r="BJ42" s="10"/>
     </row>
     <row r="43" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-    </row>
-    <row r="46" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="J46" s="44"/>
-      <c r="L46" s="44"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="BC43" s="8"/>
+      <c r="BD43" s="8"/>
+      <c r="BE43" s="8"/>
+      <c r="BF43" s="8"/>
+      <c r="BG43" s="8"/>
+      <c r="BH43" s="8"/>
+      <c r="BI43" s="10"/>
+      <c r="BJ43" s="10"/>
+    </row>
+    <row r="44" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
     </row>
     <row r="47" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="J47" s="44"/>
       <c r="L47" s="44"/>
     </row>
     <row r="48" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="J48" s="44"/>
+      <c r="L48" s="44"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="L49" s="44"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
+      <c r="J49" s="44"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L50" s="44"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B54" s="8"/>
@@ -5774,7 +5904,7 @@
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="43"/>
+      <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
     </row>
@@ -5784,7 +5914,7 @@
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="G58" s="43"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
     </row>
@@ -5801,15 +5931,19 @@
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="43"/>
+      <c r="D60" s="8"/>
       <c r="E60" s="8"/>
-      <c r="G60" s="43"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
+      <c r="D61" s="43"/>
       <c r="E61" s="8"/>
+      <c r="G61" s="43"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B62" s="8"/>
@@ -5822,9 +5956,6 @@
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B64" s="8"/>
@@ -5856,7 +5987,7 @@
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="43"/>
+      <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -5865,7 +5996,7 @@
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
+      <c r="D68" s="43"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
@@ -5885,26 +6016,35 @@
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
+      <c r="H70" s="8"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:BI37">
-    <sortCondition descending="1" ref="BG5:BG37"/>
-    <sortCondition descending="1" ref="BH5:BH37"/>
-    <sortCondition descending="1" ref="BI5:BI37"/>
-    <sortCondition ref="A5:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:BI38">
+    <sortCondition descending="1" ref="BG5:BG38"/>
+    <sortCondition descending="1" ref="BH5:BH38"/>
+    <sortCondition descending="1" ref="BI5:BI38"/>
+    <sortCondition ref="A5:A38"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" orientation="landscape"/>
   <ignoredErrors>
-    <ignoredError sqref="BC42 BC38:BH38" formulaRange="1"/>
+    <ignoredError sqref="BC43 BC39:BH39" formulaRange="1"/>
     <ignoredError sqref="BC4:BH4" formulaRange="1" emptyCellReference="1"/>
   </ignoredErrors>
 </worksheet>
@@ -5917,7 +6057,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G26"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5925,7 +6065,7 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -5948,9 +6088,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>80</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="61" t="s">
+        <v>89</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5965,16 +6105,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G35" si="0">SUM(C3*3)+D3</f>
+        <f>SUM(C3*3)+D3</f>
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>89</v>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -5989,40 +6129,40 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <f>SUM(C4*3)+D4</f>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>110</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>80</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <f>SUM(C5*3)+D5</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>91</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>110</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -6044,33 +6184,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>90</v>
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f>SUM(C7*3)+D7</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6085,16 +6225,16 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f>SUM(C8*3)+D8</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>156</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6109,17 +6249,16 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <f>SUM(C9*3)+D9</f>
         <v>3</v>
       </c>
-      <c r="H9" s="24"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6134,16 +6273,17 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <f>SUM(C10*3)+D10</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -6165,9 +6305,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6188,9 +6328,8 @@
         <f>SUM(C12*3)+D12</f>
         <v>3</v>
       </c>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -6213,8 +6352,9 @@
         <f>SUM(C13*3)+D13</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>106</v>
       </c>
@@ -6238,7 +6378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
@@ -6262,7 +6402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
@@ -6285,7 +6425,6 @@
         <f>SUM(C16*3)+D16</f>
         <v>3</v>
       </c>
-      <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -6360,7 +6499,7 @@
         <f>SUM(C19*3)+D19</f>
         <v>1</v>
       </c>
-      <c r="K19" s="38"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -6385,7 +6524,7 @@
         <f>SUM(C20*3)+D20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -6485,6 +6624,7 @@
         <f>SUM(C24*3)+D24</f>
         <v>0</v>
       </c>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
@@ -6512,7 +6652,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6527,7 +6667,7 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G26">
         <f>SUM(C26*3)+D26</f>
@@ -6536,10 +6676,25 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>112</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>-9</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G4:G29" si="1">SUM(C27*3)+D27</f>
+        <f>SUM(C27*3)+D27</f>
         <v>0</v>
       </c>
     </row>
@@ -6548,7 +6703,7 @@
         <v>75</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f>SUM(C28*3)+D28</f>
         <v>0</v>
       </c>
     </row>
@@ -6557,7 +6712,7 @@
         <v>98</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f>SUM(C29*3)+D29</f>
         <v>0</v>
       </c>
     </row>
@@ -6566,7 +6721,7 @@
         <v>19</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G30:G35" si="0">SUM(C30*3)+D30</f>
         <v>0</v>
       </c>
     </row>
@@ -6617,10 +6772,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G34" xr:uid="{CCA4218F-1ABE-CF4A-906A-71EA404D2B67}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G26">
-    <sortCondition descending="1" ref="G4:G26"/>
-    <sortCondition descending="1" ref="F4:F26"/>
-    <sortCondition ref="B4:B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G29">
+    <sortCondition descending="1" ref="G3:G29"/>
+    <sortCondition descending="1" ref="F3:F29"/>
+    <sortCondition ref="B3:B29"/>
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6634,7 +6789,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BF40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6884,7 +7039,7 @@
       <c r="AY3" s="7"/>
       <c r="AZ3" s="29"/>
       <c r="BA3" s="24">
-        <f>SUM(B3:AY3)</f>
+        <f t="shared" ref="BA3:BA36" si="0">SUM(B3:AY3)</f>
         <v>14</v>
       </c>
       <c r="BB3" s="8">
@@ -6959,7 +7114,7 @@
       <c r="AY4" s="7"/>
       <c r="AZ4" s="29"/>
       <c r="BA4" s="24">
-        <f>SUM(B4:AY4)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="BB4" s="8">
@@ -7035,7 +7190,7 @@
       <c r="AY5" s="7"/>
       <c r="AZ5" s="29"/>
       <c r="BA5" s="24">
-        <f>SUM(B5:AY5)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="BB5" s="8">
@@ -7108,7 +7263,7 @@
       <c r="AY6" s="7"/>
       <c r="AZ6" s="29"/>
       <c r="BA6" s="24">
-        <f>SUM(B6:AY6)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="BB6" s="8">
@@ -7181,7 +7336,7 @@
       <c r="AY7" s="7"/>
       <c r="AZ7" s="29"/>
       <c r="BA7" s="24">
-        <f>SUM(B7:AY7)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="BB7" s="8">
@@ -7253,7 +7408,7 @@
       <c r="AY8" s="7"/>
       <c r="AZ8" s="29"/>
       <c r="BA8" s="24">
-        <f>SUM(B8:AY8)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="BB8" s="8">
@@ -7332,7 +7487,7 @@
       <c r="AY9" s="7"/>
       <c r="AZ9" s="29"/>
       <c r="BA9" s="24">
-        <f>SUM(B9:AY9)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -7396,7 +7551,7 @@
       <c r="AY10" s="7"/>
       <c r="AZ10" s="29"/>
       <c r="BA10" s="24">
-        <f>SUM(B10:AY10)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="BB10" s="8">
@@ -7474,7 +7629,7 @@
       <c r="AY11" s="7"/>
       <c r="AZ11" s="29"/>
       <c r="BA11" s="24">
-        <f>SUM(B11:AY11)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -7542,7 +7697,7 @@
       <c r="AY12" s="7"/>
       <c r="AZ12" s="29"/>
       <c r="BA12" s="24">
-        <f>SUM(B12:AY12)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="BC12" s="8">
@@ -7612,7 +7767,7 @@
       <c r="AY13" s="7"/>
       <c r="AZ13" s="29"/>
       <c r="BA13" s="24">
-        <f>SUM(B13:AY13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="BB13" s="8">
@@ -7681,7 +7836,7 @@
       <c r="AY14" s="7"/>
       <c r="AZ14" s="29"/>
       <c r="BA14" s="24">
-        <f>SUM(B14:AY14)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="BC14" s="8">
@@ -7750,7 +7905,7 @@
       <c r="AY15" s="7"/>
       <c r="AZ15" s="29"/>
       <c r="BA15" s="24">
-        <f>SUM(B15:AY15)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -7820,7 +7975,7 @@
       <c r="AY16" s="7"/>
       <c r="AZ16" s="29"/>
       <c r="BA16" s="24">
-        <f>SUM(B16:AY16)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -7886,7 +8041,7 @@
       <c r="AY17" s="7"/>
       <c r="AZ17" s="29"/>
       <c r="BA17" s="24">
-        <f>SUM(B17:AY17)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -7950,7 +8105,7 @@
       <c r="AY18" s="7"/>
       <c r="AZ18" s="29"/>
       <c r="BA18" s="24">
-        <f>SUM(B18:AY18)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="BF18" s="24"/>
@@ -8019,7 +8174,7 @@
       <c r="AY19" s="7"/>
       <c r="AZ19" s="29"/>
       <c r="BA19" s="24">
-        <f>SUM(B19:AY19)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -8087,7 +8242,7 @@
       <c r="AY20" s="7"/>
       <c r="AZ20" s="29"/>
       <c r="BA20" s="24">
-        <f>SUM(B20:AY20)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -8151,7 +8306,7 @@
       <c r="AY21" s="7"/>
       <c r="AZ21" s="29"/>
       <c r="BA21" s="24">
-        <f>SUM(B21:AY21)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="BC21" s="8">
@@ -8220,7 +8375,7 @@
       <c r="AY22" s="7"/>
       <c r="AZ22" s="29"/>
       <c r="BA22" s="24">
-        <f>SUM(B22:AY22)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -8286,7 +8441,7 @@
       <c r="AY23" s="7"/>
       <c r="AZ23" s="29"/>
       <c r="BA23" s="24">
-        <f>SUM(B23:AY23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -8350,7 +8505,7 @@
       <c r="AY24" s="7"/>
       <c r="AZ24" s="29"/>
       <c r="BA24" s="24">
-        <f>SUM(B24:AY24)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -8412,7 +8567,7 @@
       <c r="AY25" s="7"/>
       <c r="AZ25" s="29"/>
       <c r="BA25" s="24">
-        <f>SUM(B25:AY25)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -8476,7 +8631,7 @@
       <c r="AY26" s="7"/>
       <c r="AZ26" s="29"/>
       <c r="BA26" s="24">
-        <f>SUM(B26:AY26)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -8538,7 +8693,7 @@
       <c r="AY27" s="7"/>
       <c r="AZ27" s="29"/>
       <c r="BA27" s="24">
-        <f>SUM(B27:AY27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8600,7 +8755,7 @@
       <c r="AY28" s="7"/>
       <c r="AZ28" s="29"/>
       <c r="BA28" s="24">
-        <f>SUM(B28:AY28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8660,7 +8815,7 @@
       <c r="AY29" s="7"/>
       <c r="AZ29" s="29"/>
       <c r="BA29" s="24">
-        <f>SUM(B29:AY29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8720,7 +8875,7 @@
       <c r="AY30" s="7"/>
       <c r="AZ30" s="29"/>
       <c r="BA30" s="24">
-        <f>SUM(B30:AY30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8780,7 +8935,7 @@
       <c r="AY31" s="7"/>
       <c r="AZ31" s="29"/>
       <c r="BA31" s="24">
-        <f>SUM(B31:AY31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8840,7 +8995,7 @@
       <c r="AY32" s="7"/>
       <c r="AZ32" s="29"/>
       <c r="BA32" s="24">
-        <f>SUM(B32:AY32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8900,7 +9055,7 @@
       <c r="AY33" s="7"/>
       <c r="AZ33" s="29"/>
       <c r="BA33" s="24">
-        <f>SUM(B33:AY33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8960,7 +9115,7 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="29"/>
       <c r="BA34" s="24">
-        <f>SUM(B34:AY34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9020,7 +9175,7 @@
       <c r="AY35" s="7"/>
       <c r="AZ35" s="29"/>
       <c r="BA35" s="24">
-        <f>SUM(B35:AY35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9078,7 +9233,7 @@
       <c r="AY36" s="7"/>
       <c r="AZ36" s="29"/>
       <c r="BA36" s="24">
-        <f>SUM(B36:AY36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9087,191 +9242,191 @@
         <v>43</v>
       </c>
       <c r="B38">
-        <f>'League Table'!B38</f>
+        <f>'League Table'!B39</f>
         <v>16</v>
       </c>
       <c r="C38">
-        <f>'League Table'!C38</f>
+        <f>'League Table'!C39</f>
         <v>20</v>
       </c>
       <c r="D38">
-        <f>'League Table'!D38</f>
+        <f>'League Table'!D39</f>
         <v>15</v>
       </c>
       <c r="E38">
-        <f>'League Table'!E38</f>
+        <f>'League Table'!E39</f>
         <v>13</v>
       </c>
       <c r="F38">
-        <f>'League Table'!F38</f>
+        <f>'League Table'!F39</f>
         <v>17</v>
       </c>
       <c r="G38">
-        <f>'League Table'!G38</f>
+        <f>'League Table'!G39</f>
         <v>18</v>
       </c>
       <c r="H38">
-        <f>'League Table'!H38</f>
+        <f>'League Table'!H39</f>
         <v>0</v>
       </c>
       <c r="I38">
-        <f>'League Table'!I38</f>
+        <f>'League Table'!I39</f>
         <v>12</v>
       </c>
       <c r="J38">
-        <f>'League Table'!J38</f>
+        <f>'League Table'!J39</f>
         <v>12</v>
       </c>
       <c r="K38">
-        <f>'League Table'!K38</f>
+        <f>'League Table'!K39</f>
         <v>12</v>
       </c>
       <c r="L38">
-        <f>'League Table'!L38</f>
+        <f>'League Table'!L39</f>
         <v>14</v>
       </c>
       <c r="M38">
-        <f>'League Table'!M38</f>
+        <f>'League Table'!M39</f>
         <v>17</v>
       </c>
       <c r="N38">
-        <f>'League Table'!N38</f>
+        <f>'League Table'!N39</f>
         <v>12</v>
       </c>
       <c r="O38">
-        <f>'League Table'!O38</f>
+        <f>'League Table'!O39</f>
         <v>14</v>
       </c>
       <c r="P38">
-        <f>'League Table'!P38</f>
+        <f>'League Table'!P39</f>
         <v>14</v>
       </c>
       <c r="Q38">
-        <f>'League Table'!Q38</f>
+        <f>'League Table'!Q39</f>
         <v>15</v>
       </c>
       <c r="R38">
-        <f>'League Table'!R38</f>
+        <f>'League Table'!R39</f>
         <v>0</v>
       </c>
       <c r="S38">
-        <f>'League Table'!S38</f>
+        <f>'League Table'!S39</f>
         <v>20</v>
       </c>
       <c r="T38">
-        <f>'League Table'!T38</f>
+        <f>'League Table'!T39</f>
         <v>18</v>
       </c>
       <c r="U38" s="32">
-        <f>'League Table'!U38</f>
+        <f>'League Table'!U39</f>
         <v>18</v>
       </c>
       <c r="V38">
-        <f>'League Table'!V38</f>
-        <v>0</v>
+        <f>'League Table'!V39</f>
+        <v>18</v>
       </c>
       <c r="W38">
-        <f>'League Table'!W38</f>
+        <f>'League Table'!W39</f>
         <v>0</v>
       </c>
       <c r="X38">
-        <f>'League Table'!X38</f>
+        <f>'League Table'!X39</f>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f>'League Table'!Y38</f>
+        <f>'League Table'!Y39</f>
         <v>0</v>
       </c>
       <c r="Z38">
-        <f>'League Table'!Z38</f>
+        <f>'League Table'!Z39</f>
         <v>0</v>
       </c>
       <c r="AA38">
-        <f>'League Table'!AA38</f>
+        <f>'League Table'!AA39</f>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f>'League Table'!AB38</f>
+        <f>'League Table'!AB39</f>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f>'League Table'!AC38</f>
+        <f>'League Table'!AC39</f>
         <v>0</v>
       </c>
       <c r="AD38">
-        <f>'League Table'!AD38</f>
+        <f>'League Table'!AD39</f>
         <v>0</v>
       </c>
       <c r="AE38">
-        <f>'League Table'!AE38</f>
+        <f>'League Table'!AE39</f>
         <v>0</v>
       </c>
       <c r="AF38">
-        <f>'League Table'!AF38</f>
+        <f>'League Table'!AF39</f>
         <v>0</v>
       </c>
       <c r="AG38" s="8">
-        <f>'League Table'!AG38</f>
+        <f>'League Table'!AG39</f>
         <v>0</v>
       </c>
       <c r="AH38" s="8">
-        <f>'League Table'!AH38</f>
+        <f>'League Table'!AH39</f>
         <v>0</v>
       </c>
       <c r="AI38" s="8">
-        <f>'League Table'!AI38</f>
+        <f>'League Table'!AI39</f>
         <v>0</v>
       </c>
       <c r="AJ38" s="8">
-        <f>'League Table'!AJ38</f>
+        <f>'League Table'!AJ39</f>
         <v>0</v>
       </c>
       <c r="AK38" s="8">
-        <f>'League Table'!AK38</f>
+        <f>'League Table'!AK39</f>
         <v>0</v>
       </c>
       <c r="AL38" s="8">
-        <f>'League Table'!AL38</f>
+        <f>'League Table'!AL39</f>
         <v>0</v>
       </c>
       <c r="AM38" s="8">
-        <f>'League Table'!AM38</f>
+        <f>'League Table'!AM39</f>
         <v>0</v>
       </c>
       <c r="AN38" s="8">
-        <f>'League Table'!AN38</f>
+        <f>'League Table'!AN39</f>
         <v>0</v>
       </c>
       <c r="AO38" s="8">
-        <f>'League Table'!AO38</f>
+        <f>'League Table'!AO39</f>
         <v>0</v>
       </c>
       <c r="AP38" s="8">
-        <f>'League Table'!AP38</f>
+        <f>'League Table'!AP39</f>
         <v>0</v>
       </c>
       <c r="AQ38" s="8">
-        <f>'League Table'!AQ38</f>
+        <f>'League Table'!AQ39</f>
         <v>0</v>
       </c>
       <c r="AR38" s="8">
-        <f>'League Table'!AZ38</f>
+        <f>'League Table'!AZ39</f>
         <v>0</v>
       </c>
       <c r="AS38" s="8">
-        <f>'League Table'!BA38</f>
+        <f>'League Table'!BA39</f>
         <v>0</v>
       </c>
       <c r="AT38" s="8">
-        <f>'League Table'!BB38</f>
+        <f>'League Table'!BB39</f>
         <v>0</v>
       </c>
       <c r="AU38" s="8">
-        <f>'League Table'!BC38</f>
+        <f>'League Table'!BC39</f>
         <v>0</v>
       </c>
       <c r="AV38" s="8">
-        <f>'League Table'!BD38</f>
+        <f>'League Table'!BD39</f>
         <v>0</v>
       </c>
       <c r="AW38" s="8"/>
@@ -9284,191 +9439,191 @@
         <v>63</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:AV40" si="0">SUM(B3:B36)</f>
+        <f t="shared" ref="B40:AV40" si="1">SUM(B3:B36)</f>
         <v>8</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="O40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="P40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U40" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA40" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB40" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9808,7 +9963,7 @@
       <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
       <c r="BA5">
-        <f>SUM(B5:AY5)</f>
+        <f t="shared" ref="BA5:BA38" si="0">SUM(B5:AY5)</f>
         <v>17</v>
       </c>
     </row>
@@ -9883,7 +10038,7 @@
       <c r="AX6" s="18"/>
       <c r="AY6" s="18"/>
       <c r="BA6">
-        <f>SUM(B6:AY6)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
@@ -9956,7 +10111,7 @@
       <c r="AX7" s="16"/>
       <c r="AY7" s="16"/>
       <c r="BA7">
-        <f>SUM(B7:AY7)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -10027,7 +10182,7 @@
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="BA8">
-        <f>SUM(B8:AY8)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -10094,7 +10249,7 @@
       <c r="AX9" s="19"/>
       <c r="AY9" s="19"/>
       <c r="BA9">
-        <f>SUM(B9:AY9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -10161,7 +10316,7 @@
       <c r="AX10" s="16"/>
       <c r="AY10" s="16"/>
       <c r="BA10">
-        <f>SUM(B10:AY10)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -10228,7 +10383,7 @@
       <c r="AX11" s="7"/>
       <c r="AY11" s="7"/>
       <c r="BA11">
-        <f>SUM(B11:AY11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -10295,7 +10450,7 @@
       <c r="AX12" s="16"/>
       <c r="AY12" s="16"/>
       <c r="BA12">
-        <f>SUM(B12:AY12)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -10358,7 +10513,7 @@
       <c r="AX13" s="7"/>
       <c r="AY13" s="7"/>
       <c r="BA13">
-        <f>SUM(B13:AY13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -10425,7 +10580,7 @@
       <c r="AX14" s="7"/>
       <c r="AY14" s="7"/>
       <c r="BA14">
-        <f>SUM(B14:AY14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -10490,7 +10645,7 @@
       <c r="AX15" s="7"/>
       <c r="AY15" s="7"/>
       <c r="BA15">
-        <f>SUM(B15:AY15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -10555,7 +10710,7 @@
       <c r="AX16" s="7"/>
       <c r="AY16" s="7"/>
       <c r="BA16">
-        <f>SUM(B16:AY16)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -10620,7 +10775,7 @@
       <c r="AX17" s="7"/>
       <c r="AY17" s="7"/>
       <c r="BA17">
-        <f>SUM(B17:AY17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -10685,7 +10840,7 @@
       <c r="AX18" s="7"/>
       <c r="AY18" s="7"/>
       <c r="BA18">
-        <f>SUM(B18:AY18)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -10748,7 +10903,7 @@
       <c r="AX19" s="7"/>
       <c r="AY19" s="7"/>
       <c r="BA19">
-        <f>SUM(B19:AY19)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -10809,7 +10964,7 @@
       <c r="AX20" s="7"/>
       <c r="AY20" s="7"/>
       <c r="BA20">
-        <f>SUM(B20:AY20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -10870,7 +11025,7 @@
       <c r="AX21" s="7"/>
       <c r="AY21" s="7"/>
       <c r="BA21">
-        <f>SUM(B21:AY21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -10931,7 +11086,7 @@
       <c r="AX22" s="7"/>
       <c r="AY22" s="7"/>
       <c r="BA22">
-        <f>SUM(B22:AY22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -10992,7 +11147,7 @@
       <c r="AX23" s="7"/>
       <c r="AY23" s="7"/>
       <c r="BA23">
-        <f>SUM(B23:AY23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11053,7 +11208,7 @@
       <c r="AX24" s="7"/>
       <c r="AY24" s="7"/>
       <c r="BA24">
-        <f>SUM(B24:AY24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11114,7 +11269,7 @@
       <c r="AX25" s="7"/>
       <c r="AY25" s="7"/>
       <c r="BA25">
-        <f>SUM(B25:AY25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11175,7 +11330,7 @@
       <c r="AX26" s="7"/>
       <c r="AY26" s="7"/>
       <c r="BA26">
-        <f>SUM(B26:AY26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11236,7 +11391,7 @@
       <c r="AX27" s="7"/>
       <c r="AY27" s="7"/>
       <c r="BA27">
-        <f>SUM(B27:AY27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11297,7 +11452,7 @@
       <c r="AX28" s="7"/>
       <c r="AY28" s="7"/>
       <c r="BA28">
-        <f>SUM(B28:AY28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11356,7 +11511,7 @@
       <c r="AX29" s="7"/>
       <c r="AY29" s="7"/>
       <c r="BA29">
-        <f>SUM(B29:AY29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11415,7 +11570,7 @@
       <c r="AX30" s="7"/>
       <c r="AY30" s="7"/>
       <c r="BA30">
-        <f>SUM(B30:AY30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11474,7 +11629,7 @@
       <c r="AX31" s="7"/>
       <c r="AY31" s="7"/>
       <c r="BA31">
-        <f>SUM(B31:AY31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11533,7 +11688,7 @@
       <c r="AX32" s="7"/>
       <c r="AY32" s="7"/>
       <c r="BA32">
-        <f>SUM(B32:AY32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11592,7 +11747,7 @@
       <c r="AX33" s="7"/>
       <c r="AY33" s="7"/>
       <c r="BA33">
-        <f>SUM(B33:AY33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11651,7 +11806,7 @@
       <c r="AX34" s="7"/>
       <c r="AY34" s="7"/>
       <c r="BA34">
-        <f>SUM(B34:AY34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11710,7 +11865,7 @@
       <c r="AX35" s="7"/>
       <c r="AY35" s="7"/>
       <c r="BA35">
-        <f>SUM(B35:AY35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11769,7 +11924,7 @@
       <c r="AX36" s="7"/>
       <c r="AY36" s="7"/>
       <c r="BA36">
-        <f>SUM(B36:AY36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11828,7 +11983,7 @@
       <c r="AX37" s="7"/>
       <c r="AY37" s="7"/>
       <c r="BA37">
-        <f>SUM(B37:AY37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11885,7 +12040,7 @@
       <c r="AX38" s="7"/>
       <c r="AY38" s="7"/>
       <c r="BA38">
-        <f>SUM(B38:AY38)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12000,203 +12155,203 @@
         <v>73</v>
       </c>
       <c r="B41" s="8">
-        <f t="shared" ref="B41:AH41" si="0">SUM(B5:B39)</f>
+        <f t="shared" ref="B41:AH41" si="1">SUM(B5:B39)</f>
         <v>5</v>
       </c>
       <c r="C41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="K41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="O41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Q41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="R41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="V41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI41" s="8">
-        <f t="shared" ref="AI41:AX41" si="1">SUM(AI5:AI39)</f>
+        <f t="shared" ref="AI41:AX41" si="2">SUM(AI5:AI39)</f>
         <v>0</v>
       </c>
       <c r="AJ41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AN41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AO41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AP41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AQ41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AR41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AT41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AU41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AV41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AW41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AX41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AY41" s="8">
-        <f t="shared" ref="AY41" si="2">SUM(AY5:AY39)</f>
+        <f t="shared" ref="AY41" si="3">SUM(AY5:AY39)</f>
         <v>0</v>
       </c>
       <c r="BA41">
@@ -12223,7 +12378,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12487,16 +12642,16 @@
         <v>117</v>
       </c>
       <c r="I12" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>127</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="N12" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -12527,7 +12682,7 @@
         <v>132</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N13" s="8">
         <v>3</v>
@@ -12617,16 +12772,19 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="8" t="s">
-        <v>118</v>
+        <v>123</v>
+      </c>
+      <c r="I16" s="8">
+        <v>2</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>163</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="N16" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -12647,13 +12805,13 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>168</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="N17" s="8">
         <v>2</v>
@@ -12677,13 +12835,13 @@
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>178</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="N18" s="8">
         <v>2</v>
@@ -12707,7 +12865,7 @@
         <v>117</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="N19" s="8">
         <v>2</v>
@@ -12760,7 +12918,9 @@
       <c r="H21" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="8"/>
+      <c r="K21" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="M21" s="8" t="s">
         <v>127</v>
       </c>
@@ -12792,10 +12952,18 @@
       <c r="A23" s="32">
         <v>21</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
+      <c r="B23" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>117</v>
+      </c>
       <c r="G23" s="32"/>
       <c r="H23" s="8" t="s">
         <v>182</v>
@@ -12874,7 +13042,9 @@
       <c r="E28" s="32"/>
       <c r="G28" s="32"/>
       <c r="K28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="M28" s="8" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="32">
@@ -13087,8 +13257,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M9:N20">
-    <sortCondition descending="1" ref="N9:N20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M9:N19">
+    <sortCondition descending="1" ref="N9:N19"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Update 012 Week 23
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlsmith/Desktop/Home Desktop – Carl’s iMac /Football/Season 2024 Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2B4684-417B-3F4A-9AB4-4F2F31C56A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA34B2F-81BD-984D-AB06-3F011E19831B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="3420" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6580" yWindow="4900" windowWidth="28800" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="League Table" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="199">
   <si>
     <t>WK 1</t>
   </si>
@@ -622,6 +622,21 @@
   </si>
   <si>
     <t>Drew 1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7-2</t>
+  </si>
+  <si>
+    <t>Phantom v Matt B</t>
+  </si>
+  <si>
+    <t>Lost 2-7</t>
+  </si>
+  <si>
+    <t>ZigZag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-1</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1450,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1545,22 +1560,22 @@
         <v>45060</v>
       </c>
       <c r="V2" s="46">
-        <v>45068</v>
+        <v>45067</v>
       </c>
       <c r="W2" s="46">
-        <v>45075</v>
+        <v>45074</v>
       </c>
       <c r="X2" s="46">
-        <v>45082</v>
+        <v>45081</v>
       </c>
       <c r="Y2" s="46">
-        <v>45089</v>
+        <v>45088</v>
       </c>
       <c r="Z2" s="46">
-        <v>45096</v>
+        <v>45095</v>
       </c>
       <c r="AA2" s="46">
-        <v>45103</v>
+        <v>45102</v>
       </c>
       <c r="AB2" s="46">
         <v>45110</v>
@@ -1935,7 +1950,9 @@
       <c r="W5" s="18">
         <v>0</v>
       </c>
-      <c r="X5" s="18"/>
+      <c r="X5" s="18">
+        <v>5</v>
+      </c>
       <c r="Y5" s="18"/>
       <c r="Z5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1970,11 +1987,11 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8">
         <f>COUNT(B5:AY5)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BD5" s="8">
         <f>COUNTIF($B5:$AY5, "&gt;=1")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BE5" s="8">
         <f>COUNTIF($B5:$AY5, "0")</f>
@@ -1986,43 +2003,39 @@
       </c>
       <c r="BG5" s="8">
         <f>SUM(BD5*3)+BE5</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="BH5" s="8">
         <f>SUM(B5:AY5)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="BI5" s="10">
         <f>SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.64912280701754388</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BJ5" s="10"/>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="B6" s="31">
         <v>-1</v>
       </c>
       <c r="C6" s="31">
+        <v>1</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31">
         <v>-1</v>
       </c>
-      <c r="D6" s="31">
-        <v>-9</v>
-      </c>
-      <c r="E6" s="31">
-        <v>1</v>
-      </c>
-      <c r="F6" s="57">
-        <v>1</v>
-      </c>
-      <c r="G6" s="31">
+      <c r="G6" s="57">
         <v>0</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="31">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="J6" s="31">
         <v>8</v>
@@ -2040,12 +2053,12 @@
         <v>0</v>
       </c>
       <c r="O6" s="31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P6" s="31">
         <v>2</v>
       </c>
-      <c r="Q6" s="57">
+      <c r="Q6" s="31">
         <v>3</v>
       </c>
       <c r="R6" s="52"/>
@@ -2053,14 +2066,16 @@
         <v>-2</v>
       </c>
       <c r="T6" s="31">
-        <v>-1</v>
-      </c>
-      <c r="U6" s="31">
-        <v>-4</v>
-      </c>
-      <c r="V6" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31">
+        <v>8</v>
+      </c>
       <c r="W6" s="31"/>
-      <c r="X6" s="31"/>
+      <c r="X6" s="31">
+        <v>5</v>
+      </c>
       <c r="Y6" s="31"/>
       <c r="Z6" s="31"/>
       <c r="AA6" s="31"/>
@@ -2093,7 +2108,7 @@
       </c>
       <c r="BC6" s="8">
         <f>COUNT(B6:AY6)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BD6" s="8">
         <f>COUNTIF($B6:$AY6, "&gt;=1")</f>
@@ -2105,7 +2120,7 @@
       </c>
       <c r="BF6" s="8">
         <f>COUNTIF($B6:$AY6, "&lt;0")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG6" s="8">
         <f>SUM(BD6*3)+BE6</f>
@@ -2113,22 +2128,22 @@
       </c>
       <c r="BH6" s="8">
         <f>SUM(B6:AY6)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="BI6" s="10">
         <f>SUM(BD6*3+BE6*1)/SUM(BC6*3)</f>
-        <v>0.5</v>
+        <v>0.52941176470588236</v>
       </c>
       <c r="BJ6" s="10"/>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B7" s="7">
-        <v>-1</v>
-      </c>
-      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="48">
         <v>1</v>
       </c>
       <c r="D7" s="7">
@@ -2138,50 +2153,56 @@
         <v>-1</v>
       </c>
       <c r="F7" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
       </c>
       <c r="H7" s="53"/>
-      <c r="I7" s="48">
+      <c r="I7" s="7">
         <v>-7</v>
       </c>
       <c r="J7" s="7">
-        <v>-8</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="K7" s="7"/>
       <c r="L7" s="7">
         <v>-2</v>
       </c>
       <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
+        <v>-1</v>
+      </c>
+      <c r="N7" s="48">
         <v>0</v>
       </c>
       <c r="O7" s="7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="7">
+        <v>-2</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>-3</v>
+      </c>
+      <c r="R7" s="53"/>
+      <c r="S7" s="7">
+        <v>2</v>
+      </c>
+      <c r="T7" s="7">
         <v>-1</v>
       </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7">
-        <v>1</v>
-      </c>
       <c r="U7" s="7">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="V7" s="7">
         <v>8</v>
       </c>
-      <c r="W7" s="48">
-        <v>0</v>
-      </c>
-      <c r="X7" s="7"/>
+      <c r="W7" s="7">
+        <v>0</v>
+      </c>
+      <c r="X7" s="7">
+        <v>5</v>
+      </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
@@ -2214,55 +2235,59 @@
       </c>
       <c r="BC7" s="8">
         <f>COUNT(B7:AY7)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BD7" s="8">
         <f>COUNTIF($B7:$AY7, "&gt;=1")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE7" s="8">
         <f>COUNTIF($B7:$AY7, "0")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BF7" s="8">
         <f>COUNTIF($B7:$AY7, "&lt;0")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BG7" s="8">
         <f>SUM(BD7*3)+BE7</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="BH7" s="8">
         <f>SUM(B7:AY7)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="BI7" s="10">
         <f>SUM(BD7*3+BE7*1)/SUM(BC7*3)</f>
-        <v>0.49019607843137253</v>
+        <v>0.45</v>
       </c>
       <c r="BJ7" s="10"/>
     </row>
     <row r="8" spans="1:62" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="B8" s="18">
         <v>-1</v>
       </c>
       <c r="C8" s="18">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18">
         <v>-1</v>
       </c>
-      <c r="G8" s="49">
+      <c r="D8" s="18">
+        <v>-9</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1</v>
+      </c>
+      <c r="F8" s="49">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18">
         <v>0</v>
       </c>
       <c r="H8" s="51"/>
       <c r="I8" s="18">
-        <v>-7</v>
+        <v>7</v>
       </c>
       <c r="J8" s="18">
         <v>8</v>
@@ -2280,12 +2305,12 @@
         <v>0</v>
       </c>
       <c r="O8" s="18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P8" s="18">
         <v>2</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="49">
         <v>3</v>
       </c>
       <c r="R8" s="51"/>
@@ -2293,14 +2318,16 @@
         <v>-2</v>
       </c>
       <c r="T8" s="18">
-        <v>1</v>
-      </c>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18">
-        <v>8</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="U8" s="18">
+        <v>-4</v>
+      </c>
+      <c r="V8" s="18"/>
       <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
+      <c r="X8" s="18">
+        <v>-5</v>
+      </c>
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
       <c r="AA8" s="18"/>
@@ -2333,11 +2360,11 @@
       </c>
       <c r="BC8" s="8">
         <f>COUNT(B8:AY8)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="BD8" s="8">
         <f>COUNTIF($B8:$AY8, "&gt;=1")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE8" s="8">
         <f>COUNTIF($B8:$AY8, "0")</f>
@@ -2345,30 +2372,30 @@
       </c>
       <c r="BF8" s="8">
         <f>COUNTIF($B8:$AY8, "&lt;0")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BG8" s="8">
         <f>SUM(BD8*3)+BE8</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="BH8" s="8">
         <f>SUM(B8:AY8)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="BI8" s="10">
         <f>SUM(BD8*3+BE8*1)/SUM(BC8*3)</f>
-        <v>0.5</v>
+        <v>0.47368421052631576</v>
       </c>
       <c r="BJ8" s="10"/>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="50">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="16">
         <v>1</v>
       </c>
       <c r="D9" s="16">
@@ -2378,54 +2405,52 @@
         <v>-1</v>
       </c>
       <c r="F9" s="16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G9" s="16">
         <v>0</v>
       </c>
       <c r="H9" s="54"/>
-      <c r="I9" s="16">
+      <c r="I9" s="50">
         <v>-7</v>
       </c>
       <c r="J9" s="16">
-        <v>8</v>
-      </c>
-      <c r="K9" s="16"/>
+        <v>-8</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
       <c r="L9" s="16">
         <v>-2</v>
       </c>
       <c r="M9" s="16">
+        <v>1</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0</v>
+      </c>
+      <c r="O9" s="16">
         <v>-1</v>
       </c>
-      <c r="N9" s="50">
-        <v>0</v>
-      </c>
-      <c r="O9" s="16">
-        <v>1</v>
-      </c>
-      <c r="P9" s="16">
-        <v>-2</v>
-      </c>
-      <c r="Q9" s="16">
-        <v>-3</v>
-      </c>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
       <c r="R9" s="54"/>
-      <c r="S9" s="16">
-        <v>2</v>
-      </c>
+      <c r="S9" s="16"/>
       <c r="T9" s="16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U9" s="16">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="V9" s="16">
         <v>8</v>
       </c>
-      <c r="W9" s="16">
-        <v>0</v>
-      </c>
-      <c r="X9" s="16"/>
+      <c r="W9" s="50">
+        <v>0</v>
+      </c>
+      <c r="X9" s="16">
+        <v>-5</v>
+      </c>
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
       <c r="AA9" s="16"/>
@@ -2458,7 +2483,7 @@
       </c>
       <c r="BC9" s="8">
         <f>COUNT(B9:AY9)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="BD9" s="8">
         <f>COUNTIF($B9:$AY9, "&gt;=1")</f>
@@ -2466,31 +2491,31 @@
       </c>
       <c r="BE9" s="8">
         <f>COUNTIF($B9:$AY9, "0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF9" s="8">
         <f>COUNTIF($B9:$AY9, "&lt;0")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BG9" s="8">
         <f>SUM(BD9*3)+BE9</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BH9" s="8">
         <f>SUM(B9:AY9)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BI9" s="10">
         <f>SUM(BD9*3+BE9*1)/SUM(BC9*3)</f>
-        <v>0.42105263157894735</v>
+        <v>0.46296296296296297</v>
       </c>
       <c r="BJ9" s="10"/>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="50">
+        <v>22</v>
+      </c>
+      <c r="B10" s="16">
         <v>-1</v>
       </c>
       <c r="C10" s="16">
@@ -2499,18 +2524,20 @@
       <c r="D10" s="16">
         <v>-9</v>
       </c>
-      <c r="E10" s="16">
-        <v>1</v>
-      </c>
-      <c r="F10" s="16">
+      <c r="E10" s="16"/>
+      <c r="F10" s="50">
         <v>-1</v>
       </c>
       <c r="G10" s="16">
         <v>0</v>
       </c>
       <c r="H10" s="54"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="I10" s="16">
+        <v>7</v>
+      </c>
+      <c r="J10" s="16">
+        <v>-8</v>
+      </c>
       <c r="K10" s="16">
         <v>0</v>
       </c>
@@ -2518,27 +2545,29 @@
         <v>2</v>
       </c>
       <c r="M10" s="16">
-        <v>-1</v>
-      </c>
-      <c r="N10" s="7"/>
-      <c r="O10" s="48">
-        <v>1</v>
-      </c>
-      <c r="P10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7">
+        <v>1</v>
+      </c>
+      <c r="P10" s="48">
         <v>-2</v>
       </c>
       <c r="Q10" s="7">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R10" s="54"/>
       <c r="S10" s="16">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="T10" s="16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="U10" s="16">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="V10" s="16">
         <v>8</v>
@@ -2546,7 +2575,9 @@
       <c r="W10" s="16">
         <v>0</v>
       </c>
-      <c r="X10" s="16"/>
+      <c r="X10" s="16">
+        <v>5</v>
+      </c>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="16"/>
@@ -2579,7 +2610,7 @@
       </c>
       <c r="BC10" s="8">
         <f>COUNT(B10:AY10)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BD10" s="8">
         <f>COUNTIF($B10:$AY10, "&gt;=1")</f>
@@ -2587,64 +2618,72 @@
       </c>
       <c r="BE10" s="8">
         <f>COUNTIF($B10:$AY10, "0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF10" s="8">
         <f>COUNTIF($B10:$AY10, "&lt;0")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BG10" s="8">
         <f>SUM(BD10*3)+BE10</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BH10" s="8">
         <f>SUM(B10:AY10)</f>
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="BI10" s="10">
         <f>SUM(BD10*3+BE10*1)/SUM(BC10*3)</f>
-        <v>0.47058823529411764</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="BJ10" s="10"/>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="58"/>
+        <v>106</v>
+      </c>
+      <c r="B11" s="48">
+        <v>-1</v>
+      </c>
       <c r="C11" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D11" s="7">
-        <v>9</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+        <v>-9</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-1</v>
+      </c>
       <c r="G11" s="7">
         <v>0</v>
       </c>
       <c r="H11" s="53"/>
-      <c r="I11" s="7">
-        <v>7</v>
-      </c>
-      <c r="J11" s="48">
-        <v>8</v>
-      </c>
-      <c r="K11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
       <c r="L11" s="7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="M11" s="7">
         <v>-1</v>
       </c>
       <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="O11" s="48">
+        <v>1</v>
+      </c>
       <c r="P11" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="7"/>
+        <v>-2</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>3</v>
+      </c>
       <c r="R11" s="53"/>
-      <c r="S11" s="48">
+      <c r="S11" s="7">
         <v>-2</v>
       </c>
       <c r="T11" s="7">
@@ -2653,11 +2692,15 @@
       <c r="U11" s="7">
         <v>4</v>
       </c>
-      <c r="V11" s="7"/>
+      <c r="V11" s="7">
+        <v>8</v>
+      </c>
       <c r="W11" s="7">
         <v>0</v>
       </c>
-      <c r="X11" s="7"/>
+      <c r="X11" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
@@ -2677,7 +2720,7 @@
       <c r="AO11" s="7"/>
       <c r="AP11" s="7"/>
       <c r="AQ11" s="7"/>
-      <c r="AR11" s="58"/>
+      <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
       <c r="AT11" s="7"/>
       <c r="AU11" s="7"/>
@@ -2690,7 +2733,7 @@
       </c>
       <c r="BC11" s="8">
         <f>COUNT(B11:AY11)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="BD11" s="8">
         <f>COUNTIF($B11:$AY11, "&gt;=1")</f>
@@ -2698,69 +2741,73 @@
       </c>
       <c r="BE11" s="8">
         <f>COUNTIF($B11:$AY11, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF11" s="8">
         <f>COUNTIF($B11:$AY11, "&lt;0")</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="BG11" s="8">
         <f>SUM(BD11*3)+BE11</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BH11" s="8">
         <f>SUM(B11:AY11)</f>
-        <v>27</v>
+        <v>-2</v>
       </c>
       <c r="BI11" s="10">
         <f>SUM(BD11*3+BE11*1)/SUM(BC11*3)</f>
-        <v>0.63888888888888884</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="BJ11" s="10"/>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B12" s="58"/>
       <c r="C12" s="7">
         <v>1</v>
       </c>
       <c r="D12" s="7">
         <v>9</v>
       </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="7">
         <v>0</v>
       </c>
       <c r="H12" s="53"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="7">
+        <v>7</v>
+      </c>
+      <c r="J12" s="48">
+        <v>8</v>
+      </c>
       <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="L12" s="7">
+        <v>-2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>-1</v>
+      </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="P12" s="7">
+        <v>2</v>
+      </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="53"/>
-      <c r="S12" s="7">
+      <c r="S12" s="48">
         <v>-2</v>
       </c>
-      <c r="T12" s="48">
-        <v>1</v>
-      </c>
-      <c r="U12" s="7"/>
-      <c r="V12" s="48">
-        <v>8</v>
-      </c>
+      <c r="T12" s="7">
+        <v>1</v>
+      </c>
+      <c r="U12" s="7">
+        <v>4</v>
+      </c>
+      <c r="V12" s="7"/>
       <c r="W12" s="7">
         <v>0</v>
       </c>
@@ -2784,7 +2831,7 @@
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
       <c r="AQ12" s="7"/>
-      <c r="AR12" s="7"/>
+      <c r="AR12" s="58"/>
       <c r="AS12" s="7"/>
       <c r="AT12" s="7"/>
       <c r="AU12" s="7"/>
@@ -2797,7 +2844,7 @@
       </c>
       <c r="BC12" s="8">
         <f>COUNT(B12:AY12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BD12" s="8">
         <f>COUNTIF($B12:$AY12, "&gt;=1")</f>
@@ -2809,7 +2856,7 @@
       </c>
       <c r="BF12" s="8">
         <f>COUNTIF($B12:$AY12, "&lt;0")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BG12" s="8">
         <f>SUM(BD12*3)+BE12</f>
@@ -2817,79 +2864,63 @@
       </c>
       <c r="BH12" s="8">
         <f>SUM(B12:AY12)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="BI12" s="10">
         <f>SUM(BD12*3+BE12*1)/SUM(BC12*3)</f>
-        <v>0.76666666666666672</v>
+        <v>0.63888888888888884</v>
       </c>
       <c r="BJ12" s="10"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="B13" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C13" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D13" s="7">
-        <v>-9</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="48">
-        <v>-1</v>
+        <v>9</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
       </c>
       <c r="G13" s="7">
         <v>0</v>
       </c>
       <c r="H13" s="53"/>
-      <c r="I13" s="7">
-        <v>7</v>
-      </c>
-      <c r="J13" s="7">
-        <v>-8</v>
-      </c>
-      <c r="K13" s="7">
-        <v>0</v>
-      </c>
-      <c r="L13" s="7">
-        <v>2</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
-        <v>1</v>
-      </c>
-      <c r="P13" s="48">
-        <v>-2</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>-3</v>
-      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="53"/>
       <c r="S13" s="7">
-        <v>2</v>
-      </c>
-      <c r="T13" s="7">
-        <v>-1</v>
-      </c>
-      <c r="U13" s="7">
-        <v>-4</v>
-      </c>
-      <c r="V13" s="7">
+        <v>-2</v>
+      </c>
+      <c r="T13" s="48">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7"/>
+      <c r="V13" s="48">
         <v>8</v>
       </c>
       <c r="W13" s="7">
         <v>0</v>
       </c>
-      <c r="X13" s="7"/>
+      <c r="X13" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
@@ -2922,87 +2953,95 @@
       </c>
       <c r="BC13" s="8">
         <f>COUNT(B13:AY13)</f>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="BD13" s="8">
         <f>COUNTIF($B13:$AY13, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE13" s="8">
         <f>COUNTIF($B13:$AY13, "0")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF13" s="8">
         <f>COUNTIF($B13:$AY13, "&lt;0")</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="BG13" s="8">
         <f>SUM(BD13*3)+BE13</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="BH13" s="8">
         <f>SUM(B13:AY13)</f>
-        <v>-9</v>
+        <v>15</v>
       </c>
       <c r="BI13" s="10">
         <f>SUM(BD13*3+BE13*1)/SUM(BC13*3)</f>
-        <v>0.38596491228070173</v>
+        <v>0.69696969696969702</v>
       </c>
       <c r="BJ13" s="10"/>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B14" s="7">
         <v>-1</v>
       </c>
       <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>-9</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>-1</v>
+      </c>
       <c r="G14" s="7">
         <v>0</v>
       </c>
       <c r="H14" s="53"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="48">
-        <v>-8</v>
-      </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="I14" s="7">
+        <v>7</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8</v>
+      </c>
+      <c r="K14" s="48">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>-2</v>
+      </c>
       <c r="M14" s="7">
         <v>1</v>
       </c>
       <c r="N14" s="7">
         <v>0</v>
       </c>
-      <c r="O14" s="7">
-        <v>1</v>
-      </c>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7">
-        <v>3</v>
-      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7">
+        <v>-2</v>
+      </c>
+      <c r="Q14" s="7"/>
       <c r="R14" s="53"/>
       <c r="S14" s="7">
-        <v>-2</v>
-      </c>
-      <c r="T14" s="7"/>
-      <c r="U14" s="48">
+        <v>2</v>
+      </c>
+      <c r="T14" s="48">
+        <v>-1</v>
+      </c>
+      <c r="U14" s="7">
         <v>4</v>
       </c>
       <c r="V14" s="7">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="W14" s="7">
         <v>0</v>
       </c>
-      <c r="X14" s="7"/>
+      <c r="X14" s="7">
+        <v>5</v>
+      </c>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
@@ -3035,7 +3074,7 @@
       </c>
       <c r="BC14" s="8">
         <f>COUNT(B14:AY14)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="BD14" s="8">
         <f>COUNTIF($B14:$AY14, "&gt;=1")</f>
@@ -3043,85 +3082,81 @@
       </c>
       <c r="BE14" s="8">
         <f>COUNTIF($B14:$AY14, "0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF14" s="8">
         <f>COUNTIF($B14:$AY14, "&lt;0")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BG14" s="8">
         <f>SUM(BD14*3)+BE14</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BH14" s="8">
         <f>SUM(B14:AY14)</f>
-        <v>-2</v>
+        <v>11</v>
       </c>
       <c r="BI14" s="10">
         <f>SUM(BD14*3+BE14*1)/SUM(BC14*3)</f>
-        <v>0.53846153846153844</v>
+        <v>0.43137254901960786</v>
       </c>
       <c r="BJ14" s="10"/>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B15" s="7">
         <v>-1</v>
       </c>
       <c r="C15" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>-9</v>
+      </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="7">
-        <v>-1</v>
-      </c>
+      <c r="F15" s="7"/>
       <c r="G15" s="7">
         <v>0</v>
       </c>
       <c r="H15" s="53"/>
-      <c r="I15" s="7">
-        <v>7</v>
-      </c>
-      <c r="J15" s="7">
-        <v>8</v>
-      </c>
-      <c r="K15" s="48">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7">
-        <v>-2</v>
-      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="48">
+        <v>-8</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="7">
         <v>1</v>
       </c>
       <c r="N15" s="7">
         <v>0</v>
       </c>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q15" s="7"/>
+      <c r="O15" s="7">
+        <v>1</v>
+      </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7">
+        <v>3</v>
+      </c>
       <c r="R15" s="53"/>
       <c r="S15" s="7">
-        <v>2</v>
-      </c>
-      <c r="T15" s="48">
-        <v>-1</v>
-      </c>
-      <c r="U15" s="7">
+        <v>-2</v>
+      </c>
+      <c r="T15" s="7"/>
+      <c r="U15" s="48">
         <v>4</v>
       </c>
       <c r="V15" s="7">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="W15" s="7">
         <v>0</v>
       </c>
-      <c r="X15" s="7"/>
+      <c r="X15" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
@@ -3154,85 +3189,79 @@
       </c>
       <c r="BC15" s="8">
         <f>COUNT(B15:AY15)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BD15" s="8">
         <f>COUNTIF($B15:$AY15, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE15" s="8">
         <f>COUNTIF($B15:$AY15, "0")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BF15" s="8">
         <f>COUNTIF($B15:$AY15, "&lt;0")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BG15" s="8">
         <f>SUM(BD15*3)+BE15</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="BH15" s="8">
         <f>SUM(B15:AY15)</f>
-        <v>6</v>
+        <v>-7</v>
       </c>
       <c r="BI15" s="10">
         <f>SUM(BD15*3+BE15*1)/SUM(BC15*3)</f>
-        <v>0.39583333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="BJ15" s="10"/>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B16" s="7"/>
       <c r="C16" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>9</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="48">
+        <v>1</v>
+      </c>
       <c r="F16" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="53"/>
-      <c r="I16" s="48">
-        <v>7</v>
-      </c>
-      <c r="J16" s="7">
-        <v>-8</v>
-      </c>
-      <c r="K16" s="7">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7">
+      <c r="I16" s="7">
+        <v>-7</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7">
         <v>-2</v>
       </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7">
-        <v>0</v>
-      </c>
-      <c r="O16" s="7">
-        <v>1</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7">
-        <v>3</v>
-      </c>
+      <c r="Q16" s="7"/>
       <c r="R16" s="53"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
+      <c r="S16" s="7">
+        <v>2</v>
+      </c>
+      <c r="T16" s="7">
+        <v>1</v>
+      </c>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
+      <c r="W16" s="7">
+        <v>0</v>
+      </c>
+      <c r="X16" s="48">
+        <v>5</v>
+      </c>
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
@@ -3265,44 +3294,48 @@
       </c>
       <c r="BC16" s="8">
         <f>COUNT(B16:AY16)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BD16" s="8">
         <f>COUNTIF($B16:$AY16, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE16" s="8">
         <f>COUNTIF($B16:$AY16, "0")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BF16" s="8">
         <f>COUNTIF($B16:$AY16, "&lt;0")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BG16" s="8">
         <f>SUM(BD16*3)+BE16</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BH16" s="8">
         <f>SUM(B16:AY16)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="BI16" s="10">
         <f>SUM(BD16*3+BE16*1)/SUM(BC16*3)</f>
-        <v>0.5</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="BJ16" s="10"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="B17" s="7">
+        <v>-1</v>
+      </c>
       <c r="C17" s="7">
         <v>-1</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
       <c r="F17" s="7">
         <v>-1</v>
       </c>
@@ -3310,42 +3343,44 @@
         <v>0</v>
       </c>
       <c r="H17" s="53"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7">
-        <v>8</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="48">
+      <c r="I17" s="7">
+        <v>-7</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="48">
+        <v>2</v>
+      </c>
+      <c r="M17" s="7">
         <v>1</v>
       </c>
       <c r="N17" s="7">
         <v>0</v>
       </c>
       <c r="O17" s="7">
-        <v>1</v>
-      </c>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7">
-        <v>-3</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="P17" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="7"/>
       <c r="R17" s="53"/>
-      <c r="S17" s="7">
-        <v>2</v>
-      </c>
-      <c r="T17" s="7">
-        <v>1</v>
-      </c>
-      <c r="U17" s="7">
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="48">
         <v>-4</v>
       </c>
       <c r="V17" s="7">
         <v>-8</v>
       </c>
-      <c r="W17" s="48">
-        <v>0</v>
-      </c>
-      <c r="X17" s="7"/>
+      <c r="W17" s="7">
+        <v>0</v>
+      </c>
+      <c r="X17" s="7">
+        <v>5</v>
+      </c>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
@@ -3378,7 +3413,7 @@
       </c>
       <c r="BC17" s="8">
         <f>COUNT(B17:AY17)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BD17" s="8">
         <f>COUNTIF($B17:$AY17, "&gt;=1")</f>
@@ -3386,74 +3421,76 @@
       </c>
       <c r="BE17" s="8">
         <f>COUNTIF($B17:$AY17, "0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF17" s="8">
         <f>COUNTIF($B17:$AY17, "&lt;0")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BG17" s="8">
         <f>SUM(BD17*3)+BE17</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BH17" s="8">
         <f>SUM(B17:AY17)</f>
-        <v>-4</v>
+        <v>-12</v>
       </c>
       <c r="BI17" s="10">
         <f>SUM(BD17*3+BE17*1)/SUM(BC17*3)</f>
-        <v>0.46153846153846156</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="BJ17" s="10"/>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
       <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7">
         <v>-1</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="D18" s="7">
+        <v>9</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7">
+        <v>-1</v>
+      </c>
       <c r="G18" s="7">
         <v>0</v>
       </c>
       <c r="H18" s="53"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7">
-        <v>1</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="48">
-        <v>-1</v>
+      <c r="I18" s="48">
+        <v>7</v>
+      </c>
+      <c r="J18" s="7">
+        <v>-8</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7">
+        <v>-2</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
+        <v>1</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R18" s="53"/>
-      <c r="S18" s="7">
-        <v>2</v>
-      </c>
-      <c r="T18" s="7">
-        <v>1</v>
-      </c>
-      <c r="U18" s="7">
-        <v>-4</v>
-      </c>
-      <c r="V18" s="7">
-        <v>8</v>
-      </c>
-      <c r="W18" s="7">
-        <v>0</v>
-      </c>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
@@ -3487,7 +3524,7 @@
       </c>
       <c r="BC18" s="8">
         <f>COUNT(B18:AY18)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BD18" s="8">
         <f>COUNTIF($B18:$AY18, "&gt;=1")</f>
@@ -3495,7 +3532,7 @@
       </c>
       <c r="BE18" s="8">
         <f>COUNTIF($B18:$AY18, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF18" s="8">
         <f>COUNTIF($B18:$AY18, "&lt;0")</f>
@@ -3503,48 +3540,54 @@
       </c>
       <c r="BG18" s="8">
         <f>SUM(BD18*3)+BE18</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BH18" s="8">
         <f>SUM(B18:AY18)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BI18" s="10">
         <f>SUM(BD18*3+BE18*1)/SUM(BC18*3)</f>
-        <v>0.51515151515151514</v>
+        <v>0.5</v>
       </c>
       <c r="BJ18" s="10"/>
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="48">
-        <v>1</v>
-      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="7"/>
+        <v>-1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
       <c r="H19" s="53"/>
-      <c r="I19" s="7">
-        <v>-7</v>
-      </c>
-      <c r="J19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7">
+        <v>8</v>
+      </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q19" s="7"/>
+      <c r="M19" s="48">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+      <c r="O19" s="7">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7">
+        <v>-3</v>
+      </c>
       <c r="R19" s="53"/>
       <c r="S19" s="7">
         <v>2</v>
@@ -3552,12 +3595,18 @@
       <c r="T19" s="7">
         <v>1</v>
       </c>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7">
-        <v>0</v>
-      </c>
-      <c r="X19" s="7"/>
+      <c r="U19" s="7">
+        <v>-4</v>
+      </c>
+      <c r="V19" s="7">
+        <v>-8</v>
+      </c>
+      <c r="W19" s="48">
+        <v>0</v>
+      </c>
+      <c r="X19" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
@@ -3590,7 +3639,7 @@
       </c>
       <c r="BC19" s="8">
         <f>COUNT(B19:AY19)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="BD19" s="8">
         <f>COUNTIF($B19:$AY19, "&gt;=1")</f>
@@ -3598,78 +3647,70 @@
       </c>
       <c r="BE19" s="8">
         <f>COUNTIF($B19:$AY19, "0")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF19" s="8">
         <f>COUNTIF($B19:$AY19, "&lt;0")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BG19" s="8">
         <f>SUM(BD19*3)+BE19</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="BH19" s="8">
         <f>SUM(B19:AY19)</f>
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="BI19" s="10">
         <f>SUM(BD19*3+BE19*1)/SUM(BC19*3)</f>
-        <v>0.66666666666666663</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="BJ19" s="10"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="7">
-        <v>-1</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7">
         <v>-1</v>
       </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="53"/>
-      <c r="I20" s="7">
-        <v>-7</v>
-      </c>
+      <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20" s="48">
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7">
+        <v>1</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="48">
+        <v>-1</v>
+      </c>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7">
+        <v>-3</v>
+      </c>
+      <c r="R20" s="53"/>
+      <c r="S20" s="7">
         <v>2</v>
       </c>
-      <c r="M20" s="7">
-        <v>1</v>
-      </c>
-      <c r="N20" s="7">
-        <v>0</v>
-      </c>
-      <c r="O20" s="7">
-        <v>-1</v>
-      </c>
-      <c r="P20" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="48">
+      <c r="T20" s="7">
+        <v>1</v>
+      </c>
+      <c r="U20" s="7">
         <v>-4</v>
       </c>
       <c r="V20" s="7">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="W20" s="7">
         <v>0</v>
@@ -3707,75 +3748,67 @@
       </c>
       <c r="BC20" s="8">
         <f>COUNT(B20:AY20)</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BD20" s="8">
         <f>COUNTIF($B20:$AY20, "&gt;=1")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BE20" s="8">
         <f>COUNTIF($B20:$AY20, "0")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF20" s="8">
         <f>COUNTIF($B20:$AY20, "&lt;0")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="BG20" s="8">
         <f>SUM(BD20*3)+BE20</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BH20" s="8">
         <f>SUM(B20:AY20)</f>
-        <v>-17</v>
+        <v>4</v>
       </c>
       <c r="BI20" s="10">
         <f>SUM(BD20*3+BE20*1)/SUM(BC20*3)</f>
-        <v>0.35555555555555557</v>
+        <v>0.51515151515151514</v>
       </c>
       <c r="BJ20" s="10"/>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7">
+        <v>83</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7">
+        <v>-8</v>
+      </c>
+      <c r="K21" s="48">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7">
         <v>-1</v>
       </c>
-      <c r="D21" s="7">
-        <v>-9</v>
-      </c>
-      <c r="E21" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="48">
-        <v>0</v>
-      </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="7">
-        <v>-7</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="P21" s="7">
+        <v>2</v>
+      </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="53"/>
-      <c r="S21" s="48">
+      <c r="S21" s="7">
         <v>2</v>
       </c>
-      <c r="T21" s="7">
-        <v>-1</v>
-      </c>
+      <c r="T21" s="7"/>
       <c r="U21" s="7">
         <v>4</v>
       </c>
@@ -3783,7 +3816,9 @@
       <c r="W21" s="7">
         <v>0</v>
       </c>
-      <c r="X21" s="7"/>
+      <c r="X21" s="7">
+        <v>5</v>
+      </c>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
@@ -3816,7 +3851,7 @@
       </c>
       <c r="BC21" s="8">
         <f>COUNT(B21:AY21)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BD21" s="8">
         <f>COUNTIF($B21:$AY21, "&gt;=1")</f>
@@ -3828,7 +3863,7 @@
       </c>
       <c r="BF21" s="8">
         <f>COUNTIF($B21:$AY21, "&lt;0")</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BG21" s="8">
         <f>SUM(BD21*3)+BE21</f>
@@ -3836,61 +3871,65 @@
       </c>
       <c r="BH21" s="8">
         <f>SUM(B21:AY21)</f>
-        <v>-11</v>
+        <v>4</v>
       </c>
       <c r="BI21" s="10">
         <f>SUM(BD21*3+BE21*1)/SUM(BC21*3)</f>
-        <v>0.42424242424242425</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="BJ21" s="10"/>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="58">
-        <v>1</v>
-      </c>
-      <c r="C22" s="48">
+        <v>76</v>
+      </c>
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
         <v>-1</v>
       </c>
       <c r="D22" s="7">
         <v>-9</v>
       </c>
       <c r="E22" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
       </c>
-      <c r="G22" s="7"/>
+      <c r="G22" s="48">
+        <v>0</v>
+      </c>
       <c r="H22" s="53"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7">
-        <v>-8</v>
-      </c>
+      <c r="I22" s="7">
+        <v>-7</v>
+      </c>
+      <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="7">
-        <v>2</v>
-      </c>
+      <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-      <c r="P22" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q22" s="48">
-        <v>-3</v>
-      </c>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
       <c r="R22" s="53"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
+      <c r="S22" s="48">
+        <v>2</v>
+      </c>
+      <c r="T22" s="7">
+        <v>-1</v>
+      </c>
+      <c r="U22" s="7">
+        <v>4</v>
+      </c>
       <c r="V22" s="7"/>
       <c r="W22" s="7">
         <v>0</v>
       </c>
-      <c r="X22" s="7"/>
+      <c r="X22" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="7"/>
@@ -3910,7 +3949,7 @@
       <c r="AO22" s="7"/>
       <c r="AP22" s="7"/>
       <c r="AQ22" s="7"/>
-      <c r="AR22" s="58"/>
+      <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
       <c r="AT22" s="7"/>
       <c r="AU22" s="7"/>
@@ -3918,13 +3957,12 @@
       <c r="AW22" s="7"/>
       <c r="AX22" s="7"/>
       <c r="AY22" s="7"/>
-      <c r="AZ22" s="5"/>
       <c r="BA22" s="34">
         <v>18</v>
       </c>
       <c r="BC22" s="8">
         <f>COUNT(B22:AY22)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BD22" s="8">
         <f>COUNTIF($B22:$AY22, "&gt;=1")</f>
@@ -3932,62 +3970,68 @@
       </c>
       <c r="BE22" s="8">
         <f>COUNTIF($B22:$AY22, "0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BF22" s="8">
         <f>COUNTIF($B22:$AY22, "&lt;0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BG22" s="8">
         <f>SUM(BD22*3)+BE22</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BH22" s="8">
         <f>SUM(B22:AY22)</f>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="BI22" s="10">
         <f>SUM(BD22*3+BE22*1)/SUM(BC22*3)</f>
-        <v>0.43333333333333335</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="BJ22" s="10"/>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="B23" s="58">
+        <v>1</v>
+      </c>
+      <c r="C23" s="48">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>-9</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="53"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7">
         <v>-8</v>
       </c>
-      <c r="K23" s="48">
-        <v>0</v>
-      </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7">
-        <v>-1</v>
-      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7">
+        <v>2</v>
+      </c>
+      <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="7"/>
+        <v>-2</v>
+      </c>
+      <c r="Q23" s="48">
+        <v>-3</v>
+      </c>
       <c r="R23" s="53"/>
-      <c r="S23" s="7">
-        <v>2</v>
-      </c>
+      <c r="S23" s="7"/>
       <c r="T23" s="7"/>
-      <c r="U23" s="7">
-        <v>4</v>
-      </c>
+      <c r="U23" s="7"/>
       <c r="V23" s="7"/>
       <c r="W23" s="7">
         <v>0</v>
@@ -4012,7 +4056,7 @@
       <c r="AO23" s="7"/>
       <c r="AP23" s="7"/>
       <c r="AQ23" s="7"/>
-      <c r="AR23" s="7"/>
+      <c r="AR23" s="58"/>
       <c r="AS23" s="7"/>
       <c r="AT23" s="7"/>
       <c r="AU23" s="7"/>
@@ -4020,36 +4064,37 @@
       <c r="AW23" s="7"/>
       <c r="AX23" s="7"/>
       <c r="AY23" s="7"/>
+      <c r="AZ23" s="5"/>
       <c r="BA23" s="34">
         <v>19</v>
       </c>
       <c r="BC23" s="8">
         <f>COUNT(B23:AY23)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="BD23" s="8">
         <f>COUNTIF($B23:$AY23, "&gt;=1")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BE23" s="8">
         <f>COUNTIF($B23:$AY23, "0")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF23" s="8">
         <f>COUNTIF($B23:$AY23, "&lt;0")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BG23" s="8">
         <f>SUM(BD23*3)+BE23</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BH23" s="8">
         <f>SUM(B23:AY23)</f>
-        <v>-1</v>
+        <v>-18</v>
       </c>
       <c r="BI23" s="10">
         <f>SUM(BD23*3+BE23*1)/SUM(BC23*3)</f>
-        <v>0.52380952380952384</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="BJ23" s="10"/>
     </row>
@@ -4097,7 +4142,9 @@
       </c>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
+      <c r="X24" s="48">
+        <v>-5</v>
+      </c>
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
       <c r="AA24" s="7"/>
@@ -4130,7 +4177,7 @@
       </c>
       <c r="BC24" s="8">
         <f>COUNT(B24:AY24)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BD24" s="8">
         <f>COUNTIF($B24:$AY24, "&gt;=1")</f>
@@ -4142,7 +4189,7 @@
       </c>
       <c r="BF24" s="8">
         <f>COUNTIF($B24:$AY24, "&lt;0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG24" s="8">
         <f>SUM(BD24*3)+BE24</f>
@@ -4150,17 +4197,17 @@
       </c>
       <c r="BH24" s="8">
         <f>SUM(B24:AY24)</f>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="BI24" s="10">
         <f>SUM(BD24*3+BE24*1)/SUM(BC24*3)</f>
-        <v>0.40740740740740738</v>
+        <v>0.36666666666666664</v>
       </c>
       <c r="BJ24" s="10"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -4179,20 +4226,18 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="53"/>
-      <c r="S25" s="7">
-        <v>2</v>
-      </c>
-      <c r="T25" s="7">
-        <v>-1</v>
-      </c>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7">
-        <v>8</v>
-      </c>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7">
+        <v>4</v>
+      </c>
+      <c r="V25" s="7"/>
       <c r="W25" s="7">
         <v>0</v>
       </c>
-      <c r="X25" s="7"/>
+      <c r="X25" s="7">
+        <v>5</v>
+      </c>
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="7"/>
@@ -4225,7 +4270,7 @@
       </c>
       <c r="BC25" s="8">
         <f>COUNT(B25:AY25)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BD25" s="8">
         <f>COUNTIF($B25:$AY25, "&gt;=1")</f>
@@ -4237,7 +4282,7 @@
       </c>
       <c r="BF25" s="8">
         <f>COUNTIF($B25:$AY25, "&lt;0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG25" s="8">
         <f>SUM(BD25*3)+BE25</f>
@@ -4249,30 +4294,20 @@
       </c>
       <c r="BI25" s="10">
         <f>SUM(BD25*3+BE25*1)/SUM(BC25*3)</f>
-        <v>0.58333333333333337</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="BJ25" s="10"/>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D26" s="48">
-        <v>9</v>
-      </c>
-      <c r="E26" s="7">
-        <v>-1</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="7">
-        <v>0</v>
-      </c>
+      <c r="G26" s="7"/>
       <c r="H26" s="53"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -4284,11 +4319,19 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="53"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
+      <c r="S26" s="7">
+        <v>2</v>
+      </c>
+      <c r="T26" s="7">
+        <v>-1</v>
+      </c>
       <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
+      <c r="V26" s="7">
+        <v>8</v>
+      </c>
+      <c r="W26" s="7">
+        <v>0</v>
+      </c>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
@@ -4322,7 +4365,7 @@
       </c>
       <c r="BC26" s="8">
         <f>COUNT(B26:AY26)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD26" s="8">
         <f>COUNTIF($B26:$AY26, "&gt;=1")</f>
@@ -4334,7 +4377,7 @@
       </c>
       <c r="BF26" s="8">
         <f>COUNTIF($B26:$AY26, "&lt;0")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG26" s="8">
         <f>SUM(BD26*3)+BE26</f>
@@ -4342,27 +4385,31 @@
       </c>
       <c r="BH26" s="8">
         <f>SUM(B26:AY26)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BI26" s="10">
         <f>SUM(BD26*3+BE26*1)/SUM(BC26*3)</f>
-        <v>0.46666666666666667</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="BJ26" s="10"/>
     </row>
     <row r="27" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="48">
+        <v>90</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
         <v>-1</v>
       </c>
-      <c r="F27" s="7">
-        <v>1</v>
-      </c>
+      <c r="D27" s="48">
+        <v>9</v>
+      </c>
+      <c r="E27" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="7">
         <v>0</v>
       </c>
@@ -4371,30 +4418,16 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="48">
-        <v>-1</v>
-      </c>
+      <c r="M27" s="7"/>
       <c r="N27" s="7"/>
-      <c r="O27" s="7">
-        <v>-1</v>
-      </c>
-      <c r="P27" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q27" s="7">
-        <v>3</v>
-      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
       <c r="R27" s="53"/>
-      <c r="S27" s="7">
-        <v>-2</v>
-      </c>
+      <c r="S27" s="7"/>
       <c r="T27" s="7"/>
-      <c r="U27" s="7">
-        <v>-4</v>
-      </c>
-      <c r="V27" s="7">
-        <v>-8</v>
-      </c>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
@@ -4429,7 +4462,7 @@
       </c>
       <c r="BC27" s="8">
         <f>COUNT(B27:AY27)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="BD27" s="8">
         <f>COUNTIF($B27:$AY27, "&gt;=1")</f>
@@ -4441,7 +4474,7 @@
       </c>
       <c r="BF27" s="8">
         <f>COUNTIF($B27:$AY27, "&lt;0")</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BG27" s="8">
         <f>SUM(BD27*3)+BE27</f>
@@ -4449,45 +4482,63 @@
       </c>
       <c r="BH27" s="8">
         <f>SUM(B27:AY27)</f>
-        <v>-15</v>
+        <v>8</v>
       </c>
       <c r="BI27" s="10">
         <f>SUM(BD27*3+BE27*1)/SUM(BC27*3)</f>
-        <v>0.23333333333333334</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="BJ27" s="10"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="7">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="48">
+        <v>-1</v>
+      </c>
       <c r="F28" s="7">
         <v>1</v>
       </c>
-      <c r="G28" s="7"/>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
       <c r="H28" s="53"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="M28" s="48">
+        <v>-1</v>
+      </c>
       <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
+      <c r="O28" s="7">
+        <v>-1</v>
+      </c>
+      <c r="P28" s="7">
+        <v>-2</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>3</v>
+      </c>
       <c r="R28" s="53"/>
-      <c r="S28" s="7"/>
+      <c r="S28" s="7">
+        <v>-2</v>
+      </c>
       <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
+      <c r="U28" s="7">
+        <v>-4</v>
+      </c>
+      <c r="V28" s="7">
+        <v>-8</v>
+      </c>
       <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
+      <c r="X28" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
@@ -4520,7 +4571,7 @@
       </c>
       <c r="BC28" s="8">
         <f>COUNT(B28:AY28)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="BD28" s="8">
         <f>COUNTIF($B28:$AY28, "&gt;=1")</f>
@@ -4528,35 +4579,39 @@
       </c>
       <c r="BE28" s="8">
         <f>COUNTIF($B28:$AY28, "0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF28" s="8">
         <f>COUNTIF($B28:$AY28, "&lt;0")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BG28" s="8">
         <f>SUM(BD28*3)+BE28</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BH28" s="8">
         <f>SUM(B28:AY28)</f>
-        <v>10</v>
+        <v>-20</v>
       </c>
       <c r="BI28" s="10">
         <f>SUM(BD28*3+BE28*1)/SUM(BC28*3)</f>
-        <v>1</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="BJ28" s="10"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7">
+        <v>9</v>
+      </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="53"/>
       <c r="I29" s="7"/>
@@ -4571,13 +4626,9 @@
       <c r="R29" s="53"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
-      <c r="U29" s="7">
-        <v>4</v>
-      </c>
+      <c r="U29" s="7"/>
       <c r="V29" s="7"/>
-      <c r="W29" s="7">
-        <v>0</v>
-      </c>
+      <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
@@ -4615,11 +4666,11 @@
       </c>
       <c r="BD29" s="8">
         <f>COUNTIF($B29:$AY29, "&gt;=1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE29" s="8">
         <f>COUNTIF($B29:$AY29, "0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF29" s="8">
         <f>COUNTIF($B29:$AY29, "&lt;0")</f>
@@ -4627,15 +4678,15 @@
       </c>
       <c r="BG29" s="8">
         <f>SUM(BD29*3)+BE29</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BH29" s="8">
         <f>SUM(B29:AY29)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="BI29" s="10">
         <f>SUM(BD29*3+BE29*1)/SUM(BC29*3)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="BJ29" s="10"/>
     </row>
@@ -4734,11 +4785,9 @@
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -4758,13 +4807,15 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
-      <c r="V31" s="7">
+      <c r="V31" s="48">
         <v>-8</v>
       </c>
       <c r="W31" s="7">
         <v>0</v>
       </c>
-      <c r="X31" s="7"/>
+      <c r="X31" s="7">
+        <v>5</v>
+      </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
       <c r="AA31" s="7"/>
@@ -4817,7 +4868,7 @@
       </c>
       <c r="BH31" s="8">
         <f>SUM(B31:AY31)</f>
-        <v>-7</v>
+        <v>-3</v>
       </c>
       <c r="BI31" s="10">
         <f>SUM(BD31*3+BE31*1)/SUM(BC31*3)</f>
@@ -4924,9 +4975,11 @@
     </row>
     <row r="33" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -4946,13 +4999,15 @@
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
-      <c r="V33" s="48">
+      <c r="V33" s="7">
         <v>-8</v>
       </c>
       <c r="W33" s="7">
         <v>0</v>
       </c>
-      <c r="X33" s="7"/>
+      <c r="X33" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="7"/>
@@ -4985,11 +5040,11 @@
       </c>
       <c r="BC33" s="8">
         <f>COUNT(B33:AY33)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BD33" s="8">
         <f>COUNTIF($B33:$AY33, "&gt;=1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE33" s="8">
         <f>COUNTIF($B33:$AY33, "0")</f>
@@ -4997,19 +5052,19 @@
       </c>
       <c r="BF33" s="8">
         <f>COUNTIF($B33:$AY33, "&lt;0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BG33" s="8">
         <f>SUM(BD33*3)+BE33</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BH33" s="8">
         <f>SUM(B33:AY33)</f>
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="BI33" s="10">
         <f>SUM(BD33*3+BE33*1)/SUM(BC33*3)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BJ33" s="10"/>
     </row>
@@ -5556,7 +5611,7 @@
       </c>
       <c r="X39" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y39" s="28">
         <f t="shared" si="0"/>
@@ -5738,7 +5793,12 @@
       <c r="V40" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="X40" s="8"/>
+      <c r="W40" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="X40" s="8" t="s">
+        <v>194</v>
+      </c>
       <c r="Y40" s="8"/>
       <c r="Z40" s="40"/>
       <c r="AA40" s="13"/>
@@ -6101,8 +6161,8 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G27"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6177,7 +6237,7 @@
         <v>9</v>
       </c>
       <c r="G4">
-        <f>SUM(C4*3)+D4</f>
+        <f t="shared" ref="G4:G27" si="1">SUM(C4*3)+D4</f>
         <v>6</v>
       </c>
     </row>
@@ -6201,7 +6261,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <f>SUM(C5*3)+D5</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -6225,7 +6285,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f>SUM(C6*3)+D6</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -6249,7 +6309,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>SUM(C7*3)+D7</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -6273,7 +6333,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>SUM(C8*3)+D8</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -6297,7 +6357,7 @@
         <v>9</v>
       </c>
       <c r="G9">
-        <f>SUM(C9*3)+D9</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6321,7 +6381,7 @@
         <v>8</v>
       </c>
       <c r="G10">
-        <f>SUM(C10*3)+D10</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H10" s="24"/>
@@ -6331,7 +6391,7 @@
         <v>156</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6340,13 +6400,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="G11">
-        <f>SUM(C11*3)+D11</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6358,7 +6418,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -6367,11 +6427,11 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G12">
-        <f>SUM(C12*3)+D12</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -6394,7 +6454,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUM(C13*3)+D13</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H13" s="24"/>
@@ -6419,7 +6479,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>SUM(C14*3)+D14</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6443,7 +6503,7 @@
         <v>-2</v>
       </c>
       <c r="G15">
-        <f>SUM(C15*3)+D15</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6467,7 +6527,7 @@
         <v>-4</v>
       </c>
       <c r="G16">
-        <f>SUM(C16*3)+D16</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6491,7 +6551,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUM(C17*3)+D17</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K17" s="37"/>
@@ -6516,7 +6576,7 @@
         <v>-1</v>
       </c>
       <c r="G18">
-        <f>SUM(C18*3)+D18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K18" s="37"/>
@@ -6541,7 +6601,7 @@
         <v>-2</v>
       </c>
       <c r="G19">
-        <f>SUM(C19*3)+D19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K19" s="37"/>
@@ -6566,7 +6626,7 @@
         <v>-8</v>
       </c>
       <c r="G20">
-        <f>SUM(C20*3)+D20</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K20" s="38"/>
@@ -6591,7 +6651,7 @@
         <v>-1</v>
       </c>
       <c r="G21">
-        <f>SUM(C21*3)+D21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K21" s="37"/>
@@ -6616,7 +6676,7 @@
         <v>-2</v>
       </c>
       <c r="G22">
-        <f>SUM(C22*3)+D22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K22" s="37"/>
@@ -6641,7 +6701,7 @@
         <v>-2</v>
       </c>
       <c r="G23">
-        <f>SUM(C23*3)+D23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="37"/>
@@ -6666,7 +6726,7 @@
         <v>-3</v>
       </c>
       <c r="G24">
-        <f>SUM(C24*3)+D24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K24" s="37"/>
@@ -6691,7 +6751,7 @@
         <v>-4</v>
       </c>
       <c r="G25">
-        <f>SUM(C25*3)+D25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6715,7 +6775,7 @@
         <v>-8</v>
       </c>
       <c r="G26">
-        <f>SUM(C26*3)+D26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6739,7 +6799,7 @@
         <v>-9</v>
       </c>
       <c r="G27">
-        <f>SUM(C27*3)+D27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6766,7 +6826,7 @@
         <v>19</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:G35" si="1">SUM(C30*3)+D30</f>
+        <f t="shared" ref="G30:G35" si="2">SUM(C30*3)+D30</f>
         <v>0</v>
       </c>
     </row>
@@ -6775,7 +6835,7 @@
         <v>77</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6784,7 +6844,7 @@
         <v>84</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6793,7 +6853,7 @@
         <v>101</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6802,7 +6862,7 @@
         <v>20</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6811,7 +6871,7 @@
         <v>100</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6838,7 +6898,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:BC36"/>
+      <selection pane="bottomRight" activeCell="AS24" sqref="AS24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -7354,7 +7414,9 @@
       <c r="V7" s="7">
         <v>1</v>
       </c>
-      <c r="W7" s="7"/>
+      <c r="W7" s="7">
+        <v>1</v>
+      </c>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
@@ -7386,7 +7448,7 @@
       <c r="AZ7" s="29"/>
       <c r="BA7" s="24">
         <f>SUM(B7:AY7)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB7" s="8">
         <v>1</v>
@@ -7397,36 +7459,48 @@
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
-        <v>6</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="53"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1</v>
+      </c>
       <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7">
+        <v>1</v>
+      </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="53"/>
       <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="7">
+        <v>1</v>
+      </c>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
+      <c r="W8" s="7">
+        <v>1</v>
+      </c>
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
@@ -7458,51 +7532,38 @@
       <c r="AZ8" s="29"/>
       <c r="BA8" s="24">
         <f>SUM(B8:AY8)</f>
-        <v>8</v>
-      </c>
-      <c r="BB8" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="7">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="53"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="7">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7">
-        <v>1</v>
-      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7">
-        <v>1</v>
-      </c>
-      <c r="P9" s="7">
-        <v>1</v>
-      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="53"/>
       <c r="S9" s="7"/>
-      <c r="T9" s="7">
-        <v>1</v>
-      </c>
+      <c r="T9" s="7"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
@@ -7538,6 +7599,9 @@
       <c r="BA9" s="24">
         <f>SUM(B9:AY9)</f>
         <v>8</v>
+      </c>
+      <c r="BB9" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.2">
@@ -7612,17 +7676,13 @@
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="7">
-        <v>2</v>
-      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="53"/>
       <c r="I11" s="7"/>
@@ -7630,24 +7690,22 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="7">
-        <v>1</v>
-      </c>
+      <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="7"/>
       <c r="R11" s="53"/>
-      <c r="S11" s="7">
-        <v>1</v>
-      </c>
+      <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
+      <c r="V11" s="7">
+        <v>2</v>
+      </c>
+      <c r="W11" s="7">
+        <v>3</v>
+      </c>
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
@@ -7681,10 +7739,13 @@
         <f>SUM(B11:AY11)</f>
         <v>7</v>
       </c>
+      <c r="BB11" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -7692,26 +7753,30 @@
         <v>1</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="7">
-        <v>2</v>
-      </c>
+      <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7">
-        <v>2</v>
-      </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>1</v>
+      </c>
       <c r="R12" s="53"/>
-      <c r="S12" s="7"/>
+      <c r="S12" s="7">
+        <v>1</v>
+      </c>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
@@ -7747,10 +7812,7 @@
       <c r="AZ12" s="29"/>
       <c r="BA12" s="24">
         <f>SUM(B12:AY12)</f>
-        <v>6</v>
-      </c>
-      <c r="BC12" s="8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BF12" s="24"/>
     </row>
@@ -7787,7 +7849,9 @@
       <c r="V13" s="7">
         <v>1</v>
       </c>
-      <c r="W13" s="7"/>
+      <c r="W13" s="7">
+        <v>1</v>
+      </c>
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
@@ -7819,46 +7883,42 @@
       <c r="AZ13" s="29"/>
       <c r="BA13" s="24">
         <f>SUM(B13:AY13)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
       <c r="H14" s="53"/>
       <c r="I14" s="7">
-        <v>1</v>
-      </c>
-      <c r="J14" s="7">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
-      <c r="M14" s="7">
-        <v>1</v>
-      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+      <c r="O14" s="7">
+        <v>2</v>
+      </c>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="53"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="7">
-        <v>1</v>
-      </c>
-      <c r="V14" s="7">
-        <v>1</v>
-      </c>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
@@ -7893,10 +7953,13 @@
         <f>SUM(B14:AY14)</f>
         <v>6</v>
       </c>
+      <c r="BC14" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -7905,26 +7968,32 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="53"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="I15" s="7">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
       <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
       <c r="M15" s="7">
-        <v>3</v>
-      </c>
-      <c r="N15" s="7">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="53"/>
-      <c r="S15" s="7">
-        <v>1</v>
-      </c>
+      <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="U15" s="7">
+        <v>1</v>
+      </c>
+      <c r="V15" s="7">
+        <v>1</v>
+      </c>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
@@ -7957,42 +8026,39 @@
       <c r="AZ15" s="29"/>
       <c r="BA15" s="24">
         <f>SUM(B15:AY15)</f>
-        <v>5</v>
-      </c>
-      <c r="BB15" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>3</v>
-      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="7">
-        <v>1</v>
-      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="53"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+      <c r="M16" s="7">
+        <v>3</v>
+      </c>
+      <c r="N16" s="7">
+        <v>1</v>
+      </c>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="53"/>
-      <c r="S16" s="7"/>
+      <c r="S16" s="7">
+        <v>1</v>
+      </c>
       <c r="T16" s="7"/>
-      <c r="U16" s="33"/>
+      <c r="U16" s="7"/>
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
@@ -8028,30 +8094,30 @@
         <f>SUM(B16:AY16)</f>
         <v>5</v>
       </c>
-      <c r="BC16" s="8">
+      <c r="BB16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B17" s="7"/>
       <c r="C17" s="7">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
       <c r="H17" s="53"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="7">
-        <v>1</v>
-      </c>
+      <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
@@ -8061,7 +8127,7 @@
       <c r="R17" s="53"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
+      <c r="U17" s="33"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
@@ -8095,39 +8161,48 @@
       <c r="AZ17" s="29"/>
       <c r="BA17" s="24">
         <f>SUM(B17:AY17)</f>
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="BC17" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="53"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="J18" s="7">
+        <v>1</v>
+      </c>
       <c r="K18" s="7"/>
-      <c r="L18" s="7">
-        <v>3</v>
-      </c>
+      <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="N18" s="7">
+        <v>1</v>
+      </c>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="53"/>
-      <c r="S18" s="7"/>
+      <c r="S18" s="7">
+        <v>1</v>
+      </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="7">
+        <v>1</v>
+      </c>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
@@ -8159,40 +8234,38 @@
       <c r="AZ18" s="29"/>
       <c r="BA18" s="24">
         <f>SUM(B18:AY18)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF18" s="24"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7">
-        <v>1</v>
-      </c>
+      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="53"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="7">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="7">
-        <v>1</v>
-      </c>
+      <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="53"/>
-      <c r="S19" s="7">
-        <v>1</v>
-      </c>
+      <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
@@ -8233,7 +8306,7 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
@@ -8242,14 +8315,14 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="7">
-        <v>1</v>
-      </c>
+      <c r="G20" s="7"/>
       <c r="H20" s="53"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="L20" s="7">
+        <v>3</v>
+      </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -8257,12 +8330,8 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="53"/>
       <c r="S20" s="7"/>
-      <c r="T20" s="7">
-        <v>1</v>
-      </c>
-      <c r="U20" s="7">
-        <v>1</v>
-      </c>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
@@ -8301,14 +8370,18 @@
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
       <c r="H21" s="53"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -8317,17 +8390,17 @@
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="7">
-        <v>2</v>
-      </c>
+      <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="53"/>
       <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7">
-        <v>2</v>
-      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7">
+        <v>1</v>
+      </c>
+      <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
@@ -8694,7 +8767,7 @@
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -8711,15 +8784,17 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
-      <c r="Q27" s="7">
-        <v>1</v>
-      </c>
+      <c r="Q27" s="7"/>
       <c r="R27" s="53"/>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
+      <c r="V27" s="7">
+        <v>1</v>
+      </c>
+      <c r="W27" s="7">
+        <v>2</v>
+      </c>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
@@ -8751,12 +8826,12 @@
       <c r="AZ27" s="29"/>
       <c r="BA27" s="24">
         <f>SUM(B27:AY27)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -8775,13 +8850,15 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="53"/>
-      <c r="S28" s="7">
-        <v>1</v>
-      </c>
+      <c r="S28" s="7"/>
       <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="7">
+        <v>1</v>
+      </c>
+      <c r="W28" s="7">
+        <v>1</v>
+      </c>
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
@@ -8813,12 +8890,12 @@
       <c r="AZ28" s="29"/>
       <c r="BA28" s="24">
         <f>SUM(B28:AY28)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -8835,14 +8912,14 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
+      <c r="Q29" s="7">
+        <v>1</v>
+      </c>
       <c r="R29" s="53"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
-      <c r="V29" s="7">
-        <v>1</v>
-      </c>
+      <c r="V29" s="7"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
@@ -8880,7 +8957,7 @@
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -8899,12 +8976,12 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
       <c r="R30" s="53"/>
-      <c r="S30" s="7"/>
+      <c r="S30" s="7">
+        <v>1</v>
+      </c>
       <c r="T30" s="7"/>
-      <c r="U30" s="33"/>
-      <c r="V30" s="7">
-        <v>1</v>
-      </c>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
@@ -9392,7 +9469,7 @@
       </c>
       <c r="X38">
         <f>'League Table'!X39</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y38">
         <f>'League Table'!Y39</f>
@@ -9585,7 +9662,7 @@
       </c>
       <c r="W40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X40">
         <f t="shared" si="0"/>
@@ -9709,10 +9786,10 @@
   <dimension ref="A1:BA41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:BA37"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -10026,7 +10103,7 @@
       <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
       <c r="BA5">
-        <f>SUM(B5:AY5)</f>
+        <f t="shared" ref="BA5:BA37" si="0">SUM(B5:AY5)</f>
         <v>20</v>
       </c>
     </row>
@@ -10074,7 +10151,9 @@
       <c r="W6" s="18">
         <v>1</v>
       </c>
-      <c r="X6" s="18"/>
+      <c r="X6" s="18">
+        <v>1</v>
+      </c>
       <c r="Y6" s="18"/>
       <c r="Z6" s="18"/>
       <c r="AA6" s="18"/>
@@ -10103,8 +10182,8 @@
       <c r="AX6" s="18"/>
       <c r="AY6" s="18"/>
       <c r="BA6">
-        <f>SUM(B6:AY6)</f>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
@@ -10149,7 +10228,9 @@
       </c>
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
+      <c r="X7" s="16">
+        <v>1</v>
+      </c>
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
@@ -10178,8 +10259,8 @@
       <c r="AX7" s="16"/>
       <c r="AY7" s="16"/>
       <c r="BA7">
-        <f>SUM(B7:AY7)</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -10251,7 +10332,7 @@
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="BA8">
-        <f>SUM(B8:AY8)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -10318,7 +10399,7 @@
       <c r="AX9" s="19"/>
       <c r="AY9" s="19"/>
       <c r="BA9">
-        <f>SUM(B9:AY9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -10387,7 +10468,7 @@
       <c r="AX10" s="16"/>
       <c r="AY10" s="16"/>
       <c r="BA10">
-        <f>SUM(B10:AY10)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -10454,7 +10535,7 @@
       <c r="AX11" s="7"/>
       <c r="AY11" s="7"/>
       <c r="BA11">
-        <f>SUM(B11:AY11)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -10492,7 +10573,9 @@
       </c>
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
+      <c r="X12" s="16">
+        <v>3</v>
+      </c>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
       <c r="AA12" s="16"/>
@@ -10521,8 +10604,8 @@
       <c r="AX12" s="16"/>
       <c r="AY12" s="16"/>
       <c r="BA12">
-        <f>SUM(B12:AY12)</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
@@ -10588,7 +10671,7 @@
       <c r="AX13" s="7"/>
       <c r="AY13" s="7"/>
       <c r="BA13">
-        <f>SUM(B13:AY13)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -10651,7 +10734,7 @@
       <c r="AX14" s="7"/>
       <c r="AY14" s="7"/>
       <c r="BA14">
-        <f>SUM(B14:AY14)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -10718,7 +10801,7 @@
       <c r="AX15" s="7"/>
       <c r="AY15" s="7"/>
       <c r="BA15">
-        <f>SUM(B15:AY15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -10783,7 +10866,7 @@
       <c r="AX16" s="7"/>
       <c r="AY16" s="7"/>
       <c r="BA16">
-        <f>SUM(B16:AY16)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -10848,7 +10931,7 @@
       <c r="AX17" s="7"/>
       <c r="AY17" s="7"/>
       <c r="BA17">
-        <f>SUM(B17:AY17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -10884,7 +10967,9 @@
       </c>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
+      <c r="X18" s="7">
+        <v>1</v>
+      </c>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
@@ -10913,8 +10998,8 @@
       <c r="AX18" s="7"/>
       <c r="AY18" s="7"/>
       <c r="BA18">
-        <f>SUM(B18:AY18)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.2">
@@ -10947,7 +11032,9 @@
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
+      <c r="X19" s="7">
+        <v>1</v>
+      </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
@@ -10976,8 +11063,8 @@
       <c r="AX19" s="7"/>
       <c r="AY19" s="7"/>
       <c r="BA19">
-        <f>SUM(B19:AY19)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.2">
@@ -11037,7 +11124,7 @@
       <c r="AX20" s="7"/>
       <c r="AY20" s="7"/>
       <c r="BA20">
-        <f>SUM(B20:AY20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11098,7 +11185,7 @@
       <c r="AX21" s="7"/>
       <c r="AY21" s="7"/>
       <c r="BA21">
-        <f>SUM(B21:AY21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11159,7 +11246,7 @@
       <c r="AX22" s="7"/>
       <c r="AY22" s="7"/>
       <c r="BA22">
-        <f>SUM(B22:AY22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11220,7 +11307,7 @@
       <c r="AX23" s="7"/>
       <c r="AY23" s="7"/>
       <c r="BA23">
-        <f>SUM(B23:AY23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11281,7 +11368,7 @@
       <c r="AX24" s="7"/>
       <c r="AY24" s="7"/>
       <c r="BA24">
-        <f>SUM(B24:AY24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11342,7 +11429,7 @@
       <c r="AX25" s="7"/>
       <c r="AY25" s="7"/>
       <c r="BA25">
-        <f>SUM(B25:AY25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11403,7 +11490,7 @@
       <c r="AX26" s="7"/>
       <c r="AY26" s="7"/>
       <c r="BA26">
-        <f>SUM(B26:AY26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11464,7 +11551,7 @@
       <c r="AX27" s="7"/>
       <c r="AY27" s="7"/>
       <c r="BA27">
-        <f>SUM(B27:AY27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11525,7 +11612,7 @@
       <c r="AX28" s="7"/>
       <c r="AY28" s="7"/>
       <c r="BA28">
-        <f>SUM(B28:AY28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -11584,7 +11671,7 @@
       <c r="AX29" s="7"/>
       <c r="AY29" s="7"/>
       <c r="BA29">
-        <f>SUM(B29:AY29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11614,7 +11701,9 @@
       <c r="U30" s="7"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
+      <c r="X30" s="7">
+        <v>2</v>
+      </c>
       <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
       <c r="AA30" s="7"/>
@@ -11643,8 +11732,8 @@
       <c r="AX30" s="7"/>
       <c r="AY30" s="7"/>
       <c r="BA30">
-        <f>SUM(B30:AY30)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.2">
@@ -11702,7 +11791,7 @@
       <c r="AX31" s="7"/>
       <c r="AY31" s="7"/>
       <c r="BA31">
-        <f>SUM(B31:AY31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11761,7 +11850,7 @@
       <c r="AX32" s="7"/>
       <c r="AY32" s="7"/>
       <c r="BA32">
-        <f>SUM(B32:AY32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11820,7 +11909,7 @@
       <c r="AX33" s="7"/>
       <c r="AY33" s="7"/>
       <c r="BA33">
-        <f>SUM(B33:AY33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11879,7 +11968,7 @@
       <c r="AX34" s="7"/>
       <c r="AY34" s="7"/>
       <c r="BA34">
-        <f>SUM(B34:AY34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11938,7 +12027,7 @@
       <c r="AX35" s="7"/>
       <c r="AY35" s="7"/>
       <c r="BA35">
-        <f>SUM(B35:AY35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -11997,7 +12086,7 @@
       <c r="AX36" s="7"/>
       <c r="AY36" s="7"/>
       <c r="BA36">
-        <f>SUM(B36:AY36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12056,7 +12145,7 @@
       <c r="AX37" s="7"/>
       <c r="AY37" s="7"/>
       <c r="BA37">
-        <f>SUM(B37:AY37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12113,7 +12202,7 @@
       <c r="AX38" s="7"/>
       <c r="AY38" s="7"/>
       <c r="BA38">
-        <f t="shared" ref="BA38" si="0">SUM(B38:AY38)</f>
+        <f t="shared" ref="BA38" si="1">SUM(B38:AY38)</f>
         <v>0</v>
       </c>
     </row>
@@ -12228,208 +12317,208 @@
         <v>73</v>
       </c>
       <c r="B41" s="8">
-        <f t="shared" ref="B41:AH41" si="1">SUM(B5:B39)</f>
+        <f t="shared" ref="B41:AH41" si="2">SUM(B5:B39)</f>
         <v>5</v>
       </c>
       <c r="C41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="K41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="Q41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="R41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="T41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="V41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="W41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="Y41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI41" s="8">
-        <f t="shared" ref="AI41:AX41" si="2">SUM(AI5:AI39)</f>
+        <f t="shared" ref="AI41:AX41" si="3">SUM(AI5:AI39)</f>
         <v>0</v>
       </c>
       <c r="AJ41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AL41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AN41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AR41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AS41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AT41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AU41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AV41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AW41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AX41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AY41" s="8">
-        <f t="shared" ref="AY41" si="3">SUM(AY5:AY39)</f>
+        <f t="shared" ref="AY41" si="4">SUM(AY5:AY39)</f>
         <v>0</v>
       </c>
       <c r="BA41">
         <f>SUM(B41:AZ41)</f>
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -12451,7 +12540,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12610,7 +12699,7 @@
         <v>119</v>
       </c>
       <c r="I9" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>118</v>
@@ -12622,7 +12711,7 @@
         <v>119</v>
       </c>
       <c r="N9" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -13016,7 +13105,9 @@
       <c r="H22" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="8"/>
+      <c r="K22" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="M22" s="8" t="s">
         <v>138</v>
       </c>
@@ -13075,11 +13166,22 @@
       <c r="A25" s="32">
         <v>23</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>119</v>
+      </c>
       <c r="G25" s="32"/>
+      <c r="H25" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="M25" s="8" t="s">
         <v>178</v>
@@ -13112,6 +13214,9 @@
       <c r="M27" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="N27" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="32">
@@ -13136,7 +13241,9 @@
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
       <c r="K29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="M29" s="8" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="32">

</xml_diff>

<commit_message>
Update 023 v1.3 All time stats
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlsmith/Desktop/Home Desktop – Carl’s iMac /Football/Season 2024 Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889D800B-C925-5E48-B448-606E5F05FE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0BC8D4-1008-9449-B7B1-B569B0D44266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="540" windowWidth="28800" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="1560" windowWidth="28800" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="League Table" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="216">
   <si>
     <t>WK 1</t>
   </si>
@@ -673,6 +673,21 @@
   </si>
   <si>
     <t>Matt B</t>
+  </si>
+  <si>
+    <t>Flo - Ian</t>
+  </si>
+  <si>
+    <t>Flo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5-0</t>
+  </si>
+  <si>
+    <t>Banksy - Posh</t>
+  </si>
+  <si>
+    <t>Lost 0-5</t>
   </si>
 </sst>
 </file>
@@ -1138,9 +1153,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,10 +1568,10 @@
   <dimension ref="A1:BJ74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF13" sqref="AF13"/>
+      <selection pane="bottomRight" activeCell="BA5" sqref="BA5:BA39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2073,11 +2086,15 @@
       </c>
       <c r="AC5" s="64"/>
       <c r="AD5" s="18"/>
-      <c r="AE5" s="70">
+      <c r="AE5" s="18">
         <v>-4</v>
       </c>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
+      <c r="AF5" s="47">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="18">
+        <v>5</v>
+      </c>
       <c r="AH5" s="18"/>
       <c r="AI5" s="18"/>
       <c r="AJ5" s="18"/>
@@ -2103,11 +2120,11 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8">
         <f>COUNT(B5:AY5)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="BD5" s="8">
         <f>COUNTIF($B5:$AY5, "&gt;=1")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BE5" s="8">
         <f>COUNTIF($B5:$AY5, "0")</f>
@@ -2119,21 +2136,21 @@
       </c>
       <c r="BG5" s="8">
         <f>SUM(BD5*3)+BE5</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="BH5" s="8">
         <f>SUM(B5:AY5)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="BI5" s="10">
         <f>SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.61111111111111116</v>
+        <v>0.64102564102564108</v>
       </c>
       <c r="BJ5" s="10"/>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B6" s="30">
         <v>-1</v>
@@ -2141,29 +2158,33 @@
       <c r="C6" s="30">
         <v>1</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="30">
+        <v>9</v>
+      </c>
+      <c r="E6" s="30">
+        <v>-1</v>
+      </c>
       <c r="F6" s="30">
-        <v>-1</v>
-      </c>
-      <c r="G6" s="55">
+        <v>1</v>
+      </c>
+      <c r="G6" s="30">
         <v>0</v>
       </c>
       <c r="H6" s="50"/>
-      <c r="I6" s="30">
+      <c r="I6" s="55">
         <v>-7</v>
       </c>
       <c r="J6" s="30">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="K6" s="30">
         <v>0</v>
       </c>
       <c r="L6" s="30">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M6" s="30">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N6" s="30">
         <v>0</v>
@@ -2171,46 +2192,46 @@
       <c r="O6" s="30">
         <v>-1</v>
       </c>
-      <c r="P6" s="30">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="30">
-        <v>3</v>
-      </c>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="50"/>
-      <c r="S6" s="30">
-        <v>-2</v>
-      </c>
+      <c r="S6" s="30"/>
       <c r="T6" s="30">
         <v>1</v>
       </c>
-      <c r="U6" s="30"/>
+      <c r="U6" s="30">
+        <v>4</v>
+      </c>
       <c r="V6" s="30">
         <v>8</v>
       </c>
-      <c r="W6" s="30"/>
+      <c r="W6" s="55">
+        <v>0</v>
+      </c>
       <c r="X6" s="30">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="Y6" s="30">
         <v>0</v>
       </c>
-      <c r="Z6" s="55">
-        <v>-2</v>
+      <c r="Z6" s="30">
+        <v>2</v>
       </c>
       <c r="AA6" s="50"/>
       <c r="AB6" s="30">
         <v>1</v>
       </c>
       <c r="AC6" s="65"/>
-      <c r="AD6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="30">
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="55">
         <v>4</v>
       </c>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
+      <c r="AF6" s="30">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="30">
+        <v>5</v>
+      </c>
       <c r="AH6" s="30"/>
       <c r="AI6" s="30"/>
       <c r="AJ6" s="30"/>
@@ -2234,11 +2255,11 @@
       </c>
       <c r="BC6" s="8">
         <f>COUNT(B6:AY6)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BD6" s="8">
         <f>COUNTIF($B6:$AY6, "&gt;=1")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BE6" s="8">
         <f>COUNTIF($B6:$AY6, "0")</f>
@@ -2250,15 +2271,15 @@
       </c>
       <c r="BG6" s="8">
         <f>SUM(BD6*3)+BE6</f>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="BH6" s="8">
         <f>SUM(B6:AY6)</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BI6" s="10">
         <f>SUM(BD6*3+BE6*1)/SUM(BC6*3)</f>
-        <v>0.53030303030303028</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="BJ6" s="10"/>
     </row>
@@ -2346,8 +2367,12 @@
       <c r="AE7" s="7">
         <v>4</v>
       </c>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
+      <c r="AF7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>-5</v>
+      </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
@@ -2371,11 +2396,11 @@
       </c>
       <c r="BC7" s="8">
         <f>COUNT(B7:AY7)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="BD7" s="8">
         <f>COUNTIF($B7:$AY7, "&gt;=1")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BE7" s="8">
         <f>COUNTIF($B7:$AY7, "0")</f>
@@ -2383,25 +2408,25 @@
       </c>
       <c r="BF7" s="8">
         <f>COUNTIF($B7:$AY7, "&lt;0")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BG7" s="8">
         <f>SUM(BD7*3)+BE7</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="BH7" s="8">
         <f>SUM(B7:AY7)</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="BI7" s="10">
         <f>SUM(BD7*3+BE7*1)/SUM(BC7*3)</f>
-        <v>0.46666666666666667</v>
+        <v>0.46913580246913578</v>
       </c>
       <c r="BJ7" s="10"/>
     </row>
     <row r="8" spans="1:62" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B8" s="18">
         <v>-1</v>
@@ -2409,33 +2434,29 @@
       <c r="C8" s="18">
         <v>1</v>
       </c>
-      <c r="D8" s="18">
-        <v>9</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18">
         <v>-1</v>
       </c>
-      <c r="F8" s="18">
-        <v>1</v>
-      </c>
-      <c r="G8" s="18">
+      <c r="G8" s="47">
         <v>0</v>
       </c>
       <c r="H8" s="49"/>
-      <c r="I8" s="47">
+      <c r="I8" s="18">
         <v>-7</v>
       </c>
       <c r="J8" s="18">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="K8" s="18">
         <v>0</v>
       </c>
       <c r="L8" s="18">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="M8" s="18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N8" s="18">
         <v>0</v>
@@ -2443,42 +2464,50 @@
       <c r="O8" s="18">
         <v>-1</v>
       </c>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="P8" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>3</v>
+      </c>
       <c r="R8" s="49"/>
-      <c r="S8" s="18"/>
+      <c r="S8" s="18">
+        <v>-2</v>
+      </c>
       <c r="T8" s="18">
         <v>1</v>
       </c>
-      <c r="U8" s="18">
-        <v>4</v>
-      </c>
+      <c r="U8" s="18"/>
       <c r="V8" s="18">
         <v>8</v>
       </c>
-      <c r="W8" s="47">
-        <v>0</v>
-      </c>
+      <c r="W8" s="18"/>
       <c r="X8" s="18">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="Y8" s="18">
         <v>0</v>
       </c>
-      <c r="Z8" s="18">
-        <v>2</v>
+      <c r="Z8" s="47">
+        <v>-2</v>
       </c>
       <c r="AA8" s="49"/>
       <c r="AB8" s="18">
         <v>1</v>
       </c>
       <c r="AC8" s="64"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="47">
+      <c r="AD8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="18">
         <v>4</v>
       </c>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
+      <c r="AF8" s="18">
+        <v>-2</v>
+      </c>
+      <c r="AG8" s="18">
+        <v>-5</v>
+      </c>
       <c r="AH8" s="18"/>
       <c r="AI8" s="18"/>
       <c r="AJ8" s="18"/>
@@ -2502,7 +2531,7 @@
       </c>
       <c r="BC8" s="8">
         <f>COUNT(B8:AY8)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BD8" s="8">
         <f>COUNTIF($B8:$AY8, "&gt;=1")</f>
@@ -2514,7 +2543,7 @@
       </c>
       <c r="BF8" s="8">
         <f>COUNTIF($B8:$AY8, "&lt;0")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BG8" s="8">
         <f>SUM(BD8*3)+BE8</f>
@@ -2522,11 +2551,11 @@
       </c>
       <c r="BH8" s="8">
         <f>SUM(B8:AY8)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="BI8" s="10">
         <f>SUM(BD8*3+BE8*1)/SUM(BC8*3)</f>
-        <v>0.53030303030303028</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="BJ8" s="10"/>
     </row>
@@ -2611,7 +2640,9 @@
       </c>
       <c r="AE9" s="16"/>
       <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
+      <c r="AG9" s="16">
+        <v>-5</v>
+      </c>
       <c r="AH9" s="16"/>
       <c r="AI9" s="16"/>
       <c r="AJ9" s="16"/>
@@ -2635,7 +2666,7 @@
       </c>
       <c r="BC9" s="8">
         <f>COUNT(B9:AY9)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BD9" s="8">
         <f>COUNTIF($B9:$AY9, "&gt;=1")</f>
@@ -2647,7 +2678,7 @@
       </c>
       <c r="BF9" s="8">
         <f>COUNTIF($B9:$AY9, "&lt;0")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BG9" s="8">
         <f>SUM(BD9*3)+BE9</f>
@@ -2655,11 +2686,11 @@
       </c>
       <c r="BH9" s="8">
         <f>SUM(B9:AY9)</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="BI9" s="10">
         <f>SUM(BD9*3+BE9*1)/SUM(BC9*3)</f>
-        <v>0.50724637681159424</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="BJ9" s="10"/>
     </row>
@@ -2731,8 +2762,12 @@
       <c r="AE10" s="16">
         <v>4</v>
       </c>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
+      <c r="AF10" s="16">
+        <v>-2</v>
+      </c>
+      <c r="AG10" s="16">
+        <v>-5</v>
+      </c>
       <c r="AH10" s="16"/>
       <c r="AI10" s="16"/>
       <c r="AJ10" s="16"/>
@@ -2756,7 +2791,7 @@
       </c>
       <c r="BC10" s="8">
         <f>COUNT(B10:AY10)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BD10" s="8">
         <f>COUNTIF($B10:$AY10, "&gt;=1")</f>
@@ -2768,7 +2803,7 @@
       </c>
       <c r="BF10" s="8">
         <f>COUNTIF($B10:$AY10, "&lt;0")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BG10" s="8">
         <f>SUM(BD10*3)+BE10</f>
@@ -2776,11 +2811,11 @@
       </c>
       <c r="BH10" s="8">
         <f>SUM(B10:AY10)</f>
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="BI10" s="10">
         <f>SUM(BD10*3+BE10*1)/SUM(BC10*3)</f>
-        <v>0.60784313725490191</v>
+        <v>0.54385964912280704</v>
       </c>
       <c r="BJ10" s="10"/>
     </row>
@@ -2850,8 +2885,12 @@
       <c r="AE11" s="7">
         <v>-4</v>
       </c>
-      <c r="AF11" s="7"/>
-      <c r="AG11" s="7"/>
+      <c r="AF11" s="7">
+        <v>-2</v>
+      </c>
+      <c r="AG11" s="7">
+        <v>5</v>
+      </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
@@ -2875,11 +2914,11 @@
       </c>
       <c r="BC11" s="8">
         <f>COUNT(B11:AY11)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="BD11" s="8">
         <f>COUNTIF($B11:$AY11, "&gt;=1")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BE11" s="8">
         <f>COUNTIF($B11:$AY11, "0")</f>
@@ -2887,25 +2926,25 @@
       </c>
       <c r="BF11" s="8">
         <f>COUNTIF($B11:$AY11, "&lt;0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG11" s="8">
         <f>SUM(BD11*3)+BE11</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="BH11" s="8">
         <f>SUM(B11:AY11)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BI11" s="10">
         <f>SUM(BD11*3+BE11*1)/SUM(BC11*3)</f>
-        <v>0.58333333333333337</v>
+        <v>0.57407407407407407</v>
       </c>
       <c r="BJ11" s="10"/>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="B12" s="7">
         <v>-1</v>
@@ -2913,11 +2952,9 @@
       <c r="C12" s="7">
         <v>-1</v>
       </c>
-      <c r="D12" s="7">
-        <v>-9</v>
-      </c>
+      <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="46">
+      <c r="F12" s="7">
         <v>-1</v>
       </c>
       <c r="G12" s="7">
@@ -2928,13 +2965,13 @@
         <v>7</v>
       </c>
       <c r="J12" s="7">
-        <v>-8</v>
-      </c>
-      <c r="K12" s="7">
+        <v>8</v>
+      </c>
+      <c r="K12" s="46">
         <v>0</v>
       </c>
       <c r="L12" s="7">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M12" s="7">
         <v>1</v>
@@ -2942,27 +2979,23 @@
       <c r="N12" s="7">
         <v>0</v>
       </c>
-      <c r="O12" s="7">
-        <v>1</v>
-      </c>
-      <c r="P12" s="46">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7">
         <v>-2</v>
       </c>
-      <c r="Q12" s="7">
-        <v>-3</v>
-      </c>
+      <c r="Q12" s="7"/>
       <c r="R12" s="51"/>
       <c r="S12" s="7">
         <v>2</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="46">
         <v>-1</v>
       </c>
       <c r="U12" s="7">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="V12" s="7">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="W12" s="7">
         <v>0</v>
@@ -2970,21 +3003,23 @@
       <c r="X12" s="7">
         <v>5</v>
       </c>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7">
-        <v>2</v>
-      </c>
+      <c r="Y12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="7"/>
       <c r="AA12" s="51"/>
-      <c r="AB12" s="46">
-        <v>-1</v>
-      </c>
+      <c r="AB12" s="7"/>
       <c r="AC12" s="66"/>
-      <c r="AD12" s="7"/>
+      <c r="AD12" s="7">
+        <v>0</v>
+      </c>
       <c r="AE12" s="7">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
+      <c r="AG12" s="7">
+        <v>5</v>
+      </c>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
       <c r="AJ12" s="7"/>
@@ -3008,7 +3043,7 @@
       </c>
       <c r="BC12" s="8">
         <f>COUNT(B12:AY12)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BD12" s="8">
         <f>COUNTIF($B12:$AY12, "&gt;=1")</f>
@@ -3016,33 +3051,31 @@
       </c>
       <c r="BE12" s="8">
         <f>COUNTIF($B12:$AY12, "0")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BF12" s="8">
         <f>COUNTIF($B12:$AY12, "&lt;0")</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BG12" s="8">
         <f>SUM(BD12*3)+BE12</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="BH12" s="8">
         <f>SUM(B12:AY12)</f>
-        <v>-7</v>
+        <v>20</v>
       </c>
       <c r="BI12" s="10">
         <f>SUM(BD12*3+BE12*1)/SUM(BC12*3)</f>
-        <v>0.40579710144927539</v>
+        <v>0.47619047619047616</v>
       </c>
       <c r="BJ12" s="10"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="7">
-        <v>-1</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="7">
         <v>-1</v>
       </c>
@@ -3055,54 +3088,52 @@
         <v>0</v>
       </c>
       <c r="H13" s="51"/>
-      <c r="I13" s="7">
-        <v>7</v>
-      </c>
+      <c r="I13" s="7"/>
       <c r="J13" s="7">
         <v>8</v>
       </c>
-      <c r="K13" s="46">
-        <v>0</v>
-      </c>
-      <c r="L13" s="7">
-        <v>-2</v>
-      </c>
-      <c r="M13" s="7">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="46">
         <v>1</v>
       </c>
       <c r="N13" s="7">
         <v>0</v>
       </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q13" s="7"/>
+      <c r="O13" s="7">
+        <v>1</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7">
+        <v>-3</v>
+      </c>
       <c r="R13" s="51"/>
       <c r="S13" s="7">
         <v>2</v>
       </c>
-      <c r="T13" s="46">
-        <v>-1</v>
+      <c r="T13" s="7">
+        <v>1</v>
       </c>
       <c r="U13" s="7">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="V13" s="7">
         <v>-8</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="46">
         <v>0</v>
       </c>
       <c r="X13" s="7">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="Y13" s="7">
         <v>0</v>
       </c>
       <c r="Z13" s="7"/>
       <c r="AA13" s="51"/>
-      <c r="AB13" s="7"/>
+      <c r="AB13" s="7">
+        <v>-1</v>
+      </c>
       <c r="AC13" s="66"/>
       <c r="AD13" s="7">
         <v>0</v>
@@ -3110,8 +3141,12 @@
       <c r="AE13" s="7">
         <v>4</v>
       </c>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
+      <c r="AF13" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="7">
+        <v>5</v>
+      </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
@@ -3139,11 +3174,11 @@
       </c>
       <c r="BD13" s="8">
         <f>COUNTIF($B13:$AY13, "&gt;=1")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE13" s="8">
         <f>COUNTIF($B13:$AY13, "0")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BF13" s="8">
         <f>COUNTIF($B13:$AY13, "&lt;0")</f>
@@ -3151,23 +3186,23 @@
       </c>
       <c r="BG13" s="8">
         <f>SUM(BD13*3)+BE13</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BH13" s="8">
         <f>SUM(B13:AY13)</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="BI13" s="10">
         <f>SUM(BD13*3+BE13*1)/SUM(BC13*3)</f>
-        <v>0.45</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="BJ13" s="10"/>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="46">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7">
         <v>-1</v>
       </c>
       <c r="C14" s="7">
@@ -3176,18 +3211,20 @@
       <c r="D14" s="7">
         <v>-9</v>
       </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14" s="7"/>
+      <c r="F14" s="46">
         <v>-1</v>
       </c>
       <c r="G14" s="7">
         <v>0</v>
       </c>
       <c r="H14" s="51"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="I14" s="7">
+        <v>7</v>
+      </c>
+      <c r="J14" s="7">
+        <v>-8</v>
+      </c>
       <c r="K14" s="7">
         <v>0</v>
       </c>
@@ -3195,27 +3232,29 @@
         <v>2</v>
       </c>
       <c r="M14" s="7">
-        <v>-1</v>
-      </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="46">
-        <v>1</v>
-      </c>
-      <c r="P14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <v>1</v>
+      </c>
+      <c r="P14" s="46">
         <v>-2</v>
       </c>
       <c r="Q14" s="7">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="R14" s="51"/>
       <c r="S14" s="7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="T14" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="U14" s="7">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="V14" s="7">
         <v>8</v>
@@ -3224,19 +3263,25 @@
         <v>0</v>
       </c>
       <c r="X14" s="7">
-        <v>-5</v>
-      </c>
-      <c r="Y14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7">
+        <v>2</v>
+      </c>
       <c r="AA14" s="51"/>
-      <c r="AB14" s="7"/>
+      <c r="AB14" s="46">
+        <v>-1</v>
+      </c>
       <c r="AC14" s="66"/>
       <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
+      <c r="AE14" s="7">
+        <v>-4</v>
+      </c>
       <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
+      <c r="AG14" s="7">
+        <v>-5</v>
+      </c>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
@@ -3260,11 +3305,11 @@
       </c>
       <c r="BC14" s="8">
         <f>COUNT(B14:AY14)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="BD14" s="8">
         <f>COUNTIF($B14:$AY14, "&gt;=1")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE14" s="8">
         <f>COUNTIF($B14:$AY14, "0")</f>
@@ -3272,19 +3317,19 @@
       </c>
       <c r="BF14" s="8">
         <f>COUNTIF($B14:$AY14, "&lt;0")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BG14" s="8">
         <f>SUM(BD14*3)+BE14</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="BH14" s="8">
         <f>SUM(B14:AY14)</f>
-        <v>-2</v>
+        <v>-12</v>
       </c>
       <c r="BI14" s="10">
         <f>SUM(BD14*3+BE14*1)/SUM(BC14*3)</f>
-        <v>0.43859649122807015</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="BJ14" s="10"/>
     </row>
@@ -3362,8 +3407,12 @@
       <c r="AE15" s="7">
         <v>-4</v>
       </c>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
+      <c r="AF15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="46">
+        <v>-5</v>
+      </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
@@ -3387,11 +3436,11 @@
       </c>
       <c r="BC15" s="8">
         <f>COUNT(B15:AY15)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BD15" s="8">
         <f>COUNTIF($B15:$AY15, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE15" s="8">
         <f>COUNTIF($B15:$AY15, "0")</f>
@@ -3399,32 +3448,38 @@
       </c>
       <c r="BF15" s="8">
         <f>COUNTIF($B15:$AY15, "&lt;0")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BG15" s="8">
         <f>SUM(BD15*3)+BE15</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="BH15" s="8">
         <f>SUM(B15:AY15)</f>
-        <v>-14</v>
+        <v>-17</v>
       </c>
       <c r="BI15" s="10">
         <f>SUM(BD15*3+BE15*1)/SUM(BC15*3)</f>
-        <v>0.4</v>
+        <v>0.40909090909090912</v>
       </c>
       <c r="BJ15" s="10"/>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="B16" s="46">
+        <v>-1</v>
+      </c>
       <c r="C16" s="7">
         <v>-1</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="7">
+        <v>-9</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
       <c r="F16" s="7">
         <v>-1</v>
       </c>
@@ -3433,38 +3488,40 @@
       </c>
       <c r="H16" s="51"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="7">
-        <v>8</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="46">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7">
-        <v>0</v>
-      </c>
-      <c r="O16" s="7">
-        <v>1</v>
-      </c>
-      <c r="P16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>2</v>
+      </c>
+      <c r="M16" s="7">
+        <v>-1</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="46">
+        <v>1</v>
+      </c>
+      <c r="P16" s="7">
+        <v>-2</v>
+      </c>
       <c r="Q16" s="7">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="R16" s="51"/>
       <c r="S16" s="7">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="T16" s="7">
         <v>1</v>
       </c>
       <c r="U16" s="7">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="V16" s="7">
-        <v>-8</v>
-      </c>
-      <c r="W16" s="46">
+        <v>8</v>
+      </c>
+      <c r="W16" s="7">
         <v>0</v>
       </c>
       <c r="X16" s="7">
@@ -3475,16 +3532,10 @@
       </c>
       <c r="Z16" s="7"/>
       <c r="AA16" s="51"/>
-      <c r="AB16" s="7">
-        <v>-1</v>
-      </c>
+      <c r="AB16" s="7"/>
       <c r="AC16" s="66"/>
-      <c r="AD16" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="7">
-        <v>4</v>
-      </c>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="7"/>
       <c r="AH16" s="7"/>
@@ -3510,68 +3561,62 @@
       </c>
       <c r="BC16" s="8">
         <f>COUNT(B16:AY16)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BD16" s="8">
         <f>COUNTIF($B16:$AY16, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE16" s="8">
         <f>COUNTIF($B16:$AY16, "0")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF16" s="8">
         <f>COUNTIF($B16:$AY16, "&lt;0")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BG16" s="8">
         <f>SUM(BD16*3)+BE16</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BH16" s="8">
         <f>SUM(B16:AY16)</f>
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="BI16" s="10">
         <f>SUM(BD16*3+BE16*1)/SUM(BC16*3)</f>
-        <v>0.42592592592592593</v>
+        <v>0.43859649122807015</v>
       </c>
       <c r="BJ16" s="10"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B17" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C17" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D17" s="7">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="7">
-        <v>-1</v>
-      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="7">
         <v>0</v>
       </c>
       <c r="H17" s="51"/>
-      <c r="I17" s="46">
-        <v>7</v>
-      </c>
-      <c r="J17" s="7">
+      <c r="I17" s="7"/>
+      <c r="J17" s="46">
         <v>-8</v>
       </c>
-      <c r="K17" s="7">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7">
-        <v>-2</v>
-      </c>
-      <c r="M17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7">
+        <v>1</v>
+      </c>
       <c r="N17" s="7">
         <v>0</v>
       </c>
@@ -3583,25 +3628,39 @@
         <v>3</v>
       </c>
       <c r="R17" s="51"/>
-      <c r="S17" s="7"/>
+      <c r="S17" s="7">
+        <v>-2</v>
+      </c>
       <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
+      <c r="U17" s="46">
+        <v>4</v>
+      </c>
+      <c r="V17" s="7">
+        <v>8</v>
+      </c>
+      <c r="W17" s="7">
+        <v>0</v>
+      </c>
+      <c r="X17" s="7">
+        <v>-5</v>
+      </c>
       <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
+      <c r="Z17" s="7">
+        <v>-2</v>
+      </c>
       <c r="AA17" s="51"/>
-      <c r="AB17" s="46">
-        <v>1</v>
-      </c>
+      <c r="AB17" s="7"/>
       <c r="AC17" s="66"/>
       <c r="AD17" s="7">
         <v>0</v>
       </c>
-      <c r="AE17" s="7"/>
+      <c r="AE17" s="46">
+        <v>-4</v>
+      </c>
       <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
+      <c r="AG17" s="7">
+        <v>5</v>
+      </c>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
@@ -3625,11 +3684,11 @@
       </c>
       <c r="BC17" s="8">
         <f>COUNT(B17:AY17)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="BD17" s="8">
         <f>COUNTIF($B17:$AY17, "&gt;=1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE17" s="8">
         <f>COUNTIF($B17:$AY17, "0")</f>
@@ -3637,83 +3696,87 @@
       </c>
       <c r="BF17" s="8">
         <f>COUNTIF($B17:$AY17, "&lt;0")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BG17" s="8">
         <f>SUM(BD17*3)+BE17</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="BH17" s="8">
         <f>SUM(B17:AY17)</f>
-        <v>10</v>
+        <v>-8</v>
       </c>
       <c r="BI17" s="10">
         <f>SUM(BD17*3+BE17*1)/SUM(BC17*3)</f>
-        <v>0.52380952380952384</v>
+        <v>0.46296296296296297</v>
       </c>
       <c r="BJ17" s="10"/>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>9</v>
+      </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
       <c r="H18" s="51"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="46">
+        <v>7</v>
+      </c>
       <c r="J18" s="7">
         <v>-8</v>
       </c>
-      <c r="K18" s="46">
-        <v>0</v>
-      </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7">
-        <v>-1</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="7"/>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7">
+        <v>-2</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
+        <v>1</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7">
+        <v>3</v>
+      </c>
       <c r="R18" s="51"/>
-      <c r="S18" s="7">
-        <v>2</v>
-      </c>
+      <c r="S18" s="7"/>
       <c r="T18" s="7"/>
-      <c r="U18" s="7">
-        <v>4</v>
-      </c>
+      <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7">
-        <v>0</v>
-      </c>
-      <c r="X18" s="7">
-        <v>5</v>
-      </c>
-      <c r="Y18" s="46">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>2</v>
-      </c>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
       <c r="AA18" s="51"/>
-      <c r="AB18" s="7">
-        <v>-1</v>
+      <c r="AB18" s="46">
+        <v>1</v>
       </c>
       <c r="AC18" s="66"/>
       <c r="AD18" s="7">
         <v>0</v>
       </c>
-      <c r="AE18" s="7">
-        <v>4</v>
-      </c>
-      <c r="AF18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7">
+        <v>-2</v>
+      </c>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
@@ -3738,7 +3801,7 @@
       </c>
       <c r="BC18" s="8">
         <f>COUNT(B18:AY18)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BD18" s="8">
         <f>COUNTIF($B18:$AY18, "&gt;=1")</f>
@@ -3750,7 +3813,7 @@
       </c>
       <c r="BF18" s="8">
         <f>COUNTIF($B18:$AY18, "&lt;0")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BG18" s="8">
         <f>SUM(BD18*3)+BE18</f>
@@ -3758,11 +3821,11 @@
       </c>
       <c r="BH18" s="8">
         <f>SUM(B18:AY18)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BI18" s="10">
         <f>SUM(BD18*3+BE18*1)/SUM(BC18*3)</f>
-        <v>0.5641025641025641</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="BJ18" s="10"/>
     </row>
@@ -3883,74 +3946,70 @@
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="7">
-        <v>-1</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <v>-9</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
+      <c r="G20" s="7"/>
       <c r="H20" s="51"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="46">
+      <c r="J20" s="7">
         <v>-8</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20" s="46">
+        <v>0</v>
+      </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7">
-        <v>1</v>
-      </c>
-      <c r="N20" s="7">
-        <v>0</v>
-      </c>
-      <c r="O20" s="7">
-        <v>1</v>
-      </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7">
-        <v>3</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="7"/>
       <c r="R20" s="51"/>
       <c r="S20" s="7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="T20" s="7"/>
-      <c r="U20" s="46">
+      <c r="U20" s="7">
         <v>4</v>
       </c>
-      <c r="V20" s="7">
-        <v>8</v>
-      </c>
+      <c r="V20" s="7"/>
       <c r="W20" s="7">
         <v>0</v>
       </c>
       <c r="X20" s="7">
-        <v>-5</v>
-      </c>
-      <c r="Y20" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="Y20" s="46">
+        <v>0</v>
+      </c>
       <c r="Z20" s="7">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="AA20" s="51"/>
-      <c r="AB20" s="7"/>
+      <c r="AB20" s="7">
+        <v>-1</v>
+      </c>
       <c r="AC20" s="66"/>
       <c r="AD20" s="7">
         <v>0</v>
       </c>
-      <c r="AE20" s="46">
-        <v>-4</v>
-      </c>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="7"/>
+      <c r="AE20" s="7">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="46">
+        <v>-2</v>
+      </c>
+      <c r="AG20" s="7">
+        <v>-5</v>
+      </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
       <c r="AJ20" s="7"/>
@@ -3974,7 +4033,7 @@
       </c>
       <c r="BC20" s="8">
         <f>COUNT(B20:AY20)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BD20" s="8">
         <f>COUNTIF($B20:$AY20, "&gt;=1")</f>
@@ -3986,7 +4045,7 @@
       </c>
       <c r="BF20" s="8">
         <f>COUNTIF($B20:$AY20, "&lt;0")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BG20" s="8">
         <f>SUM(BD20*3)+BE20</f>
@@ -3994,30 +4053,36 @@
       </c>
       <c r="BH20" s="8">
         <f>SUM(B20:AY20)</f>
-        <v>-13</v>
+        <v>2</v>
       </c>
       <c r="BI20" s="10">
         <f>SUM(BD20*3+BE20*1)/SUM(BC20*3)</f>
-        <v>0.43137254901960786</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="BJ20" s="10"/>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
       <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="46">
-        <v>1</v>
+        <v>-1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>-9</v>
+      </c>
+      <c r="E21" s="7">
+        <v>-1</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="7"/>
+      <c r="G21" s="46">
+        <v>0</v>
+      </c>
       <c r="H21" s="51"/>
       <c r="I21" s="7">
         <v>-7</v>
@@ -4028,40 +4093,46 @@
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="7">
-        <v>-2</v>
-      </c>
+      <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="51"/>
-      <c r="S21" s="7">
+      <c r="S21" s="46">
         <v>2</v>
       </c>
       <c r="T21" s="7">
-        <v>1</v>
-      </c>
-      <c r="U21" s="7"/>
+        <v>-1</v>
+      </c>
+      <c r="U21" s="7">
+        <v>4</v>
+      </c>
       <c r="V21" s="7"/>
       <c r="W21" s="7">
         <v>0</v>
       </c>
-      <c r="X21" s="46">
-        <v>5</v>
+      <c r="X21" s="7">
+        <v>-5</v>
       </c>
       <c r="Y21" s="7">
         <v>0</v>
       </c>
-      <c r="Z21" s="7"/>
+      <c r="Z21" s="7">
+        <v>-2</v>
+      </c>
       <c r="AA21" s="51"/>
       <c r="AB21" s="7">
         <v>-1</v>
       </c>
       <c r="AC21" s="66"/>
-      <c r="AD21" s="7"/>
+      <c r="AD21" s="7">
+        <v>0</v>
+      </c>
       <c r="AE21" s="7">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
+      <c r="AG21" s="46">
+        <v>5</v>
+      </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
@@ -4085,7 +4156,7 @@
       </c>
       <c r="BC21" s="8">
         <f>COUNT(B21:AY21)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="BD21" s="8">
         <f>COUNTIF($B21:$AY21, "&gt;=1")</f>
@@ -4093,48 +4164,42 @@
       </c>
       <c r="BE21" s="8">
         <f>COUNTIF($B21:$AY21, "0")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BF21" s="8">
         <f>COUNTIF($B21:$AY21, "&lt;0")</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="BG21" s="8">
         <f>SUM(BD21*3)+BE21</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BH21" s="8">
         <f>SUM(B21:AY21)</f>
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="BI21" s="10">
         <f>SUM(BD21*3+BE21*1)/SUM(BC21*3)</f>
-        <v>0.55555555555555558</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="BJ21" s="10"/>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>-9</v>
-      </c>
-      <c r="E22" s="7">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="46">
+        <v>1</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
       </c>
-      <c r="G22" s="46">
-        <v>0</v>
-      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="51"/>
       <c r="I22" s="7">
         <v>-7</v>
@@ -4145,41 +4210,37 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="P22" s="7">
+        <v>-2</v>
+      </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="51"/>
-      <c r="S22" s="46">
+      <c r="S22" s="7">
         <v>2</v>
       </c>
       <c r="T22" s="7">
-        <v>-1</v>
-      </c>
-      <c r="U22" s="7">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7">
         <v>0</v>
       </c>
-      <c r="X22" s="7">
-        <v>-5</v>
+      <c r="X22" s="46">
+        <v>5</v>
       </c>
       <c r="Y22" s="7">
         <v>0</v>
       </c>
-      <c r="Z22" s="7">
-        <v>-2</v>
-      </c>
+      <c r="Z22" s="7"/>
       <c r="AA22" s="51"/>
       <c r="AB22" s="7">
         <v>-1</v>
       </c>
       <c r="AC22" s="66"/>
-      <c r="AD22" s="7">
-        <v>0</v>
-      </c>
+      <c r="AD22" s="7"/>
       <c r="AE22" s="7">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="AF22" s="7"/>
       <c r="AG22" s="7"/>
@@ -4206,31 +4267,31 @@
       </c>
       <c r="BC22" s="8">
         <f>COUNT(B22:AY22)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="BD22" s="8">
         <f>COUNTIF($B22:$AY22, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE22" s="8">
         <f>COUNTIF($B22:$AY22, "0")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF22" s="8">
         <f>COUNTIF($B22:$AY22, "&lt;0")</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="BG22" s="8">
         <f>SUM(BD22*3)+BE22</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BH22" s="8">
         <f>SUM(B22:AY22)</f>
-        <v>-15</v>
+        <v>-3</v>
       </c>
       <c r="BI22" s="10">
         <f>SUM(BD22*3+BE22*1)/SUM(BC22*3)</f>
-        <v>0.37254901960784315</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="BJ22" s="10"/>
     </row>
@@ -4296,7 +4357,9 @@
       <c r="AE23" s="7">
         <v>-4</v>
       </c>
-      <c r="AF23" s="7"/>
+      <c r="AF23" s="7">
+        <v>2</v>
+      </c>
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
       <c r="AI23" s="7"/>
@@ -4322,11 +4385,11 @@
       </c>
       <c r="BC23" s="8">
         <f>COUNT(B23:AY23)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BD23" s="8">
         <f>COUNTIF($B23:$AY23, "&gt;=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BE23" s="8">
         <f>COUNTIF($B23:$AY23, "0")</f>
@@ -4338,15 +4401,15 @@
       </c>
       <c r="BG23" s="8">
         <f>SUM(BD23*3)+BE23</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BH23" s="8">
         <f>SUM(B23:AY23)</f>
-        <v>-23</v>
+        <v>-21</v>
       </c>
       <c r="BI23" s="10">
         <f>SUM(BD23*3+BE23*1)/SUM(BC23*3)</f>
-        <v>0.40476190476190477</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="BJ23" s="10"/>
     </row>
@@ -4606,7 +4669,9 @@
       <c r="AE26" s="7">
         <v>-4</v>
       </c>
-      <c r="AF26" s="7"/>
+      <c r="AF26" s="7">
+        <v>-2</v>
+      </c>
       <c r="AG26" s="7"/>
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
@@ -4631,7 +4696,7 @@
       </c>
       <c r="BC26" s="8">
         <f>COUNT(B26:AY26)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD26" s="8">
         <f>COUNTIF($B26:$AY26, "&gt;=1")</f>
@@ -4643,7 +4708,7 @@
       </c>
       <c r="BF26" s="8">
         <f>COUNTIF($B26:$AY26, "&lt;0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BG26" s="8">
         <f>SUM(BD26*3)+BE26</f>
@@ -4651,11 +4716,11 @@
       </c>
       <c r="BH26" s="8">
         <f>SUM(B26:AY26)</f>
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="BI26" s="10">
         <f>SUM(BD26*3+BE26*1)/SUM(BC26*3)</f>
-        <v>0.44444444444444442</v>
+        <v>0.38095238095238093</v>
       </c>
       <c r="BJ26" s="10"/>
     </row>
@@ -6010,11 +6075,11 @@
       </c>
       <c r="AF40" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AG40" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AH40" s="27">
         <f t="shared" si="1"/>
@@ -6183,8 +6248,12 @@
       <c r="AE41" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="AF41" s="13"/>
-      <c r="AG41" s="8"/>
+      <c r="AF41" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG41" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="AH41" s="13"/>
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>
@@ -6539,7 +6608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6578,7 +6647,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" s="63">
         <v>3</v>
@@ -6593,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="63">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G3" s="63">
         <f>SUM(C3*3)+D3</f>
@@ -6602,58 +6671,58 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4">
+        <v>80</v>
+      </c>
+      <c r="B4" s="70">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
+      <c r="C4" s="70">
+        <v>2</v>
+      </c>
+      <c r="D4" s="70">
+        <v>1</v>
+      </c>
+      <c r="E4" s="70">
+        <v>0</v>
+      </c>
+      <c r="F4" s="70">
+        <v>4</v>
+      </c>
+      <c r="G4" s="70">
         <f>SUM(C4*3)+D4</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f>SUM(C5*3)+D5</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B6" s="63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="63">
         <v>2</v>
@@ -6662,10 +6731,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="63">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="63">
         <f>SUM(C6*3)+D6</f>
@@ -6674,88 +6743,88 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
+        <v>99</v>
+      </c>
+      <c r="B7" s="70">
+        <v>2</v>
+      </c>
+      <c r="C7" s="70">
+        <v>2</v>
+      </c>
+      <c r="D7" s="70">
+        <v>0</v>
+      </c>
+      <c r="E7" s="70">
+        <v>0</v>
+      </c>
+      <c r="F7" s="70">
+        <v>9</v>
+      </c>
+      <c r="G7" s="70">
         <f>SUM(C7*3)+D7</f>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f>SUM(C8*3)+D8</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <f>SUM(C9*3)+D9</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -6765,7 +6834,7 @@
       </c>
       <c r="G10">
         <f>SUM(C10*3)+D10</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="23"/>
     </row>
@@ -6868,7 +6937,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>65</v>
+        <v>156</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -6883,7 +6952,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="G15">
         <f>SUM(C15*3)+D15</f>
@@ -6892,10 +6961,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>156</v>
+        <v>65</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6904,10 +6973,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="G16">
         <f>SUM(C16*3)+D16</f>
@@ -6944,7 +7013,7 @@
         <v>83</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -6953,10 +7022,10 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="G18">
         <f>SUM(C18*3)+D18</f>
@@ -7278,10 +7347,10 @@
   <dimension ref="A1:BF40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU22" sqref="AU22"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:BC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -7622,44 +7691,44 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
       <c r="H5" s="51"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
       <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
       <c r="N5" s="7">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
-      <c r="P5" s="7">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="51"/>
-      <c r="S5" s="7">
-        <v>3</v>
-      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7">
         <v>1</v>
       </c>
-      <c r="W5" s="7">
-        <v>3</v>
-      </c>
+      <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
@@ -7668,7 +7737,9 @@
       <c r="AC5" s="69"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
+      <c r="AF5" s="7">
+        <v>1</v>
+      </c>
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
@@ -7691,23 +7762,26 @@
       <c r="AZ5" s="28"/>
       <c r="BA5" s="23">
         <f>SUM(B5:AY5)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB5" s="8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="BC5" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="7">
-        <v>2</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
       <c r="G6" s="7">
         <v>2</v>
       </c>
@@ -7715,16 +7789,12 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
-        <v>4</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -7732,21 +7802,31 @@
       <c r="R6" s="51"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7">
-        <v>1</v>
-      </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
+      <c r="U6" s="7">
+        <v>2</v>
+      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7">
+        <v>1</v>
+      </c>
+      <c r="X6" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>1</v>
+      </c>
       <c r="Z6" s="7"/>
       <c r="AA6" s="51"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="69"/>
       <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
+      <c r="AE6" s="7">
+        <v>2</v>
+      </c>
       <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
+      <c r="AG6" s="7">
+        <v>1</v>
+      </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
@@ -7768,67 +7848,63 @@
       <c r="AZ6" s="28"/>
       <c r="BA6" s="23">
         <f>SUM(B6:AY6)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC6" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2</v>
-      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="51"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7">
         <v>1</v>
       </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="O7" s="7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="7">
+        <v>3</v>
+      </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="51"/>
-      <c r="S7" s="7"/>
+      <c r="S7" s="7">
+        <v>3</v>
+      </c>
       <c r="T7" s="7"/>
-      <c r="U7" s="7">
-        <v>2</v>
-      </c>
-      <c r="V7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7">
+        <v>1</v>
+      </c>
       <c r="W7" s="7">
-        <v>1</v>
-      </c>
-      <c r="X7" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="7">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="51"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="69"/>
       <c r="AD7" s="7"/>
-      <c r="AE7" s="7">
-        <v>2</v>
-      </c>
+      <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
       <c r="AG7" s="7"/>
       <c r="AH7" s="7"/>
@@ -7855,61 +7931,52 @@
         <v>13</v>
       </c>
       <c r="BB7" s="8">
-        <v>1</v>
-      </c>
-      <c r="BC7" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="51"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
-        <v>1</v>
-      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="7">
-        <v>1</v>
-      </c>
+      <c r="M8" s="7"/>
       <c r="N8" s="7">
         <v>1</v>
       </c>
-      <c r="O8" s="7">
-        <v>1</v>
-      </c>
+      <c r="O8" s="7"/>
       <c r="P8" s="7">
         <v>1</v>
       </c>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="7">
+        <v>1</v>
+      </c>
       <c r="R8" s="51"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7">
-        <v>1</v>
-      </c>
+      <c r="S8" s="7">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="7">
-        <v>1</v>
-      </c>
+      <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-      <c r="X8" s="7">
-        <v>1</v>
-      </c>
+      <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="Z8" s="7">
+        <v>2</v>
+      </c>
       <c r="AA8" s="51"/>
       <c r="AB8" s="7">
         <v>1</v>
@@ -7917,7 +7984,9 @@
       <c r="AC8" s="69"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
+      <c r="AF8" s="7">
+        <v>3</v>
+      </c>
       <c r="AG8" s="7"/>
       <c r="AH8" s="7"/>
       <c r="AI8" s="7"/>
@@ -7940,61 +8009,75 @@
       <c r="AZ8" s="28"/>
       <c r="BA8" s="23">
         <f>SUM(B8:AY8)</f>
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="BB8" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC8" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="51"/>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
+      <c r="I9" s="7"/>
       <c r="J9" s="7">
         <v>1</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
-        <v>1</v>
-      </c>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7"/>
       <c r="M9" s="7">
         <v>1</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1</v>
+      </c>
+      <c r="P9" s="7">
+        <v>1</v>
+      </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="51"/>
       <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7">
-        <v>1</v>
-      </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7">
-        <v>1</v>
-      </c>
-      <c r="X9" s="7"/>
+      <c r="T9" s="7">
+        <v>1</v>
+      </c>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7">
+        <v>1</v>
+      </c>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7">
+        <v>1</v>
+      </c>
       <c r="Y9" s="7"/>
-      <c r="Z9" s="7">
-        <v>2</v>
-      </c>
+      <c r="Z9" s="7"/>
       <c r="AA9" s="51"/>
-      <c r="AB9" s="7"/>
+      <c r="AB9" s="7">
+        <v>1</v>
+      </c>
       <c r="AC9" s="69"/>
       <c r="AD9" s="7"/>
-      <c r="AE9" s="7">
-        <v>2</v>
-      </c>
+      <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
+      <c r="AG9" s="7">
+        <v>1</v>
+      </c>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7"/>
       <c r="AJ9" s="7"/>
@@ -8016,64 +8099,59 @@
       <c r="AZ9" s="28"/>
       <c r="BA9" s="23">
         <f>SUM(B9:AY9)</f>
-        <v>10</v>
-      </c>
-      <c r="BC9" s="8">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="7">
-        <v>1</v>
-      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="7">
-        <v>2</v>
-      </c>
-      <c r="G10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
       <c r="H10" s="51"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="7">
-        <v>1</v>
-      </c>
+      <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>1</v>
-      </c>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
       <c r="R10" s="51"/>
-      <c r="S10" s="7">
-        <v>1</v>
-      </c>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7">
+        <v>1</v>
+      </c>
+      <c r="U10" s="7">
+        <v>1</v>
+      </c>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7">
-        <v>2</v>
-      </c>
+      <c r="Y10" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="7"/>
       <c r="AA10" s="51"/>
-      <c r="AB10" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB10" s="7"/>
       <c r="AC10" s="69"/>
       <c r="AD10" s="7"/>
-      <c r="AE10" s="7"/>
+      <c r="AE10" s="7">
+        <v>1</v>
+      </c>
       <c r="AF10" s="7"/>
-      <c r="AG10" s="7"/>
+      <c r="AG10" s="7">
+        <v>4</v>
+      </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="7"/>
       <c r="AJ10" s="7"/>
@@ -8097,32 +8175,34 @@
         <f>SUM(B10:AY10)</f>
         <v>10</v>
       </c>
-      <c r="BC10" s="8">
+      <c r="BB10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="51"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="I11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <v>1</v>
+      </c>
       <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <v>1</v>
+      </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -8130,19 +8210,25 @@
       <c r="R11" s="51"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
+      <c r="U11" s="7">
+        <v>1</v>
+      </c>
       <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
+      <c r="W11" s="7">
+        <v>1</v>
+      </c>
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
+      <c r="Z11" s="7">
+        <v>2</v>
+      </c>
       <c r="AA11" s="51"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="69"/>
-      <c r="AD11" s="7">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7">
+        <v>2</v>
+      </c>
       <c r="AF11" s="7"/>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
@@ -8166,22 +8252,25 @@
       <c r="AZ11" s="28"/>
       <c r="BA11" s="23">
         <f>SUM(B11:AY11)</f>
-        <v>9</v>
-      </c>
-      <c r="BB11" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="BC11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+        <v>99</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -8193,30 +8282,24 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="7">
-        <v>2</v>
-      </c>
+      <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="51"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-      <c r="W12" s="7">
-        <v>2</v>
-      </c>
-      <c r="X12" s="7">
-        <v>3</v>
-      </c>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="51"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="69"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7">
-        <v>1</v>
-      </c>
+      <c r="AD12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
@@ -8240,26 +8323,25 @@
       <c r="AZ12" s="28"/>
       <c r="BA12" s="23">
         <f>SUM(B12:AY12)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB12" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="8">
         <v>1</v>
       </c>
       <c r="BF12" s="23"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="7">
-        <v>3</v>
-      </c>
+      <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7">
-        <v>4</v>
-      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="51"/>
       <c r="I13" s="7"/>
@@ -8269,22 +8351,30 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="P13" s="7">
+        <v>2</v>
+      </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="51"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
+      <c r="W13" s="7">
+        <v>2</v>
+      </c>
+      <c r="X13" s="7">
+        <v>3</v>
+      </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="51"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="69"/>
       <c r="AD13" s="7"/>
-      <c r="AE13" s="7"/>
+      <c r="AE13" s="7">
+        <v>1</v>
+      </c>
       <c r="AF13" s="7"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
@@ -8308,41 +8398,34 @@
       <c r="AZ13" s="28"/>
       <c r="BA13" s="23">
         <f>SUM(B13:AY13)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB13" s="8">
-        <v>1</v>
-      </c>
-      <c r="BC13" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="51"/>
-      <c r="I14" s="7">
-        <v>2</v>
-      </c>
+      <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="7">
-        <v>2</v>
-      </c>
+      <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="51"/>
@@ -8355,9 +8438,7 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="51"/>
-      <c r="AB14" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB14" s="7"/>
       <c r="AC14" s="69"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
@@ -8386,51 +8467,54 @@
         <f>SUM(B14:AY14)</f>
         <v>7</v>
       </c>
+      <c r="BB14" s="8">
+        <v>1</v>
+      </c>
       <c r="BC14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>3</v>
-      </c>
-      <c r="G15" s="7"/>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
       <c r="H15" s="51"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7">
+        <v>2</v>
+      </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7">
-        <v>1</v>
-      </c>
+      <c r="O15" s="7">
+        <v>2</v>
+      </c>
+      <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="51"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
-      <c r="W15" s="7">
-        <v>1</v>
-      </c>
-      <c r="X15" s="7">
-        <v>1</v>
-      </c>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="51"/>
-      <c r="AB15" s="7"/>
+      <c r="AB15" s="7">
+        <v>1</v>
+      </c>
       <c r="AC15" s="69"/>
       <c r="AD15" s="7"/>
       <c r="AE15" s="7"/>
@@ -8459,55 +8543,54 @@
         <f>SUM(B15:AY15)</f>
         <v>7</v>
       </c>
+      <c r="BC15" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
       <c r="F16" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="51"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="7">
-        <v>1</v>
-      </c>
+      <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="7">
-        <v>1</v>
-      </c>
+      <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="P16" s="7">
+        <v>1</v>
+      </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="51"/>
-      <c r="S16" s="7">
-        <v>1</v>
-      </c>
+      <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
+      <c r="W16" s="7">
+        <v>1</v>
+      </c>
       <c r="X16" s="7">
         <v>1</v>
       </c>
-      <c r="Y16" s="7">
-        <v>1</v>
-      </c>
+      <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="51"/>
       <c r="AB16" s="7"/>
       <c r="AC16" s="69"/>
       <c r="AD16" s="7"/>
-      <c r="AE16" s="7">
-        <v>1</v>
-      </c>
+      <c r="AE16" s="7"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="7"/>
       <c r="AH16" s="7"/>
@@ -8536,22 +8619,24 @@
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="51"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="J17" s="7">
+        <v>1</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="7">
-        <v>3</v>
-      </c>
+      <c r="M17" s="7"/>
       <c r="N17" s="7">
         <v>1</v>
       </c>
@@ -8566,8 +8651,12 @@
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
+      <c r="X17" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>1</v>
+      </c>
       <c r="Z17" s="7"/>
       <c r="AA17" s="51"/>
       <c r="AB17" s="7"/>
@@ -8599,10 +8688,7 @@
       <c r="AZ17" s="28"/>
       <c r="BA17" s="23">
         <f>SUM(B17:AY17)</f>
-        <v>6</v>
-      </c>
-      <c r="BB17" s="8">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.2">
@@ -8647,7 +8733,9 @@
       <c r="AC18" s="69"/>
       <c r="AD18" s="7"/>
       <c r="AE18" s="7"/>
-      <c r="AF18" s="7"/>
+      <c r="AF18" s="7">
+        <v>1</v>
+      </c>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
@@ -8670,48 +8758,44 @@
       <c r="AZ18" s="28"/>
       <c r="BA18" s="23">
         <f>SUM(B18:AY18)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF18" s="23"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="7">
-        <v>1</v>
-      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="51"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="M19" s="7">
+        <v>3</v>
+      </c>
+      <c r="N19" s="7">
+        <v>1</v>
+      </c>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="51"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7">
-        <v>1</v>
-      </c>
-      <c r="U19" s="7">
-        <v>1</v>
-      </c>
+      <c r="S19" s="7">
+        <v>1</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
-      <c r="Y19" s="7">
-        <v>1</v>
-      </c>
+      <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="51"/>
       <c r="AB19" s="7"/>
@@ -8744,6 +8828,9 @@
       <c r="BA19" s="23">
         <f>SUM(B19:AY19)</f>
         <v>6</v>
+      </c>
+      <c r="BB19" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.2">
@@ -9846,7 +9933,7 @@
       <c r="AY36" s="7"/>
       <c r="AZ36" s="28"/>
       <c r="BA36" s="23">
-        <f>SUM(B36:AY36)</f>
+        <f t="shared" ref="BA3:BA36" si="0">SUM(B36:AY36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9976,11 +10063,11 @@
       </c>
       <c r="AF38">
         <f>'League Table'!AF40</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AG38" s="8">
         <f>'League Table'!AG40</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AH38" s="8">
         <f>'League Table'!AH40</f>
@@ -10052,199 +10139,199 @@
         <v>63</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:AV40" si="0">SUM(B3:B36)</f>
+        <f t="shared" ref="B40:AV40" si="1">SUM(B3:B36)</f>
         <v>8</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="O40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="P40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U40" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="W40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="X40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AA40" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB40" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="AC40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AE40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="AF40" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="AG40" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="AH40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV40" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BC36">
-    <sortCondition descending="1" ref="BA3:BA36"/>
-    <sortCondition descending="1" ref="BB3:BB36"/>
-    <sortCondition descending="1" ref="BC3:BC36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BC35">
+    <sortCondition descending="1" ref="BA3:BA35"/>
+    <sortCondition descending="1" ref="BB3:BB35"/>
+    <sortCondition descending="1" ref="BC3:BC35"/>
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10261,7 +10348,7 @@
   <dimension ref="A1:BA41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AO2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A5" sqref="A5:BA37"/>
@@ -10503,53 +10590,49 @@
     </row>
     <row r="5" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="18">
-        <v>2</v>
-      </c>
-      <c r="C5" s="18"/>
+        <v>107</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
       <c r="D5" s="18"/>
-      <c r="E5" s="18">
-        <v>4</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18">
-        <v>1</v>
-      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+      <c r="G5" s="18"/>
       <c r="H5" s="49"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>3</v>
+      </c>
       <c r="K5" s="18">
         <v>2</v>
       </c>
-      <c r="L5" s="18">
-        <v>1</v>
-      </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18">
-        <v>1</v>
-      </c>
-      <c r="P5" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>3</v>
-      </c>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18">
+        <v>1</v>
+      </c>
+      <c r="N5" s="18">
+        <v>1</v>
+      </c>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
-      <c r="T5" s="18">
-        <v>1</v>
-      </c>
+      <c r="T5" s="18"/>
       <c r="U5" s="18">
-        <v>1</v>
-      </c>
-      <c r="V5" s="18">
         <v>3</v>
       </c>
+      <c r="V5" s="18"/>
       <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
+      <c r="X5" s="18">
+        <v>1</v>
+      </c>
       <c r="Y5" s="18">
         <v>1</v>
       </c>
@@ -10557,10 +10640,18 @@
       <c r="AA5" s="18"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
+      <c r="AD5" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="18">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="18">
+        <v>3</v>
+      </c>
       <c r="AH5" s="18"/>
       <c r="AI5" s="18"/>
       <c r="AJ5" s="18"/>
@@ -10581,54 +10672,58 @@
       <c r="AY5" s="18"/>
       <c r="BA5">
         <f>SUM(B5:AY5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45">
-        <v>1</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B6" s="45">
+        <v>2</v>
+      </c>
+      <c r="C6" s="45"/>
       <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45">
-        <v>1</v>
-      </c>
-      <c r="G6" s="45"/>
+      <c r="E6" s="45">
+        <v>4</v>
+      </c>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45">
+        <v>1</v>
+      </c>
       <c r="H6" s="53"/>
-      <c r="I6" s="45">
-        <v>2</v>
-      </c>
-      <c r="J6" s="45">
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="59">
+        <v>2</v>
+      </c>
+      <c r="L6" s="16">
+        <v>1</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16">
+        <v>1</v>
+      </c>
+      <c r="P6" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="16">
         <v>3</v>
       </c>
-      <c r="K6" s="59">
-        <v>2</v>
-      </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16">
-        <v>1</v>
-      </c>
-      <c r="N6" s="16">
-        <v>1</v>
-      </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
+      <c r="T6" s="16">
+        <v>1</v>
+      </c>
       <c r="U6" s="16">
+        <v>1</v>
+      </c>
+      <c r="V6" s="16">
         <v>3</v>
       </c>
-      <c r="V6" s="16"/>
       <c r="W6" s="16"/>
-      <c r="X6" s="16">
-        <v>1</v>
-      </c>
+      <c r="X6" s="16"/>
       <c r="Y6" s="16">
         <v>1</v>
       </c>
@@ -10636,12 +10731,8 @@
       <c r="AA6" s="16"/>
       <c r="AB6" s="16"/>
       <c r="AC6" s="16"/>
-      <c r="AD6" s="16">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="16">
-        <v>2</v>
-      </c>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
       <c r="AF6" s="16"/>
       <c r="AG6" s="16"/>
       <c r="AH6" s="16"/>
@@ -10664,7 +10755,7 @@
       <c r="AY6" s="16"/>
       <c r="BA6">
         <f>SUM(B6:AY6)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
@@ -10723,8 +10814,12 @@
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
+      <c r="AF7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>2</v>
+      </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
@@ -10745,7 +10840,7 @@
       <c r="AY7" s="7"/>
       <c r="BA7">
         <f>SUM(B7:AY7)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -12951,11 +13046,11 @@
       </c>
       <c r="AF41" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG41" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH41" s="8">
         <f t="shared" si="1"/>
@@ -13031,7 +13126,7 @@
       </c>
       <c r="BA41">
         <f>SUM(B41:AZ41)</f>
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -13052,8 +13147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13217,7 +13312,7 @@
       <c r="K9" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="8">
         <v>3</v>
       </c>
       <c r="M9" s="8" t="s">
@@ -13253,7 +13348,7 @@
       <c r="K10" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="8">
         <v>2</v>
       </c>
       <c r="M10" s="8" t="s">
@@ -13284,19 +13379,19 @@
         <v>131</v>
       </c>
       <c r="I11" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="8">
         <v>2</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>131</v>
       </c>
       <c r="N11" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -13323,7 +13418,10 @@
         <v>3</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>117</v>
@@ -13351,14 +13449,15 @@
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
       <c r="H13" s="8" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="I13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>127</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="L13" s="8"/>
       <c r="M13" s="8" t="s">
         <v>121</v>
       </c>
@@ -13383,20 +13482,21 @@
         <v>119</v>
       </c>
       <c r="G14" s="31"/>
-      <c r="H14" s="57" t="s">
-        <v>132</v>
+      <c r="H14" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="I14" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>132</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="L14" s="8"/>
       <c r="M14" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="N14" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -13416,17 +13516,18 @@
         <v>142</v>
       </c>
       <c r="G15" s="31"/>
-      <c r="H15" s="8" t="s">
-        <v>168</v>
+      <c r="H15" s="57" t="s">
+        <v>132</v>
       </c>
       <c r="I15" s="8">
         <v>2</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>148</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="L15" s="8"/>
       <c r="M15" s="8" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="N15" s="8">
         <v>3</v>
@@ -13450,16 +13551,17 @@
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="8" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="I16" s="8">
         <v>2</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>163</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="L16" s="8"/>
       <c r="M16" s="8" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="N16" s="8">
         <v>3</v>
@@ -13483,14 +13585,15 @@
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I17" s="8">
         <v>2</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>168</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="L17" s="8"/>
       <c r="M17" s="8" t="s">
         <v>118</v>
       </c>
@@ -13516,19 +13619,20 @@
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="8">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="I18" s="8">
-        <v>2</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="N18" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -13546,13 +13650,14 @@
         <v>118</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="L19" s="8"/>
       <c r="M19" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N19" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -13576,10 +13681,11 @@
         <v>122</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>123</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="L20" s="8"/>
       <c r="M20" s="8" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="N20" s="8">
         <v>2</v>
@@ -13608,8 +13714,9 @@
       <c r="K21" s="8" t="s">
         <v>190</v>
       </c>
+      <c r="L21" s="8"/>
       <c r="M21" s="8" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="N21" s="8">
         <v>2</v>
@@ -13636,6 +13743,7 @@
       <c r="K22" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="L22" s="8"/>
       <c r="M22" s="8" t="s">
         <v>152</v>
       </c>
@@ -13666,8 +13774,12 @@
       <c r="K23" s="8" t="s">
         <v>203</v>
       </c>
+      <c r="L23" s="8"/>
       <c r="M23" s="8" t="s">
-        <v>122</v>
+        <v>203</v>
+      </c>
+      <c r="N23" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -13690,9 +13802,12 @@
       <c r="H24" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="K24" s="8"/>
+      <c r="K24" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="L24" s="8"/>
       <c r="M24" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -13717,7 +13832,7 @@
       </c>
       <c r="K25" s="8"/>
       <c r="M25" s="8" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -13742,7 +13857,7 @@
       </c>
       <c r="K26" s="8"/>
       <c r="M26" s="8" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -13767,7 +13882,7 @@
       </c>
       <c r="K27" s="8"/>
       <c r="M27" s="8" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -13781,9 +13896,12 @@
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
       <c r="G28" s="31"/>
+      <c r="H28" s="8" t="s">
+        <v>203</v>
+      </c>
       <c r="K28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -13804,7 +13922,7 @@
       </c>
       <c r="K29" s="8"/>
       <c r="M29" s="8" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -13818,7 +13936,7 @@
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
       <c r="M30" s="8" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -13857,24 +13975,43 @@
       <c r="E32" s="31" t="s">
         <v>210</v>
       </c>
+      <c r="M32" s="8" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="31">
         <v>31</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
+      <c r="B33" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="31">
         <v>32</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
+      <c r="B34" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="31">
@@ -14031,8 +14168,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M9:N26">
-    <sortCondition descending="1" ref="N9:N26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M9:N23">
+    <sortCondition descending="1" ref="N9:N23"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Week 39 latest data
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlsmith/Desktop/Home Desktop – Carl’s iMac /Football/Season 2024 Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F525536-362C-5249-BA1E-2963C0BD964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF573D18-FEFE-B14D-B553-C83D98BD2B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8780" yWindow="3660" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="230">
   <si>
     <t>WK 1</t>
   </si>
@@ -721,6 +721,15 @@
   </si>
   <si>
     <t>Mick</t>
+  </si>
+  <si>
+    <t>STRAIGHT ROB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRAIGHT ROB </t>
+  </si>
+  <si>
+    <t>Straight Rob v Woger</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1187,7 +1196,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1602,10 +1610,10 @@
   <dimension ref="A1:BJ74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA5" sqref="BA5:BA39"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2145,7 +2153,9 @@
       <c r="AM5" s="18">
         <v>0</v>
       </c>
-      <c r="AN5" s="18"/>
+      <c r="AN5" s="18">
+        <v>0</v>
+      </c>
       <c r="AO5" s="18"/>
       <c r="AP5" s="18"/>
       <c r="AQ5" s="18"/>
@@ -2164,7 +2174,7 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8">
         <f>COUNT(B5:AY5)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BD5" s="8">
         <f>COUNTIF($B5:$AY5, "&gt;=1")</f>
@@ -2172,7 +2182,7 @@
       </c>
       <c r="BE5" s="8">
         <f>COUNTIF($B5:$AY5, "0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF5" s="8">
         <f>COUNTIF($B5:$AY5, "&lt;0")</f>
@@ -2180,7 +2190,7 @@
       </c>
       <c r="BG5" s="8">
         <f>SUM(BD5*3)+BE5</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BH5" s="8">
         <f>SUM(B5:AY5)</f>
@@ -2188,7 +2198,7 @@
       </c>
       <c r="BI5" s="10">
         <f>SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.61290322580645162</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="BJ5" s="10"/>
     </row>
@@ -2294,7 +2304,9 @@
       <c r="AM6" s="30">
         <v>0</v>
       </c>
-      <c r="AN6" s="30"/>
+      <c r="AN6" s="30">
+        <v>0</v>
+      </c>
       <c r="AO6" s="30"/>
       <c r="AP6" s="30"/>
       <c r="AQ6" s="30"/>
@@ -2311,7 +2323,7 @@
       </c>
       <c r="BC6" s="8">
         <f>COUNT(B6:AY6)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BD6" s="8">
         <f>COUNTIF($B6:$AY6, "&gt;=1")</f>
@@ -2319,7 +2331,7 @@
       </c>
       <c r="BE6" s="8">
         <f>COUNTIF($B6:$AY6, "0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF6" s="8">
         <f>COUNTIF($B6:$AY6, "&lt;0")</f>
@@ -2327,7 +2339,7 @@
       </c>
       <c r="BG6" s="8">
         <f>SUM(BD6*3)+BE6</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BH6" s="8">
         <f>SUM(B6:AY6)</f>
@@ -2335,7 +2347,7 @@
       </c>
       <c r="BI6" s="10">
         <f>SUM(BD6*3+BE6*1)/SUM(BC6*3)</f>
-        <v>0.56666666666666665</v>
+        <v>0.55913978494623651</v>
       </c>
       <c r="BJ6" s="10"/>
     </row>
@@ -2445,7 +2457,9 @@
       <c r="AM7" s="7">
         <v>0</v>
       </c>
-      <c r="AN7" s="7"/>
+      <c r="AN7" s="7">
+        <v>0</v>
+      </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
@@ -2462,7 +2476,7 @@
       </c>
       <c r="BC7" s="8">
         <f>COUNT(B7:AY7)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BD7" s="8">
         <f>COUNTIF($B7:$AY7, "&gt;=1")</f>
@@ -2470,7 +2484,7 @@
       </c>
       <c r="BE7" s="8">
         <f>COUNTIF($B7:$AY7, "0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF7" s="8">
         <f>COUNTIF($B7:$AY7, "&lt;0")</f>
@@ -2478,7 +2492,7 @@
       </c>
       <c r="BG7" s="8">
         <f>SUM(BD7*3)+BE7</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="BH7" s="8">
         <f>SUM(B7:AY7)</f>
@@ -2486,7 +2500,7 @@
       </c>
       <c r="BI7" s="10">
         <f>SUM(BD7*3+BE7*1)/SUM(BC7*3)</f>
-        <v>0.46875</v>
+        <v>0.46464646464646464</v>
       </c>
       <c r="BJ7" s="10"/>
     </row>
@@ -2588,7 +2602,9 @@
       <c r="AM8" s="18">
         <v>0</v>
       </c>
-      <c r="AN8" s="18"/>
+      <c r="AN8" s="18">
+        <v>0</v>
+      </c>
       <c r="AO8" s="18"/>
       <c r="AP8" s="18"/>
       <c r="AQ8" s="18"/>
@@ -2605,7 +2621,7 @@
       </c>
       <c r="BC8" s="8">
         <f>COUNT(B8:AY8)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD8" s="8">
         <f>COUNTIF($B8:$AY8, "&gt;=1")</f>
@@ -2613,7 +2629,7 @@
       </c>
       <c r="BE8" s="8">
         <f>COUNTIF($B8:$AY8, "0")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF8" s="8">
         <f>COUNTIF($B8:$AY8, "&lt;0")</f>
@@ -2621,7 +2637,7 @@
       </c>
       <c r="BG8" s="8">
         <f>SUM(BD8*3)+BE8</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="BH8" s="8">
         <f>SUM(B8:AY8)</f>
@@ -2629,7 +2645,7 @@
       </c>
       <c r="BI8" s="10">
         <f>SUM(BD8*3+BE8*1)/SUM(BC8*3)</f>
-        <v>0.5357142857142857</v>
+        <v>0.52873563218390807</v>
       </c>
       <c r="BJ8" s="10"/>
     </row>
@@ -2723,7 +2739,9 @@
       <c r="AM9" s="47">
         <v>0</v>
       </c>
-      <c r="AN9" s="16"/>
+      <c r="AN9" s="16">
+        <v>0</v>
+      </c>
       <c r="AO9" s="16"/>
       <c r="AP9" s="16"/>
       <c r="AQ9" s="16"/>
@@ -2740,7 +2758,7 @@
       </c>
       <c r="BC9" s="8">
         <f>COUNT(B9:AY9)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BD9" s="8">
         <f>COUNTIF($B9:$AY9, "&gt;=1")</f>
@@ -2748,7 +2766,7 @@
       </c>
       <c r="BE9" s="8">
         <f>COUNTIF($B9:$AY9, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF9" s="8">
         <f>COUNTIF($B9:$AY9, "&lt;0")</f>
@@ -2756,7 +2774,7 @@
       </c>
       <c r="BG9" s="8">
         <f>SUM(BD9*3)+BE9</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BH9" s="8">
         <f>SUM(B9:AY9)</f>
@@ -2764,7 +2782,7 @@
       </c>
       <c r="BI9" s="10">
         <f>SUM(BD9*3+BE9*1)/SUM(BC9*3)</f>
-        <v>0.56944444444444442</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="BJ9" s="10"/>
     </row>
@@ -2866,7 +2884,9 @@
       </c>
       <c r="AL10" s="16"/>
       <c r="AM10" s="16"/>
-      <c r="AN10" s="16"/>
+      <c r="AN10" s="16">
+        <v>0</v>
+      </c>
       <c r="AO10" s="16"/>
       <c r="AP10" s="16"/>
       <c r="AQ10" s="16"/>
@@ -2883,7 +2903,7 @@
       </c>
       <c r="BC10" s="8">
         <f>COUNT(B10:AY10)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD10" s="8">
         <f>COUNTIF($B10:$AY10, "&gt;=1")</f>
@@ -2891,7 +2911,7 @@
       </c>
       <c r="BE10" s="8">
         <f>COUNTIF($B10:$AY10, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF10" s="8">
         <f>COUNTIF($B10:$AY10, "&lt;0")</f>
@@ -2899,7 +2919,7 @@
       </c>
       <c r="BG10" s="8">
         <f>SUM(BD10*3)+BE10</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BH10" s="8">
         <f>SUM(B10:AY10)</f>
@@ -2907,7 +2927,7 @@
       </c>
       <c r="BI10" s="10">
         <f>SUM(BD10*3+BE10*1)/SUM(BC10*3)</f>
-        <v>0.48809523809523808</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="BJ10" s="10"/>
     </row>
@@ -3140,7 +3160,9 @@
       <c r="AM12" s="45">
         <v>0</v>
       </c>
-      <c r="AN12" s="7"/>
+      <c r="AN12" s="7">
+        <v>0</v>
+      </c>
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
       <c r="AQ12" s="7"/>
@@ -3157,7 +3179,7 @@
       </c>
       <c r="BC12" s="8">
         <f>COUNT(B12:AY12)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="BD12" s="8">
         <f>COUNTIF($B12:$AY12, "&gt;=1")</f>
@@ -3165,7 +3187,7 @@
       </c>
       <c r="BE12" s="8">
         <f>COUNTIF($B12:$AY12, "0")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BF12" s="8">
         <f>COUNTIF($B12:$AY12, "&lt;0")</f>
@@ -3173,7 +3195,7 @@
       </c>
       <c r="BG12" s="8">
         <f>SUM(BD12*3)+BE12</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BH12" s="8">
         <f>SUM(B12:AY12)</f>
@@ -3181,7 +3203,7 @@
       </c>
       <c r="BI12" s="10">
         <f>SUM(BD12*3+BE12*1)/SUM(BC12*3)</f>
-        <v>0.45333333333333331</v>
+        <v>0.44871794871794873</v>
       </c>
       <c r="BJ12" s="10"/>
     </row>
@@ -3283,7 +3305,9 @@
       <c r="AM13" s="7">
         <v>0</v>
       </c>
-      <c r="AN13" s="7"/>
+      <c r="AN13" s="7">
+        <v>0</v>
+      </c>
       <c r="AO13" s="7"/>
       <c r="AP13" s="7"/>
       <c r="AQ13" s="7"/>
@@ -3300,7 +3324,7 @@
       </c>
       <c r="BC13" s="8">
         <f>COUNT(B13:AY13)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD13" s="8">
         <f>COUNTIF($B13:$AY13, "&gt;=1")</f>
@@ -3308,7 +3332,7 @@
       </c>
       <c r="BE13" s="8">
         <f>COUNTIF($B13:$AY13, "0")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BF13" s="8">
         <f>COUNTIF($B13:$AY13, "&lt;0")</f>
@@ -3316,7 +3340,7 @@
       </c>
       <c r="BG13" s="8">
         <f>SUM(BD13*3)+BE13</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BH13" s="8">
         <f>SUM(B13:AY13)</f>
@@ -3324,7 +3348,7 @@
       </c>
       <c r="BI13" s="10">
         <f>SUM(BD13*3+BE13*1)/SUM(BC13*3)</f>
-        <v>0.40476190476190477</v>
+        <v>0.40229885057471265</v>
       </c>
       <c r="BJ13" s="10"/>
     </row>
@@ -3412,7 +3436,9 @@
       <c r="AM14" s="7">
         <v>0</v>
       </c>
-      <c r="AN14" s="7"/>
+      <c r="AN14" s="7">
+        <v>0</v>
+      </c>
       <c r="AO14" s="7"/>
       <c r="AP14" s="7"/>
       <c r="AQ14" s="7"/>
@@ -3429,7 +3455,7 @@
       </c>
       <c r="BC14" s="8">
         <f>COUNT(B14:AY14)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BD14" s="8">
         <f>COUNTIF($B14:$AY14, "&gt;=1")</f>
@@ -3437,7 +3463,7 @@
       </c>
       <c r="BE14" s="8">
         <f>COUNTIF($B14:$AY14, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF14" s="8">
         <f>COUNTIF($B14:$AY14, "&lt;0")</f>
@@ -3445,7 +3471,7 @@
       </c>
       <c r="BG14" s="8">
         <f>SUM(BD14*3)+BE14</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BH14" s="8">
         <f>SUM(B14:AY14)</f>
@@ -3453,7 +3479,7 @@
       </c>
       <c r="BI14" s="10">
         <f>SUM(BD14*3+BE14*1)/SUM(BC14*3)</f>
-        <v>0.50793650793650791</v>
+        <v>0.5</v>
       </c>
       <c r="BJ14" s="10"/>
     </row>
@@ -3557,7 +3583,9 @@
         <v>-1</v>
       </c>
       <c r="AM15" s="7"/>
-      <c r="AN15" s="7"/>
+      <c r="AN15" s="7">
+        <v>0</v>
+      </c>
       <c r="AO15" s="7"/>
       <c r="AP15" s="7"/>
       <c r="AQ15" s="7"/>
@@ -3574,7 +3602,7 @@
       </c>
       <c r="BC15" s="8">
         <f>COUNT(B15:AY15)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BD15" s="8">
         <f>COUNTIF($B15:$AY15, "&gt;=1")</f>
@@ -3582,7 +3610,7 @@
       </c>
       <c r="BE15" s="8">
         <f>COUNTIF($B15:$AY15, "0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF15" s="8">
         <f>COUNTIF($B15:$AY15, "&lt;0")</f>
@@ -3590,7 +3618,7 @@
       </c>
       <c r="BG15" s="8">
         <f>SUM(BD15*3)+BE15</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BH15" s="8">
         <f>SUM(B15:AY15)</f>
@@ -3598,7 +3626,7 @@
       </c>
       <c r="BI15" s="10">
         <f>SUM(BD15*3+BE15*1)/SUM(BC15*3)</f>
-        <v>0.35632183908045978</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="BJ15" s="10"/>
     </row>
@@ -3682,7 +3710,9 @@
       <c r="AM16" s="7">
         <v>0</v>
       </c>
-      <c r="AN16" s="7"/>
+      <c r="AN16" s="7">
+        <v>0</v>
+      </c>
       <c r="AO16" s="7"/>
       <c r="AP16" s="7"/>
       <c r="AQ16" s="7"/>
@@ -3699,7 +3729,7 @@
       </c>
       <c r="BC16" s="8">
         <f>COUNT(B16:AY16)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BD16" s="8">
         <f>COUNTIF($B16:$AY16, "&gt;=1")</f>
@@ -3707,7 +3737,7 @@
       </c>
       <c r="BE16" s="8">
         <f>COUNTIF($B16:$AY16, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF16" s="8">
         <f>COUNTIF($B16:$AY16, "&lt;0")</f>
@@ -3715,7 +3745,7 @@
       </c>
       <c r="BG16" s="8">
         <f>SUM(BD16*3)+BE16</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BH16" s="8">
         <f>SUM(B16:AY16)</f>
@@ -3723,89 +3753,99 @@
       </c>
       <c r="BI16" s="10">
         <f>SUM(BD16*3+BE16*1)/SUM(BC16*3)</f>
-        <v>0.50877192982456143</v>
+        <v>0.5</v>
       </c>
       <c r="BJ16" s="10"/>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="B17" s="45">
+        <v>-1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>-9</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
       <c r="H17" s="50"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7">
-        <v>-8</v>
-      </c>
-      <c r="K17" s="45">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>2</v>
+      </c>
       <c r="M17" s="7">
         <v>-1</v>
       </c>
       <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="O17" s="45">
+        <v>1</v>
+      </c>
       <c r="P17" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="7"/>
+        <v>-2</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>3</v>
+      </c>
       <c r="R17" s="50"/>
       <c r="S17" s="7">
-        <v>2</v>
-      </c>
-      <c r="T17" s="7"/>
+        <v>-2</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
       <c r="U17" s="7">
         <v>4</v>
       </c>
-      <c r="V17" s="7"/>
+      <c r="V17" s="7">
+        <v>8</v>
+      </c>
       <c r="W17" s="7">
         <v>0</v>
       </c>
       <c r="X17" s="7">
-        <v>5</v>
-      </c>
-      <c r="Y17" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="7">
-        <v>2</v>
-      </c>
+        <v>-5</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="7"/>
       <c r="AA17" s="50"/>
-      <c r="AB17" s="7">
-        <v>-1</v>
-      </c>
+      <c r="AB17" s="7"/>
       <c r="AC17" s="65"/>
-      <c r="AD17" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="7">
-        <v>4</v>
-      </c>
-      <c r="AF17" s="45">
-        <v>-2</v>
-      </c>
-      <c r="AG17" s="7">
-        <v>-5</v>
-      </c>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
-      <c r="AK17" s="7">
+      <c r="AK17" s="45">
         <v>1</v>
       </c>
       <c r="AL17" s="7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AM17" s="7">
         <v>0</v>
       </c>
-      <c r="AN17" s="7"/>
+      <c r="AN17" s="7">
+        <v>0</v>
+      </c>
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
       <c r="AQ17" s="7"/>
@@ -3822,7 +3862,7 @@
       </c>
       <c r="BC17" s="8">
         <f>COUNT(B17:AY17)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="BD17" s="8">
         <f>COUNTIF($B17:$AY17, "&gt;=1")</f>
@@ -3830,108 +3870,100 @@
       </c>
       <c r="BE17" s="8">
         <f>COUNTIF($B17:$AY17, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF17" s="8">
         <f>COUNTIF($B17:$AY17, "&lt;0")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="BG17" s="8">
         <f>SUM(BD17*3)+BE17</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BH17" s="8">
         <f>SUM(B17:AY17)</f>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="BI17" s="10">
         <f>SUM(BD17*3+BE17*1)/SUM(BC17*3)</f>
-        <v>0.53703703703703709</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="BJ17" s="10"/>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="45">
-        <v>-1</v>
-      </c>
-      <c r="C18" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D18" s="7">
-        <v>-9</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="50"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7">
-        <v>0</v>
-      </c>
-      <c r="L18" s="7">
-        <v>2</v>
-      </c>
+      <c r="J18" s="7">
+        <v>-8</v>
+      </c>
+      <c r="K18" s="45">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7"/>
       <c r="M18" s="7">
         <v>-1</v>
       </c>
       <c r="N18" s="7"/>
-      <c r="O18" s="45">
-        <v>1</v>
-      </c>
+      <c r="O18" s="7"/>
       <c r="P18" s="7">
-        <v>-2</v>
-      </c>
-      <c r="Q18" s="7">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="Q18" s="7"/>
       <c r="R18" s="50"/>
       <c r="S18" s="7">
-        <v>-2</v>
-      </c>
-      <c r="T18" s="7">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="T18" s="7"/>
       <c r="U18" s="7">
         <v>4</v>
       </c>
-      <c r="V18" s="7">
-        <v>8</v>
-      </c>
+      <c r="V18" s="7"/>
       <c r="W18" s="7">
         <v>0</v>
       </c>
       <c r="X18" s="7">
+        <v>5</v>
+      </c>
+      <c r="Y18" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AC18" s="65"/>
+      <c r="AD18" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="7">
+        <v>4</v>
+      </c>
+      <c r="AF18" s="45">
+        <v>-2</v>
+      </c>
+      <c r="AG18" s="7">
         <v>-5</v>
       </c>
-      <c r="Y18" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="50"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="65"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
-      <c r="AF18" s="7"/>
-      <c r="AG18" s="7"/>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
-      <c r="AK18" s="45">
+      <c r="AK18" s="7">
         <v>1</v>
       </c>
       <c r="AL18" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AM18" s="7">
         <v>0</v>
@@ -3953,7 +3985,7 @@
       </c>
       <c r="BC18" s="8">
         <f>COUNT(B18:AY18)</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="BD18" s="8">
         <f>COUNTIF($B18:$AY18, "&gt;=1")</f>
@@ -3965,7 +3997,7 @@
       </c>
       <c r="BF18" s="8">
         <f>COUNTIF($B18:$AY18, "&lt;0")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="BG18" s="8">
         <f>SUM(BD18*3)+BE18</f>
@@ -3973,11 +4005,11 @@
       </c>
       <c r="BH18" s="8">
         <f>SUM(B18:AY18)</f>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="BI18" s="10">
         <f>SUM(BD18*3+BE18*1)/SUM(BC18*3)</f>
-        <v>0.43939393939393939</v>
+        <v>0.53703703703703709</v>
       </c>
       <c r="BJ18" s="10"/>
     </row>
@@ -4065,7 +4097,9 @@
         <v>-1</v>
       </c>
       <c r="AM19" s="7"/>
-      <c r="AN19" s="7"/>
+      <c r="AN19" s="7">
+        <v>0</v>
+      </c>
       <c r="AO19" s="7"/>
       <c r="AP19" s="7"/>
       <c r="AQ19" s="7"/>
@@ -4082,7 +4116,7 @@
       </c>
       <c r="BC19" s="8">
         <f>COUNT(B19:AY19)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BD19" s="8">
         <f>COUNTIF($B19:$AY19, "&gt;=1")</f>
@@ -4090,7 +4124,7 @@
       </c>
       <c r="BE19" s="8">
         <f>COUNTIF($B19:$AY19, "0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF19" s="8">
         <f>COUNTIF($B19:$AY19, "&lt;0")</f>
@@ -4098,7 +4132,7 @@
       </c>
       <c r="BG19" s="8">
         <f>SUM(BD19*3)+BE19</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BH19" s="8">
         <f>SUM(B19:AY19)</f>
@@ -4106,7 +4140,7 @@
       </c>
       <c r="BI19" s="10">
         <f>SUM(BD19*3+BE19*1)/SUM(BC19*3)</f>
-        <v>0.44444444444444442</v>
+        <v>0.43939393939393939</v>
       </c>
       <c r="BJ19" s="10"/>
     </row>
@@ -4186,7 +4220,9 @@
       <c r="AM20" s="7">
         <v>0</v>
       </c>
-      <c r="AN20" s="7"/>
+      <c r="AN20" s="7">
+        <v>0</v>
+      </c>
       <c r="AO20" s="7"/>
       <c r="AP20" s="7"/>
       <c r="AQ20" s="7"/>
@@ -4203,7 +4239,7 @@
       </c>
       <c r="BC20" s="8">
         <f>COUNT(B20:AY20)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BD20" s="8">
         <f>COUNTIF($B20:$AY20, "&gt;=1")</f>
@@ -4211,7 +4247,7 @@
       </c>
       <c r="BE20" s="8">
         <f>COUNTIF($B20:$AY20, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF20" s="8">
         <f>COUNTIF($B20:$AY20, "&lt;0")</f>
@@ -4219,7 +4255,7 @@
       </c>
       <c r="BG20" s="8">
         <f>SUM(BD20*3)+BE20</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BH20" s="8">
         <f>SUM(B20:AY20)</f>
@@ -4227,7 +4263,7 @@
       </c>
       <c r="BI20" s="10">
         <f>SUM(BD20*3+BE20*1)/SUM(BC20*3)</f>
-        <v>0.50980392156862742</v>
+        <v>0.5</v>
       </c>
       <c r="BJ20" s="10"/>
     </row>
@@ -4305,7 +4341,9 @@
       <c r="AM21" s="7">
         <v>0</v>
       </c>
-      <c r="AN21" s="7"/>
+      <c r="AN21" s="7">
+        <v>0</v>
+      </c>
       <c r="AO21" s="7"/>
       <c r="AP21" s="7"/>
       <c r="AQ21" s="7"/>
@@ -4322,7 +4360,7 @@
       </c>
       <c r="BC21" s="8">
         <f>COUNT(B21:AY21)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BD21" s="8">
         <f>COUNTIF($B21:$AY21, "&gt;=1")</f>
@@ -4330,7 +4368,7 @@
       </c>
       <c r="BE21" s="8">
         <f>COUNTIF($B21:$AY21, "0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF21" s="8">
         <f>COUNTIF($B21:$AY21, "&lt;0")</f>
@@ -4338,7 +4376,7 @@
       </c>
       <c r="BG21" s="8">
         <f>SUM(BD21*3)+BE21</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BH21" s="8">
         <f>SUM(B21:AY21)</f>
@@ -4346,7 +4384,7 @@
       </c>
       <c r="BI21" s="10">
         <f>SUM(BD21*3+BE21*1)/SUM(BC21*3)</f>
-        <v>0.5</v>
+        <v>0.49019607843137253</v>
       </c>
       <c r="BJ21" s="10"/>
     </row>
@@ -4434,7 +4472,9 @@
       <c r="AM22" s="7">
         <v>0</v>
       </c>
-      <c r="AN22" s="7"/>
+      <c r="AN22" s="7">
+        <v>0</v>
+      </c>
       <c r="AO22" s="7"/>
       <c r="AP22" s="7"/>
       <c r="AQ22" s="7"/>
@@ -4451,7 +4491,7 @@
       </c>
       <c r="BC22" s="8">
         <f>COUNT(B22:AY22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BD22" s="8">
         <f>COUNTIF($B22:$AY22, "&gt;=1")</f>
@@ -4459,7 +4499,7 @@
       </c>
       <c r="BE22" s="8">
         <f>COUNTIF($B22:$AY22, "0")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF22" s="8">
         <f>COUNTIF($B22:$AY22, "&lt;0")</f>
@@ -4467,7 +4507,7 @@
       </c>
       <c r="BG22" s="8">
         <f>SUM(BD22*3)+BE22</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BH22" s="8">
         <f>SUM(B22:AY22)</f>
@@ -4475,7 +4515,7 @@
       </c>
       <c r="BI22" s="10">
         <f>SUM(BD22*3+BE22*1)/SUM(BC22*3)</f>
-        <v>0.36507936507936506</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="BJ22" s="10"/>
     </row>
@@ -4553,7 +4593,9 @@
       <c r="AK23" s="7"/>
       <c r="AL23" s="7"/>
       <c r="AM23" s="7"/>
-      <c r="AN23" s="7"/>
+      <c r="AN23" s="7">
+        <v>0</v>
+      </c>
       <c r="AO23" s="7"/>
       <c r="AP23" s="7"/>
       <c r="AQ23" s="7"/>
@@ -4571,7 +4613,7 @@
       </c>
       <c r="BC23" s="8">
         <f>COUNT(B23:AY23)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BD23" s="8">
         <f>COUNTIF($B23:$AY23, "&gt;=1")</f>
@@ -4579,7 +4621,7 @@
       </c>
       <c r="BE23" s="8">
         <f>COUNTIF($B23:$AY23, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF23" s="8">
         <f>COUNTIF($B23:$AY23, "&lt;0")</f>
@@ -4587,7 +4629,7 @@
       </c>
       <c r="BG23" s="8">
         <f>SUM(BD23*3)+BE23</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BH23" s="8">
         <f>SUM(B23:AY23)</f>
@@ -4595,7 +4637,7 @@
       </c>
       <c r="BI23" s="10">
         <f>SUM(BD23*3+BE23*1)/SUM(BC23*3)</f>
-        <v>0.47916666666666669</v>
+        <v>0.47058823529411764</v>
       </c>
       <c r="BJ23" s="10"/>
     </row>
@@ -5427,7 +5469,7 @@
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -5475,7 +5517,9 @@
       <c r="AM32" s="7">
         <v>0</v>
       </c>
-      <c r="AN32" s="7"/>
+      <c r="AN32" s="45">
+        <v>0</v>
+      </c>
       <c r="AO32" s="7"/>
       <c r="AP32" s="7"/>
       <c r="AQ32" s="7"/>
@@ -5492,7 +5536,7 @@
       </c>
       <c r="BC32" s="8">
         <f>COUNT(B32:AY32)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD32" s="8">
         <f>COUNTIF($B32:$AY32, "&gt;=1")</f>
@@ -5500,7 +5544,7 @@
       </c>
       <c r="BE32" s="8">
         <f>COUNTIF($B32:$AY32, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF32" s="8">
         <f>COUNTIF($B32:$AY32, "&lt;0")</f>
@@ -5508,7 +5552,7 @@
       </c>
       <c r="BG32" s="8">
         <f>SUM(BD32*3)+BE32</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BH32" s="8">
         <f>SUM(B32:AY32)</f>
@@ -5516,7 +5560,7 @@
       </c>
       <c r="BI32" s="10">
         <f>SUM(BD32*3+BE32*1)/SUM(BC32*3)</f>
-        <v>0.41666666666666669</v>
+        <v>0.4</v>
       </c>
       <c r="BJ32" s="10"/>
     </row>
@@ -5574,7 +5618,9 @@
         <v>0</v>
       </c>
       <c r="AM33" s="7"/>
-      <c r="AN33" s="7"/>
+      <c r="AN33" s="7">
+        <v>0</v>
+      </c>
       <c r="AO33" s="7"/>
       <c r="AP33" s="7"/>
       <c r="AQ33" s="7"/>
@@ -5591,7 +5637,7 @@
       </c>
       <c r="BC33" s="8">
         <f>COUNT(B33:AY33)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD33" s="8">
         <f>COUNTIF($B33:$AY33, "&gt;=1")</f>
@@ -5599,7 +5645,7 @@
       </c>
       <c r="BE33" s="8">
         <f>COUNTIF($B33:$AY33, "0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF33" s="8">
         <f>COUNTIF($B33:$AY33, "&lt;0")</f>
@@ -5607,7 +5653,7 @@
       </c>
       <c r="BG33" s="8">
         <f>SUM(BD33*3)+BE33</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BH33" s="8">
         <f>SUM(B33:AY33)</f>
@@ -5615,18 +5661,16 @@
       </c>
       <c r="BI33" s="10">
         <f>SUM(BD33*3+BE33*1)/SUM(BC33*3)</f>
-        <v>0.27777777777777779</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="BJ33" s="10"/>
     </row>
     <row r="34" spans="1:62" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="7">
-        <v>1</v>
-      </c>
+      <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -5634,9 +5678,7 @@
       <c r="H34" s="50"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
-      <c r="K34" s="7">
-        <v>0</v>
-      </c>
+      <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
@@ -5644,9 +5686,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="50"/>
-      <c r="S34" s="7">
-        <v>-2</v>
-      </c>
+      <c r="S34" s="7"/>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
@@ -5663,11 +5703,17 @@
       <c r="AG34" s="7"/>
       <c r="AH34" s="7"/>
       <c r="AI34" s="7"/>
-      <c r="AJ34" s="7"/>
-      <c r="AK34" s="7"/>
+      <c r="AJ34" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AK34" s="7">
+        <v>1</v>
+      </c>
       <c r="AL34" s="7"/>
       <c r="AM34" s="7"/>
-      <c r="AN34" s="7"/>
+      <c r="AN34" s="45">
+        <v>0</v>
+      </c>
       <c r="AO34" s="7"/>
       <c r="AP34" s="7"/>
       <c r="AQ34" s="7"/>
@@ -5704,7 +5750,7 @@
       </c>
       <c r="BH34" s="8">
         <f>SUM(B34:AY34)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BI34" s="10">
         <f>SUM(BD34*3+BE34*1)/SUM(BC34*3)</f>
@@ -5714,10 +5760,12 @@
     </row>
     <row r="35" spans="1:62" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -5728,25 +5776,19 @@
       <c r="K35" s="7">
         <v>0</v>
       </c>
-      <c r="L35" s="45">
-        <v>-2</v>
-      </c>
-      <c r="M35" s="7">
-        <v>-1</v>
-      </c>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
-      <c r="Q35" s="7">
-        <v>3</v>
-      </c>
+      <c r="Q35" s="7"/>
       <c r="R35" s="50"/>
-      <c r="S35" s="7"/>
+      <c r="S35" s="7">
+        <v>-2</v>
+      </c>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="7">
-        <v>-8</v>
-      </c>
+      <c r="V35" s="7"/>
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
@@ -5759,9 +5801,7 @@
       <c r="AF35" s="7"/>
       <c r="AG35" s="7"/>
       <c r="AH35" s="7"/>
-      <c r="AI35" s="45">
-        <v>-1</v>
-      </c>
+      <c r="AI35" s="7"/>
       <c r="AJ35" s="7"/>
       <c r="AK35" s="7"/>
       <c r="AL35" s="7"/>
@@ -5783,7 +5823,7 @@
       </c>
       <c r="BC35" s="8">
         <f>COUNT(B35:AY35)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="BD35" s="8">
         <f>COUNTIF($B35:$AY35, "&gt;=1")</f>
@@ -5795,7 +5835,7 @@
       </c>
       <c r="BF35" s="8">
         <f>COUNTIF($B35:$AY35, "&lt;0")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BG35" s="8">
         <f>SUM(BD35*3)+BE35</f>
@@ -5803,17 +5843,17 @@
       </c>
       <c r="BH35" s="8">
         <f>SUM(B35:AY35)</f>
-        <v>-9</v>
+        <v>-1</v>
       </c>
       <c r="BI35" s="10">
         <f>SUM(BD35*3+BE35*1)/SUM(BC35*3)</f>
-        <v>0.22222222222222221</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="BJ35" s="10"/>
     </row>
     <row r="36" spans="1:62" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -5824,18 +5864,28 @@
       <c r="H36" s="50"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+      <c r="K36" s="7">
+        <v>0</v>
+      </c>
+      <c r="L36" s="45">
+        <v>-2</v>
+      </c>
+      <c r="M36" s="7">
+        <v>-1</v>
+      </c>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="Q36" s="7">
+        <v>3</v>
+      </c>
       <c r="R36" s="50"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
-      <c r="V36" s="7"/>
+      <c r="V36" s="7">
+        <v>-8</v>
+      </c>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
@@ -5848,13 +5898,11 @@
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
       <c r="AH36" s="7"/>
-      <c r="AI36" s="7"/>
-      <c r="AJ36" s="7">
+      <c r="AI36" s="45">
         <v>-1</v>
       </c>
-      <c r="AK36" s="7">
-        <v>1</v>
-      </c>
+      <c r="AJ36" s="7"/>
+      <c r="AK36" s="7"/>
       <c r="AL36" s="7"/>
       <c r="AM36" s="7"/>
       <c r="AN36" s="7"/>
@@ -5874,7 +5922,7 @@
       </c>
       <c r="BC36" s="8">
         <f>COUNT(B36:AY36)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BD36" s="8">
         <f>COUNTIF($B36:$AY36, "&gt;=1")</f>
@@ -5882,23 +5930,23 @@
       </c>
       <c r="BE36" s="8">
         <f>COUNTIF($B36:$AY36, "0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF36" s="8">
         <f>COUNTIF($B36:$AY36, "&lt;0")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BG36" s="8">
         <f>SUM(BD36*3)+BE36</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BH36" s="8">
         <f>SUM(B36:AY36)</f>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="BI36" s="10">
         <f>SUM(BD36*3+BE36*1)/SUM(BC36*3)</f>
-        <v>0.5</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="BJ36" s="10"/>
     </row>
@@ -6329,7 +6377,7 @@
       </c>
       <c r="AN40" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO40" s="27">
         <f t="shared" si="1"/>
@@ -6494,7 +6542,9 @@
       <c r="AM41" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AN41" s="8"/>
+      <c r="AN41" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="AO41" s="8"/>
       <c r="AP41" s="8"/>
       <c r="AQ41" s="8"/>
@@ -6842,7 +6892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G30"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6900,7 +6950,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="62">
-        <f>SUM(C3*3)+D3</f>
+        <f t="shared" ref="G3:G30" si="0">SUM(C3*3)+D3</f>
         <v>9</v>
       </c>
       <c r="K3">
@@ -6938,7 +6988,7 @@
         <v>24</v>
       </c>
       <c r="L4" s="69">
-        <f t="shared" ref="L4:L27" si="0">K4/B4</f>
+        <f t="shared" ref="L4:L27" si="1">K4/B4</f>
         <v>8</v>
       </c>
     </row>
@@ -6969,7 +7019,7 @@
         <v>27</v>
       </c>
       <c r="L5" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -7000,7 +7050,7 @@
         <v>19</v>
       </c>
       <c r="L6" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.333333333333333</v>
       </c>
     </row>
@@ -7008,22 +7058,22 @@
       <c r="A7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="70">
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="70">
-        <v>2</v>
-      </c>
-      <c r="D7" s="70">
-        <v>1</v>
-      </c>
-      <c r="E7" s="70">
-        <v>0</v>
-      </c>
-      <c r="F7" s="70">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7">
         <f>SUM(C7*3)+D7</f>
         <v>7</v>
       </c>
@@ -7031,7 +7081,7 @@
         <v>19</v>
       </c>
       <c r="L7" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.333333333333333</v>
       </c>
     </row>
@@ -7065,7 +7115,7 @@
         <v>16</v>
       </c>
       <c r="L8" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="M8" t="s">
@@ -7099,7 +7149,7 @@
         <v>13</v>
       </c>
       <c r="L9" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
     </row>
@@ -7134,7 +7184,7 @@
         <v>28</v>
       </c>
       <c r="L10" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="M10" t="s">
@@ -7168,7 +7218,7 @@
         <v>21</v>
       </c>
       <c r="L11" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -7199,7 +7249,7 @@
         <v>25</v>
       </c>
       <c r="L12" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
     </row>
@@ -7231,7 +7281,7 @@
         <v>5</v>
       </c>
       <c r="L13" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -7262,7 +7312,7 @@
         <v>19</v>
       </c>
       <c r="L14" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -7293,7 +7343,7 @@
         <v>12</v>
       </c>
       <c r="L15" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -7324,7 +7374,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
     </row>
@@ -7355,7 +7405,7 @@
         <v>19</v>
       </c>
       <c r="L17" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.333333333333333</v>
       </c>
     </row>
@@ -7386,7 +7436,7 @@
         <v>15</v>
       </c>
       <c r="L18" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -7417,7 +7467,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.333333333333333</v>
       </c>
     </row>
@@ -7448,7 +7498,7 @@
         <v>14</v>
       </c>
       <c r="L20" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
     </row>
@@ -7479,16 +7529,16 @@
         <v>25</v>
       </c>
       <c r="L21" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>108</v>
+        <v>227</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -7497,10 +7547,10 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <f>SUM(C22*3)+D22</f>
@@ -7510,16 +7560,16 @@
         <v>5</v>
       </c>
       <c r="L22" s="69">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -7528,10 +7578,10 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f>SUM(C23*3)+D23</f>
@@ -7541,22 +7591,22 @@
         <v>12</v>
       </c>
       <c r="L23" s="69">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>184</v>
+        <v>108</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -7566,53 +7616,53 @@
       </c>
       <c r="G24">
         <f>SUM(C24*3)+D24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="36">
         <v>15</v>
       </c>
       <c r="L24" s="69">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="G25">
         <f>SUM(C25*3)+D25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="36">
         <v>25</v>
       </c>
       <c r="L25" s="69">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7621,10 +7671,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G26">
         <f>SUM(C26*3)+D26</f>
@@ -7634,16 +7684,16 @@
         <v>8</v>
       </c>
       <c r="L26" s="69">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -7652,10 +7702,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G27">
         <f>SUM(C27*3)+D27</f>
@@ -7665,16 +7715,16 @@
         <v>1</v>
       </c>
       <c r="L27" s="69">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -7683,10 +7733,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="G28">
         <f>SUM(C28*3)+D28</f>
@@ -7698,10 +7748,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -7710,10 +7760,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>-8</v>
+        <v>-3</v>
       </c>
       <c r="G29">
         <f>SUM(C29*3)+D29</f>
@@ -7725,10 +7775,10 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -7737,10 +7787,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>-9</v>
+        <v>-4</v>
       </c>
       <c r="G30">
         <f>SUM(C30*3)+D30</f>
@@ -7752,10 +7802,25 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>-8</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G3:G34" si="1">SUM(C31*3)+D31</f>
+        <f>SUM(C31*3)+D31</f>
         <v>0</v>
       </c>
       <c r="K31">
@@ -7764,10 +7829,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>-9</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f>SUM(C32*3)+D32</f>
         <v>0</v>
       </c>
       <c r="K32">
@@ -7779,7 +7859,7 @@
         <v>19</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G31:G34" si="2">SUM(C33*3)+D33</f>
         <v>0</v>
       </c>
       <c r="K33">
@@ -7791,7 +7871,7 @@
         <v>84</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K34">
@@ -7803,7 +7883,7 @@
         <v>20</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35" si="2">SUM(C35*3)+D35</f>
+        <f t="shared" ref="G35" si="3">SUM(C35*3)+D35</f>
         <v>0</v>
       </c>
       <c r="K35">
@@ -7812,10 +7892,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G34" xr:uid="{CCA4218F-1ABE-CF4A-906A-71EA404D2B67}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G30">
-    <sortCondition descending="1" ref="G3:G30"/>
-    <sortCondition descending="1" ref="F3:F30"/>
-    <sortCondition ref="B3:B30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G32">
+    <sortCondition descending="1" ref="G4:G32"/>
+    <sortCondition descending="1" ref="F4:F32"/>
+    <sortCondition ref="B4:B32"/>
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7830,7 +7910,7 @@
   <dimension ref="A1:BF40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3:BC35"/>
@@ -8087,7 +8167,7 @@
       <c r="AY3" s="7"/>
       <c r="AZ3" s="28"/>
       <c r="BA3" s="23">
-        <f>SUM(B3:AY3)</f>
+        <f t="shared" ref="BA3:BA35" si="0">SUM(B3:AY3)</f>
         <v>19</v>
       </c>
       <c r="BB3" s="8">
@@ -8165,7 +8245,7 @@
       <c r="AY4" s="7"/>
       <c r="AZ4" s="28"/>
       <c r="BA4" s="23">
-        <f>SUM(B4:AY4)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="BB4" s="8">
@@ -8174,44 +8254,44 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
       <c r="H5" s="50"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
       <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
       <c r="N5" s="7">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
-      <c r="P5" s="7">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="50"/>
-      <c r="S5" s="7">
-        <v>3</v>
-      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7">
         <v>1</v>
       </c>
-      <c r="W5" s="7">
-        <v>3</v>
-      </c>
+      <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
@@ -8220,16 +8300,18 @@
       <c r="AC5" s="67"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
+      <c r="AF5" s="7">
+        <v>1</v>
+      </c>
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
-      <c r="AI5" s="7">
-        <v>1</v>
-      </c>
+      <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
       <c r="AK5" s="7"/>
       <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
+      <c r="AM5" s="7">
+        <v>1</v>
+      </c>
       <c r="AN5" s="7"/>
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
@@ -8244,53 +8326,56 @@
       <c r="AY5" s="7"/>
       <c r="AZ5" s="28"/>
       <c r="BA5" s="23">
-        <f>SUM(B5:AY5)</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="BB5" s="8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="BC5" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="7">
-        <v>2</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="7">
-        <v>2</v>
-      </c>
+      <c r="G6" s="7"/>
       <c r="H6" s="50"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7">
-        <v>1</v>
-      </c>
+      <c r="K6" s="7"/>
       <c r="L6" s="7">
-        <v>4</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M6" s="7"/>
       <c r="N6" s="7">
-        <v>2</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7">
+        <v>3</v>
+      </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="50"/>
-      <c r="S6" s="7"/>
+      <c r="S6" s="7">
+        <v>3</v>
+      </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="7">
         <v>1</v>
       </c>
-      <c r="W6" s="7"/>
+      <c r="W6" s="7">
+        <v>3</v>
+      </c>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
@@ -8299,12 +8384,12 @@
       <c r="AC6" s="67"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="7">
-        <v>1</v>
-      </c>
+      <c r="AF6" s="7"/>
       <c r="AG6" s="7"/>
       <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
+      <c r="AI6" s="7">
+        <v>1</v>
+      </c>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
       <c r="AL6" s="7"/>
@@ -8323,14 +8408,11 @@
       <c r="AY6" s="7"/>
       <c r="AZ6" s="28"/>
       <c r="BA6" s="23">
-        <f>SUM(B6:AY6)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="BB6" s="8">
-        <v>2</v>
-      </c>
-      <c r="BC6" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.2">
@@ -8409,7 +8491,7 @@
       <c r="AY7" s="7"/>
       <c r="AZ7" s="28"/>
       <c r="BA7" s="23">
-        <f>SUM(B7:AY7)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="BB7" s="8">
@@ -8485,7 +8567,7 @@
       <c r="AY8" s="7"/>
       <c r="AZ8" s="28"/>
       <c r="BA8" s="23">
-        <f>SUM(B8:AY8)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="BB8" s="8">
@@ -8569,7 +8651,7 @@
       <c r="AY9" s="7"/>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="23">
-        <f>SUM(B9:AY9)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="BB9" s="8">
@@ -8661,7 +8743,7 @@
       <c r="AY10" s="7"/>
       <c r="AZ10" s="28"/>
       <c r="BA10" s="23">
-        <f>SUM(B10:AY10)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -8731,7 +8813,7 @@
       <c r="AY11" s="7"/>
       <c r="AZ11" s="28"/>
       <c r="BA11" s="23">
-        <f>SUM(B11:AY11)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="BB11" s="8">
@@ -8740,18 +8822,18 @@
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="50"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -8760,40 +8842,40 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="50"/>
       <c r="S12" s="7"/>
-      <c r="T12" s="7">
-        <v>1</v>
-      </c>
-      <c r="U12" s="7">
-        <v>1</v>
-      </c>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7">
-        <v>1</v>
-      </c>
+      <c r="W12" s="7">
+        <v>1</v>
+      </c>
+      <c r="X12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="50"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="67"/>
       <c r="AD12" s="7"/>
-      <c r="AE12" s="7">
-        <v>1</v>
-      </c>
+      <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
-      <c r="AG12" s="7">
-        <v>4</v>
-      </c>
+      <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
-      <c r="AI12" s="7"/>
+      <c r="AI12" s="7">
+        <v>3</v>
+      </c>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
       <c r="AL12" s="7"/>
-      <c r="AM12" s="7"/>
+      <c r="AM12" s="7">
+        <v>1</v>
+      </c>
       <c r="AN12" s="7"/>
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
@@ -8808,66 +8890,61 @@
       <c r="AY12" s="7"/>
       <c r="AZ12" s="28"/>
       <c r="BA12" s="23">
-        <f>SUM(B12:AY12)</f>
-        <v>10</v>
-      </c>
-      <c r="BB12" s="8">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="BF12" s="23"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
       <c r="H13" s="50"/>
-      <c r="I13" s="7">
-        <v>1</v>
-      </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="7">
-        <v>1</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="50"/>
       <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
+      <c r="T13" s="7">
+        <v>1</v>
+      </c>
       <c r="U13" s="7">
         <v>1</v>
       </c>
       <c r="V13" s="7"/>
-      <c r="W13" s="7">
-        <v>1</v>
-      </c>
+      <c r="W13" s="7"/>
       <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7">
-        <v>2</v>
-      </c>
+      <c r="Y13" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="7"/>
       <c r="AA13" s="50"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="67"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
+      <c r="AG13" s="7">
+        <v>4</v>
+      </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
@@ -8888,63 +8965,67 @@
       <c r="AY13" s="7"/>
       <c r="AZ13" s="28"/>
       <c r="BA13" s="23">
-        <f>SUM(B13:AY13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="BC13" s="8">
-        <v>2</v>
+      <c r="BB13" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>3</v>
-      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="50"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="I14" s="7">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
+        <v>1</v>
+      </c>
       <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="L14" s="7">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="7">
-        <v>1</v>
-      </c>
+      <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="50"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
+      <c r="U14" s="7">
+        <v>1</v>
+      </c>
       <c r="V14" s="7"/>
       <c r="W14" s="7">
         <v>1</v>
       </c>
-      <c r="X14" s="7">
-        <v>1</v>
-      </c>
+      <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
+      <c r="Z14" s="7">
+        <v>2</v>
+      </c>
       <c r="AA14" s="50"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="67"/>
       <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
+      <c r="AE14" s="7">
+        <v>2</v>
+      </c>
       <c r="AF14" s="7"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
-      <c r="AI14" s="7">
-        <v>3</v>
-      </c>
+      <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
       <c r="AK14" s="7"/>
       <c r="AL14" s="7"/>
@@ -8963,8 +9044,11 @@
       <c r="AY14" s="7"/>
       <c r="AZ14" s="28"/>
       <c r="BA14" s="23">
-        <f>SUM(B14:AY14)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="BC14" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
@@ -9029,7 +9113,7 @@
       <c r="AY15" s="7"/>
       <c r="AZ15" s="28"/>
       <c r="BA15" s="23">
-        <f>SUM(B15:AY15)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="BB15" s="8">
@@ -9101,7 +9185,7 @@
       <c r="AY16" s="7"/>
       <c r="AZ16" s="28"/>
       <c r="BA16" s="23">
-        <f>SUM(B16:AY16)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="BB16" s="8">
@@ -9113,52 +9197,48 @@
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
       <c r="H17" s="50"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7">
-        <v>1</v>
-      </c>
+      <c r="I17" s="7">
+        <v>2</v>
+      </c>
+      <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7">
-        <v>1</v>
-      </c>
-      <c r="O17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7">
+        <v>2</v>
+      </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="50"/>
-      <c r="S17" s="7">
-        <v>1</v>
-      </c>
+      <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
-      <c r="X17" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="7">
-        <v>1</v>
-      </c>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="50"/>
-      <c r="AB17" s="7"/>
+      <c r="AB17" s="7">
+        <v>1</v>
+      </c>
       <c r="AC17" s="67"/>
       <c r="AD17" s="7"/>
-      <c r="AE17" s="7">
-        <v>1</v>
-      </c>
+      <c r="AE17" s="7"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="7"/>
       <c r="AH17" s="7">
@@ -9166,11 +9246,11 @@
       </c>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
-      <c r="AK17" s="7">
-        <v>1</v>
-      </c>
+      <c r="AK17" s="7"/>
       <c r="AL17" s="7"/>
-      <c r="AM17" s="7"/>
+      <c r="AM17" s="7">
+        <v>1</v>
+      </c>
       <c r="AN17" s="7"/>
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
@@ -9185,54 +9265,61 @@
       <c r="AY17" s="7"/>
       <c r="AZ17" s="28"/>
       <c r="BA17" s="23">
-        <f>SUM(B17:AY17)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
+      </c>
+      <c r="BC17" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
+      <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7">
-        <v>1</v>
-      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="50"/>
-      <c r="I18" s="7">
-        <v>2</v>
-      </c>
-      <c r="J18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7">
+        <v>1</v>
+      </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7">
-        <v>2</v>
-      </c>
+      <c r="N18" s="7">
+        <v>1</v>
+      </c>
+      <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="50"/>
-      <c r="S18" s="7"/>
+      <c r="S18" s="7">
+        <v>1</v>
+      </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
+      <c r="X18" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="7">
+        <v>1</v>
+      </c>
       <c r="Z18" s="7"/>
       <c r="AA18" s="50"/>
-      <c r="AB18" s="7">
-        <v>1</v>
-      </c>
+      <c r="AB18" s="7"/>
       <c r="AC18" s="67"/>
       <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
+      <c r="AE18" s="7">
+        <v>1</v>
+      </c>
       <c r="AF18" s="7"/>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7">
@@ -9240,7 +9327,9 @@
       </c>
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
-      <c r="AK18" s="7"/>
+      <c r="AK18" s="7">
+        <v>1</v>
+      </c>
       <c r="AL18" s="7"/>
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
@@ -9257,11 +9346,8 @@
       <c r="AY18" s="7"/>
       <c r="AZ18" s="28"/>
       <c r="BA18" s="23">
-        <f>SUM(B18:AY18)</f>
-        <v>8</v>
-      </c>
-      <c r="BC18" s="8">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="BF18" s="23"/>
     </row>
@@ -9333,20 +9419,16 @@
       <c r="AY19" s="7"/>
       <c r="AZ19" s="28"/>
       <c r="BA19" s="23">
-        <f>SUM(B19:AY19)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="7">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7">
-        <v>2</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -9354,9 +9436,7 @@
       <c r="H20" s="50"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="7">
-        <v>1</v>
-      </c>
+      <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -9366,29 +9446,37 @@
       <c r="R20" s="50"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
+      <c r="U20" s="32"/>
       <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
+      <c r="W20" s="7">
+        <v>1</v>
+      </c>
+      <c r="X20" s="7">
+        <v>1</v>
+      </c>
       <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
+      <c r="Z20" s="7">
+        <v>1</v>
+      </c>
       <c r="AA20" s="50"/>
       <c r="AB20" s="7"/>
       <c r="AC20" s="67"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7">
-        <v>1</v>
-      </c>
+      <c r="AD20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="7"/>
       <c r="AF20" s="7"/>
       <c r="AG20" s="7"/>
-      <c r="AH20" s="7">
-        <v>2</v>
-      </c>
+      <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
-      <c r="AJ20" s="7"/>
+      <c r="AJ20" s="7">
+        <v>1</v>
+      </c>
       <c r="AK20" s="7"/>
       <c r="AL20" s="7"/>
-      <c r="AM20" s="7"/>
+      <c r="AM20" s="7">
+        <v>2</v>
+      </c>
       <c r="AN20" s="7"/>
       <c r="AO20" s="7"/>
       <c r="AP20" s="7"/>
@@ -9403,19 +9491,23 @@
       <c r="AY20" s="7"/>
       <c r="AZ20" s="28"/>
       <c r="BA20" s="23">
-        <f>SUM(B20:AY20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="BC20" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -9423,21 +9515,17 @@
       <c r="H21" s="50"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="K21" s="7">
+        <v>1</v>
+      </c>
       <c r="L21" s="7"/>
-      <c r="M21" s="7">
-        <v>3</v>
-      </c>
-      <c r="N21" s="7">
-        <v>1</v>
-      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="50"/>
-      <c r="S21" s="7">
-        <v>1</v>
-      </c>
+      <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
       <c r="V21" s="7"/>
@@ -9454,7 +9542,9 @@
       </c>
       <c r="AF21" s="7"/>
       <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
+      <c r="AH21" s="7">
+        <v>2</v>
+      </c>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
       <c r="AK21" s="7"/>
@@ -9474,43 +9564,43 @@
       <c r="AY21" s="7"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="23">
-        <f>SUM(B21:AY21)</f>
-        <v>6</v>
-      </c>
-      <c r="BB21" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="BC21" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3</v>
-      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="7">
-        <v>1</v>
-      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="50"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
+      <c r="M22" s="7">
+        <v>3</v>
+      </c>
+      <c r="N22" s="7">
+        <v>1</v>
+      </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="50"/>
-      <c r="S22" s="7"/>
+      <c r="S22" s="7">
+        <v>1</v>
+      </c>
       <c r="T22" s="7"/>
-      <c r="U22" s="32"/>
+      <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
@@ -9520,7 +9610,9 @@
       <c r="AB22" s="7"/>
       <c r="AC22" s="67"/>
       <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
+      <c r="AE22" s="7">
+        <v>1</v>
+      </c>
       <c r="AF22" s="7"/>
       <c r="AG22" s="7"/>
       <c r="AH22" s="7"/>
@@ -9543,23 +9635,29 @@
       <c r="AY22" s="7"/>
       <c r="AZ22" s="28"/>
       <c r="BA22" s="23">
-        <f>SUM(B22:AY22)</f>
-        <v>5</v>
-      </c>
-      <c r="BC22" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="BB22" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>184</v>
+        <v>90</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>3</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
       <c r="H23" s="50"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -9575,30 +9673,20 @@
       <c r="T23" s="7"/>
       <c r="U23" s="32"/>
       <c r="V23" s="7"/>
-      <c r="W23" s="7">
-        <v>1</v>
-      </c>
-      <c r="X23" s="7">
-        <v>1</v>
-      </c>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
       <c r="Y23" s="7"/>
-      <c r="Z23" s="7">
-        <v>1</v>
-      </c>
+      <c r="Z23" s="7"/>
       <c r="AA23" s="50"/>
       <c r="AB23" s="7"/>
       <c r="AC23" s="67"/>
-      <c r="AD23" s="7">
-        <v>1</v>
-      </c>
+      <c r="AD23" s="7"/>
       <c r="AE23" s="7"/>
       <c r="AF23" s="7"/>
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
       <c r="AI23" s="7"/>
-      <c r="AJ23" s="7">
-        <v>1</v>
-      </c>
+      <c r="AJ23" s="7"/>
       <c r="AK23" s="7"/>
       <c r="AL23" s="7"/>
       <c r="AM23" s="7"/>
@@ -9616,7 +9704,7 @@
       <c r="AY23" s="7"/>
       <c r="AZ23" s="28"/>
       <c r="BA23" s="23">
-        <f>SUM(B23:AY23)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="BC23" s="8">
@@ -9685,7 +9773,7 @@
       <c r="AY24" s="7"/>
       <c r="AZ24" s="28"/>
       <c r="BA24" s="23">
-        <f>SUM(B24:AY24)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -9755,7 +9843,7 @@
       <c r="AY25" s="7"/>
       <c r="AZ25" s="28"/>
       <c r="BA25" s="23">
-        <f>SUM(B25:AY25)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -9825,7 +9913,7 @@
       <c r="AY26" s="7"/>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="23">
-        <f>SUM(B26:AY26)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -9893,7 +9981,7 @@
       <c r="AY27" s="7"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="23">
-        <f>SUM(B27:AY27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -9961,7 +10049,7 @@
       <c r="AY28" s="7"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="23">
-        <f>SUM(B28:AY28)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -10025,7 +10113,7 @@
       <c r="AY29" s="7"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="23">
-        <f>SUM(B29:AY29)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="BC29" s="8">
@@ -10034,7 +10122,7 @@
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -10059,9 +10147,7 @@
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="7">
-        <v>2</v>
-      </c>
+      <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
       <c r="AA30" s="50"/>
       <c r="AB30" s="7"/>
@@ -10075,7 +10161,9 @@
       <c r="AJ30" s="7"/>
       <c r="AK30" s="7"/>
       <c r="AL30" s="7"/>
-      <c r="AM30" s="7"/>
+      <c r="AM30" s="7">
+        <v>2</v>
+      </c>
       <c r="AN30" s="7"/>
       <c r="AO30" s="7"/>
       <c r="AP30" s="7"/>
@@ -10090,13 +10178,16 @@
       <c r="AY30" s="7"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="23">
-        <f>SUM(B30:AY30)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BC30" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -10115,15 +10206,15 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="50"/>
-      <c r="S31" s="7">
-        <v>1</v>
-      </c>
+      <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
+      <c r="Y31" s="7">
+        <v>2</v>
+      </c>
       <c r="Z31" s="7"/>
       <c r="AA31" s="50"/>
       <c r="AB31" s="7"/>
@@ -10152,13 +10243,13 @@
       <c r="AY31" s="7"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="23">
-        <f>SUM(B31:AY31)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>19</v>
+        <v>156</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -10177,7 +10268,9 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="50"/>
-      <c r="S32" s="7"/>
+      <c r="S32" s="7">
+        <v>1</v>
+      </c>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
@@ -10212,13 +10305,13 @@
       <c r="AY32" s="7"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="23">
-        <f>SUM(B32:AY32)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -10272,13 +10365,13 @@
       <c r="AY33" s="7"/>
       <c r="AZ33" s="28"/>
       <c r="BA33" s="23">
-        <f>SUM(B33:AY33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -10332,13 +10425,13 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="28"/>
       <c r="BA34" s="23">
-        <f>SUM(B34:AY34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -10392,7 +10485,7 @@
       <c r="AY35" s="7"/>
       <c r="AZ35" s="28"/>
       <c r="BA35" s="23">
-        <f>SUM(B35:AY35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -10450,7 +10543,7 @@
       <c r="AY36" s="7"/>
       <c r="AZ36" s="28"/>
       <c r="BA36" s="23">
-        <f t="shared" ref="BA36" si="0">SUM(B36:AY36)</f>
+        <f t="shared" ref="BA36" si="1">SUM(B36:AY36)</f>
         <v>0</v>
       </c>
     </row>
@@ -10612,7 +10705,7 @@
       </c>
       <c r="AN38" s="8">
         <f>'League Table'!AN40</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AO38" s="8">
         <f>'League Table'!AO40</f>
@@ -10656,191 +10749,191 @@
         <v>63</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:AV40" si="1">SUM(B3:B36)</f>
+        <f t="shared" ref="B40:AV40" si="2">SUM(B3:B36)</f>
         <v>8</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="M40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="N40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="R40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="T40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="U40" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="W40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="X40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AA40" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB40" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AC40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AE40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AF40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AG40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AH40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AI40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AJ40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AK40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AL40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM40" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="AN40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AO40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AP40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AQ40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AR40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AT40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AU40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AV40" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10865,10 +10958,10 @@
   <dimension ref="A1:BA41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV9" sqref="AV9"/>
+      <selection pane="bottomRight" activeCell="BA39" sqref="BA39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -11353,7 +11446,9 @@
         <v>1</v>
       </c>
       <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
+      <c r="AN7" s="7">
+        <v>1</v>
+      </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
@@ -11367,7 +11462,7 @@
       <c r="AY7" s="7"/>
       <c r="BA7">
         <f>SUM(B7:AY7)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -11432,7 +11527,9 @@
         <v>1</v>
       </c>
       <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
+      <c r="AN8" s="18">
+        <v>1</v>
+      </c>
       <c r="AO8" s="18"/>
       <c r="AP8" s="18"/>
       <c r="AQ8" s="18"/>
@@ -11446,7 +11543,7 @@
       <c r="AY8" s="18"/>
       <c r="BA8">
         <f>SUM(B8:AY8)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
@@ -12021,20 +12118,16 @@
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="50"/>
-      <c r="I17" s="7">
-        <v>1</v>
-      </c>
+      <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -12042,16 +12135,16 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
+      <c r="Q17" s="7">
+        <v>1</v>
+      </c>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
-      <c r="X17" s="7">
-        <v>1</v>
-      </c>
+      <c r="X17" s="7"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
@@ -12060,18 +12153,20 @@
       <c r="AD17" s="7">
         <v>1</v>
       </c>
-      <c r="AE17" s="7">
-        <v>1</v>
-      </c>
+      <c r="AE17" s="7"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="7"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
-      <c r="AJ17" s="7"/>
+      <c r="AJ17" s="7">
+        <v>2</v>
+      </c>
       <c r="AK17" s="7"/>
       <c r="AL17" s="7"/>
       <c r="AM17" s="7"/>
-      <c r="AN17" s="7"/>
+      <c r="AN17" s="7">
+        <v>1</v>
+      </c>
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
       <c r="AQ17" s="7"/>
@@ -12090,29 +12185,27 @@
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="50"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7">
-        <v>1</v>
-      </c>
-      <c r="K18" s="7">
-        <v>1</v>
-      </c>
+      <c r="I18" s="7">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-      <c r="P18" s="7">
-        <v>1</v>
-      </c>
+      <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
@@ -12120,21 +12213,25 @@
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
+      <c r="X18" s="7">
+        <v>1</v>
+      </c>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
       <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
+      <c r="AD18" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="7">
+        <v>1</v>
+      </c>
       <c r="AF18" s="7"/>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
-      <c r="AJ18" s="7">
-        <v>1</v>
-      </c>
+      <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
       <c r="AL18" s="7"/>
       <c r="AM18" s="7"/>
@@ -12152,12 +12249,12 @@
       <c r="AY18" s="7"/>
       <c r="BA18">
         <f>SUM(B18:AY18)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -12167,16 +12264,20 @@
       <c r="G19" s="7"/>
       <c r="H19" s="50"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7">
-        <v>1</v>
-      </c>
+      <c r="P19" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
@@ -12189,16 +12290,14 @@
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
       <c r="AC19" s="7"/>
-      <c r="AD19" s="7">
-        <v>1</v>
-      </c>
+      <c r="AD19" s="7"/>
       <c r="AE19" s="7"/>
       <c r="AF19" s="7"/>
       <c r="AG19" s="7"/>
       <c r="AH19" s="7"/>
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="7"/>
       <c r="AL19" s="7"/>
@@ -12415,15 +12514,13 @@
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>136</v>
+        <v>228</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7">
-        <v>1</v>
-      </c>
+      <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="50"/>
       <c r="I23" s="7"/>
@@ -12452,14 +12549,18 @@
       <c r="AF23" s="7"/>
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
-      <c r="AI23" s="7">
-        <v>1</v>
-      </c>
+      <c r="AI23" s="7"/>
       <c r="AJ23" s="7"/>
-      <c r="AK23" s="7"/>
+      <c r="AK23" s="7">
+        <v>1</v>
+      </c>
       <c r="AL23" s="7"/>
-      <c r="AM23" s="7"/>
-      <c r="AN23" s="7"/>
+      <c r="AM23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="7">
+        <v>1</v>
+      </c>
       <c r="AO23" s="7"/>
       <c r="AP23" s="7"/>
       <c r="AQ23" s="7"/>
@@ -12473,12 +12574,12 @@
       <c r="AY23" s="7"/>
       <c r="BA23">
         <f>SUM(B23:AY23)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -12511,13 +12612,13 @@
       <c r="AB24" s="7"/>
       <c r="AC24" s="7"/>
       <c r="AD24" s="7"/>
-      <c r="AE24" s="7">
-        <v>1</v>
-      </c>
+      <c r="AE24" s="7"/>
       <c r="AF24" s="7"/>
       <c r="AG24" s="7"/>
       <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
+      <c r="AI24" s="7">
+        <v>1</v>
+      </c>
       <c r="AJ24" s="7"/>
       <c r="AK24" s="7"/>
       <c r="AL24" s="7"/>
@@ -12541,13 +12642,15 @@
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>218</v>
+        <v>111</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="50"/>
       <c r="I25" s="7"/>
@@ -12572,19 +12675,17 @@
       <c r="AB25" s="7"/>
       <c r="AC25" s="7"/>
       <c r="AD25" s="7"/>
-      <c r="AE25" s="7"/>
+      <c r="AE25" s="7">
+        <v>1</v>
+      </c>
       <c r="AF25" s="7"/>
       <c r="AG25" s="7"/>
       <c r="AH25" s="7"/>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
-      <c r="AK25" s="7">
-        <v>1</v>
-      </c>
+      <c r="AK25" s="7"/>
       <c r="AL25" s="7"/>
-      <c r="AM25" s="7">
-        <v>1</v>
-      </c>
+      <c r="AM25" s="7"/>
       <c r="AN25" s="7"/>
       <c r="AO25" s="7"/>
       <c r="AP25" s="7"/>
@@ -13376,10 +13477,6 @@
       <c r="AW38" s="7"/>
       <c r="AX38" s="7"/>
       <c r="AY38" s="7"/>
-      <c r="BA38">
-        <f t="shared" ref="BA38" si="0">SUM(B38:AY38)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
@@ -13492,208 +13589,208 @@
         <v>73</v>
       </c>
       <c r="B41" s="8">
-        <f t="shared" ref="B41:AH41" si="1">SUM(B5:B39)</f>
+        <f t="shared" ref="B41:AH41" si="0">SUM(B5:B39)</f>
         <v>5</v>
       </c>
       <c r="C41" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J41" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K41" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N41" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O41" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P41" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q41" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T41" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U41" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="V41" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="W41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X41" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Y41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Z41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AA41" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AB41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AE41" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AF41" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AG41" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AH41" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AI41" s="8">
+        <f t="shared" ref="AI41:AX41" si="1">SUM(AI5:AI39)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ41" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D41" s="8">
+      <c r="AK41" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="E41" s="8">
+        <v>3</v>
+      </c>
+      <c r="AL41" s="8">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F41" s="8">
+        <v>7</v>
+      </c>
+      <c r="AM41" s="8">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G41" s="8">
+        <v>2</v>
+      </c>
+      <c r="AN41" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H41" s="8">
+      <c r="AO41" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I41" s="8">
+      <c r="AP41" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="J41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ41" s="8">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="K41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR41" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS41" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT41" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU41" s="8">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="O41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV41" s="8">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="P41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AW41" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="Q41" s="8">
+        <v>0</v>
+      </c>
+      <c r="AX41" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="R41" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S41" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="T41" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U41" s="8">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="V41" s="8">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="W41" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="X41" s="8">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="Y41" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Z41" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AA41" s="8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AB41" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC41" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AD41" s="8">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AE41" s="8">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AF41" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AG41" s="8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AH41" s="8">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="AI41" s="8">
-        <f t="shared" ref="AI41:AX41" si="2">SUM(AI5:AI39)</f>
-        <v>5</v>
-      </c>
-      <c r="AJ41" s="8">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="AK41" s="8">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="AL41" s="8">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="AM41" s="8">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="AN41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AO41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AP41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AQ41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AR41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AS41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AT41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AU41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AV41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AW41" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AX41" s="8">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AY41" s="8">
-        <f t="shared" ref="AY41" si="3">SUM(AY5:AY39)</f>
+        <f t="shared" ref="AY41" si="2">SUM(AY5:AY39)</f>
         <v>0</v>
       </c>
       <c r="BA41">
         <f>SUM(B41:AZ41)</f>
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -13714,8 +13811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14720,10 +14817,18 @@
       <c r="A41" s="31">
         <v>39</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
+      <c r="B41" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="31">

</xml_diff>

<commit_message>
042 Week 48 latest data
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="YBb/v89E9RD7p/e82SSZhRrUZN6W6DhdfVypsnUF/TA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="HvgkgCul3x9/XnxcfAWwp+i3J6tG0O7IAFunAUKadpA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="240">
   <si>
     <t>MARLOW DUKES 2024</t>
   </si>
@@ -216,10 +216,10 @@
     <t>KERMIT</t>
   </si>
   <si>
-    <t>FATHER TED</t>
+    <t>ZIGZAG</t>
   </si>
   <si>
-    <t>ZIGZAG</t>
+    <t>FATHER TED</t>
   </si>
   <si>
     <t>VINCE</t>
@@ -249,13 +249,13 @@
     <t>POSH CHRIS</t>
   </si>
   <si>
-    <t>DWARF</t>
-  </si>
-  <si>
     <t>FLO</t>
   </si>
   <si>
     <t>MATT B</t>
+  </si>
+  <si>
+    <t>DWARF</t>
   </si>
   <si>
     <t>PHANTOM</t>
@@ -273,6 +273,9 @@
     <t>DOGGER</t>
   </si>
   <si>
+    <t>CARZOLA</t>
+  </si>
+  <si>
     <t>MICK</t>
   </si>
   <si>
@@ -286,9 +289,6 @@
   </si>
   <si>
     <t>GAZZA</t>
-  </si>
-  <si>
-    <t>CARZOLA</t>
   </si>
   <si>
     <t>PANDA</t>
@@ -522,13 +522,16 @@
     <t>No game</t>
   </si>
   <si>
+    <t>Bruce</t>
+  </si>
+  <si>
     <t>Bruce - Carlos</t>
   </si>
   <si>
     <t>Lost 1-8</t>
   </si>
   <si>
-    <t>Bruce</t>
+    <t>ZigZag</t>
   </si>
   <si>
     <t>Captain Kirk - Father Ted</t>
@@ -540,16 +543,13 @@
     <t>Dwarf</t>
   </si>
   <si>
+    <t>Captain Kirk</t>
+  </si>
+  <si>
     <t>Flo - Kermit</t>
   </si>
   <si>
     <t>Drew 5-5</t>
-  </si>
-  <si>
-    <t>ZigZag</t>
-  </si>
-  <si>
-    <t>Captain Kirk</t>
   </si>
   <si>
     <t>Casale - Banksy</t>
@@ -576,6 +576,9 @@
     <t>Drew 3-3</t>
   </si>
   <si>
+    <t>Matt B</t>
+  </si>
+  <si>
     <t>Dom - Duncan</t>
   </si>
   <si>
@@ -594,19 +597,16 @@
     <t>Lost 4-6</t>
   </si>
   <si>
-    <t>Dom</t>
-  </si>
-  <si>
     <t>Dwarf - Gadget</t>
   </si>
   <si>
     <t>Lost 3-6</t>
   </si>
   <si>
-    <t>Woody</t>
+    <t>Dom</t>
   </si>
   <si>
-    <t>Matt B</t>
+    <t>Woody</t>
   </si>
   <si>
     <t>Father Ted - Posh</t>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>Lost 4-5</t>
+  </si>
+  <si>
+    <t>Capt Kirk - Flo</t>
   </si>
 </sst>
 </file>
@@ -1386,8 +1389,8 @@
     <col customWidth="1" min="42" max="42" width="6.43" outlineLevel="1"/>
     <col customWidth="1" min="43" max="49" width="6.71" outlineLevel="1"/>
     <col customWidth="1" min="50" max="50" width="8.29" outlineLevel="1"/>
-    <col customWidth="1" min="51" max="53" width="9.14"/>
-    <col customWidth="1" min="54" max="56" width="8.86"/>
+    <col customWidth="1" min="51" max="54" width="9.14"/>
+    <col customWidth="1" min="55" max="56" width="8.86"/>
     <col customWidth="1" min="57" max="57" width="10.29"/>
     <col customWidth="1" min="58" max="62" width="8.86"/>
   </cols>
@@ -1942,17 +1945,19 @@
       <c r="AV5" s="15">
         <v>4.0</v>
       </c>
-      <c r="AW5" s="16"/>
+      <c r="AW5" s="16">
+        <v>-3.0</v>
+      </c>
       <c r="AX5" s="16"/>
       <c r="AY5" s="19"/>
       <c r="AZ5" s="19"/>
       <c r="BA5" s="19">
         <v>1.0</v>
       </c>
-      <c r="BB5" s="5"/>
+      <c r="BB5" s="19"/>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC39" si="1">COUNT(B5:AX5)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD39" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
@@ -1964,7 +1969,7 @@
       </c>
       <c r="BF5" s="5">
         <f t="shared" ref="BF5:BF39" si="4">COUNTIF($B5:$AX5, "&lt;0")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BG5" s="5">
         <f t="shared" ref="BG5:BG39" si="5">SUM(BD5*3)+BE5</f>
@@ -1972,11 +1977,11 @@
       </c>
       <c r="BH5" s="5">
         <f t="shared" ref="BH5:BH39" si="6">SUM(B5:AX5)</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="BI5" s="20">
         <f t="shared" ref="BI5:BI39" si="7">SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.5982905983</v>
+        <v>0.5833333333</v>
       </c>
       <c r="BJ5" s="20"/>
     </row>
@@ -2109,17 +2114,19 @@
       <c r="AV6" s="24">
         <v>-4.0</v>
       </c>
-      <c r="AW6" s="22"/>
+      <c r="AW6" s="22">
+        <v>-3.0</v>
+      </c>
       <c r="AX6" s="22"/>
       <c r="AY6" s="19"/>
       <c r="AZ6" s="19"/>
       <c r="BA6" s="19">
         <v>2.0</v>
       </c>
-      <c r="BB6" s="5"/>
+      <c r="BB6" s="19"/>
       <c r="BC6" s="5">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="2"/>
@@ -2131,7 +2138,7 @@
       </c>
       <c r="BF6" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BG6" s="5">
         <f t="shared" si="5"/>
@@ -2139,11 +2146,11 @@
       </c>
       <c r="BH6" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BI6" s="20">
         <f t="shared" si="7"/>
-        <v>0.5213675214</v>
+        <v>0.5083333333</v>
       </c>
       <c r="BJ6" s="20"/>
     </row>
@@ -2283,7 +2290,7 @@
       <c r="BA7" s="19">
         <v>3.0</v>
       </c>
-      <c r="BB7" s="5"/>
+      <c r="BB7" s="19"/>
       <c r="BC7" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2437,21 +2444,23 @@
       <c r="AV8" s="16">
         <v>-4.0</v>
       </c>
-      <c r="AW8" s="16"/>
+      <c r="AW8" s="16">
+        <v>3.0</v>
+      </c>
       <c r="AX8" s="16"/>
       <c r="AY8" s="19"/>
       <c r="AZ8" s="19"/>
       <c r="BA8" s="19">
         <v>4.0</v>
       </c>
-      <c r="BB8" s="5"/>
+      <c r="BB8" s="19"/>
       <c r="BC8" s="5">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="3"/>
@@ -2463,15 +2472,15 @@
       </c>
       <c r="BG8" s="5">
         <f t="shared" si="5"/>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="BH8" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BI8" s="20">
         <f t="shared" si="7"/>
-        <v>0.5092592593</v>
+        <v>0.5225225225</v>
       </c>
       <c r="BJ8" s="20"/>
     </row>
@@ -2601,7 +2610,7 @@
       <c r="BA9" s="19">
         <v>5.0</v>
       </c>
-      <c r="BB9" s="5"/>
+      <c r="BB9" s="19"/>
       <c r="BC9" s="5">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2636,57 +2645,55 @@
       <c r="A10" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="32">
+        <v>1.0</v>
+      </c>
       <c r="C10" s="32">
         <v>1.0</v>
       </c>
       <c r="D10" s="32">
         <v>9.0</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>1.0</v>
+      </c>
       <c r="G10" s="32">
         <v>0.0</v>
       </c>
       <c r="H10" s="33"/>
-      <c r="I10" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="J10" s="34">
-        <v>8.0</v>
-      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="32">
-        <v>-2.0</v>
-      </c>
-      <c r="M10" s="32">
-        <v>-1.0</v>
-      </c>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
-      <c r="P10" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
       <c r="R10" s="33"/>
-      <c r="S10" s="34">
+      <c r="S10" s="32">
         <v>-2.0</v>
       </c>
-      <c r="T10" s="32">
+      <c r="T10" s="34">
         <v>1.0</v>
       </c>
-      <c r="U10" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="V10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="34">
+        <v>8.0</v>
+      </c>
       <c r="W10" s="32">
         <v>0.0</v>
       </c>
-      <c r="X10" s="32"/>
+      <c r="X10" s="32">
+        <v>-5.0</v>
+      </c>
       <c r="Y10" s="32">
         <v>0.0</v>
       </c>
-      <c r="Z10" s="34">
+      <c r="Z10" s="32">
         <v>2.0</v>
       </c>
       <c r="AA10" s="33"/>
@@ -2698,22 +2705,30 @@
         <v>0.0</v>
       </c>
       <c r="AE10" s="32">
-        <v>4.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AF10" s="32">
         <v>-2.0</v>
       </c>
       <c r="AG10" s="32">
-        <v>-5.0</v>
-      </c>
-      <c r="AH10" s="32"/>
-      <c r="AI10" s="32"/>
+        <v>5.0</v>
+      </c>
+      <c r="AH10" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="AI10" s="32">
+        <v>1.0</v>
+      </c>
       <c r="AJ10" s="32">
         <v>-1.0</v>
       </c>
-      <c r="AK10" s="32"/>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="32">
+      <c r="AK10" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="AL10" s="32">
+        <v>-1.0</v>
+      </c>
+      <c r="AM10" s="34">
         <v>0.0</v>
       </c>
       <c r="AN10" s="32">
@@ -2722,38 +2737,44 @@
       <c r="AO10" s="32">
         <v>4.0</v>
       </c>
-      <c r="AP10" s="32"/>
+      <c r="AP10" s="32">
+        <v>-1.0</v>
+      </c>
       <c r="AQ10" s="32">
         <v>-4.0</v>
       </c>
       <c r="AR10" s="32">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AS10" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="AT10" s="32"/>
+        <v>-2.0</v>
+      </c>
+      <c r="AT10" s="32">
+        <v>-1.0</v>
+      </c>
       <c r="AU10" s="32">
         <v>1.0</v>
       </c>
       <c r="AV10" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="AW10" s="32"/>
+        <v>-4.0</v>
+      </c>
+      <c r="AW10" s="32">
+        <v>3.0</v>
+      </c>
       <c r="AX10" s="32"/>
       <c r="AY10" s="19"/>
       <c r="AZ10" s="19"/>
       <c r="BA10" s="19">
         <v>6.0</v>
       </c>
-      <c r="BB10" s="5"/>
+      <c r="BB10" s="19"/>
       <c r="BC10" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="3"/>
@@ -2761,19 +2782,19 @@
       </c>
       <c r="BF10" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="BG10" s="5">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="BH10" s="5">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="BI10" s="20">
         <f t="shared" si="7"/>
-        <v>0.5714285714</v>
+        <v>0.5</v>
       </c>
       <c r="BJ10" s="20"/>
     </row>
@@ -2781,55 +2802,57 @@
       <c r="A11" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="B11" s="27"/>
       <c r="C11" s="27">
         <v>1.0</v>
       </c>
       <c r="D11" s="27">
         <v>9.0</v>
       </c>
-      <c r="E11" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="F11" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="27">
         <v>0.0</v>
       </c>
       <c r="H11" s="29"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="I11" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>8.0</v>
+      </c>
       <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+      <c r="L11" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="M11" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
+      <c r="P11" s="27">
+        <v>2.0</v>
+      </c>
       <c r="Q11" s="27"/>
       <c r="R11" s="29"/>
-      <c r="S11" s="27">
+      <c r="S11" s="28">
         <v>-2.0</v>
       </c>
-      <c r="T11" s="28">
+      <c r="T11" s="27">
         <v>1.0</v>
       </c>
-      <c r="U11" s="27"/>
-      <c r="V11" s="28">
-        <v>8.0</v>
-      </c>
+      <c r="U11" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="V11" s="27"/>
       <c r="W11" s="27">
         <v>0.0</v>
       </c>
-      <c r="X11" s="27">
-        <v>-5.0</v>
-      </c>
+      <c r="X11" s="27"/>
       <c r="Y11" s="27">
         <v>0.0</v>
       </c>
-      <c r="Z11" s="27">
+      <c r="Z11" s="28">
         <v>2.0</v>
       </c>
       <c r="AA11" s="29"/>
@@ -2841,30 +2864,22 @@
         <v>0.0</v>
       </c>
       <c r="AE11" s="27">
-        <v>-4.0</v>
+        <v>4.0</v>
       </c>
       <c r="AF11" s="27">
         <v>-2.0</v>
       </c>
       <c r="AG11" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="AH11" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AI11" s="27">
-        <v>1.0</v>
-      </c>
+        <v>-5.0</v>
+      </c>
+      <c r="AH11" s="27"/>
+      <c r="AI11" s="27"/>
       <c r="AJ11" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AK11" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AL11" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AM11" s="28">
+      <c r="AK11" s="27"/>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27">
         <v>0.0</v>
       </c>
       <c r="AN11" s="27">
@@ -2873,38 +2888,36 @@
       <c r="AO11" s="27">
         <v>4.0</v>
       </c>
-      <c r="AP11" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="AP11" s="27"/>
       <c r="AQ11" s="27">
         <v>-4.0</v>
       </c>
       <c r="AR11" s="27">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AS11" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="AT11" s="27">
-        <v>-1.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="AT11" s="27"/>
       <c r="AU11" s="27">
         <v>1.0</v>
       </c>
       <c r="AV11" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="AW11" s="27"/>
+        <v>4.0</v>
+      </c>
+      <c r="AW11" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AX11" s="27"/>
       <c r="AY11" s="19"/>
       <c r="AZ11" s="19"/>
       <c r="BA11" s="19">
         <v>7.0</v>
       </c>
-      <c r="BB11" s="5"/>
+      <c r="BB11" s="19"/>
       <c r="BC11" s="5">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="2"/>
@@ -2916,7 +2929,7 @@
       </c>
       <c r="BF11" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="BG11" s="5">
         <f t="shared" si="5"/>
@@ -2924,11 +2937,11 @@
       </c>
       <c r="BH11" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="BI11" s="20">
         <f t="shared" si="7"/>
-        <v>0.4848484848</v>
+        <v>0.5517241379</v>
       </c>
       <c r="BJ11" s="20"/>
     </row>
@@ -3058,7 +3071,7 @@
       <c r="BA12" s="19">
         <v>8.0</v>
       </c>
-      <c r="BB12" s="5"/>
+      <c r="BB12" s="19"/>
       <c r="BC12" s="5">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -3212,17 +3225,19 @@
       <c r="AV13" s="27">
         <v>4.0</v>
       </c>
-      <c r="AW13" s="27"/>
+      <c r="AW13" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AX13" s="27"/>
       <c r="AY13" s="19"/>
       <c r="AZ13" s="19"/>
       <c r="BA13" s="19">
         <v>9.0</v>
       </c>
-      <c r="BB13" s="5"/>
+      <c r="BB13" s="19"/>
       <c r="BC13" s="5">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="2"/>
@@ -3234,7 +3249,7 @@
       </c>
       <c r="BF13" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BG13" s="5">
         <f t="shared" si="5"/>
@@ -3242,11 +3257,11 @@
       </c>
       <c r="BH13" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="BI13" s="20">
         <f t="shared" si="7"/>
-        <v>0.4351851852</v>
+        <v>0.4234234234</v>
       </c>
       <c r="BJ13" s="20"/>
     </row>
@@ -3356,7 +3371,7 @@
       <c r="BA14" s="19">
         <v>10.0</v>
       </c>
-      <c r="BB14" s="5"/>
+      <c r="BB14" s="19"/>
       <c r="BC14" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -3498,17 +3513,19 @@
         <v>1.0</v>
       </c>
       <c r="AV15" s="27"/>
-      <c r="AW15" s="27"/>
+      <c r="AW15" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AX15" s="27"/>
       <c r="AY15" s="19"/>
       <c r="AZ15" s="19"/>
       <c r="BA15" s="19">
         <v>11.0</v>
       </c>
-      <c r="BB15" s="5"/>
+      <c r="BB15" s="19"/>
       <c r="BC15" s="5">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="2"/>
@@ -3520,7 +3537,7 @@
       </c>
       <c r="BF15" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BG15" s="5">
         <f t="shared" si="5"/>
@@ -3528,11 +3545,11 @@
       </c>
       <c r="BH15" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="BI15" s="20">
         <f t="shared" si="7"/>
-        <v>0.4666666667</v>
+        <v>0.4516129032</v>
       </c>
       <c r="BJ15" s="20"/>
     </row>
@@ -3643,17 +3660,19 @@
       <c r="AV16" s="27">
         <v>4.0</v>
       </c>
-      <c r="AW16" s="27"/>
+      <c r="AW16" s="28">
+        <v>-3.0</v>
+      </c>
       <c r="AX16" s="27"/>
       <c r="AY16" s="19"/>
       <c r="AZ16" s="19"/>
       <c r="BA16" s="19">
         <v>12.0</v>
       </c>
-      <c r="BB16" s="5"/>
+      <c r="BB16" s="19"/>
       <c r="BC16" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="2"/>
@@ -3665,7 +3684,7 @@
       </c>
       <c r="BF16" s="5">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BG16" s="5">
         <f t="shared" si="5"/>
@@ -3673,11 +3692,11 @@
       </c>
       <c r="BH16" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="BI16" s="20">
         <f t="shared" si="7"/>
-        <v>0.4880952381</v>
+        <v>0.4712643678</v>
       </c>
       <c r="BJ16" s="20"/>
     </row>
@@ -3786,17 +3805,19 @@
       <c r="AV17" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AW17" s="27"/>
+      <c r="AW17" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AX17" s="27"/>
       <c r="AY17" s="19"/>
       <c r="AZ17" s="19"/>
       <c r="BA17" s="19">
         <v>13.0</v>
       </c>
-      <c r="BB17" s="5"/>
+      <c r="BB17" s="19"/>
       <c r="BC17" s="5">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="2"/>
@@ -3808,7 +3829,7 @@
       </c>
       <c r="BF17" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BG17" s="5">
         <f t="shared" si="5"/>
@@ -3816,11 +3837,11 @@
       </c>
       <c r="BH17" s="5">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="BI17" s="20">
         <f t="shared" si="7"/>
-        <v>0.4814814815</v>
+        <v>0.4642857143</v>
       </c>
       <c r="BJ17" s="20"/>
     </row>
@@ -3938,7 +3959,7 @@
       <c r="BA18" s="19">
         <v>14.0</v>
       </c>
-      <c r="BB18" s="5"/>
+      <c r="BB18" s="19"/>
       <c r="BC18" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -4093,7 +4114,7 @@
       <c r="BA19" s="19">
         <v>15.0</v>
       </c>
-      <c r="BB19" s="5"/>
+      <c r="BB19" s="19"/>
       <c r="BC19" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -4231,21 +4252,23 @@
       <c r="AV20" s="27">
         <v>4.0</v>
       </c>
-      <c r="AW20" s="27"/>
+      <c r="AW20" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AX20" s="27"/>
       <c r="AY20" s="19"/>
       <c r="AZ20" s="19"/>
       <c r="BA20" s="19">
         <v>16.0</v>
       </c>
-      <c r="BB20" s="5"/>
+      <c r="BB20" s="19"/>
       <c r="BC20" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="3"/>
@@ -4257,15 +4280,15 @@
       </c>
       <c r="BG20" s="5">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="BH20" s="5">
         <f t="shared" si="6"/>
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="BI20" s="20">
         <f t="shared" si="7"/>
-        <v>0.3928571429</v>
+        <v>0.4137931034</v>
       </c>
       <c r="BJ20" s="20"/>
     </row>
@@ -4273,110 +4296,112 @@
       <c r="A21" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="C21" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D21" s="27">
-        <v>-9.0</v>
-      </c>
-      <c r="E21" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="29"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27">
         <v>-8.0</v>
       </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="M21" s="27"/>
+      <c r="K21" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="N21" s="27"/>
       <c r="O21" s="27"/>
       <c r="P21" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="Q21" s="28">
-        <v>-3.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="Q21" s="27"/>
       <c r="R21" s="29"/>
-      <c r="S21" s="27"/>
+      <c r="S21" s="27">
+        <v>2.0</v>
+      </c>
       <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
+      <c r="U21" s="27">
+        <v>4.0</v>
+      </c>
       <c r="V21" s="27"/>
       <c r="W21" s="27">
         <v>0.0</v>
       </c>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
+      <c r="X21" s="27">
+        <v>5.0</v>
+      </c>
+      <c r="Y21" s="28">
+        <v>0.0</v>
+      </c>
       <c r="Z21" s="27">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AA21" s="29"/>
       <c r="AB21" s="27">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AC21" s="30"/>
       <c r="AD21" s="27">
         <v>0.0</v>
       </c>
       <c r="AE21" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AF21" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="AG21" s="27">
+        <v>-5.0</v>
+      </c>
+      <c r="AH21" s="27"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AL21" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AM21" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AN21" s="27"/>
+      <c r="AO21" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AF21" s="27">
+      <c r="AP21" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="AQ21" s="27"/>
+      <c r="AR21" s="27">
         <v>2.0</v>
-      </c>
-      <c r="AG21" s="27"/>
-      <c r="AH21" s="27"/>
-      <c r="AI21" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="27"/>
-      <c r="AL21" s="27"/>
-      <c r="AM21" s="27"/>
-      <c r="AN21" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="AO21" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AP21" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AQ21" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="AR21" s="27">
-        <v>-2.0</v>
       </c>
       <c r="AS21" s="27">
         <v>-2.0</v>
       </c>
       <c r="AT21" s="27"/>
-      <c r="AU21" s="27"/>
-      <c r="AV21" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AW21" s="27"/>
+      <c r="AU21" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="AV21" s="27"/>
+      <c r="AW21" s="28">
+        <v>3.0</v>
+      </c>
       <c r="AX21" s="27"/>
       <c r="AY21" s="19"/>
       <c r="AZ21" s="19"/>
       <c r="BA21" s="19">
         <v>17.0</v>
       </c>
-      <c r="BB21" s="5"/>
+      <c r="BB21" s="19"/>
       <c r="BC21" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BD21" s="5">
         <f t="shared" si="2"/>
@@ -4384,23 +4409,23 @@
       </c>
       <c r="BE21" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BF21" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BG21" s="5">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="BH21" s="5">
         <f t="shared" si="6"/>
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="BI21" s="20">
         <f t="shared" si="7"/>
-        <v>0.4782608696</v>
+        <v>0.4861111111</v>
       </c>
       <c r="BJ21" s="20"/>
     </row>
@@ -4409,133 +4434,135 @@
         <v>76</v>
       </c>
       <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="C22" s="27">
+        <v>1.0</v>
+      </c>
       <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
+      <c r="E22" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="27">
+        <v>1.0</v>
+      </c>
       <c r="G22" s="27"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27">
-        <v>-8.0</v>
-      </c>
-      <c r="K22" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="I22" s="27">
+        <v>-7.0</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
       <c r="L22" s="27"/>
-      <c r="M22" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="M22" s="27"/>
       <c r="N22" s="27"/>
       <c r="O22" s="27"/>
       <c r="P22" s="27">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="Q22" s="27"/>
       <c r="R22" s="29"/>
       <c r="S22" s="27">
         <v>2.0</v>
       </c>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="T22" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="U22" s="27"/>
       <c r="V22" s="27"/>
       <c r="W22" s="27">
         <v>0.0</v>
       </c>
-      <c r="X22" s="27">
+      <c r="X22" s="28">
         <v>5.0</v>
       </c>
-      <c r="Y22" s="28">
+      <c r="Y22" s="27">
         <v>0.0</v>
       </c>
-      <c r="Z22" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="Z22" s="27"/>
       <c r="AA22" s="29"/>
       <c r="AB22" s="27">
         <v>-1.0</v>
       </c>
       <c r="AC22" s="30"/>
-      <c r="AD22" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AD22" s="27"/>
       <c r="AE22" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AF22" s="28">
+        <v>-4.0</v>
+      </c>
+      <c r="AF22" s="27"/>
+      <c r="AG22" s="27"/>
+      <c r="AH22" s="27">
         <v>-2.0</v>
       </c>
-      <c r="AG22" s="27">
-        <v>-5.0</v>
-      </c>
-      <c r="AH22" s="27"/>
-      <c r="AI22" s="27"/>
+      <c r="AI22" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ22" s="27"/>
       <c r="AK22" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AL22" s="27">
-        <v>1.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="AL22" s="27"/>
       <c r="AM22" s="27">
         <v>0.0</v>
       </c>
-      <c r="AN22" s="27"/>
-      <c r="AO22" s="27">
+      <c r="AN22" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AO22" s="28">
         <v>-4.0</v>
       </c>
       <c r="AP22" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AQ22" s="27"/>
-      <c r="AR22" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AQ22" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AR22" s="27"/>
       <c r="AS22" s="27">
         <v>-2.0</v>
       </c>
       <c r="AT22" s="27"/>
       <c r="AU22" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AV22" s="27"/>
-      <c r="AW22" s="27"/>
+        <v>1.0</v>
+      </c>
+      <c r="AV22" s="27">
+        <v>-4.0</v>
+      </c>
+      <c r="AW22" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AX22" s="27"/>
       <c r="AY22" s="19"/>
       <c r="AZ22" s="19"/>
       <c r="BA22" s="19">
         <v>18.0</v>
       </c>
-      <c r="BB22" s="5"/>
+      <c r="BB22" s="19"/>
       <c r="BC22" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BD22" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BE22" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF22" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BG22" s="5">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="BH22" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="BI22" s="20">
         <f t="shared" si="7"/>
-        <v>0.4637681159</v>
+        <v>0.4722222222</v>
       </c>
       <c r="BJ22" s="20"/>
     </row>
@@ -4543,12 +4570,16 @@
       <c r="A23" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27">
+      <c r="B23" s="27">
         <v>1.0</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28">
+      <c r="C23" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="D23" s="27">
+        <v>-9.0</v>
+      </c>
+      <c r="E23" s="27">
         <v>1.0</v>
       </c>
       <c r="F23" s="27">
@@ -4556,85 +4587,81 @@
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="29"/>
-      <c r="I23" s="27">
-        <v>-7.0</v>
-      </c>
-      <c r="J23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27">
+        <v>-8.0</v>
+      </c>
       <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+      <c r="L23" s="27">
+        <v>2.0</v>
+      </c>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27">
         <v>-2.0</v>
       </c>
-      <c r="Q23" s="27"/>
+      <c r="Q23" s="28">
+        <v>-3.0</v>
+      </c>
       <c r="R23" s="29"/>
-      <c r="S23" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="T23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
       <c r="W23" s="27">
         <v>0.0</v>
       </c>
-      <c r="X23" s="28">
-        <v>5.0</v>
-      </c>
-      <c r="Y23" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="Z23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="AA23" s="29"/>
       <c r="AB23" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AC23" s="30"/>
-      <c r="AD23" s="27"/>
+      <c r="AD23" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AE23" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AF23" s="27"/>
+      <c r="AF23" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AG23" s="27"/>
-      <c r="AH23" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="AI23" s="27">
+      <c r="AH23" s="27"/>
+      <c r="AI23" s="28">
         <v>1.0</v>
       </c>
       <c r="AJ23" s="27"/>
-      <c r="AK23" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="AK23" s="27"/>
       <c r="AL23" s="27"/>
-      <c r="AM23" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AM23" s="27"/>
       <c r="AN23" s="27">
         <v>0.0</v>
       </c>
-      <c r="AO23" s="28">
+      <c r="AO23" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AP23" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AQ23" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AP23" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AQ23" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AR23" s="27"/>
+      <c r="AR23" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="AS23" s="27">
         <v>-2.0</v>
       </c>
       <c r="AT23" s="27"/>
-      <c r="AU23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AU23" s="27"/>
       <c r="AV23" s="27">
-        <v>-4.0</v>
+        <v>4.0</v>
       </c>
       <c r="AW23" s="27"/>
       <c r="AX23" s="27"/>
@@ -4643,18 +4670,18 @@
       <c r="BA23" s="19">
         <v>19.0</v>
       </c>
-      <c r="BB23" s="5"/>
+      <c r="BB23" s="19"/>
       <c r="BC23" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BE23" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BF23" s="5">
         <f t="shared" si="4"/>
@@ -4662,15 +4689,15 @@
       </c>
       <c r="BG23" s="5">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="BH23" s="5">
         <f t="shared" si="6"/>
-        <v>-11</v>
+        <v>-19</v>
       </c>
       <c r="BI23" s="20">
         <f t="shared" si="7"/>
-        <v>0.4492753623</v>
+        <v>0.4782608696</v>
       </c>
       <c r="BJ23" s="20"/>
     </row>
@@ -4760,7 +4787,7 @@
       <c r="BA24" s="19">
         <v>20.0</v>
       </c>
-      <c r="BB24" s="5"/>
+      <c r="BB24" s="19"/>
       <c r="BC24" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4873,7 +4900,7 @@
       <c r="BA25" s="19">
         <v>21.0</v>
       </c>
-      <c r="BB25" s="5"/>
+      <c r="BB25" s="19"/>
       <c r="BC25" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4980,7 +5007,7 @@
       <c r="BA26" s="19">
         <v>22.0</v>
       </c>
-      <c r="BB26" s="5"/>
+      <c r="BB26" s="19"/>
       <c r="BC26" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -5093,7 +5120,7 @@
       <c r="BA27" s="19">
         <v>23.0</v>
       </c>
-      <c r="BB27" s="5"/>
+      <c r="BB27" s="19"/>
       <c r="BC27" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5198,7 +5225,7 @@
       <c r="BA28" s="19">
         <v>24.0</v>
       </c>
-      <c r="BB28" s="5"/>
+      <c r="BB28" s="19"/>
       <c r="BC28" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -5242,21 +5269,25 @@
       <c r="H29" s="29"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
+      <c r="K29" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="L29" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="M29" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="N29" s="27"/>
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
       <c r="Q29" s="27">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="R29" s="29"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
-      <c r="U29" s="27">
-        <v>-4.0</v>
-      </c>
+      <c r="U29" s="27"/>
       <c r="V29" s="27">
         <v>-8.0</v>
       </c>
@@ -5267,62 +5298,58 @@
       <c r="AA29" s="29"/>
       <c r="AB29" s="27"/>
       <c r="AC29" s="30"/>
-      <c r="AD29" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AD29" s="27"/>
       <c r="AE29" s="27"/>
       <c r="AF29" s="27"/>
       <c r="AG29" s="27"/>
       <c r="AH29" s="27"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI29" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="AJ29" s="27"/>
       <c r="AK29" s="27"/>
-      <c r="AL29" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="AL29" s="27"/>
       <c r="AM29" s="27"/>
-      <c r="AN29" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AN29" s="27"/>
       <c r="AO29" s="27"/>
-      <c r="AP29" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="AQ29" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="27"/>
       <c r="AR29" s="27">
         <v>-2.0</v>
       </c>
       <c r="AS29" s="27"/>
-      <c r="AT29" s="27"/>
-      <c r="AU29" s="27"/>
+      <c r="AT29" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AU29" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AV29" s="27"/>
-      <c r="AW29" s="27"/>
+      <c r="AW29" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AX29" s="27"/>
       <c r="AY29" s="19"/>
       <c r="AZ29" s="19"/>
       <c r="BA29" s="19">
         <v>25.0</v>
       </c>
-      <c r="BB29" s="5"/>
+      <c r="BB29" s="19"/>
       <c r="BC29" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD29" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BE29" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BF29" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BG29" s="5">
         <f t="shared" si="5"/>
@@ -5330,7 +5357,7 @@
       </c>
       <c r="BH29" s="5">
         <f t="shared" si="6"/>
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="BI29" s="20">
         <f t="shared" si="7"/>
@@ -5344,13 +5371,9 @@
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
-      <c r="D30" s="27">
-        <v>9.0</v>
-      </c>
+      <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="F30" s="27"/>
       <c r="G30" s="27"/>
       <c r="H30" s="29"/>
       <c r="I30" s="27"/>
@@ -5361,12 +5384,18 @@
       <c r="N30" s="27"/>
       <c r="O30" s="27"/>
       <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
+      <c r="Q30" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="R30" s="29"/>
       <c r="S30" s="27"/>
       <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
+      <c r="U30" s="27">
+        <v>-4.0</v>
+      </c>
+      <c r="V30" s="27">
+        <v>-8.0</v>
+      </c>
       <c r="W30" s="27"/>
       <c r="X30" s="27"/>
       <c r="Y30" s="27"/>
@@ -5374,25 +5403,35 @@
       <c r="AA30" s="29"/>
       <c r="AB30" s="27"/>
       <c r="AC30" s="30"/>
-      <c r="AD30" s="27"/>
+      <c r="AD30" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AE30" s="27"/>
       <c r="AF30" s="27"/>
       <c r="AG30" s="27"/>
-      <c r="AH30" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AI30" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AJ30" s="27"/>
+      <c r="AH30" s="27"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AK30" s="27"/>
-      <c r="AL30" s="27"/>
+      <c r="AL30" s="28">
+        <v>0.0</v>
+      </c>
       <c r="AM30" s="27"/>
-      <c r="AN30" s="27"/>
+      <c r="AN30" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AO30" s="27"/>
-      <c r="AP30" s="27"/>
-      <c r="AQ30" s="27"/>
-      <c r="AR30" s="27"/>
+      <c r="AP30" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AQ30" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AR30" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="AS30" s="27"/>
       <c r="AT30" s="27"/>
       <c r="AU30" s="27"/>
@@ -5404,34 +5443,34 @@
       <c r="BA30" s="19">
         <v>26.0</v>
       </c>
-      <c r="BB30" s="5"/>
+      <c r="BB30" s="19"/>
       <c r="BC30" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="BD30" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BE30" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BF30" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BG30" s="5">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BH30" s="5">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>-12</v>
       </c>
       <c r="BI30" s="20">
         <f t="shared" si="7"/>
-        <v>0.75</v>
+        <v>0.3333333333</v>
       </c>
       <c r="BJ30" s="20"/>
     </row>
@@ -5441,52 +5480,32 @@
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="D31" s="27">
+        <v>9.0</v>
+      </c>
+      <c r="E31" s="27"/>
       <c r="F31" s="27">
         <v>1.0</v>
       </c>
-      <c r="G31" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="G31" s="27"/>
       <c r="H31" s="29"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
-      <c r="M31" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="M31" s="27"/>
       <c r="N31" s="27"/>
-      <c r="O31" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="P31" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="Q31" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
       <c r="R31" s="29"/>
-      <c r="S31" s="27">
-        <v>-2.0</v>
-      </c>
+      <c r="S31" s="27"/>
       <c r="T31" s="27"/>
-      <c r="U31" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="V31" s="27">
-        <v>-8.0</v>
-      </c>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
       <c r="W31" s="27"/>
-      <c r="X31" s="27">
-        <v>-5.0</v>
-      </c>
-      <c r="Y31" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
       <c r="Z31" s="27"/>
       <c r="AA31" s="29"/>
       <c r="AB31" s="27"/>
@@ -5495,8 +5514,12 @@
       <c r="AE31" s="27"/>
       <c r="AF31" s="27"/>
       <c r="AG31" s="27"/>
-      <c r="AH31" s="27"/>
-      <c r="AI31" s="27"/>
+      <c r="AH31" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AI31" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AJ31" s="27"/>
       <c r="AK31" s="27"/>
       <c r="AL31" s="27"/>
@@ -5517,34 +5540,34 @@
       <c r="BA31" s="19">
         <v>27.0</v>
       </c>
-      <c r="BB31" s="5"/>
+      <c r="BB31" s="19"/>
       <c r="BC31" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="BD31" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BE31" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF31" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="BG31" s="5">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BH31" s="5">
         <f t="shared" si="6"/>
-        <v>-20</v>
+        <v>11</v>
       </c>
       <c r="BI31" s="20">
         <f t="shared" si="7"/>
-        <v>0.2222222222</v>
+        <v>0.75</v>
       </c>
       <c r="BJ31" s="20"/>
     </row>
@@ -5555,35 +5578,51 @@
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
+      <c r="E32" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="F32" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0.0</v>
+      </c>
       <c r="H32" s="29"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
       <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
+      <c r="M32" s="28">
+        <v>-1.0</v>
+      </c>
       <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
+      <c r="O32" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="P32" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="Q32" s="27">
+        <v>3.0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="T32" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="U32" s="27"/>
+        <v>-2.0</v>
+      </c>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27">
+        <v>-4.0</v>
+      </c>
       <c r="V32" s="27">
-        <v>8.0</v>
-      </c>
-      <c r="W32" s="27">
+        <v>-8.0</v>
+      </c>
+      <c r="W32" s="27"/>
+      <c r="X32" s="27">
+        <v>-5.0</v>
+      </c>
+      <c r="Y32" s="27">
         <v>0.0</v>
       </c>
-      <c r="X32" s="27"/>
-      <c r="Y32" s="27"/>
       <c r="Z32" s="27"/>
       <c r="AA32" s="29"/>
       <c r="AB32" s="27"/>
@@ -5614,10 +5653,10 @@
       <c r="BA32" s="19">
         <v>28.0</v>
       </c>
-      <c r="BB32" s="5"/>
+      <c r="BB32" s="19"/>
       <c r="BC32" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="BD32" s="5">
         <f t="shared" si="2"/>
@@ -5625,23 +5664,23 @@
       </c>
       <c r="BE32" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BF32" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="BG32" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BH32" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>-20</v>
       </c>
       <c r="BI32" s="20">
         <f t="shared" si="7"/>
-        <v>0.5833333333</v>
+        <v>0.2222222222</v>
       </c>
       <c r="BJ32" s="20"/>
     </row>
@@ -5649,22 +5688,12 @@
       <c r="A33" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="C33" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="D33" s="28">
-        <v>9.0</v>
-      </c>
-      <c r="E33" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="G33" s="27"/>
       <c r="H33" s="29"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
@@ -5676,11 +5705,19 @@
       <c r="P33" s="27"/>
       <c r="Q33" s="27"/>
       <c r="R33" s="29"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
+      <c r="S33" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="T33" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-      <c r="W33" s="27"/>
+      <c r="V33" s="27">
+        <v>8.0</v>
+      </c>
+      <c r="W33" s="27">
+        <v>0.0</v>
+      </c>
       <c r="X33" s="27"/>
       <c r="Y33" s="27"/>
       <c r="Z33" s="27"/>
@@ -5713,10 +5750,10 @@
       <c r="BA33" s="19">
         <v>29.0</v>
       </c>
-      <c r="BB33" s="5"/>
+      <c r="BB33" s="19"/>
       <c r="BC33" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD33" s="5">
         <f t="shared" si="2"/>
@@ -5728,7 +5765,7 @@
       </c>
       <c r="BF33" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG33" s="5">
         <f t="shared" si="5"/>
@@ -5736,11 +5773,11 @@
       </c>
       <c r="BH33" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BI33" s="20">
         <f t="shared" si="7"/>
-        <v>0.4666666667</v>
+        <v>0.5833333333</v>
       </c>
       <c r="BJ33" s="20"/>
     </row>
@@ -5748,37 +5785,37 @@
       <c r="A34" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+      <c r="B34" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="C34" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="D34" s="28">
+        <v>9.0</v>
+      </c>
+      <c r="E34" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
+      <c r="G34" s="27">
+        <v>0.0</v>
+      </c>
       <c r="H34" s="29"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
-      <c r="K34" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="L34" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="M34" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
       <c r="N34" s="27"/>
       <c r="O34" s="27"/>
       <c r="P34" s="27"/>
-      <c r="Q34" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="Q34" s="27"/>
       <c r="R34" s="29"/>
       <c r="S34" s="27"/>
       <c r="T34" s="27"/>
       <c r="U34" s="27"/>
-      <c r="V34" s="27">
-        <v>-8.0</v>
-      </c>
+      <c r="V34" s="27"/>
       <c r="W34" s="27"/>
       <c r="X34" s="27"/>
       <c r="Y34" s="27"/>
@@ -5791,9 +5828,7 @@
       <c r="AF34" s="27"/>
       <c r="AG34" s="27"/>
       <c r="AH34" s="27"/>
-      <c r="AI34" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="AI34" s="27"/>
       <c r="AJ34" s="27"/>
       <c r="AK34" s="27"/>
       <c r="AL34" s="27"/>
@@ -5802,16 +5837,10 @@
       <c r="AO34" s="27"/>
       <c r="AP34" s="27"/>
       <c r="AQ34" s="27"/>
-      <c r="AR34" s="27">
-        <v>-2.0</v>
-      </c>
+      <c r="AR34" s="27"/>
       <c r="AS34" s="27"/>
-      <c r="AT34" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AU34" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="AT34" s="27"/>
+      <c r="AU34" s="27"/>
       <c r="AV34" s="27"/>
       <c r="AW34" s="27"/>
       <c r="AX34" s="27"/>
@@ -5820,10 +5849,10 @@
       <c r="BA34" s="19">
         <v>30.0</v>
       </c>
-      <c r="BB34" s="5"/>
+      <c r="BB34" s="19"/>
       <c r="BC34" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="BD34" s="5">
         <f t="shared" si="2"/>
@@ -5835,7 +5864,7 @@
       </c>
       <c r="BF34" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="BG34" s="5">
         <f t="shared" si="5"/>
@@ -5843,11 +5872,11 @@
       </c>
       <c r="BH34" s="5">
         <f t="shared" si="6"/>
-        <v>-11</v>
+        <v>8</v>
       </c>
       <c r="BI34" s="20">
         <f t="shared" si="7"/>
-        <v>0.2592592593</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BJ34" s="20"/>
     </row>
@@ -5915,7 +5944,7 @@
       <c r="BA35" s="19">
         <v>31.0</v>
       </c>
-      <c r="BB35" s="5"/>
+      <c r="BB35" s="19"/>
       <c r="BC35" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -6016,7 +6045,7 @@
       <c r="BA36" s="19">
         <v>32.0</v>
       </c>
-      <c r="BB36" s="5"/>
+      <c r="BB36" s="19"/>
       <c r="BC36" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6109,7 +6138,7 @@
       <c r="BA37" s="19">
         <v>33.0</v>
       </c>
-      <c r="BB37" s="5"/>
+      <c r="BB37" s="19"/>
       <c r="BC37" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -6200,7 +6229,7 @@
       <c r="BA38" s="19">
         <v>34.0</v>
       </c>
-      <c r="BB38" s="5"/>
+      <c r="BB38" s="19"/>
       <c r="BC38" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -6291,7 +6320,7 @@
       <c r="BA39" s="19">
         <v>35.0</v>
       </c>
-      <c r="BB39" s="5"/>
+      <c r="BB39" s="19"/>
       <c r="BC39" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -6516,13 +6545,12 @@
       </c>
       <c r="AW40" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AX40" s="32">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
       <c r="BD40" s="5"/>
       <c r="BE40" s="5"/>
@@ -6669,9 +6697,10 @@
       <c r="AV41" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AW41" s="5"/>
+      <c r="AW41" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="AX41" s="5"/>
-      <c r="BB41" s="5"/>
       <c r="BC41" s="5"/>
       <c r="BD41" s="5"/>
       <c r="BE41" s="5"/>
@@ -6732,7 +6761,6 @@
       <c r="AV42" s="5"/>
       <c r="AW42" s="5"/>
       <c r="AX42" s="5"/>
-      <c r="BB42" s="5"/>
       <c r="BC42" s="5"/>
       <c r="BD42" s="5"/>
       <c r="BE42" s="5"/>
@@ -6777,7 +6805,6 @@
       <c r="AV43" s="5"/>
       <c r="AW43" s="5"/>
       <c r="AX43" s="5"/>
-      <c r="BB43" s="5"/>
       <c r="BC43" s="5"/>
       <c r="BD43" s="5"/>
       <c r="BE43" s="5"/>
@@ -6815,7 +6842,6 @@
       <c r="AV44" s="6"/>
       <c r="AW44" s="6"/>
       <c r="AX44" s="6"/>
-      <c r="BB44" s="5"/>
       <c r="BC44" s="5"/>
       <c r="BD44" s="5"/>
       <c r="BE44" s="5"/>
@@ -27056,9 +27082,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.71"/>
-    <col customWidth="1" min="2" max="10" width="8.86"/>
-    <col customWidth="1" hidden="1" min="11" max="12" width="8.86"/>
-    <col customWidth="1" min="13" max="26" width="8.86"/>
+    <col customWidth="1" min="2" max="8" width="8.86"/>
+    <col customWidth="1" hidden="1" min="9" max="10" width="8.86"/>
+    <col customWidth="1" min="11" max="26" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -27083,10 +27109,10 @@
       <c r="G1" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="I1" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="J1" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -27113,11 +27139,11 @@
         <f t="shared" ref="G3:G32" si="1">SUM(C3*3)+D3</f>
         <v>10</v>
       </c>
-      <c r="K3" s="44">
+      <c r="I3" s="44">
         <v>18.0</v>
       </c>
-      <c r="L3" s="46">
-        <f t="shared" ref="L3:L7" si="2">K3/B3</f>
+      <c r="J3" s="46">
+        <f t="shared" ref="J3:J7" si="2">I3/B3</f>
         <v>3.6</v>
       </c>
     </row>
@@ -27144,10 +27170,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K4" s="44">
+      <c r="I4" s="44">
         <v>24.0</v>
       </c>
-      <c r="L4" s="46">
+      <c r="J4" s="46">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -27175,10 +27201,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K5" s="44">
+      <c r="I5" s="44">
         <v>27.0</v>
       </c>
-      <c r="L5" s="46">
+      <c r="J5" s="46">
         <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
@@ -27206,17 +27232,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K6" s="44">
+      <c r="I6" s="44">
         <v>19.0</v>
       </c>
-      <c r="L6" s="46">
+      <c r="J6" s="46">
         <f t="shared" si="2"/>
         <v>4.75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="44">
         <v>3.0</v>
@@ -27237,10 +27263,10 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K7" s="44">
+      <c r="I7" s="44">
         <v>19.0</v>
       </c>
-      <c r="L7" s="46">
+      <c r="J7" s="46">
         <f t="shared" si="2"/>
         <v>6.333333333</v>
       </c>
@@ -27268,7 +27294,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L8" s="46"/>
+      <c r="J8" s="46"/>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
@@ -27293,7 +27319,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
@@ -27319,11 +27345,11 @@
         <v>7</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="L10" s="46"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="44">
         <v>3.0</v>
@@ -27344,11 +27370,11 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="44">
         <v>3.0</v>
@@ -27369,11 +27395,11 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K12" s="44">
+      <c r="I12" s="44">
         <v>25.0</v>
       </c>
-      <c r="L12" s="46">
-        <f t="shared" ref="L12:L27" si="3">K12/B12</f>
+      <c r="J12" s="46">
+        <f t="shared" ref="J12:J27" si="3">I12/B12</f>
         <v>8.333333333</v>
       </c>
     </row>
@@ -27401,17 +27427,17 @@
         <v>6</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="K13" s="44">
+      <c r="I13" s="44">
         <v>5.0</v>
       </c>
-      <c r="L13" s="46">
+      <c r="J13" s="46">
         <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B14" s="44">
         <v>4.0</v>
@@ -27426,57 +27452,57 @@
         <v>1.0</v>
       </c>
       <c r="F14" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="44">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K14" s="44">
+      <c r="I14" s="44">
         <v>19.0</v>
       </c>
-      <c r="L14" s="46">
+      <c r="J14" s="46">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B15" s="44">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C15" s="44">
         <v>1.0</v>
       </c>
       <c r="D15" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E15" s="44">
         <v>1.0</v>
       </c>
       <c r="F15" s="44">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="G15" s="44">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="K15" s="44">
+        <v>5</v>
+      </c>
+      <c r="I15" s="44">
         <v>12.0</v>
       </c>
-      <c r="L15" s="46">
+      <c r="J15" s="46">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B16" s="44">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C16" s="44">
         <v>1.0</v>
@@ -27485,57 +27511,57 @@
         <v>1.0</v>
       </c>
       <c r="E16" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="44">
         <v>3.0</v>
-      </c>
-      <c r="F16" s="44">
-        <v>-9.0</v>
       </c>
       <c r="G16" s="44">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K16" s="44">
+      <c r="I16" s="44">
         <v>23.0</v>
       </c>
-      <c r="L16" s="46">
+      <c r="J16" s="46">
         <f t="shared" si="3"/>
-        <v>4.6</v>
+        <v>7.666666667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B17" s="44">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="44">
         <v>1.0</v>
       </c>
       <c r="D17" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E17" s="44">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="F17" s="44">
-        <v>9.0</v>
+        <v>-9.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="K17" s="47">
+        <v>4</v>
+      </c>
+      <c r="I17" s="47">
         <v>19.0</v>
       </c>
-      <c r="L17" s="46">
+      <c r="J17" s="46">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B18" s="44">
         <v>1.0</v>
@@ -27550,26 +27576,26 @@
         <v>0.0</v>
       </c>
       <c r="F18" s="44">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="G18" s="44">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K18" s="47">
+      <c r="I18" s="47">
         <v>15.0</v>
       </c>
-      <c r="L18" s="46">
+      <c r="J18" s="46">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B19" s="44">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" s="44">
         <v>1.0</v>
@@ -27578,29 +27604,29 @@
         <v>0.0</v>
       </c>
       <c r="E19" s="44">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F19" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G19" s="44">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K19" s="47">
+      <c r="I19" s="47">
         <v>22.0</v>
       </c>
-      <c r="L19" s="46">
+      <c r="J19" s="46">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B20" s="44">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C20" s="44">
         <v>1.0</v>
@@ -27609,29 +27635,29 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="44">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F20" s="44">
-        <v>-3.0</v>
+        <v>0.0</v>
       </c>
       <c r="G20" s="44">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K20" s="48">
+      <c r="I20" s="48">
         <v>14.0</v>
       </c>
-      <c r="L20" s="46">
+      <c r="J20" s="46">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B21" s="44">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C21" s="44">
         <v>1.0</v>
@@ -27640,7 +27666,7 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="44">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F21" s="44">
         <v>-3.0</v>
@@ -27649,17 +27675,17 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K21" s="47">
+      <c r="I21" s="47">
         <v>25.0</v>
       </c>
-      <c r="L21" s="46">
+      <c r="J21" s="46">
         <f t="shared" si="3"/>
-        <v>8.333333333</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B22" s="44">
         <v>3.0</v>
@@ -27674,49 +27700,49 @@
         <v>2.0</v>
       </c>
       <c r="F22" s="44">
-        <v>-8.0</v>
+        <v>-3.0</v>
       </c>
       <c r="G22" s="44">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K22" s="47">
+      <c r="I22" s="47">
         <v>5.0</v>
       </c>
-      <c r="L22" s="46">
+      <c r="J22" s="46">
         <f t="shared" si="3"/>
         <v>1.666666667</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B23" s="44">
+        <v>4.0</v>
+      </c>
+      <c r="C23" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="E23" s="44">
         <v>3.0</v>
       </c>
-      <c r="C23" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="D23" s="44">
-        <v>2.0</v>
-      </c>
-      <c r="E23" s="44">
-        <v>1.0</v>
-      </c>
       <c r="F23" s="44">
-        <v>-2.0</v>
+        <v>-11.0</v>
       </c>
       <c r="G23" s="44">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K23" s="47">
+        <v>3</v>
+      </c>
+      <c r="I23" s="47">
         <v>12.0</v>
       </c>
-      <c r="L23" s="46">
+      <c r="J23" s="46">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -27742,10 +27768,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K24" s="47">
+      <c r="I24" s="47">
         <v>15.0</v>
       </c>
-      <c r="L24" s="46">
+      <c r="J24" s="46">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
@@ -27773,10 +27799,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K25" s="47">
+      <c r="I25" s="47">
         <v>25.0</v>
       </c>
-      <c r="L25" s="46">
+      <c r="J25" s="46">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
@@ -27804,17 +27830,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K26" s="47">
+      <c r="I26" s="47">
         <v>8.0</v>
       </c>
-      <c r="L26" s="46">
+      <c r="J26" s="46">
         <f t="shared" si="3"/>
         <v>2.666666667</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B27" s="44">
         <v>1.0</v>
@@ -27835,10 +27861,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K27" s="47">
+      <c r="I27" s="47">
         <v>1.0</v>
       </c>
-      <c r="L27" s="46">
+      <c r="J27" s="46">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -27866,13 +27892,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="47">
+      <c r="I28" s="47">
         <v>4.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B29" s="44">
         <v>2.0</v>
@@ -27893,13 +27919,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K29" s="47">
+      <c r="I29" s="47">
         <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B30" s="44">
         <v>2.0</v>
@@ -27920,7 +27946,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K30" s="47">
+      <c r="I30" s="47">
         <v>0.0</v>
       </c>
     </row>
@@ -27947,7 +27973,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K31" s="44">
+      <c r="I31" s="44">
         <v>0.0</v>
       </c>
     </row>
@@ -27974,7 +28000,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K32" s="44">
+      <c r="I32" s="44">
         <v>0.0</v>
       </c>
     </row>
@@ -28971,7 +28997,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.14"/>
     <col customWidth="1" min="2" max="11" width="7.29"/>
-    <col customWidth="1" min="12" max="51" width="7.29" outlineLevel="1"/>
+    <col customWidth="1" min="12" max="50" width="7.29" outlineLevel="1"/>
+    <col customWidth="1" hidden="1" min="51" max="51" width="7.29" outlineLevel="1"/>
     <col customWidth="1" min="52" max="52" width="7.29"/>
     <col customWidth="1" min="53" max="53" width="9.14"/>
     <col customWidth="1" min="54" max="58" width="8.86"/>
@@ -29176,173 +29203,173 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="E3" s="27">
-        <v>6.0</v>
-      </c>
+      <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="29"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27">
+      <c r="L3" s="27">
         <v>1.0</v>
       </c>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="O3" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="P3" s="27">
+        <v>3.0</v>
+      </c>
       <c r="Q3" s="27"/>
       <c r="R3" s="29"/>
       <c r="S3" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27">
         <v>1.0</v>
       </c>
-      <c r="T3" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="U3" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="V3" s="27">
+      <c r="W3" s="27">
         <v>3.0</v>
       </c>
-      <c r="W3" s="27"/>
       <c r="X3" s="27"/>
-      <c r="Y3" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="Y3" s="27"/>
       <c r="Z3" s="27"/>
       <c r="AA3" s="29"/>
-      <c r="AB3" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AB3" s="27"/>
       <c r="AC3" s="50"/>
-      <c r="AD3" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AD3" s="27"/>
       <c r="AE3" s="27"/>
       <c r="AF3" s="27"/>
       <c r="AG3" s="27"/>
       <c r="AH3" s="27"/>
-      <c r="AI3" s="27"/>
+      <c r="AI3" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="27"/>
       <c r="AL3" s="27"/>
       <c r="AM3" s="27"/>
-      <c r="AN3" s="27">
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="AP3" s="27">
         <v>1.0</v>
       </c>
-      <c r="AO3" s="27">
+      <c r="AQ3" s="27">
         <v>1.0</v>
       </c>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AR3" s="27">
+      <c r="AR3" s="27"/>
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="27">
         <v>1.0</v>
       </c>
-      <c r="AS3" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AT3" s="27"/>
       <c r="AU3" s="27">
         <v>1.0</v>
       </c>
-      <c r="AV3" s="27"/>
+      <c r="AV3" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AW3" s="27"/>
       <c r="AX3" s="27"/>
       <c r="AY3" s="27"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6">
         <f t="shared" ref="BA3:BA35" si="1">SUM(B3:AY3)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BB3" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="BC3" s="5">
-        <v>2.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="BC3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="E4" s="27">
+        <v>6.0</v>
+      </c>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="29"/>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
-      <c r="L4" s="27">
+      <c r="L4" s="27"/>
+      <c r="M4" s="27">
         <v>1.0</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="O4" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="P4" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
       <c r="Q4" s="27"/>
       <c r="R4" s="29"/>
       <c r="S4" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="T4" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="U4" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="V4" s="27">
         <v>3.0</v>
       </c>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="W4" s="27">
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27">
         <v>3.0</v>
       </c>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
       <c r="Z4" s="27"/>
       <c r="AA4" s="29"/>
-      <c r="AB4" s="27"/>
+      <c r="AB4" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AC4" s="50"/>
-      <c r="AD4" s="27"/>
+      <c r="AD4" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AE4" s="27"/>
       <c r="AF4" s="27"/>
       <c r="AG4" s="27"/>
       <c r="AH4" s="27"/>
-      <c r="AI4" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI4" s="27"/>
       <c r="AJ4" s="27"/>
       <c r="AK4" s="27"/>
       <c r="AL4" s="27"/>
       <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
+      <c r="AN4" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AO4" s="27">
-        <v>7.0</v>
-      </c>
-      <c r="AP4" s="27">
         <v>1.0</v>
       </c>
+      <c r="AP4" s="27"/>
       <c r="AQ4" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AR4" s="27">
         <v>1.0</v>
       </c>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AS4" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AT4" s="27"/>
       <c r="AU4" s="27">
         <v>1.0</v>
       </c>
@@ -29353,50 +29380,56 @@
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="BB4" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="BC4" s="5"/>
+        <v>3.0</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="27">
-        <v>2.0</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="27">
+      <c r="E5" s="27"/>
+      <c r="F5" s="27">
         <v>1.0</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="G5" s="27">
+        <v>2.0</v>
+      </c>
       <c r="H5" s="29"/>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="K5" s="27">
+        <v>2.0</v>
+      </c>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27">
-        <v>5.0</v>
-      </c>
+      <c r="N5" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="O5" s="27"/>
       <c r="P5" s="27"/>
-      <c r="Q5" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="Q5" s="27"/>
       <c r="R5" s="29"/>
       <c r="S5" s="27"/>
-      <c r="T5" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="U5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27">
+        <v>2.0</v>
+      </c>
       <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
+      <c r="W5" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="X5" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Y5" s="27">
         <v>1.0</v>
       </c>
@@ -29405,9 +29438,13 @@
       <c r="AB5" s="27"/>
       <c r="AC5" s="50"/>
       <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
+      <c r="AG5" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AH5" s="27"/>
       <c r="AI5" s="27"/>
       <c r="AJ5" s="27"/>
@@ -29415,201 +29452,197 @@
       <c r="AL5" s="27"/>
       <c r="AM5" s="27"/>
       <c r="AN5" s="27"/>
-      <c r="AO5" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AO5" s="27"/>
       <c r="AP5" s="27"/>
       <c r="AQ5" s="27"/>
       <c r="AR5" s="27"/>
-      <c r="AS5" s="27"/>
+      <c r="AS5" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AT5" s="27"/>
       <c r="AU5" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AV5" s="27"/>
+        <v>2.0</v>
+      </c>
+      <c r="AV5" s="27">
+        <v>4.0</v>
+      </c>
       <c r="AW5" s="27"/>
       <c r="AX5" s="27"/>
       <c r="AY5" s="27"/>
       <c r="AZ5" s="6"/>
       <c r="BA5" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="BB5" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="BC5" s="5"/>
+        <v>2.0</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="27"/>
+        <v>66</v>
+      </c>
+      <c r="B6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
-      <c r="F6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="G6" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="29"/>
       <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="J6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="K6" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="M6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="N6" s="27">
         <v>1.0</v>
       </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
+      <c r="O6" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="P6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Q6" s="27"/>
       <c r="R6" s="29"/>
       <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27">
+      <c r="T6" s="27">
         <v>1.0</v>
       </c>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="W6" s="27"/>
       <c r="X6" s="27">
         <v>1.0</v>
       </c>
-      <c r="Y6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="29"/>
-      <c r="AB6" s="27"/>
+      <c r="AB6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AC6" s="50"/>
       <c r="AD6" s="27"/>
-      <c r="AE6" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AE6" s="27"/>
       <c r="AF6" s="27"/>
       <c r="AG6" s="27">
         <v>1.0</v>
       </c>
       <c r="AH6" s="27"/>
-      <c r="AI6" s="27"/>
+      <c r="AI6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ6" s="27"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="27"/>
       <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
+      <c r="AN6" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AO6" s="27"/>
       <c r="AP6" s="27"/>
-      <c r="AQ6" s="27"/>
+      <c r="AQ6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AR6" s="27"/>
-      <c r="AS6" s="27">
+      <c r="AS6" s="27"/>
+      <c r="AT6" s="27"/>
+      <c r="AU6" s="27"/>
+      <c r="AV6" s="27">
         <v>1.0</v>
       </c>
-      <c r="AT6" s="27"/>
-      <c r="AU6" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AV6" s="27"/>
       <c r="AW6" s="27"/>
       <c r="AX6" s="27"/>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="6"/>
       <c r="BA6" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="BB6" s="5">
+        <v>18</v>
+      </c>
+      <c r="BB6" s="5"/>
+      <c r="BC6" s="5">
         <v>1.0</v>
-      </c>
-      <c r="BC6" s="5">
-        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B7" s="27">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="29"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="K7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="27"/>
-      <c r="M7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="N7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
       <c r="O7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="P7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Q7" s="27"/>
+        <v>5.0</v>
+      </c>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27">
+        <v>3.0</v>
+      </c>
       <c r="R7" s="29"/>
       <c r="S7" s="27"/>
       <c r="T7" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27">
         <v>1.0</v>
       </c>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Y7" s="27"/>
       <c r="Z7" s="27"/>
       <c r="AA7" s="29"/>
-      <c r="AB7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AB7" s="27"/>
       <c r="AC7" s="50"/>
       <c r="AD7" s="27"/>
       <c r="AE7" s="27"/>
       <c r="AF7" s="27"/>
-      <c r="AG7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AG7" s="27"/>
       <c r="AH7" s="27"/>
-      <c r="AI7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI7" s="27"/>
       <c r="AJ7" s="27"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="27"/>
       <c r="AM7" s="27"/>
-      <c r="AN7" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="AO7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AP7" s="27"/>
-      <c r="AQ7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AQ7" s="27"/>
       <c r="AR7" s="27"/>
       <c r="AS7" s="27"/>
       <c r="AT7" s="27"/>
-      <c r="AU7" s="27"/>
+      <c r="AU7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AV7" s="27"/>
       <c r="AW7" s="27"/>
       <c r="AX7" s="27"/>
@@ -29619,10 +29652,10 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="BB7" s="5"/>
-      <c r="BC7" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BB7" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="BC7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
@@ -29800,7 +29833,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="27">
         <v>1.0</v>
@@ -29966,30 +29999,38 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="27">
+        <v>59</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27">
         <v>1.0</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="F12" s="27">
+        <v>2.0</v>
+      </c>
       <c r="G12" s="27"/>
       <c r="H12" s="29"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
-      <c r="L12" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="L12" s="27"/>
       <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
+      <c r="N12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
+      <c r="P12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="Q12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="R12" s="29"/>
-      <c r="S12" s="27"/>
+      <c r="S12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
       <c r="V12" s="27"/>
@@ -29997,7 +30038,7 @@
       <c r="X12" s="27"/>
       <c r="Y12" s="27"/>
       <c r="Z12" s="27">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="AA12" s="29"/>
       <c r="AB12" s="27">
@@ -30007,32 +30048,26 @@
       <c r="AD12" s="27"/>
       <c r="AE12" s="27"/>
       <c r="AF12" s="27">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AG12" s="27"/>
       <c r="AH12" s="27"/>
-      <c r="AI12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI12" s="27"/>
       <c r="AJ12" s="27"/>
       <c r="AK12" s="27"/>
       <c r="AL12" s="27"/>
       <c r="AM12" s="27"/>
-      <c r="AN12" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="AO12" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AP12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="27"/>
+      <c r="AP12" s="27"/>
       <c r="AQ12" s="27"/>
       <c r="AR12" s="27"/>
       <c r="AS12" s="27"/>
       <c r="AT12" s="27"/>
       <c r="AU12" s="27"/>
-      <c r="AV12" s="27"/>
+      <c r="AV12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AW12" s="27"/>
       <c r="AX12" s="27"/>
       <c r="AY12" s="27"/>
@@ -30041,7 +30076,9 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="BB12" s="5"/>
+      <c r="BB12" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC12" s="5">
         <v>1.0</v>
       </c>
@@ -30051,70 +30088,70 @@
       <c r="A13" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
-      <c r="E13" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="29"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="L13" s="27">
+        <v>3.0</v>
+      </c>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
-      <c r="P13" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="P13" s="27"/>
       <c r="Q13" s="27"/>
       <c r="R13" s="29"/>
       <c r="S13" s="27"/>
       <c r="T13" s="27"/>
       <c r="U13" s="27"/>
       <c r="V13" s="27"/>
-      <c r="W13" s="27">
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27">
         <v>1.0</v>
       </c>
-      <c r="X13" s="27">
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="27">
         <v>1.0</v>
       </c>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="27"/>
       <c r="AC13" s="50"/>
       <c r="AD13" s="27"/>
       <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
+      <c r="AF13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AG13" s="27"/>
       <c r="AH13" s="27"/>
       <c r="AI13" s="27">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="AJ13" s="27"/>
       <c r="AK13" s="27"/>
       <c r="AL13" s="27"/>
-      <c r="AM13" s="27">
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AO13" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AP13" s="27">
         <v>1.0</v>
       </c>
-      <c r="AN13" s="27"/>
-      <c r="AO13" s="27"/>
-      <c r="AP13" s="27"/>
-      <c r="AQ13" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AQ13" s="27"/>
       <c r="AR13" s="27"/>
       <c r="AS13" s="27"/>
       <c r="AT13" s="27"/>
-      <c r="AU13" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AU13" s="27"/>
       <c r="AV13" s="27"/>
       <c r="AW13" s="27"/>
       <c r="AX13" s="27"/>
@@ -30125,20 +30162,22 @@
         <v>14</v>
       </c>
       <c r="BB13" s="5"/>
-      <c r="BC13" s="5"/>
+      <c r="BC13" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
-      <c r="D14" s="27">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27">
         <v>1.0</v>
       </c>
-      <c r="E14" s="27"/>
       <c r="F14" s="27">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="29"/>
@@ -30147,54 +30186,54 @@
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
-      <c r="N14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="N14" s="27"/>
       <c r="O14" s="27"/>
       <c r="P14" s="27">
         <v>1.0</v>
       </c>
-      <c r="Q14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="Q14" s="27"/>
       <c r="R14" s="29"/>
-      <c r="S14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="S14" s="27"/>
       <c r="T14" s="27"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
+      <c r="W14" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="X14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Y14" s="27"/>
-      <c r="Z14" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="Z14" s="27"/>
       <c r="AA14" s="29"/>
-      <c r="AB14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AB14" s="27"/>
       <c r="AC14" s="50"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
-      <c r="AF14" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="AF14" s="27"/>
       <c r="AG14" s="27"/>
       <c r="AH14" s="27"/>
-      <c r="AI14" s="27"/>
+      <c r="AI14" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AJ14" s="27"/>
       <c r="AK14" s="27"/>
       <c r="AL14" s="27"/>
-      <c r="AM14" s="27"/>
+      <c r="AM14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AN14" s="27"/>
       <c r="AO14" s="27"/>
       <c r="AP14" s="27"/>
-      <c r="AQ14" s="27"/>
+      <c r="AQ14" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AR14" s="27"/>
       <c r="AS14" s="27"/>
       <c r="AT14" s="27"/>
-      <c r="AU14" s="27"/>
+      <c r="AU14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AV14" s="27"/>
       <c r="AW14" s="27"/>
       <c r="AX14" s="27"/>
@@ -30202,18 +30241,14 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="BB14" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC14" s="5">
-        <v>1.0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="BB14" s="5"/>
+      <c r="BC14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
@@ -30369,7 +30404,7 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -30445,7 +30480,7 @@
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -30670,14 +30705,16 @@
         <v>3.0</v>
       </c>
       <c r="AU20" s="27"/>
-      <c r="AV20" s="27"/>
+      <c r="AV20" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AW20" s="27"/>
       <c r="AX20" s="27"/>
       <c r="AY20" s="27"/>
       <c r="AZ20" s="6"/>
       <c r="BA20" s="6">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB20" s="5"/>
       <c r="BC20" s="5">
@@ -30766,7 +30803,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -30914,7 +30951,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -31134,7 +31171,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27">
@@ -31204,7 +31241,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -31666,7 +31703,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -31999,13 +32036,13 @@
         <f>'League Table'!AT40</f>
         <v>15</v>
       </c>
-      <c r="AU38" s="5" t="str">
-        <f>'League Table'!BC40</f>
-        <v/>
-      </c>
-      <c r="AV38" s="5" t="str">
-        <f>'League Table'!BD40</f>
-        <v/>
+      <c r="AU38" s="5">
+        <f>'League Table'!AU40</f>
+        <v>17</v>
+      </c>
+      <c r="AV38" s="5">
+        <f>'League Table'!AV40</f>
+        <v>14</v>
       </c>
       <c r="AW38" s="5"/>
       <c r="AX38" s="5"/>
@@ -32237,7 +32274,7 @@
       </c>
       <c r="AV40" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AW40" s="6"/>
       <c r="AX40" s="6"/>
@@ -62992,7 +63029,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="22.29"/>
     <col customWidth="1" min="2" max="11" width="8.86"/>
-    <col customWidth="1" min="12" max="51" width="9.14" outlineLevel="1"/>
+    <col customWidth="1" min="12" max="50" width="9.14" outlineLevel="1"/>
+    <col customWidth="1" hidden="1" min="51" max="51" width="9.14" outlineLevel="1"/>
     <col customWidth="1" min="52" max="53" width="8.86"/>
   </cols>
   <sheetData>
@@ -63407,12 +63445,14 @@
         <v>2.0</v>
       </c>
       <c r="AV6" s="32"/>
-      <c r="AW6" s="32"/>
+      <c r="AW6" s="32">
+        <v>2.0</v>
+      </c>
       <c r="AX6" s="32"/>
       <c r="AY6" s="32"/>
       <c r="BA6" s="44">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -63502,12 +63542,14 @@
       <c r="AV7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AW7" s="27"/>
+      <c r="AW7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX7" s="27"/>
       <c r="AY7" s="27"/>
       <c r="BA7" s="44">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -63601,7 +63643,7 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -63670,17 +63712,19 @@
       <c r="AT9" s="32"/>
       <c r="AU9" s="32"/>
       <c r="AV9" s="32"/>
-      <c r="AW9" s="32"/>
+      <c r="AW9" s="32">
+        <v>3.0</v>
+      </c>
       <c r="AX9" s="32"/>
       <c r="AY9" s="32"/>
       <c r="BA9" s="44">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="27">
         <v>2.0</v>
@@ -63747,12 +63791,14 @@
       </c>
       <c r="AU10" s="27"/>
       <c r="AV10" s="27"/>
-      <c r="AW10" s="27"/>
+      <c r="AW10" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AX10" s="27"/>
       <c r="AY10" s="27"/>
       <c r="BA10" s="44">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -63972,7 +64018,7 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27">
@@ -64110,7 +64156,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -64585,7 +64631,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -64705,17 +64751,19 @@
       </c>
       <c r="AU24" s="27"/>
       <c r="AV24" s="27"/>
-      <c r="AW24" s="27"/>
+      <c r="AW24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX24" s="27"/>
       <c r="AY24" s="27"/>
       <c r="BA24" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -65024,7 +65072,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
@@ -65085,7 +65133,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -65327,7 +65375,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -65855,7 +65903,7 @@
       </c>
       <c r="AW41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AX41" s="5">
         <f t="shared" si="2"/>
@@ -65867,7 +65915,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -67029,16 +67077,16 @@
         <v>7.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="L9" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>156</v>
       </c>
       <c r="N9" s="5">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
@@ -67046,10 +67094,10 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D10" s="49" t="s">
         <v>157</v>
@@ -67059,13 +67107,13 @@
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="I10" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="L10" s="5">
         <v>3.0</v>
@@ -67082,13 +67130,13 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>164</v>
@@ -67098,19 +67146,19 @@
         <v>156</v>
       </c>
       <c r="I11" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="L11" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="N11" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="12">
@@ -67118,10 +67166,10 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D12" s="49" t="s">
         <v>164</v>
@@ -67131,13 +67179,13 @@
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="5" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="I12" s="5">
         <v>6.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L12" s="5">
         <v>2.0</v>
@@ -67146,7 +67194,7 @@
         <v>146</v>
       </c>
       <c r="N12" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="13">
@@ -67180,7 +67228,7 @@
         <v>2.0</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="N13" s="5">
         <v>6.0</v>
@@ -67204,10 +67252,10 @@
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I14" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>181</v>
@@ -67240,10 +67288,10 @@
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="5" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="I15" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>180</v>
@@ -67252,7 +67300,7 @@
         <v>2.0</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N15" s="5">
         <v>5.0</v>
@@ -67263,35 +67311,35 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>179</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="5" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="I16" s="5">
         <v>3.0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L16" s="5">
         <v>2.0</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="N16" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
@@ -67299,10 +67347,10 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>152</v>
@@ -67312,7 +67360,7 @@
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="5" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="I17" s="5">
         <v>3.0</v>
@@ -67324,10 +67372,10 @@
         <v>2.0</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="N17" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="18">
@@ -67341,14 +67389,14 @@
         <v>192</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E18" s="49" t="s">
         <v>157</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="5" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="I18" s="5">
         <v>3.0</v>
@@ -67358,7 +67406,7 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="N18" s="5">
         <v>5.0</v>
@@ -67376,17 +67424,17 @@
       <c r="E19" s="49"/>
       <c r="G19" s="49"/>
       <c r="H19" s="5" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="I19" s="5">
         <v>3.0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="N19" s="5">
         <v>4.0</v>
@@ -67410,7 +67458,7 @@
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="5" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="I20" s="5">
         <v>3.0</v>
@@ -67420,10 +67468,10 @@
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N20" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -67450,11 +67498,11 @@
         <v>2.0</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="N21" s="5">
         <v>3.0</v>
@@ -67484,7 +67532,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N22" s="5">
         <v>3.0</v>
@@ -67516,10 +67564,10 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="N23" s="5">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -67548,10 +67596,10 @@
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="N24" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -67565,7 +67613,7 @@
         <v>209</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E25" s="49" t="s">
         <v>152</v>
@@ -67580,7 +67628,7 @@
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="N25" s="5">
         <v>2.0</v>
@@ -67629,7 +67677,7 @@
         <v>177</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E27" s="49" t="s">
         <v>156</v>
@@ -67688,17 +67736,17 @@
         <v>213</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>211</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N29" s="5">
         <v>2.0</v>
@@ -67745,14 +67793,14 @@
         <v>164</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="5" t="s">
         <v>213</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N31" s="5"/>
     </row>
@@ -67770,7 +67818,7 @@
         <v>156</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>218</v>
@@ -67796,7 +67844,7 @@
         <v>181</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>220</v>
@@ -67838,7 +67886,7 @@
         <v>223</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D35" s="49" t="s">
         <v>224</v>
@@ -67913,7 +67961,7 @@
         <v>149</v>
       </c>
       <c r="E38" s="49" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -67930,7 +67978,7 @@
         <v>229</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E39" s="49" t="s">
         <v>146</v>
@@ -68013,7 +68061,7 @@
         <v>214</v>
       </c>
       <c r="E43" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -68030,7 +68078,7 @@
         <v>232</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E44" s="49" t="s">
         <v>152</v>
@@ -68050,7 +68098,7 @@
         <v>234</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E45" s="49" t="s">
         <v>152</v>
@@ -68073,7 +68121,7 @@
         <v>224</v>
       </c>
       <c r="E46" s="49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -68123,12 +68171,38 @@
       <c r="A49" s="49">
         <v>47.0</v>
       </c>
+      <c r="B49" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="49" t="s">
+        <v>169</v>
+      </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="N49" s="5"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="6"/>
+      <c r="A50" s="49">
+        <v>48.0</v>
+      </c>
+      <c r="B50" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" s="49" t="s">
+        <v>146</v>
+      </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="N50" s="5"/>

</xml_diff>

<commit_message>
044 Week 48 Data Fix
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="HvgkgCul3x9/XnxcfAWwp+i3J6tG0O7IAFunAUKadpA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="KCSWMUleTP2KA5AUJ8UtnNfMBPncuC/m+G++KNWuD2A="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="241">
   <si>
     <t>MARLOW DUKES 2024</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 5-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7-3</t>
   </si>
   <si>
     <t>P</t>
@@ -1946,7 +1949,7 @@
         <v>4.0</v>
       </c>
       <c r="AW5" s="16">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX5" s="16"/>
       <c r="AY5" s="19"/>
@@ -1977,7 +1980,7 @@
       </c>
       <c r="BH5" s="5">
         <f t="shared" ref="BH5:BH39" si="6">SUM(B5:AX5)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BI5" s="20">
         <f t="shared" ref="BI5:BI39" si="7">SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
@@ -2115,7 +2118,7 @@
         <v>-4.0</v>
       </c>
       <c r="AW6" s="22">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX6" s="22"/>
       <c r="AY6" s="19"/>
@@ -2146,7 +2149,7 @@
       </c>
       <c r="BH6" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BI6" s="20">
         <f t="shared" si="7"/>
@@ -2445,7 +2448,7 @@
         <v>-4.0</v>
       </c>
       <c r="AW8" s="16">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX8" s="16"/>
       <c r="AY8" s="19"/>
@@ -2476,7 +2479,7 @@
       </c>
       <c r="BH8" s="5">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BI8" s="20">
         <f t="shared" si="7"/>
@@ -2759,7 +2762,7 @@
         <v>-4.0</v>
       </c>
       <c r="AW10" s="32">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX10" s="32"/>
       <c r="AY10" s="19"/>
@@ -2790,7 +2793,7 @@
       </c>
       <c r="BH10" s="5">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BI10" s="20">
         <f t="shared" si="7"/>
@@ -2906,7 +2909,7 @@
         <v>4.0</v>
       </c>
       <c r="AW11" s="27">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX11" s="27"/>
       <c r="AY11" s="19"/>
@@ -2937,7 +2940,7 @@
       </c>
       <c r="BH11" s="5">
         <f t="shared" si="6"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BI11" s="20">
         <f t="shared" si="7"/>
@@ -3226,7 +3229,7 @@
         <v>4.0</v>
       </c>
       <c r="AW13" s="27">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX13" s="27"/>
       <c r="AY13" s="19"/>
@@ -3257,7 +3260,7 @@
       </c>
       <c r="BH13" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="BI13" s="20">
         <f t="shared" si="7"/>
@@ -3514,7 +3517,7 @@
       </c>
       <c r="AV15" s="27"/>
       <c r="AW15" s="27">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX15" s="27"/>
       <c r="AY15" s="19"/>
@@ -3545,7 +3548,7 @@
       </c>
       <c r="BH15" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="BI15" s="20">
         <f t="shared" si="7"/>
@@ -3661,7 +3664,7 @@
         <v>4.0</v>
       </c>
       <c r="AW16" s="28">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX16" s="27"/>
       <c r="AY16" s="19"/>
@@ -3692,7 +3695,7 @@
       </c>
       <c r="BH16" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="BI16" s="20">
         <f t="shared" si="7"/>
@@ -3806,7 +3809,7 @@
         <v>-4.0</v>
       </c>
       <c r="AW17" s="27">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AX17" s="27"/>
       <c r="AY17" s="19"/>
@@ -3837,7 +3840,7 @@
       </c>
       <c r="BH17" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BI17" s="20">
         <f t="shared" si="7"/>
@@ -4253,7 +4256,7 @@
         <v>4.0</v>
       </c>
       <c r="AW20" s="27">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX20" s="27"/>
       <c r="AY20" s="19"/>
@@ -4284,7 +4287,7 @@
       </c>
       <c r="BH20" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="BI20" s="20">
         <f t="shared" si="7"/>
@@ -4390,7 +4393,7 @@
       </c>
       <c r="AV21" s="27"/>
       <c r="AW21" s="28">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX21" s="27"/>
       <c r="AY21" s="19"/>
@@ -4421,7 +4424,7 @@
       </c>
       <c r="BH21" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BI21" s="20">
         <f t="shared" si="7"/>
@@ -4527,7 +4530,7 @@
         <v>-4.0</v>
       </c>
       <c r="AW22" s="27">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX22" s="27"/>
       <c r="AY22" s="19"/>
@@ -4558,7 +4561,7 @@
       </c>
       <c r="BH22" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="BI22" s="20">
         <f t="shared" si="7"/>
@@ -5326,7 +5329,7 @@
       </c>
       <c r="AV29" s="27"/>
       <c r="AW29" s="27">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AX29" s="27"/>
       <c r="AY29" s="19"/>
@@ -5357,7 +5360,7 @@
       </c>
       <c r="BH29" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="BI29" s="20">
         <f t="shared" si="7"/>
@@ -6356,7 +6359,7 @@
         <v>94</v>
       </c>
       <c r="B40" s="32">
-        <f t="shared" ref="B40:AX40" si="8">COUNT(B5:B39)</f>
+        <f t="shared" ref="B40:AW40" si="8">COUNT(B5:B39)</f>
         <v>16</v>
       </c>
       <c r="C40" s="32">
@@ -6547,10 +6550,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="AX40" s="32">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
+      <c r="AX40" s="32"/>
       <c r="BC40" s="5"/>
       <c r="BD40" s="5"/>
       <c r="BE40" s="5"/>
@@ -6698,7 +6698,7 @@
         <v>109</v>
       </c>
       <c r="AW41" s="5" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="AX41" s="5"/>
       <c r="BC41" s="5"/>
@@ -27092,28 +27092,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>56</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
@@ -27747,7 +27747,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B24" s="44">
         <v>1.0</v>
@@ -29156,17 +29156,17 @@
         <v>50</v>
       </c>
       <c r="AY1" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2">
@@ -29280,13 +29280,15 @@
       <c r="AV3" s="27">
         <v>3.0</v>
       </c>
-      <c r="AW3" s="27"/>
+      <c r="AW3" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX3" s="27"/>
       <c r="AY3" s="27"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6">
         <f t="shared" ref="BA3:BA35" si="1">SUM(B3:AY3)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BB3" s="5">
         <v>4.0</v>
@@ -29483,88 +29485,72 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="27">
         <v>1.0</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="27">
+        <v>6.0</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
       <c r="H6" s="29"/>
       <c r="I6" s="27"/>
-      <c r="J6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="K6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="27"/>
-      <c r="M6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="N6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="O6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="P6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="29"/>
       <c r="S6" s="27"/>
-      <c r="T6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="T6" s="27"/>
       <c r="U6" s="27"/>
-      <c r="V6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="V6" s="27"/>
       <c r="W6" s="27"/>
-      <c r="X6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="X6" s="27"/>
       <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="29"/>
-      <c r="AB6" s="27">
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="50"/>
+      <c r="AD6" s="27">
         <v>1.0</v>
       </c>
-      <c r="AC6" s="50"/>
-      <c r="AD6" s="27"/>
       <c r="AE6" s="27"/>
       <c r="AF6" s="27"/>
-      <c r="AG6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AG6" s="27"/>
       <c r="AH6" s="27"/>
       <c r="AI6" s="27">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="AJ6" s="27"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="27"/>
       <c r="AM6" s="27"/>
-      <c r="AN6" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="AO6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AP6" s="27"/>
-      <c r="AQ6" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AQ6" s="27"/>
       <c r="AR6" s="27"/>
       <c r="AS6" s="27"/>
-      <c r="AT6" s="27"/>
+      <c r="AT6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AU6" s="27"/>
-      <c r="AV6" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AW6" s="27"/>
+      <c r="AV6" s="27"/>
+      <c r="AW6" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AX6" s="27"/>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="6"/>
@@ -29572,128 +29558,146 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="BB6" s="5"/>
+      <c r="BB6" s="5">
+        <v>2.0</v>
+      </c>
       <c r="BC6" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B7" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="29"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="K7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
+      <c r="M7" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="N7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="O7" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27">
-        <v>3.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="P7" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="Q7" s="27"/>
       <c r="R7" s="29"/>
       <c r="S7" s="27"/>
       <c r="T7" s="27">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
+      <c r="V7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27">
+      <c r="X7" s="27">
         <v>1.0</v>
       </c>
+      <c r="Y7" s="27"/>
       <c r="Z7" s="27"/>
       <c r="AA7" s="29"/>
-      <c r="AB7" s="27"/>
+      <c r="AB7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AC7" s="50"/>
       <c r="AD7" s="27"/>
       <c r="AE7" s="27"/>
       <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
+      <c r="AG7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AH7" s="27"/>
-      <c r="AI7" s="27"/>
+      <c r="AI7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ7" s="27"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="27"/>
       <c r="AM7" s="27"/>
-      <c r="AN7" s="27"/>
-      <c r="AO7" s="27">
+      <c r="AN7" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AP7" s="27"/>
-      <c r="AQ7" s="27"/>
       <c r="AR7" s="27"/>
       <c r="AS7" s="27"/>
       <c r="AT7" s="27"/>
-      <c r="AU7" s="27">
+      <c r="AU7" s="27"/>
+      <c r="AV7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AV7" s="27"/>
       <c r="AW7" s="27"/>
       <c r="AX7" s="27"/>
       <c r="AY7" s="27"/>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="BB7" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="BC7" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="27"/>
+        <v>69</v>
+      </c>
+      <c r="B8" s="27">
+        <v>2.0</v>
+      </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27">
+      <c r="E8" s="27">
         <v>1.0</v>
       </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="29"/>
       <c r="I8" s="27"/>
-      <c r="J8" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="J8" s="27"/>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
-      <c r="N8" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="O8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27">
+        <v>5.0</v>
+      </c>
       <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
+      <c r="Q8" s="27">
+        <v>3.0</v>
+      </c>
       <c r="R8" s="29"/>
-      <c r="S8" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="T8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27">
+        <v>3.0</v>
+      </c>
       <c r="U8" s="27"/>
       <c r="V8" s="27"/>
       <c r="W8" s="27"/>
-      <c r="X8" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="X8" s="27"/>
       <c r="Y8" s="27">
         <v>1.0</v>
       </c>
@@ -29702,37 +29706,27 @@
       <c r="AB8" s="27"/>
       <c r="AC8" s="50"/>
       <c r="AD8" s="27"/>
-      <c r="AE8" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AE8" s="27"/>
       <c r="AF8" s="27"/>
       <c r="AG8" s="27"/>
-      <c r="AH8" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AH8" s="27"/>
       <c r="AI8" s="27"/>
       <c r="AJ8" s="27"/>
-      <c r="AK8" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AK8" s="27"/>
       <c r="AL8" s="27"/>
       <c r="AM8" s="27"/>
       <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="AO8" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AP8" s="27"/>
       <c r="AQ8" s="27"/>
-      <c r="AR8" s="27">
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="27"/>
+      <c r="AT8" s="27"/>
+      <c r="AU8" s="27">
         <v>1.0</v>
       </c>
-      <c r="AS8" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AT8" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AU8" s="27"/>
       <c r="AV8" s="27"/>
       <c r="AW8" s="27"/>
       <c r="AX8" s="27"/>
@@ -29740,80 +29734,88 @@
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BB8" s="5">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="BC8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B9" s="27"/>
-      <c r="C9" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="F9" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="27"/>
       <c r="H9" s="29"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27">
+      <c r="J9" s="27">
         <v>1.0</v>
       </c>
-      <c r="L9" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="M9" s="27">
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27">
         <v>1.0</v>
-      </c>
-      <c r="N9" s="27">
-        <v>2.0</v>
       </c>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="29"/>
-      <c r="S9" s="27"/>
+      <c r="S9" s="27">
+        <v>1.0</v>
+      </c>
       <c r="T9" s="27"/>
       <c r="U9" s="27"/>
-      <c r="V9" s="27">
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27">
         <v>1.0</v>
       </c>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
+      <c r="Y9" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Z9" s="27"/>
       <c r="AA9" s="29"/>
       <c r="AB9" s="27"/>
       <c r="AC9" s="50"/>
       <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27">
+      <c r="AE9" s="27">
         <v>1.0</v>
       </c>
+      <c r="AF9" s="27"/>
       <c r="AG9" s="27"/>
-      <c r="AH9" s="27"/>
+      <c r="AH9" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AI9" s="27"/>
       <c r="AJ9" s="27"/>
-      <c r="AK9" s="27"/>
+      <c r="AK9" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AL9" s="27"/>
-      <c r="AM9" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AM9" s="27"/>
       <c r="AN9" s="27"/>
       <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
+      <c r="AP9" s="27">
+        <v>4.0</v>
+      </c>
       <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
-      <c r="AS9" s="27"/>
-      <c r="AT9" s="27"/>
+      <c r="AR9" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AS9" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AT9" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AU9" s="27"/>
       <c r="AV9" s="27"/>
       <c r="AW9" s="27"/>
@@ -29822,38 +29824,42 @@
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BB9" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="BC9" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="27">
-        <v>1.0</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B10" s="27"/>
       <c r="C10" s="27">
-        <v>6.0</v>
-      </c>
-      <c r="D10" s="27">
-        <v>1.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="27">
+        <v>2.0</v>
+      </c>
       <c r="H10" s="29"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
+      <c r="K10" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="M10" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="N10" s="27">
+        <v>2.0</v>
+      </c>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
@@ -29861,7 +29867,9 @@
       <c r="S10" s="27"/>
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
+      <c r="V10" s="27">
+        <v>1.0</v>
+      </c>
       <c r="W10" s="27"/>
       <c r="X10" s="27"/>
       <c r="Y10" s="27"/>
@@ -29869,31 +29877,27 @@
       <c r="AA10" s="29"/>
       <c r="AB10" s="27"/>
       <c r="AC10" s="50"/>
-      <c r="AD10" s="27">
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27">
         <v>1.0</v>
       </c>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
       <c r="AG10" s="27"/>
       <c r="AH10" s="27"/>
-      <c r="AI10" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="AI10" s="27"/>
       <c r="AJ10" s="27"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="27"/>
-      <c r="AM10" s="27"/>
+      <c r="AM10" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AN10" s="27"/>
-      <c r="AO10" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AO10" s="27"/>
       <c r="AP10" s="27"/>
       <c r="AQ10" s="27"/>
       <c r="AR10" s="27"/>
       <c r="AS10" s="27"/>
-      <c r="AT10" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AT10" s="27"/>
       <c r="AU10" s="27"/>
       <c r="AV10" s="27"/>
       <c r="AW10" s="27"/>
@@ -29982,13 +29986,15 @@
       </c>
       <c r="AU11" s="27"/>
       <c r="AV11" s="27"/>
-      <c r="AW11" s="27"/>
+      <c r="AW11" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX11" s="27"/>
       <c r="AY11" s="27"/>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BB11" s="5">
         <v>1.0</v>
@@ -29999,17 +30005,13 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
-      <c r="D12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="D12" s="27"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="F12" s="27"/>
       <c r="G12" s="27"/>
       <c r="H12" s="29"/>
       <c r="I12" s="27"/>
@@ -30017,58 +30019,56 @@
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
-      <c r="N12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="N12" s="27"/>
       <c r="O12" s="27"/>
       <c r="P12" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Q12" s="27">
-        <v>1.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="Q12" s="27"/>
       <c r="R12" s="29"/>
-      <c r="S12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="S12" s="27"/>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
       <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
+      <c r="W12" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="X12" s="27">
+        <v>3.0</v>
+      </c>
       <c r="Y12" s="27"/>
-      <c r="Z12" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="Z12" s="27"/>
       <c r="AA12" s="29"/>
-      <c r="AB12" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AB12" s="27"/>
       <c r="AC12" s="50"/>
       <c r="AD12" s="27"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="AE12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AF12" s="27"/>
       <c r="AG12" s="27"/>
       <c r="AH12" s="27"/>
       <c r="AI12" s="27"/>
       <c r="AJ12" s="27"/>
-      <c r="AK12" s="27"/>
+      <c r="AK12" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AL12" s="27"/>
       <c r="AM12" s="27"/>
       <c r="AN12" s="27"/>
       <c r="AO12" s="27"/>
       <c r="AP12" s="27"/>
       <c r="AQ12" s="27"/>
-      <c r="AR12" s="27"/>
+      <c r="AR12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AS12" s="27"/>
       <c r="AT12" s="27"/>
       <c r="AU12" s="27"/>
-      <c r="AV12" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AW12" s="27"/>
+      <c r="AV12" s="27"/>
+      <c r="AW12" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AX12" s="27"/>
       <c r="AY12" s="27"/>
       <c r="AZ12" s="6"/>
@@ -30077,39 +30077,45 @@
         <v>14</v>
       </c>
       <c r="BB12" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC12" s="5">
-        <v>1.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="BC12" s="5"/>
       <c r="BF12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="27">
+        <v>59</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27">
         <v>1.0</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="F13" s="27">
+        <v>2.0</v>
+      </c>
       <c r="G13" s="27"/>
       <c r="H13" s="29"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="L13" s="27"/>
       <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
+      <c r="N13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
+      <c r="P13" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="Q13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="R13" s="29"/>
-      <c r="S13" s="27"/>
+      <c r="S13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="T13" s="27"/>
       <c r="U13" s="27"/>
       <c r="V13" s="27"/>
@@ -30117,7 +30123,7 @@
       <c r="X13" s="27"/>
       <c r="Y13" s="27"/>
       <c r="Z13" s="27">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="AA13" s="29"/>
       <c r="AB13" s="27">
@@ -30127,32 +30133,26 @@
       <c r="AD13" s="27"/>
       <c r="AE13" s="27"/>
       <c r="AF13" s="27">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AG13" s="27"/>
       <c r="AH13" s="27"/>
-      <c r="AI13" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI13" s="27"/>
       <c r="AJ13" s="27"/>
       <c r="AK13" s="27"/>
       <c r="AL13" s="27"/>
       <c r="AM13" s="27"/>
-      <c r="AN13" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="AO13" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AP13" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="27"/>
+      <c r="AP13" s="27"/>
       <c r="AQ13" s="27"/>
       <c r="AR13" s="27"/>
       <c r="AS13" s="27"/>
       <c r="AT13" s="27"/>
       <c r="AU13" s="27"/>
-      <c r="AV13" s="27"/>
+      <c r="AV13" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AW13" s="27"/>
       <c r="AX13" s="27"/>
       <c r="AY13" s="27"/>
@@ -30161,79 +30161,81 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="BB13" s="5"/>
+      <c r="BB13" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC13" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="27"/>
+        <v>77</v>
+      </c>
+      <c r="B14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="F14" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="29"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="L14" s="27">
+        <v>3.0</v>
+      </c>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
-      <c r="P14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="P14" s="27"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="29"/>
       <c r="S14" s="27"/>
       <c r="T14" s="27"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27"/>
-      <c r="W14" s="27">
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27">
         <v>1.0</v>
       </c>
-      <c r="X14" s="27">
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="27">
         <v>1.0</v>
       </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AA14" s="29"/>
-      <c r="AB14" s="27"/>
       <c r="AC14" s="50"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
-      <c r="AF14" s="27"/>
+      <c r="AF14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AG14" s="27"/>
       <c r="AH14" s="27"/>
       <c r="AI14" s="27">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="AJ14" s="27"/>
       <c r="AK14" s="27"/>
       <c r="AL14" s="27"/>
-      <c r="AM14" s="27">
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AO14" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AP14" s="27">
         <v>1.0</v>
       </c>
-      <c r="AN14" s="27"/>
-      <c r="AO14" s="27"/>
-      <c r="AP14" s="27"/>
-      <c r="AQ14" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AQ14" s="27"/>
       <c r="AR14" s="27"/>
       <c r="AS14" s="27"/>
       <c r="AT14" s="27"/>
-      <c r="AU14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AU14" s="27"/>
       <c r="AV14" s="27"/>
       <c r="AW14" s="27"/>
       <c r="AX14" s="27"/>
@@ -30244,17 +30246,23 @@
         <v>14</v>
       </c>
       <c r="BB14" s="5"/>
-      <c r="BC14" s="5"/>
+      <c r="BC14" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="E15" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="27">
+        <v>3.0</v>
+      </c>
       <c r="G15" s="27"/>
       <c r="H15" s="29"/>
       <c r="I15" s="27"/>
@@ -30265,7 +30273,7 @@
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
       <c r="P15" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q15" s="27"/>
       <c r="R15" s="29"/>
@@ -30274,10 +30282,10 @@
       <c r="U15" s="27"/>
       <c r="V15" s="27"/>
       <c r="W15" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="X15" s="27">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="Y15" s="27"/>
       <c r="Z15" s="27"/>
@@ -30285,29 +30293,31 @@
       <c r="AB15" s="27"/>
       <c r="AC15" s="50"/>
       <c r="AD15" s="27"/>
-      <c r="AE15" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AE15" s="27"/>
       <c r="AF15" s="27"/>
       <c r="AG15" s="27"/>
       <c r="AH15" s="27"/>
-      <c r="AI15" s="27"/>
+      <c r="AI15" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AJ15" s="27"/>
-      <c r="AK15" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="AK15" s="27"/>
       <c r="AL15" s="27"/>
-      <c r="AM15" s="27"/>
+      <c r="AM15" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AN15" s="27"/>
       <c r="AO15" s="27"/>
       <c r="AP15" s="27"/>
-      <c r="AQ15" s="27"/>
-      <c r="AR15" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AQ15" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AR15" s="27"/>
       <c r="AS15" s="27"/>
       <c r="AT15" s="27"/>
-      <c r="AU15" s="27"/>
+      <c r="AU15" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AV15" s="27"/>
       <c r="AW15" s="27"/>
       <c r="AX15" s="27"/>
@@ -30315,63 +30325,63 @@
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="BB15" s="5">
-        <v>2.0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="BB15" s="5"/>
       <c r="BC15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="27">
-        <v>1.0</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="27">
+      <c r="G16" s="27"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="27">
         <v>1.0</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
+      <c r="J16" s="27">
+        <v>1.0</v>
+      </c>
       <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
+      <c r="L16" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="M16" s="27">
+        <v>1.0</v>
+      </c>
       <c r="N16" s="27"/>
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
       <c r="R16" s="29"/>
       <c r="S16" s="27"/>
-      <c r="T16" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="T16" s="27"/>
       <c r="U16" s="27">
         <v>1.0</v>
       </c>
       <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
+      <c r="W16" s="27">
+        <v>1.0</v>
+      </c>
       <c r="X16" s="27"/>
-      <c r="Y16" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Z16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AA16" s="29"/>
       <c r="AB16" s="27"/>
       <c r="AC16" s="50"/>
       <c r="AD16" s="27"/>
       <c r="AE16" s="27">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="AF16" s="27"/>
-      <c r="AG16" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="AG16" s="27"/>
       <c r="AH16" s="27"/>
       <c r="AI16" s="27"/>
       <c r="AJ16" s="27"/>
@@ -30383,35 +30393,43 @@
       <c r="AP16" s="27"/>
       <c r="AQ16" s="27"/>
       <c r="AR16" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="AS16" s="27"/>
       <c r="AT16" s="27"/>
-      <c r="AU16" s="27"/>
+      <c r="AU16" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AV16" s="27"/>
-      <c r="AW16" s="27"/>
+      <c r="AW16" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX16" s="27"/>
       <c r="AY16" s="27"/>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="BB16" s="5">
+        <v>13</v>
+      </c>
+      <c r="BB16" s="5"/>
+      <c r="BC16" s="5">
         <v>2.0</v>
       </c>
-      <c r="BC16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="27"/>
+        <v>74</v>
+      </c>
+      <c r="B17" s="27">
+        <v>1.0</v>
+      </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="G17" s="27">
+        <v>1.0</v>
+      </c>
       <c r="H17" s="29"/>
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
@@ -30421,44 +30439,46 @@
       <c r="N17" s="27"/>
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
-      <c r="Q17" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="Q17" s="27"/>
       <c r="R17" s="29"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
+      <c r="T17" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="U17" s="27">
+        <v>1.0</v>
+      </c>
       <c r="V17" s="27"/>
       <c r="W17" s="27"/>
       <c r="X17" s="27"/>
-      <c r="Y17" s="27"/>
+      <c r="Y17" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Z17" s="27"/>
       <c r="AA17" s="29"/>
       <c r="AB17" s="27"/>
       <c r="AC17" s="50"/>
-      <c r="AD17" s="27">
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27">
         <v>1.0</v>
       </c>
-      <c r="AE17" s="27"/>
       <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
+      <c r="AG17" s="27">
+        <v>4.0</v>
+      </c>
       <c r="AH17" s="27"/>
       <c r="AI17" s="27"/>
-      <c r="AJ17" s="27">
-        <v>7.0</v>
-      </c>
+      <c r="AJ17" s="27"/>
       <c r="AK17" s="27"/>
       <c r="AL17" s="27"/>
       <c r="AM17" s="27"/>
-      <c r="AN17" s="27">
+      <c r="AN17" s="27"/>
+      <c r="AO17" s="27"/>
+      <c r="AP17" s="27"/>
+      <c r="AQ17" s="27"/>
+      <c r="AR17" s="27">
         <v>2.0</v>
       </c>
-      <c r="AO17" s="27"/>
-      <c r="AP17" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AQ17" s="27"/>
-      <c r="AR17" s="27"/>
       <c r="AS17" s="27"/>
       <c r="AT17" s="27"/>
       <c r="AU17" s="27"/>
@@ -30472,15 +30492,13 @@
         <v>12</v>
       </c>
       <c r="BB17" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC17" s="5">
-        <v>1.0</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="BC17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -30489,65 +30507,55 @@
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
       <c r="H18" s="29"/>
-      <c r="I18" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="J18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="27"/>
-      <c r="L18" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="M18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
+      <c r="Q18" s="27">
+        <v>1.0</v>
+      </c>
       <c r="R18" s="29"/>
       <c r="S18" s="27"/>
       <c r="T18" s="27"/>
-      <c r="U18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="U18" s="27"/>
       <c r="V18" s="27"/>
-      <c r="W18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="W18" s="27"/>
       <c r="X18" s="27"/>
       <c r="Y18" s="27"/>
-      <c r="Z18" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="Z18" s="27"/>
       <c r="AA18" s="29"/>
       <c r="AB18" s="27"/>
       <c r="AC18" s="50"/>
-      <c r="AD18" s="27"/>
-      <c r="AE18" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AD18" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AE18" s="27"/>
       <c r="AF18" s="27"/>
       <c r="AG18" s="27"/>
       <c r="AH18" s="27"/>
       <c r="AI18" s="27"/>
-      <c r="AJ18" s="27"/>
+      <c r="AJ18" s="27">
+        <v>7.0</v>
+      </c>
       <c r="AK18" s="27"/>
       <c r="AL18" s="27"/>
       <c r="AM18" s="27"/>
-      <c r="AN18" s="27"/>
+      <c r="AN18" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AO18" s="27"/>
-      <c r="AP18" s="27"/>
+      <c r="AP18" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AQ18" s="27"/>
-      <c r="AR18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AR18" s="27"/>
       <c r="AS18" s="27"/>
       <c r="AT18" s="27"/>
-      <c r="AU18" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AU18" s="27"/>
       <c r="AV18" s="27"/>
       <c r="AW18" s="27"/>
       <c r="AX18" s="27"/>
@@ -30557,9 +30565,11 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="BB18" s="5"/>
+      <c r="BB18" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC18" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="BF18" s="6"/>
     </row>
@@ -30875,7 +30885,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -30886,72 +30896,72 @@
       <c r="H23" s="29"/>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
+      <c r="K23" s="27">
+        <v>1.0</v>
+      </c>
       <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="M23" s="27">
+        <v>1.0</v>
+      </c>
       <c r="N23" s="27"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
+      <c r="Q23" s="27">
+        <v>1.0</v>
+      </c>
       <c r="R23" s="29"/>
       <c r="S23" s="27"/>
       <c r="T23" s="27"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27">
+      <c r="U23" s="27"/>
+      <c r="V23" s="27">
         <v>1.0</v>
       </c>
-      <c r="X23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
       <c r="Y23" s="27"/>
-      <c r="Z23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="Z23" s="27"/>
       <c r="AA23" s="29"/>
       <c r="AB23" s="27"/>
       <c r="AC23" s="50"/>
-      <c r="AD23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AD23" s="27"/>
       <c r="AE23" s="27"/>
       <c r="AF23" s="27"/>
       <c r="AG23" s="27"/>
       <c r="AH23" s="27"/>
       <c r="AI23" s="27"/>
-      <c r="AJ23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AJ23" s="27"/>
       <c r="AK23" s="27"/>
       <c r="AL23" s="27"/>
-      <c r="AM23" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="AM23" s="27"/>
       <c r="AN23" s="27"/>
       <c r="AO23" s="27"/>
       <c r="AP23" s="27"/>
       <c r="AQ23" s="27"/>
       <c r="AR23" s="27"/>
       <c r="AS23" s="27"/>
-      <c r="AT23" s="27"/>
+      <c r="AT23" s="27">
+        <v>3.0</v>
+      </c>
       <c r="AU23" s="27"/>
       <c r="AV23" s="27"/>
-      <c r="AW23" s="27"/>
+      <c r="AW23" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX23" s="27"/>
       <c r="AY23" s="27"/>
       <c r="AZ23" s="6"/>
       <c r="BA23" s="6">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB23" s="5"/>
       <c r="BC23" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -30962,52 +30972,54 @@
       <c r="H24" s="29"/>
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
-      <c r="K24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="K24" s="27"/>
       <c r="L24" s="27"/>
-      <c r="M24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="M24" s="27"/>
       <c r="N24" s="27"/>
       <c r="O24" s="27"/>
       <c r="P24" s="27"/>
-      <c r="Q24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="Q24" s="27"/>
       <c r="R24" s="29"/>
       <c r="S24" s="27"/>
       <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27">
+      <c r="U24" s="51"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27">
         <v>1.0</v>
       </c>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
+      <c r="X24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
+      <c r="Z24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AA24" s="29"/>
       <c r="AB24" s="27"/>
       <c r="AC24" s="50"/>
-      <c r="AD24" s="27"/>
+      <c r="AD24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AE24" s="27"/>
       <c r="AF24" s="27"/>
       <c r="AG24" s="27"/>
       <c r="AH24" s="27"/>
       <c r="AI24" s="27"/>
-      <c r="AJ24" s="27"/>
+      <c r="AJ24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AK24" s="27"/>
       <c r="AL24" s="27"/>
-      <c r="AM24" s="27"/>
+      <c r="AM24" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AN24" s="27"/>
       <c r="AO24" s="27"/>
       <c r="AP24" s="27"/>
       <c r="AQ24" s="27"/>
       <c r="AR24" s="27"/>
       <c r="AS24" s="27"/>
-      <c r="AT24" s="27">
-        <v>3.0</v>
-      </c>
+      <c r="AT24" s="27"/>
       <c r="AU24" s="27"/>
       <c r="AV24" s="27"/>
       <c r="AW24" s="27"/>
@@ -31020,7 +31032,7 @@
       </c>
       <c r="BB24" s="5"/>
       <c r="BC24" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -31449,7 +31461,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -32086,7 +32098,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B40" s="44">
         <f t="shared" ref="B40:AV40" si="2">SUM(B3:B36)</f>
@@ -63036,7 +63048,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="2"/>
@@ -63201,10 +63213,10 @@
         <v>50</v>
       </c>
       <c r="AY3" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="BA3" s="54" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4">
@@ -64225,7 +64237,7 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -64436,13 +64448,15 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="27">
+        <v>1.0</v>
+      </c>
       <c r="G20" s="27"/>
       <c r="H20" s="29"/>
       <c r="I20" s="27"/>
@@ -64471,29 +64485,27 @@
       <c r="AF20" s="27"/>
       <c r="AG20" s="27"/>
       <c r="AH20" s="27"/>
-      <c r="AI20" s="27"/>
+      <c r="AI20" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ20" s="27"/>
-      <c r="AK20" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AK20" s="27"/>
       <c r="AL20" s="27"/>
-      <c r="AM20" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AN20" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
       <c r="AO20" s="27"/>
       <c r="AP20" s="27"/>
       <c r="AQ20" s="27"/>
       <c r="AR20" s="27"/>
       <c r="AS20" s="27"/>
-      <c r="AT20" s="27"/>
-      <c r="AU20" s="27">
+      <c r="AT20" s="27">
         <v>1.0</v>
       </c>
+      <c r="AU20" s="27"/>
       <c r="AV20" s="27"/>
-      <c r="AW20" s="27"/>
+      <c r="AW20" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX20" s="27"/>
       <c r="AY20" s="27"/>
       <c r="BA20" s="44">
@@ -64503,7 +64515,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -64517,9 +64529,7 @@
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="N21" s="27"/>
       <c r="O21" s="27"/>
       <c r="P21" s="27"/>
       <c r="Q21" s="27"/>
@@ -64536,39 +64546,43 @@
       <c r="AB21" s="27"/>
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
-      <c r="AE21" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AE21" s="27"/>
       <c r="AF21" s="27"/>
       <c r="AG21" s="27"/>
       <c r="AH21" s="27"/>
-      <c r="AI21" s="27">
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="27">
         <v>1.0</v>
       </c>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="27"/>
       <c r="AL21" s="27"/>
-      <c r="AM21" s="27"/>
-      <c r="AN21" s="27"/>
+      <c r="AM21" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AN21" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AO21" s="27"/>
       <c r="AP21" s="27"/>
       <c r="AQ21" s="27"/>
       <c r="AR21" s="27"/>
       <c r="AS21" s="27"/>
       <c r="AT21" s="27"/>
-      <c r="AU21" s="27"/>
+      <c r="AU21" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AV21" s="27"/>
       <c r="AW21" s="27"/>
       <c r="AX21" s="27"/>
       <c r="AY21" s="27"/>
       <c r="BA21" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -64582,7 +64596,9 @@
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
+      <c r="N22" s="27">
+        <v>1.0</v>
+      </c>
       <c r="O22" s="27"/>
       <c r="P22" s="27"/>
       <c r="Q22" s="27"/>
@@ -64592,22 +64608,22 @@
       <c r="U22" s="27"/>
       <c r="V22" s="27"/>
       <c r="W22" s="27"/>
-      <c r="X22" s="27">
-        <v>2.0</v>
-      </c>
+      <c r="X22" s="27"/>
       <c r="Y22" s="27"/>
       <c r="Z22" s="27"/>
       <c r="AA22" s="27"/>
       <c r="AB22" s="27"/>
       <c r="AC22" s="27"/>
       <c r="AD22" s="27"/>
-      <c r="AE22" s="27"/>
+      <c r="AE22" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AF22" s="27"/>
       <c r="AG22" s="27"/>
-      <c r="AH22" s="27">
+      <c r="AH22" s="27"/>
+      <c r="AI22" s="27">
         <v>1.0</v>
       </c>
-      <c r="AI22" s="27"/>
       <c r="AJ22" s="27"/>
       <c r="AK22" s="27"/>
       <c r="AL22" s="27"/>
@@ -64631,29 +64647,23 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="29"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="J23" s="27"/>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
       <c r="O23" s="27"/>
-      <c r="P23" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
@@ -64661,7 +64671,9 @@
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
       <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
+      <c r="X23" s="27">
+        <v>2.0</v>
+      </c>
       <c r="Y23" s="27"/>
       <c r="Z23" s="27"/>
       <c r="AA23" s="27"/>
@@ -64671,7 +64683,9 @@
       <c r="AE23" s="27"/>
       <c r="AF23" s="27"/>
       <c r="AG23" s="27"/>
-      <c r="AH23" s="27"/>
+      <c r="AH23" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AI23" s="27"/>
       <c r="AJ23" s="27"/>
       <c r="AK23" s="27"/>
@@ -64696,25 +64710,29 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27">
+      <c r="E24" s="27">
         <v>1.0</v>
       </c>
+      <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="29"/>
       <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
+      <c r="J24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
       <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
+      <c r="P24" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Q24" s="27"/>
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
@@ -64733,9 +64751,7 @@
       <c r="AF24" s="27"/>
       <c r="AG24" s="27"/>
       <c r="AH24" s="27"/>
-      <c r="AI24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AI24" s="27"/>
       <c r="AJ24" s="27"/>
       <c r="AK24" s="27"/>
       <c r="AL24" s="27"/>
@@ -64746,19 +64762,15 @@
       <c r="AQ24" s="27"/>
       <c r="AR24" s="27"/>
       <c r="AS24" s="27"/>
-      <c r="AT24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AT24" s="27"/>
       <c r="AU24" s="27"/>
       <c r="AV24" s="27"/>
-      <c r="AW24" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AW24" s="27"/>
       <c r="AX24" s="27"/>
       <c r="AY24" s="27"/>
       <c r="BA24" s="44">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -64816,12 +64828,14 @@
       <c r="AT25" s="27"/>
       <c r="AU25" s="27"/>
       <c r="AV25" s="27"/>
-      <c r="AW25" s="27"/>
+      <c r="AW25" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AX25" s="27"/>
       <c r="AY25" s="27"/>
       <c r="BA25" s="44">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -65255,7 +65269,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -65711,7 +65725,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" ref="B41:AY41" si="2">SUM(B5:B39)</f>
@@ -65903,7 +65917,7 @@
       </c>
       <c r="AW41" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AX41" s="5">
         <f t="shared" si="2"/>
@@ -65915,7 +65929,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66902,19 +66916,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -66930,16 +66944,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="5"/>
@@ -66951,16 +66965,16 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="5"/>
@@ -66972,16 +66986,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="5"/>
@@ -66993,16 +67007,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="5"/>
@@ -67014,27 +67028,27 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I7" s="5"/>
       <c r="K7" s="44" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -67043,16 +67057,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="5"/>
@@ -67064,26 +67078,26 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
       <c r="G9" s="49"/>
       <c r="H9" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I9" s="5">
         <v>7.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L9" s="5">
         <v>4.0</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N9" s="5">
         <v>9.0</v>
@@ -67094,32 +67108,32 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I10" s="5">
         <v>7.0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L10" s="5">
         <v>3.0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N10" s="5">
         <v>8.0</v>
@@ -67130,32 +67144,32 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I11" s="5">
         <v>7.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L11" s="5">
         <v>3.0</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N11" s="5">
         <v>7.0</v>
@@ -67166,32 +67180,32 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I12" s="5">
         <v>6.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L12" s="5">
         <v>2.0</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N12" s="5">
         <v>7.0</v>
@@ -67202,33 +67216,33 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
       <c r="H13" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I13" s="5">
         <v>4.0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L13" s="5">
         <v>2.0</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N13" s="5">
         <v>6.0</v>
@@ -67239,32 +67253,32 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I14" s="5">
         <v>4.0</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L14" s="5">
         <v>2.0</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N14" s="5">
         <v>6.0</v>
@@ -67275,32 +67289,32 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I15" s="5">
         <v>4.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L15" s="5">
         <v>2.0</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N15" s="5">
         <v>5.0</v>
@@ -67311,32 +67325,32 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I16" s="5">
         <v>3.0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L16" s="5">
         <v>2.0</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N16" s="5">
         <v>5.0</v>
@@ -67347,32 +67361,32 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I17" s="5">
         <v>3.0</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L17" s="5">
         <v>2.0</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N17" s="5">
         <v>5.0</v>
@@ -67383,30 +67397,30 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I18" s="5">
         <v>3.0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N18" s="5">
         <v>5.0</v>
@@ -67417,24 +67431,24 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
       <c r="G19" s="49"/>
       <c r="H19" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I19" s="5">
         <v>3.0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N19" s="5">
         <v>4.0</v>
@@ -67445,30 +67459,30 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I20" s="5">
         <v>3.0</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N20" s="5">
         <v>4.0</v>
@@ -67479,30 +67493,30 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="63" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I21" s="5">
         <v>2.0</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N21" s="5">
         <v>3.0</v>
@@ -67513,26 +67527,26 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E22" s="49"/>
       <c r="G22" s="49"/>
       <c r="H22" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N22" s="5">
         <v>3.0</v>
@@ -67543,28 +67557,28 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N23" s="5">
         <v>3.0</v>
@@ -67575,28 +67589,28 @@
         <v>22.0</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="63" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N24" s="5">
         <v>3.0</v>
@@ -67607,28 +67621,28 @@
         <v>23.0</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N25" s="5">
         <v>2.0</v>
@@ -67639,28 +67653,28 @@
         <v>24.0</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N26" s="5">
         <v>2.0</v>
@@ -67671,27 +67685,27 @@
         <v>25.0</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N27" s="5">
         <v>2.0</v>
@@ -67702,21 +67716,21 @@
         <v>26.0</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
       <c r="E28" s="49"/>
       <c r="G28" s="49"/>
       <c r="H28" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N28" s="5">
         <v>2.0</v>
@@ -67727,26 +67741,26 @@
         <v>27.0</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N29" s="5">
         <v>2.0</v>
@@ -67757,20 +67771,20 @@
         <v>28.0</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="49"/>
       <c r="H30" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N30" s="5">
         <v>2.0</v>
@@ -67781,26 +67795,26 @@
         <v>29.0</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E31" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N31" s="5"/>
     </row>
@@ -67809,24 +67823,24 @@
         <v>30.0</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I32" s="5"/>
       <c r="K32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N32" s="5"/>
     </row>
@@ -67835,23 +67849,23 @@
         <v>31.0</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N33" s="5"/>
     </row>
@@ -67860,21 +67874,21 @@
         <v>32.0</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E34" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N34" s="5"/>
     </row>
@@ -67883,21 +67897,21 @@
         <v>33.0</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E35" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N35" s="5"/>
     </row>
@@ -67906,21 +67920,21 @@
         <v>34.0</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E36" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N36" s="5"/>
     </row>
@@ -67929,21 +67943,21 @@
         <v>35.0</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N37" s="5"/>
     </row>
@@ -67952,16 +67966,16 @@
         <v>36.0</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E38" s="49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -67972,16 +67986,16 @@
         <v>37.0</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -67992,16 +68006,16 @@
         <v>38.0</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E40" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -68012,16 +68026,16 @@
         <v>39.0</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E41" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -68032,16 +68046,16 @@
         <v>40.0</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E42" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -68052,16 +68066,16 @@
         <v>41.0</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E43" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -68072,16 +68086,16 @@
         <v>42.0</v>
       </c>
       <c r="B44" s="49" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="49" t="s">
         <v>233</v>
       </c>
-      <c r="C44" s="49" t="s">
-        <v>232</v>
-      </c>
       <c r="D44" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E44" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -68092,16 +68106,16 @@
         <v>43.0</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C45" s="49" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E45" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -68112,16 +68126,16 @@
         <v>44.0</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E46" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -68132,16 +68146,16 @@
         <v>45.0</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -68152,16 +68166,16 @@
         <v>46.0</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C48" s="49" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E48" s="49" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -68172,16 +68186,16 @@
         <v>47.0</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -68192,16 +68206,16 @@
         <v>48.0</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C50" s="49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E50" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>

</xml_diff>

<commit_message>
Week 49 Final data update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="KCSWMUleTP2KA5AUJ8UtnNfMBPncuC/m+G++KNWuD2A="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="XynpmnBcZ8TxnAVm9yCxVsUZr5Gtla3t2urMy1hsZhk="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="245">
   <si>
     <t>MARLOW DUKES 2024</t>
   </si>
@@ -213,13 +213,10 @@
     <t>INSPECTOR GADGET</t>
   </si>
   <si>
-    <t>KERMIT</t>
-  </si>
-  <si>
     <t>ZIGZAG</t>
   </si>
   <si>
-    <t>FATHER TED</t>
+    <t>KERMIT</t>
   </si>
   <si>
     <t>VINCE</t>
@@ -228,13 +225,16 @@
     <t>PRESTON</t>
   </si>
   <si>
+    <t>FATHER TED</t>
+  </si>
+  <si>
     <t>DOM</t>
   </si>
   <si>
-    <t>DUNCAN</t>
+    <t>CAPTAIN KIRK</t>
   </si>
   <si>
-    <t>CAPTAIN KIRK</t>
+    <t>DUNCAN</t>
   </si>
   <si>
     <t>SMUDGE</t>
@@ -420,6 +420,9 @@
     <t>DAY OFF DICKIE</t>
   </si>
   <si>
+    <t>MAMAS</t>
+  </si>
+  <si>
     <t># VOTES</t>
   </si>
   <si>
@@ -570,9 +573,6 @@
     <t>Carzola</t>
   </si>
   <si>
-    <t>Vince</t>
-  </si>
-  <si>
     <t>Ian - Wilson</t>
   </si>
   <si>
@@ -580,6 +580,9 @@
   </si>
   <si>
     <t>Matt B</t>
+  </si>
+  <si>
+    <t>Vince</t>
   </si>
   <si>
     <t>Dom - Duncan</t>
@@ -591,13 +594,13 @@
     <t>Fred?</t>
   </si>
   <si>
-    <t>Moo</t>
-  </si>
-  <si>
     <t>Preston - Phantom</t>
   </si>
   <si>
     <t>Lost 4-6</t>
+  </si>
+  <si>
+    <t>Moo</t>
   </si>
   <si>
     <t>Dwarf - Gadget</t>
@@ -696,10 +699,16 @@
     <t>Lost 0-5</t>
   </si>
   <si>
+    <t>Straight Rob</t>
+  </si>
+  <si>
     <t>Vince - Artist</t>
   </si>
   <si>
     <t>Matt</t>
+  </si>
+  <si>
+    <t>Mamas</t>
   </si>
   <si>
     <t>Carzola - Dwarf</t>
@@ -745,6 +754,9 @@
   </si>
   <si>
     <t>Capt Kirk - Flo</t>
+  </si>
+  <si>
+    <t>Gadget - Bruce</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1404,8 @@
     <col customWidth="1" min="42" max="42" width="6.43" outlineLevel="1"/>
     <col customWidth="1" min="43" max="49" width="6.71" outlineLevel="1"/>
     <col customWidth="1" min="50" max="50" width="8.29" outlineLevel="1"/>
-    <col customWidth="1" min="51" max="54" width="9.14"/>
-    <col customWidth="1" min="55" max="56" width="8.86"/>
+    <col customWidth="1" min="51" max="53" width="9.14"/>
+    <col customWidth="1" min="54" max="56" width="8.86"/>
     <col customWidth="1" min="57" max="57" width="10.29"/>
     <col customWidth="1" min="58" max="62" width="8.86"/>
   </cols>
@@ -1951,20 +1963,22 @@
       <c r="AW5" s="16">
         <v>-4.0</v>
       </c>
-      <c r="AX5" s="16"/>
+      <c r="AX5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AY5" s="19"/>
       <c r="AZ5" s="19"/>
       <c r="BA5" s="19">
         <v>1.0</v>
       </c>
-      <c r="BB5" s="19"/>
+      <c r="BB5" s="5"/>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC39" si="1">COUNT(B5:AX5)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD39" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE39" si="3">COUNTIF($B5:$AX5, "0")</f>
@@ -1976,15 +1990,15 @@
       </c>
       <c r="BG5" s="5">
         <f t="shared" ref="BG5:BG39" si="5">SUM(BD5*3)+BE5</f>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="BH5" s="5">
         <f t="shared" ref="BH5:BH39" si="6">SUM(B5:AX5)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="BI5" s="20">
         <f t="shared" ref="BI5:BI39" si="7">SUM(BD5*3+BE5*1)/SUM(BC5*3)</f>
-        <v>0.5833333333</v>
+        <v>0.593495935</v>
       </c>
       <c r="BJ5" s="20"/>
     </row>
@@ -2120,20 +2134,22 @@
       <c r="AW6" s="22">
         <v>-4.0</v>
       </c>
-      <c r="AX6" s="22"/>
+      <c r="AX6" s="24">
+        <v>1.0</v>
+      </c>
       <c r="AY6" s="19"/>
       <c r="AZ6" s="19"/>
       <c r="BA6" s="19">
         <v>2.0</v>
       </c>
-      <c r="BB6" s="19"/>
+      <c r="BB6" s="5"/>
       <c r="BC6" s="5">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="3"/>
@@ -2145,15 +2161,15 @@
       </c>
       <c r="BG6" s="5">
         <f t="shared" si="5"/>
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="BH6" s="5">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BI6" s="20">
         <f t="shared" si="7"/>
-        <v>0.5083333333</v>
+        <v>0.5203252033</v>
       </c>
       <c r="BJ6" s="20"/>
     </row>
@@ -2293,7 +2309,7 @@
       <c r="BA7" s="19">
         <v>3.0</v>
       </c>
-      <c r="BB7" s="19"/>
+      <c r="BB7" s="5"/>
       <c r="BC7" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2450,16 +2466,18 @@
       <c r="AW8" s="16">
         <v>4.0</v>
       </c>
-      <c r="AX8" s="16"/>
+      <c r="AX8" s="15">
+        <v>-1.0</v>
+      </c>
       <c r="AY8" s="19"/>
       <c r="AZ8" s="19"/>
       <c r="BA8" s="19">
         <v>4.0</v>
       </c>
-      <c r="BB8" s="19"/>
+      <c r="BB8" s="5"/>
       <c r="BC8" s="5">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="2"/>
@@ -2471,7 +2489,7 @@
       </c>
       <c r="BF8" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BG8" s="5">
         <f t="shared" si="5"/>
@@ -2479,11 +2497,11 @@
       </c>
       <c r="BH8" s="5">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BI8" s="20">
         <f t="shared" si="7"/>
-        <v>0.5225225225</v>
+        <v>0.5087719298</v>
       </c>
       <c r="BJ8" s="20"/>
     </row>
@@ -2492,90 +2510,88 @@
         <v>63</v>
       </c>
       <c r="B9" s="32">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" s="32">
-        <v>-1.0</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="32">
+        <v>9.0</v>
+      </c>
+      <c r="E9" s="32">
+        <v>1.0</v>
+      </c>
       <c r="F9" s="32">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="G9" s="32">
         <v>0.0</v>
       </c>
       <c r="H9" s="33"/>
-      <c r="I9" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="J9" s="32">
-        <v>8.0</v>
-      </c>
-      <c r="K9" s="34">
-        <v>0.0</v>
-      </c>
-      <c r="L9" s="32">
-        <v>-2.0</v>
-      </c>
-      <c r="M9" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="N9" s="32">
-        <v>0.0</v>
-      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
       <c r="O9" s="32"/>
-      <c r="P9" s="32">
-        <v>-2.0</v>
-      </c>
+      <c r="P9" s="32"/>
       <c r="Q9" s="32"/>
       <c r="R9" s="33"/>
       <c r="S9" s="32">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="T9" s="34">
-        <v>-1.0</v>
-      </c>
-      <c r="U9" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="V9" s="32">
-        <v>-8.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="U9" s="32"/>
+      <c r="V9" s="34">
+        <v>8.0</v>
       </c>
       <c r="W9" s="32">
         <v>0.0</v>
       </c>
       <c r="X9" s="32">
-        <v>5.0</v>
+        <v>-5.0</v>
       </c>
       <c r="Y9" s="32">
         <v>0.0</v>
       </c>
-      <c r="Z9" s="32"/>
+      <c r="Z9" s="32">
+        <v>2.0</v>
+      </c>
       <c r="AA9" s="33"/>
-      <c r="AB9" s="32"/>
+      <c r="AB9" s="32">
+        <v>-1.0</v>
+      </c>
       <c r="AC9" s="35"/>
       <c r="AD9" s="32">
         <v>0.0</v>
       </c>
       <c r="AE9" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="AF9" s="32"/>
+        <v>-4.0</v>
+      </c>
+      <c r="AF9" s="32">
+        <v>-2.0</v>
+      </c>
       <c r="AG9" s="32">
         <v>5.0</v>
       </c>
       <c r="AH9" s="32">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AI9" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="AJ9" s="32">
         <v>-1.0</v>
       </c>
-      <c r="AJ9" s="32"/>
       <c r="AK9" s="32">
         <v>1.0</v>
       </c>
-      <c r="AL9" s="32"/>
+      <c r="AL9" s="32">
+        <v>-1.0</v>
+      </c>
       <c r="AM9" s="34">
         <v>0.0</v>
       </c>
@@ -2583,64 +2599,68 @@
         <v>0.0</v>
       </c>
       <c r="AO9" s="32">
-        <v>-4.0</v>
+        <v>4.0</v>
       </c>
       <c r="AP9" s="32">
         <v>-1.0</v>
       </c>
       <c r="AQ9" s="32">
+        <v>-4.0</v>
+      </c>
+      <c r="AR9" s="32">
+        <v>-2.0</v>
+      </c>
+      <c r="AS9" s="32">
+        <v>-2.0</v>
+      </c>
+      <c r="AT9" s="32">
+        <v>-1.0</v>
+      </c>
+      <c r="AU9" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="AV9" s="32">
+        <v>-4.0</v>
+      </c>
+      <c r="AW9" s="32">
         <v>4.0</v>
       </c>
-      <c r="AR9" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="AS9" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="AT9" s="34">
+      <c r="AX9" s="32">
         <v>1.0</v>
       </c>
-      <c r="AU9" s="32">
-        <v>0.0</v>
-      </c>
-      <c r="AV9" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="AW9" s="32"/>
-      <c r="AX9" s="32"/>
       <c r="AY9" s="19"/>
       <c r="AZ9" s="19"/>
       <c r="BA9" s="19">
         <v>5.0</v>
       </c>
-      <c r="BB9" s="19"/>
+      <c r="BB9" s="5"/>
       <c r="BC9" s="5">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="BF9" s="5">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BG9" s="5">
         <f t="shared" si="5"/>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="BH9" s="5">
         <f t="shared" si="6"/>
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="BI9" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.5142857143</v>
       </c>
       <c r="BJ9" s="20"/>
     </row>
@@ -2649,88 +2669,90 @@
         <v>64</v>
       </c>
       <c r="B10" s="32">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="C10" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="32">
-        <v>9.0</v>
-      </c>
-      <c r="E10" s="32">
-        <v>1.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="32">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G10" s="32">
         <v>0.0</v>
       </c>
       <c r="H10" s="33"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="27"/>
+      <c r="I10" s="32">
+        <v>7.0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>8.0</v>
+      </c>
+      <c r="K10" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="32">
+        <v>-2.0</v>
+      </c>
+      <c r="M10" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="N10" s="27">
+        <v>0.0</v>
+      </c>
       <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
+      <c r="P10" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="33"/>
       <c r="S10" s="32">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="T10" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="U10" s="32"/>
-      <c r="V10" s="34">
-        <v>8.0</v>
+        <v>-1.0</v>
+      </c>
+      <c r="U10" s="32">
+        <v>4.0</v>
+      </c>
+      <c r="V10" s="32">
+        <v>-8.0</v>
       </c>
       <c r="W10" s="32">
         <v>0.0</v>
       </c>
       <c r="X10" s="32">
-        <v>-5.0</v>
+        <v>5.0</v>
       </c>
       <c r="Y10" s="32">
         <v>0.0</v>
       </c>
-      <c r="Z10" s="32">
-        <v>2.0</v>
-      </c>
+      <c r="Z10" s="32"/>
       <c r="AA10" s="33"/>
-      <c r="AB10" s="32">
-        <v>-1.0</v>
-      </c>
+      <c r="AB10" s="32"/>
       <c r="AC10" s="35"/>
       <c r="AD10" s="32">
         <v>0.0</v>
       </c>
       <c r="AE10" s="32">
-        <v>-4.0</v>
-      </c>
-      <c r="AF10" s="32">
-        <v>-2.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="AF10" s="32"/>
       <c r="AG10" s="32">
         <v>5.0</v>
       </c>
       <c r="AH10" s="32">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AI10" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="AJ10" s="32">
         <v>-1.0</v>
       </c>
+      <c r="AJ10" s="32"/>
       <c r="AK10" s="32">
         <v>1.0</v>
       </c>
-      <c r="AL10" s="32">
-        <v>-1.0</v>
-      </c>
+      <c r="AL10" s="32"/>
       <c r="AM10" s="34">
         <v>0.0</v>
       </c>
@@ -2738,54 +2760,54 @@
         <v>0.0</v>
       </c>
       <c r="AO10" s="32">
-        <v>4.0</v>
+        <v>-4.0</v>
       </c>
       <c r="AP10" s="32">
         <v>-1.0</v>
       </c>
       <c r="AQ10" s="32">
-        <v>-4.0</v>
+        <v>4.0</v>
       </c>
       <c r="AR10" s="32">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AS10" s="32">
-        <v>-2.0</v>
-      </c>
-      <c r="AT10" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="AT10" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="AU10" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="AV10" s="32">
+        <v>4.0</v>
+      </c>
+      <c r="AW10" s="32"/>
+      <c r="AX10" s="32">
         <v>-1.0</v>
       </c>
-      <c r="AU10" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="AV10" s="32">
-        <v>-4.0</v>
-      </c>
-      <c r="AW10" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="AX10" s="32"/>
       <c r="AY10" s="19"/>
       <c r="AZ10" s="19"/>
       <c r="BA10" s="19">
         <v>6.0</v>
       </c>
-      <c r="BB10" s="19"/>
+      <c r="BB10" s="5"/>
       <c r="BC10" s="5">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BF10" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BG10" s="5">
         <f t="shared" si="5"/>
@@ -2793,11 +2815,11 @@
       </c>
       <c r="BH10" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="BI10" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4857142857</v>
       </c>
       <c r="BJ10" s="20"/>
     </row>
@@ -2805,62 +2827,72 @@
       <c r="A11" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="C11" s="27">
         <v>1.0</v>
       </c>
-      <c r="D11" s="27">
-        <v>9.0</v>
-      </c>
+      <c r="D11" s="27"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27">
+      <c r="F11" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="G11" s="28">
         <v>0.0</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="27">
-        <v>7.0</v>
-      </c>
-      <c r="J11" s="28">
+        <v>-7.0</v>
+      </c>
+      <c r="J11" s="27">
         <v>8.0</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="27">
+        <v>0.0</v>
+      </c>
       <c r="L11" s="27">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="M11" s="27">
         <v>-1.0</v>
       </c>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
+      <c r="N11" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="O11" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="P11" s="27">
         <v>2.0</v>
       </c>
-      <c r="Q11" s="27"/>
+      <c r="Q11" s="27">
+        <v>3.0</v>
+      </c>
       <c r="R11" s="29"/>
-      <c r="S11" s="28">
+      <c r="S11" s="27">
         <v>-2.0</v>
       </c>
       <c r="T11" s="27">
         <v>1.0</v>
       </c>
-      <c r="U11" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="X11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27">
+        <v>8.0</v>
+      </c>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27">
+        <v>5.0</v>
+      </c>
       <c r="Y11" s="27">
         <v>0.0</v>
       </c>
       <c r="Z11" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AA11" s="29"/>
       <c r="AB11" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AC11" s="30"/>
       <c r="AD11" s="27">
@@ -2875,22 +2907,24 @@
       <c r="AG11" s="27">
         <v>-5.0</v>
       </c>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="27"/>
+      <c r="AH11" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="AI11" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AJ11" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AK11" s="27"/>
+        <v>1.0</v>
+      </c>
+      <c r="AK11" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AL11" s="27"/>
-      <c r="AM11" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AM11" s="27"/>
       <c r="AN11" s="27">
         <v>0.0</v>
       </c>
-      <c r="AO11" s="27">
-        <v>4.0</v>
-      </c>
+      <c r="AO11" s="27"/>
       <c r="AP11" s="27"/>
       <c r="AQ11" s="27">
         <v>-4.0</v>
@@ -2899,32 +2933,32 @@
         <v>2.0</v>
       </c>
       <c r="AS11" s="27">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AT11" s="27"/>
       <c r="AU11" s="27">
         <v>1.0</v>
       </c>
       <c r="AV11" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AW11" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AX11" s="27"/>
+      <c r="AW11" s="27"/>
+      <c r="AX11" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY11" s="19"/>
       <c r="AZ11" s="19"/>
       <c r="BA11" s="19">
         <v>7.0</v>
       </c>
-      <c r="BB11" s="19"/>
+      <c r="BB11" s="5"/>
       <c r="BC11" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="3"/>
@@ -2932,19 +2966,19 @@
       </c>
       <c r="BF11" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="BG11" s="5">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="BH11" s="5">
         <f t="shared" si="6"/>
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="BI11" s="20">
         <f t="shared" si="7"/>
-        <v>0.5517241379</v>
+        <v>0.4857142857</v>
       </c>
       <c r="BJ11" s="20"/>
     </row>
@@ -2956,22 +2990,24 @@
         <v>-1.0</v>
       </c>
       <c r="C12" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="27"/>
+        <v>-1.0</v>
+      </c>
+      <c r="D12" s="27">
+        <v>-9.0</v>
+      </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="27">
+      <c r="F12" s="28">
         <v>-1.0</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>0.0</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="27">
-        <v>-7.0</v>
+        <v>7.0</v>
       </c>
       <c r="J12" s="27">
-        <v>8.0</v>
+        <v>-8.0</v>
       </c>
       <c r="K12" s="27">
         <v>0.0</v>
@@ -2980,128 +3016,134 @@
         <v>2.0</v>
       </c>
       <c r="M12" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N12" s="27">
         <v>0.0</v>
       </c>
       <c r="O12" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="P12" s="27">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="P12" s="28">
+        <v>-2.0</v>
       </c>
       <c r="Q12" s="27">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="R12" s="29"/>
       <c r="S12" s="27">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="T12" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="U12" s="27"/>
+        <v>-1.0</v>
+      </c>
+      <c r="U12" s="27">
+        <v>-4.0</v>
+      </c>
       <c r="V12" s="27">
         <v>8.0</v>
       </c>
-      <c r="W12" s="27"/>
+      <c r="W12" s="27">
+        <v>0.0</v>
+      </c>
       <c r="X12" s="27">
         <v>5.0</v>
       </c>
-      <c r="Y12" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="Z12" s="28">
-        <v>-2.0</v>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27">
+        <v>2.0</v>
       </c>
       <c r="AA12" s="29"/>
-      <c r="AB12" s="27">
-        <v>1.0</v>
+      <c r="AB12" s="28">
+        <v>-1.0</v>
       </c>
       <c r="AC12" s="30"/>
-      <c r="AD12" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AD12" s="27"/>
       <c r="AE12" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AF12" s="27">
-        <v>-2.0</v>
-      </c>
+        <v>-4.0</v>
+      </c>
+      <c r="AF12" s="27"/>
       <c r="AG12" s="27">
         <v>-5.0</v>
       </c>
-      <c r="AH12" s="28">
+      <c r="AH12" s="27">
         <v>-2.0</v>
       </c>
       <c r="AI12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AJ12" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AJ12" s="27">
-        <v>1.0</v>
-      </c>
       <c r="AK12" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AL12" s="27"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AL12" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AM12" s="27"/>
       <c r="AN12" s="27">
         <v>0.0</v>
       </c>
-      <c r="AO12" s="27"/>
-      <c r="AP12" s="27"/>
-      <c r="AQ12" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="AR12" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AS12" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="AT12" s="27"/>
+      <c r="AO12" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AP12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AQ12" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="AR12" s="27"/>
+      <c r="AS12" s="27"/>
+      <c r="AT12" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AU12" s="27">
         <v>1.0</v>
       </c>
       <c r="AV12" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AW12" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AW12" s="27"/>
-      <c r="AX12" s="27"/>
+      <c r="AX12" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY12" s="19"/>
       <c r="AZ12" s="19"/>
       <c r="BA12" s="19">
         <v>8.0</v>
       </c>
-      <c r="BB12" s="19"/>
+      <c r="BB12" s="5"/>
       <c r="BC12" s="5">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BF12" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="BG12" s="5">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="BH12" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="BI12" s="20">
         <f t="shared" si="7"/>
-        <v>0.4705882353</v>
+        <v>0.4385964912</v>
       </c>
       <c r="BJ12" s="20"/>
     </row>
@@ -3109,19 +3151,15 @@
       <c r="A13" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="B13" s="27"/>
       <c r="C13" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13" s="27">
-        <v>-9.0</v>
+        <v>9.0</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="F13" s="27"/>
       <c r="G13" s="27">
         <v>0.0</v>
       </c>
@@ -3129,99 +3167,87 @@
       <c r="I13" s="27">
         <v>7.0</v>
       </c>
-      <c r="J13" s="27">
-        <v>-8.0</v>
-      </c>
-      <c r="K13" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="J13" s="28">
+        <v>8.0</v>
+      </c>
+      <c r="K13" s="27"/>
       <c r="L13" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="M13" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27">
         <v>2.0</v>
       </c>
-      <c r="M13" s="27">
+      <c r="Q13" s="27"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="T13" s="27">
         <v>1.0</v>
       </c>
-      <c r="N13" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="O13" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="P13" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="Q13" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="R13" s="29"/>
-      <c r="S13" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="T13" s="27">
-        <v>-1.0</v>
-      </c>
       <c r="U13" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="V13" s="27">
-        <v>8.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="V13" s="27"/>
       <c r="W13" s="27">
         <v>0.0</v>
       </c>
-      <c r="X13" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27">
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" s="28">
         <v>2.0</v>
       </c>
       <c r="AA13" s="29"/>
-      <c r="AB13" s="28">
+      <c r="AB13" s="27">
         <v>-1.0</v>
       </c>
       <c r="AC13" s="30"/>
-      <c r="AD13" s="27"/>
+      <c r="AD13" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AE13" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="AF13" s="27"/>
+        <v>4.0</v>
+      </c>
+      <c r="AF13" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="AG13" s="27">
         <v>-5.0</v>
       </c>
-      <c r="AH13" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="AI13" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
       <c r="AJ13" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AK13" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AL13" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AM13" s="27"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AN13" s="27">
         <v>0.0</v>
       </c>
       <c r="AO13" s="27">
         <v>4.0</v>
       </c>
-      <c r="AP13" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AQ13" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="AR13" s="27"/>
-      <c r="AS13" s="27"/>
-      <c r="AT13" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27">
+        <v>-4.0</v>
+      </c>
+      <c r="AR13" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AS13" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AT13" s="27"/>
       <c r="AU13" s="27">
         <v>1.0</v>
       </c>
@@ -3231,16 +3257,18 @@
       <c r="AW13" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AX13" s="27"/>
+      <c r="AX13" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AY13" s="19"/>
       <c r="AZ13" s="19"/>
       <c r="BA13" s="19">
         <v>9.0</v>
       </c>
-      <c r="BB13" s="19"/>
+      <c r="BB13" s="5"/>
       <c r="BC13" s="5">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="2"/>
@@ -3248,23 +3276,23 @@
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF13" s="5">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="BG13" s="5">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="BH13" s="5">
         <f t="shared" si="6"/>
-        <v>-7</v>
+        <v>28</v>
       </c>
       <c r="BI13" s="20">
         <f t="shared" si="7"/>
-        <v>0.4234234234</v>
+        <v>0.5333333333</v>
       </c>
       <c r="BJ13" s="20"/>
     </row>
@@ -3368,20 +3396,22 @@
       </c>
       <c r="AV14" s="27"/>
       <c r="AW14" s="27"/>
-      <c r="AX14" s="27"/>
+      <c r="AX14" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY14" s="19"/>
       <c r="AZ14" s="19"/>
       <c r="BA14" s="19">
         <v>10.0</v>
       </c>
-      <c r="BB14" s="19"/>
+      <c r="BB14" s="5"/>
       <c r="BC14" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="3"/>
@@ -3393,15 +3423,15 @@
       </c>
       <c r="BG14" s="5">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="BH14" s="5">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BI14" s="20">
         <f t="shared" si="7"/>
-        <v>0.5833333333</v>
+        <v>0.6</v>
       </c>
       <c r="BJ14" s="20"/>
     </row>
@@ -3409,43 +3439,37 @@
       <c r="A15" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="27">
         <v>-1.0</v>
       </c>
       <c r="C15" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D15" s="27">
         <v>-9.0</v>
       </c>
-      <c r="E15" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="F15" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="27">
         <v>0.0</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27">
+      <c r="J15" s="28">
+        <v>-8.0</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="N15" s="27">
         <v>0.0</v>
       </c>
-      <c r="L15" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="M15" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28">
+      <c r="O15" s="27">
         <v>1.0</v>
       </c>
-      <c r="P15" s="27">
-        <v>-2.0</v>
-      </c>
+      <c r="P15" s="27"/>
       <c r="Q15" s="27">
         <v>3.0</v>
       </c>
@@ -3453,10 +3477,8 @@
       <c r="S15" s="27">
         <v>-2.0</v>
       </c>
-      <c r="T15" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="U15" s="27">
+      <c r="T15" s="27"/>
+      <c r="U15" s="28">
         <v>4.0</v>
       </c>
       <c r="V15" s="27">
@@ -3468,43 +3490,47 @@
       <c r="X15" s="27">
         <v>-5.0</v>
       </c>
-      <c r="Y15" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="Z15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="AA15" s="29"/>
       <c r="AB15" s="27"/>
       <c r="AC15" s="30"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="27"/>
+      <c r="AD15" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AE15" s="28">
+        <v>-4.0</v>
+      </c>
       <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="27"/>
-      <c r="AI15" s="27"/>
+      <c r="AG15" s="27">
+        <v>5.0</v>
+      </c>
+      <c r="AH15" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="AI15" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AJ15" s="27"/>
-      <c r="AK15" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="AK15" s="27"/>
       <c r="AL15" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AM15" s="27">
-        <v>0.0</v>
-      </c>
+      <c r="AM15" s="27"/>
       <c r="AN15" s="27">
         <v>0.0</v>
       </c>
       <c r="AO15" s="27">
         <v>4.0</v>
       </c>
-      <c r="AP15" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="AP15" s="27"/>
       <c r="AQ15" s="27">
         <v>-4.0</v>
       </c>
       <c r="AR15" s="27">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AS15" s="27">
         <v>-2.0</v>
@@ -3512,47 +3538,49 @@
       <c r="AT15" s="27">
         <v>1.0</v>
       </c>
-      <c r="AU15" s="27">
+      <c r="AU15" s="27"/>
+      <c r="AV15" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="AW15" s="28">
+        <v>-4.0</v>
+      </c>
+      <c r="AX15" s="27">
         <v>1.0</v>
       </c>
-      <c r="AV15" s="27"/>
-      <c r="AW15" s="27">
-        <v>-4.0</v>
-      </c>
-      <c r="AX15" s="27"/>
       <c r="AY15" s="19"/>
       <c r="AZ15" s="19"/>
       <c r="BA15" s="19">
         <v>11.0</v>
       </c>
-      <c r="BB15" s="19"/>
+      <c r="BB15" s="5"/>
       <c r="BC15" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BF15" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BG15" s="5">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BH15" s="5">
         <f t="shared" si="6"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="BI15" s="20">
         <f t="shared" si="7"/>
-        <v>0.4516129032</v>
+        <v>0.4888888889</v>
       </c>
       <c r="BJ15" s="20"/>
     </row>
@@ -3560,37 +3588,43 @@
       <c r="A16" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="28">
         <v>-1.0</v>
       </c>
       <c r="C16" s="27">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D16" s="27">
         <v>-9.0</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="E16" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="G16" s="27">
         <v>0.0</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="28">
-        <v>-8.0</v>
-      </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="L16" s="27">
+        <v>2.0</v>
+      </c>
       <c r="M16" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="N16" s="27"/>
+      <c r="O16" s="28">
         <v>1.0</v>
       </c>
-      <c r="N16" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="O16" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="P16" s="27"/>
+      <c r="P16" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="Q16" s="27">
         <v>3.0</v>
       </c>
@@ -3598,8 +3632,10 @@
       <c r="S16" s="27">
         <v>-2.0</v>
       </c>
-      <c r="T16" s="27"/>
-      <c r="U16" s="28">
+      <c r="T16" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="U16" s="27">
         <v>4.0</v>
       </c>
       <c r="V16" s="27">
@@ -3611,47 +3647,43 @@
       <c r="X16" s="27">
         <v>-5.0</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27">
-        <v>-2.0</v>
-      </c>
+      <c r="Y16" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="Z16" s="27"/>
       <c r="AA16" s="29"/>
       <c r="AB16" s="27"/>
       <c r="AC16" s="30"/>
-      <c r="AD16" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="AE16" s="28">
-        <v>-4.0</v>
-      </c>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
       <c r="AF16" s="27"/>
-      <c r="AG16" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="AH16" s="27">
-        <v>-2.0</v>
-      </c>
-      <c r="AI16" s="27">
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
+      <c r="AI16" s="27"/>
+      <c r="AJ16" s="27"/>
+      <c r="AK16" s="28">
         <v>1.0</v>
       </c>
-      <c r="AJ16" s="27"/>
-      <c r="AK16" s="27"/>
       <c r="AL16" s="27">
         <v>-1.0</v>
       </c>
-      <c r="AM16" s="27"/>
+      <c r="AM16" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AN16" s="27">
         <v>0.0</v>
       </c>
       <c r="AO16" s="27">
         <v>4.0</v>
       </c>
-      <c r="AP16" s="27"/>
+      <c r="AP16" s="28">
+        <v>1.0</v>
+      </c>
       <c r="AQ16" s="27">
         <v>-4.0</v>
       </c>
       <c r="AR16" s="27">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AS16" s="27">
         <v>-2.0</v>
@@ -3659,23 +3691,25 @@
       <c r="AT16" s="27">
         <v>1.0</v>
       </c>
-      <c r="AU16" s="27"/>
-      <c r="AV16" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="AW16" s="28">
+      <c r="AU16" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AV16" s="27"/>
+      <c r="AW16" s="27">
         <v>-4.0</v>
       </c>
-      <c r="AX16" s="27"/>
+      <c r="AX16" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AY16" s="19"/>
       <c r="AZ16" s="19"/>
       <c r="BA16" s="19">
         <v>12.0</v>
       </c>
-      <c r="BB16" s="19"/>
+      <c r="BB16" s="5"/>
       <c r="BC16" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="2"/>
@@ -3683,23 +3717,23 @@
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BF16" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BG16" s="5">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BH16" s="5">
         <f t="shared" si="6"/>
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="BI16" s="20">
         <f t="shared" si="7"/>
-        <v>0.4712643678</v>
+        <v>0.4375</v>
       </c>
       <c r="BJ16" s="20"/>
     </row>
@@ -3817,7 +3851,7 @@
       <c r="BA17" s="19">
         <v>13.0</v>
       </c>
-      <c r="BB17" s="19"/>
+      <c r="BB17" s="5"/>
       <c r="BC17" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -3962,7 +3996,7 @@
       <c r="BA18" s="19">
         <v>14.0</v>
       </c>
-      <c r="BB18" s="19"/>
+      <c r="BB18" s="5"/>
       <c r="BC18" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -4117,7 +4151,7 @@
       <c r="BA19" s="19">
         <v>15.0</v>
       </c>
-      <c r="BB19" s="19"/>
+      <c r="BB19" s="5"/>
       <c r="BC19" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -4264,7 +4298,7 @@
       <c r="BA20" s="19">
         <v>16.0</v>
       </c>
-      <c r="BB20" s="19"/>
+      <c r="BB20" s="5"/>
       <c r="BC20" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -4401,7 +4435,7 @@
       <c r="BA21" s="19">
         <v>17.0</v>
       </c>
-      <c r="BB21" s="19"/>
+      <c r="BB21" s="5"/>
       <c r="BC21" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4538,7 +4572,7 @@
       <c r="BA22" s="19">
         <v>18.0</v>
       </c>
-      <c r="BB22" s="19"/>
+      <c r="BB22" s="5"/>
       <c r="BC22" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4667,16 +4701,18 @@
         <v>4.0</v>
       </c>
       <c r="AW23" s="27"/>
-      <c r="AX23" s="27"/>
+      <c r="AX23" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AY23" s="19"/>
       <c r="AZ23" s="19"/>
       <c r="BA23" s="19">
         <v>19.0</v>
       </c>
-      <c r="BB23" s="19"/>
+      <c r="BB23" s="5"/>
       <c r="BC23" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="2"/>
@@ -4688,7 +4724,7 @@
       </c>
       <c r="BF23" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BG23" s="5">
         <f t="shared" si="5"/>
@@ -4696,11 +4732,11 @@
       </c>
       <c r="BH23" s="5">
         <f t="shared" si="6"/>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="BI23" s="20">
         <f t="shared" si="7"/>
-        <v>0.4782608696</v>
+        <v>0.4583333333</v>
       </c>
       <c r="BJ23" s="20"/>
     </row>
@@ -4790,7 +4826,7 @@
       <c r="BA24" s="19">
         <v>20.0</v>
       </c>
-      <c r="BB24" s="19"/>
+      <c r="BB24" s="5"/>
       <c r="BC24" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4897,16 +4933,18 @@
         <v>-4.0</v>
       </c>
       <c r="AW25" s="27"/>
-      <c r="AX25" s="27"/>
+      <c r="AX25" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AY25" s="19"/>
       <c r="AZ25" s="19"/>
       <c r="BA25" s="19">
         <v>21.0</v>
       </c>
-      <c r="BB25" s="19"/>
+      <c r="BB25" s="5"/>
       <c r="BC25" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="2"/>
@@ -4918,7 +4956,7 @@
       </c>
       <c r="BF25" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG25" s="5">
         <f t="shared" si="5"/>
@@ -4926,11 +4964,11 @@
       </c>
       <c r="BH25" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BI25" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4615384615</v>
       </c>
       <c r="BJ25" s="20"/>
     </row>
@@ -5010,7 +5048,7 @@
       <c r="BA26" s="19">
         <v>22.0</v>
       </c>
-      <c r="BB26" s="19"/>
+      <c r="BB26" s="5"/>
       <c r="BC26" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -5123,7 +5161,7 @@
       <c r="BA27" s="19">
         <v>23.0</v>
       </c>
-      <c r="BB27" s="19"/>
+      <c r="BB27" s="5"/>
       <c r="BC27" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5228,7 +5266,7 @@
       <c r="BA28" s="19">
         <v>24.0</v>
       </c>
-      <c r="BB28" s="19"/>
+      <c r="BB28" s="5"/>
       <c r="BC28" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -5337,7 +5375,7 @@
       <c r="BA29" s="19">
         <v>25.0</v>
       </c>
-      <c r="BB29" s="19"/>
+      <c r="BB29" s="5"/>
       <c r="BC29" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -5446,7 +5484,7 @@
       <c r="BA30" s="19">
         <v>26.0</v>
       </c>
-      <c r="BB30" s="19"/>
+      <c r="BB30" s="5"/>
       <c r="BC30" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -5543,7 +5581,7 @@
       <c r="BA31" s="19">
         <v>27.0</v>
       </c>
-      <c r="BB31" s="19"/>
+      <c r="BB31" s="5"/>
       <c r="BC31" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -5656,7 +5694,7 @@
       <c r="BA32" s="19">
         <v>28.0</v>
       </c>
-      <c r="BB32" s="19"/>
+      <c r="BB32" s="5"/>
       <c r="BC32" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -5753,7 +5791,7 @@
       <c r="BA33" s="19">
         <v>29.0</v>
       </c>
-      <c r="BB33" s="19"/>
+      <c r="BB33" s="5"/>
       <c r="BC33" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -5852,7 +5890,7 @@
       <c r="BA34" s="19">
         <v>30.0</v>
       </c>
-      <c r="BB34" s="19"/>
+      <c r="BB34" s="5"/>
       <c r="BC34" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -5947,7 +5985,7 @@
       <c r="BA35" s="19">
         <v>31.0</v>
       </c>
-      <c r="BB35" s="19"/>
+      <c r="BB35" s="5"/>
       <c r="BC35" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -6048,7 +6086,7 @@
       <c r="BA36" s="19">
         <v>32.0</v>
       </c>
-      <c r="BB36" s="19"/>
+      <c r="BB36" s="5"/>
       <c r="BC36" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6141,7 +6179,7 @@
       <c r="BA37" s="19">
         <v>33.0</v>
       </c>
-      <c r="BB37" s="19"/>
+      <c r="BB37" s="5"/>
       <c r="BC37" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -6232,7 +6270,7 @@
       <c r="BA38" s="19">
         <v>34.0</v>
       </c>
-      <c r="BB38" s="19"/>
+      <c r="BB38" s="5"/>
       <c r="BC38" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -6323,7 +6361,7 @@
       <c r="BA39" s="19">
         <v>35.0</v>
       </c>
-      <c r="BB39" s="19"/>
+      <c r="BB39" s="5"/>
       <c r="BC39" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -6359,7 +6397,7 @@
         <v>94</v>
       </c>
       <c r="B40" s="32">
-        <f t="shared" ref="B40:AW40" si="8">COUNT(B5:B39)</f>
+        <f t="shared" ref="B40:AX40" si="8">COUNT(B5:B39)</f>
         <v>16</v>
       </c>
       <c r="C40" s="32">
@@ -6550,7 +6588,11 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="AX40" s="32"/>
+      <c r="AX40" s="32">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
       <c r="BD40" s="5"/>
       <c r="BE40" s="5"/>
@@ -6700,7 +6742,10 @@
       <c r="AW41" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AX41" s="5"/>
+      <c r="AX41" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB41" s="5"/>
       <c r="BC41" s="5"/>
       <c r="BD41" s="5"/>
       <c r="BE41" s="5"/>
@@ -6761,6 +6806,7 @@
       <c r="AV42" s="5"/>
       <c r="AW42" s="5"/>
       <c r="AX42" s="5"/>
+      <c r="BB42" s="5"/>
       <c r="BC42" s="5"/>
       <c r="BD42" s="5"/>
       <c r="BE42" s="5"/>
@@ -6805,6 +6851,7 @@
       <c r="AV43" s="5"/>
       <c r="AW43" s="5"/>
       <c r="AX43" s="5"/>
+      <c r="BB43" s="5"/>
       <c r="BC43" s="5"/>
       <c r="BD43" s="5"/>
       <c r="BE43" s="5"/>
@@ -6842,6 +6889,7 @@
       <c r="AV44" s="6"/>
       <c r="AW44" s="6"/>
       <c r="AX44" s="6"/>
+      <c r="BB44" s="5"/>
       <c r="BC44" s="5"/>
       <c r="BD44" s="5"/>
       <c r="BE44" s="5"/>
@@ -27180,7 +27228,7 @@
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="44">
         <v>4.0</v>
@@ -27242,7 +27290,7 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="44">
         <v>3.0</v>
@@ -27298,10 +27346,10 @@
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B9" s="44">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" s="44">
         <v>2.0</v>
@@ -27310,10 +27358,10 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="44">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F9" s="44">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="G9" s="44">
         <f t="shared" si="1"/>
@@ -27323,10 +27371,10 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B10" s="44">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C10" s="44">
         <v>2.0</v>
@@ -27335,7 +27383,7 @@
         <v>1.0</v>
       </c>
       <c r="E10" s="44">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="F10" s="44">
         <v>3.0</v>
@@ -27349,32 +27397,32 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B11" s="44">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C11" s="44">
         <v>2.0</v>
       </c>
       <c r="D11" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E11" s="44">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F11" s="44">
-        <v>10.0</v>
+        <v>-8.0</v>
       </c>
       <c r="G11" s="44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J11" s="46"/>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B12" s="44">
         <v>3.0</v>
@@ -27389,7 +27437,7 @@
         <v>1.0</v>
       </c>
       <c r="F12" s="44">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="G12" s="44">
         <f t="shared" si="1"/>
@@ -27405,10 +27453,10 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B13" s="44">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C13" s="44">
         <v>2.0</v>
@@ -27417,10 +27465,10 @@
         <v>0.0</v>
       </c>
       <c r="E13" s="44">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F13" s="44">
-        <v>-5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="1"/>
@@ -27432,31 +27480,31 @@
       </c>
       <c r="J13" s="46">
         <f t="shared" si="3"/>
-        <v>1.25</v>
+        <v>1.666666667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" s="44">
         <v>4.0</v>
       </c>
       <c r="C14" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D14" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="44">
         <v>2.0</v>
       </c>
-      <c r="E14" s="44">
-        <v>1.0</v>
-      </c>
       <c r="F14" s="44">
-        <v>1.0</v>
+        <v>-5.0</v>
       </c>
       <c r="G14" s="44">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I14" s="44">
         <v>19.0</v>
@@ -27468,7 +27516,7 @@
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B15" s="44">
         <v>4.0</v>
@@ -27483,7 +27531,7 @@
         <v>1.0</v>
       </c>
       <c r="F15" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" s="44">
         <f t="shared" si="1"/>
@@ -27499,41 +27547,41 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B16" s="44">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C16" s="44">
         <v>1.0</v>
       </c>
       <c r="D16" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E16" s="44">
         <v>1.0</v>
       </c>
       <c r="F16" s="44">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="G16" s="44">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I16" s="44">
         <v>23.0</v>
       </c>
       <c r="J16" s="46">
         <f t="shared" si="3"/>
-        <v>7.666666667</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B17" s="44">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C17" s="44">
         <v>1.0</v>
@@ -27542,10 +27590,10 @@
         <v>1.0</v>
       </c>
       <c r="E17" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="44">
         <v>3.0</v>
-      </c>
-      <c r="F17" s="44">
-        <v>-9.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
@@ -27556,7 +27604,7 @@
       </c>
       <c r="J17" s="46">
         <f t="shared" si="3"/>
-        <v>3.8</v>
+        <v>6.333333333</v>
       </c>
     </row>
     <row r="18">
@@ -27623,7 +27671,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="44">
         <v>4.0</v>
@@ -27716,7 +27764,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="44">
         <v>4.0</v>
@@ -27809,7 +27857,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="44">
         <v>3.0</v>
@@ -29203,7 +29251,7 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -29283,15 +29331,17 @@
       <c r="AW3" s="27">
         <v>1.0</v>
       </c>
-      <c r="AX3" s="27"/>
+      <c r="AX3" s="27">
+        <v>4.0</v>
+      </c>
       <c r="AY3" s="27"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6">
         <f t="shared" ref="BA3:BA35" si="1">SUM(B3:AY3)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BB3" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="BC3" s="5"/>
     </row>
@@ -29377,12 +29427,14 @@
       </c>
       <c r="AV4" s="27"/>
       <c r="AW4" s="27"/>
-      <c r="AX4" s="27"/>
+      <c r="AX4" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AY4" s="27"/>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BB4" s="5">
         <v>3.0</v>
@@ -29393,7 +29445,7 @@
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
@@ -29485,7 +29537,7 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="27">
         <v>1.0</v>
@@ -29551,12 +29603,14 @@
       <c r="AW6" s="27">
         <v>3.0</v>
       </c>
-      <c r="AX6" s="27"/>
+      <c r="AX6" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="6"/>
       <c r="BA6" s="6">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BB6" s="5">
         <v>2.0</v>
@@ -29567,7 +29621,7 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="27">
         <v>1.0</v>
@@ -29649,12 +29703,14 @@
         <v>1.0</v>
       </c>
       <c r="AW7" s="27"/>
-      <c r="AX7" s="27"/>
+      <c r="AX7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY7" s="27"/>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BB7" s="5"/>
       <c r="BC7" s="5">
@@ -29663,7 +29719,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="27">
         <v>2.0</v>
@@ -30332,7 +30388,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -30653,7 +30709,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -31653,7 +31709,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
@@ -31703,19 +31759,21 @@
       <c r="AU34" s="27"/>
       <c r="AV34" s="27"/>
       <c r="AW34" s="27"/>
-      <c r="AX34" s="27"/>
+      <c r="AX34" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY34" s="27"/>
       <c r="AZ34" s="6"/>
       <c r="BA34" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB34" s="5"/>
       <c r="BC34" s="5"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -31765,12 +31823,14 @@
       <c r="AU35" s="27"/>
       <c r="AV35" s="27"/>
       <c r="AW35" s="27"/>
-      <c r="AX35" s="27"/>
+      <c r="AX35" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY35" s="27"/>
       <c r="AZ35" s="6"/>
       <c r="BA35" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB35" s="5"/>
       <c r="BC35" s="5"/>
@@ -32098,7 +32158,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B40" s="44">
         <f t="shared" ref="B40:AV40" si="2">SUM(B3:B36)</f>
@@ -63048,7 +63108,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="2"/>
@@ -63216,7 +63276,7 @@
         <v>127</v>
       </c>
       <c r="BA3" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4">
@@ -63275,7 +63335,7 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16">
@@ -63365,16 +63425,18 @@
         <v>3.0</v>
       </c>
       <c r="AW5" s="16"/>
-      <c r="AX5" s="16"/>
+      <c r="AX5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AY5" s="16"/>
       <c r="BA5" s="44">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" s="55">
         <v>2.0</v>
@@ -63460,11 +63522,13 @@
       <c r="AW6" s="32">
         <v>2.0</v>
       </c>
-      <c r="AX6" s="32"/>
+      <c r="AX6" s="32">
+        <v>2.0</v>
+      </c>
       <c r="AY6" s="32"/>
       <c r="BA6" s="44">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -63557,11 +63621,13 @@
       <c r="AW7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AX7" s="27"/>
+      <c r="AX7" s="27">
+        <v>1.0</v>
+      </c>
       <c r="AY7" s="27"/>
       <c r="BA7" s="44">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -63646,11 +63712,13 @@
       </c>
       <c r="AV8" s="16"/>
       <c r="AW8" s="16"/>
-      <c r="AX8" s="16"/>
+      <c r="AX8" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AY8" s="16"/>
       <c r="BA8" s="44">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -63736,7 +63804,7 @@
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="27">
         <v>2.0</v>
@@ -63806,16 +63874,18 @@
       <c r="AW10" s="27">
         <v>2.0</v>
       </c>
-      <c r="AX10" s="27"/>
+      <c r="AX10" s="27">
+        <v>2.0</v>
+      </c>
       <c r="AY10" s="27"/>
       <c r="BA10" s="44">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
@@ -64237,7 +64307,7 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -64448,7 +64518,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -64840,7 +64910,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -65025,7 +65095,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -65147,7 +65217,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -65269,7 +65339,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -65725,7 +65795,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" ref="B41:AY41" si="2">SUM(B5:B39)</f>
@@ -65921,7 +65991,7 @@
       </c>
       <c r="AX41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AY41" s="5">
         <f t="shared" si="2"/>
@@ -65929,7 +65999,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66916,19 +66986,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -66944,16 +67014,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="5"/>
@@ -66965,16 +67035,16 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="5"/>
@@ -66986,16 +67056,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="5"/>
@@ -67007,16 +67077,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="5"/>
@@ -67028,27 +67098,27 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I7" s="5"/>
       <c r="K7" s="44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -67057,16 +67127,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="5"/>
@@ -67078,26 +67148,26 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
       <c r="G9" s="49"/>
       <c r="H9" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I9" s="5">
         <v>7.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L9" s="5">
         <v>4.0</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N9" s="5">
         <v>9.0</v>
@@ -67108,32 +67178,32 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I10" s="5">
         <v>7.0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L10" s="5">
         <v>3.0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N10" s="5">
         <v>8.0</v>
@@ -67144,32 +67214,32 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I11" s="5">
         <v>7.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L11" s="5">
         <v>3.0</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N11" s="5">
         <v>7.0</v>
@@ -67180,32 +67250,32 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I12" s="5">
         <v>6.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="L12" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N12" s="5">
         <v>7.0</v>
@@ -67216,33 +67286,33 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
       <c r="H13" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I13" s="5">
         <v>4.0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="L13" s="5">
         <v>2.0</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N13" s="5">
         <v>6.0</v>
@@ -67253,32 +67323,32 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I14" s="5">
         <v>4.0</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="L14" s="5">
         <v>2.0</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N14" s="5">
         <v>6.0</v>
@@ -67295,10 +67365,10 @@
         <v>184</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="5" t="s">
@@ -67308,16 +67378,16 @@
         <v>4.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="L15" s="5">
         <v>2.0</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="N15" s="5">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="16">
@@ -67325,32 +67395,32 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I16" s="5">
         <v>3.0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="L16" s="5">
         <v>2.0</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="N16" s="5">
         <v>5.0</v>
@@ -67367,26 +67437,26 @@
         <v>191</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I17" s="5">
         <v>3.0</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="L17" s="5">
         <v>2.0</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N17" s="5">
         <v>5.0</v>
@@ -67397,26 +67467,26 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I18" s="5">
         <v>3.0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
@@ -67431,24 +67501,24 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
       <c r="G19" s="49"/>
       <c r="H19" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I19" s="5">
         <v>3.0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N19" s="5">
         <v>4.0</v>
@@ -67459,30 +67529,30 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G20" s="49"/>
       <c r="H20" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I20" s="5">
         <v>3.0</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N20" s="5">
         <v>4.0</v>
@@ -67493,30 +67563,30 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="63" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I21" s="5">
         <v>2.0</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N21" s="5">
         <v>3.0</v>
@@ -67527,26 +67597,26 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E22" s="49"/>
       <c r="G22" s="49"/>
       <c r="H22" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="N22" s="5">
         <v>3.0</v>
@@ -67557,28 +67627,28 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N23" s="5">
         <v>3.0</v>
@@ -67589,28 +67659,28 @@
         <v>22.0</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G24" s="49"/>
       <c r="H24" s="63" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N24" s="5">
         <v>3.0</v>
@@ -67621,28 +67691,28 @@
         <v>23.0</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N25" s="5">
         <v>2.0</v>
@@ -67653,28 +67723,28 @@
         <v>24.0</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N26" s="5">
         <v>2.0</v>
@@ -67685,27 +67755,27 @@
         <v>25.0</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N27" s="5">
         <v>2.0</v>
@@ -67716,21 +67786,21 @@
         <v>26.0</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
       <c r="E28" s="49"/>
       <c r="G28" s="49"/>
       <c r="H28" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N28" s="5">
         <v>2.0</v>
@@ -67741,26 +67811,26 @@
         <v>27.0</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I29" s="5"/>
       <c r="K29" s="5" t="s">
         <v>185</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N29" s="5">
         <v>2.0</v>
@@ -67771,20 +67841,20 @@
         <v>28.0</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="49"/>
       <c r="H30" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N30" s="5">
         <v>2.0</v>
@@ -67795,26 +67865,26 @@
         <v>29.0</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C31" s="49" t="s">
         <v>184</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E31" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I31" s="5"/>
       <c r="K31" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="N31" s="5"/>
     </row>
@@ -67823,24 +67893,24 @@
         <v>30.0</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E32" s="49" t="s">
         <v>185</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I32" s="5"/>
       <c r="K32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="N32" s="5"/>
     </row>
@@ -67849,23 +67919,23 @@
         <v>31.0</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N33" s="5"/>
     </row>
@@ -67874,21 +67944,23 @@
         <v>32.0</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E34" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N34" s="5"/>
     </row>
@@ -67897,21 +67969,23 @@
         <v>33.0</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C35" s="49" t="s">
         <v>191</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E35" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="H35" s="5"/>
+        <v>148</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="I35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N35" s="5"/>
     </row>
@@ -67920,21 +67994,21 @@
         <v>34.0</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E36" s="49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N36" s="5"/>
     </row>
@@ -67943,21 +68017,21 @@
         <v>35.0</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N37" s="5"/>
     </row>
@@ -67966,16 +68040,16 @@
         <v>36.0</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E38" s="49" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -67986,16 +68060,16 @@
         <v>37.0</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -68006,16 +68080,16 @@
         <v>38.0</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E40" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -68026,16 +68100,16 @@
         <v>39.0</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E41" s="49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -68046,16 +68120,16 @@
         <v>40.0</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E42" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -68066,16 +68140,16 @@
         <v>41.0</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E43" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -68086,16 +68160,16 @@
         <v>42.0</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C44" s="49" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E44" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -68109,13 +68183,13 @@
         <v>183</v>
       </c>
       <c r="C45" s="49" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E45" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -68126,16 +68200,16 @@
         <v>44.0</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E46" s="49" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -68146,16 +68220,16 @@
         <v>45.0</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -68166,16 +68240,16 @@
         <v>46.0</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C48" s="49" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48" s="49" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -68186,16 +68260,16 @@
         <v>47.0</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -68206,23 +68280,37 @@
         <v>48.0</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C50" s="49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E50" s="49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="N50" s="5"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="6"/>
+      <c r="A51" s="49">
+        <v>49.0</v>
+      </c>
+      <c r="B51" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="C51" s="49" t="s">
+        <v>242</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" s="49" t="s">
+        <v>228</v>
+      </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="N51" s="5"/>

</xml_diff>

<commit_message>
Week 14 data correction
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="+5CrHHmSKXHoltAV9WQ3iFcB5dL0HKn6G89GI7UABFw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="kI5myAL6QbpvUS+fDkMpbnCSLArKRlzUdWbOn1uoCx8="/>
     </ext>
   </extLst>
 </workbook>
@@ -3828,7 +3828,7 @@
       <c r="J26" s="29"/>
       <c r="K26" s="27"/>
       <c r="L26" s="28">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="M26" s="29">
         <v>1.0</v>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB26" s="5">
         <f t="shared" si="3"/>
@@ -3889,19 +3889,19 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="BF26" s="20">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="BG26" s="20"/>
     </row>

</xml_diff>

<commit_message>
062 Game week 17 update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="7e87VVOEGS+PnThWZgTqzJR+JRuIdF4JHle1tltmElo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="6gNUf0hGLVgnOgh7+iO1a49nYPtIhHgVVQWqCdorvyA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -201,19 +201,19 @@
     <t>%</t>
   </si>
   <si>
-    <t>DOM</t>
+    <t>POSH CHRIS</t>
   </si>
   <si>
-    <t>POSH CHRIS</t>
+    <t>DOM</t>
   </si>
   <si>
     <t>KERMIT</t>
   </si>
   <si>
-    <t>CAPTAIN KIRK</t>
+    <t xml:space="preserve">MAMAS </t>
   </si>
   <si>
-    <t xml:space="preserve">MAMAS </t>
+    <t>CAPTAIN KIRK</t>
   </si>
   <si>
     <t>BRUCE</t>
@@ -225,13 +225,28 @@
     <t>CARLOS</t>
   </si>
   <si>
+    <t>PRESTON</t>
+  </si>
+  <si>
     <t>INSPECTOR GADGET</t>
   </si>
   <si>
     <t>DUNCAN</t>
   </si>
   <si>
-    <t>PRESTON</t>
+    <t>DWARF</t>
+  </si>
+  <si>
+    <t>KRYTON</t>
+  </si>
+  <si>
+    <t>ZIGZAG</t>
+  </si>
+  <si>
+    <t>ARTIST</t>
+  </si>
+  <si>
+    <t>FLO</t>
   </si>
   <si>
     <t>TUNDE</t>
@@ -240,22 +255,7 @@
     <t>TOY BOY</t>
   </si>
   <si>
-    <t>ARTIST</t>
-  </si>
-  <si>
-    <t>DWARF</t>
-  </si>
-  <si>
-    <t>KRYTON</t>
-  </si>
-  <si>
-    <t>FLO</t>
-  </si>
-  <si>
     <t>IAN</t>
-  </si>
-  <si>
-    <t>ZIGZAG</t>
   </si>
   <si>
     <t>FATHER TED</t>
@@ -270,10 +270,10 @@
     <t xml:space="preserve">STRAIGHT ROB </t>
   </si>
   <si>
-    <t>STEPTOE</t>
+    <t>RYAN</t>
   </si>
   <si>
-    <t>DOGGER</t>
+    <t>STEPTOE</t>
   </si>
   <si>
     <t>ELBOW</t>
@@ -282,7 +282,7 @@
     <t>FRED</t>
   </si>
   <si>
-    <t>GAZZA</t>
+    <t>DOGGER</t>
   </si>
   <si>
     <t>MICK</t>
@@ -348,6 +348,9 @@
     <t xml:space="preserve"> 4-3</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2-2</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
@@ -373,6 +376,9 @@
   </si>
   <si>
     <t>BAZ</t>
+  </si>
+  <si>
+    <t>GAZZA</t>
   </si>
   <si>
     <t>STEVE P</t>
@@ -510,6 +516,9 @@
     <t>Carzola</t>
   </si>
   <si>
+    <t>Ian</t>
+  </si>
+  <si>
     <t>Duncan - Dom</t>
   </si>
   <si>
@@ -517,9 +526,6 @@
   </si>
   <si>
     <t>Carlos</t>
-  </si>
-  <si>
-    <t>Father Ted</t>
   </si>
   <si>
     <t>Duncan</t>
@@ -534,13 +540,13 @@
     <t>Flo</t>
   </si>
   <si>
+    <t>Father Ted</t>
+  </si>
+  <si>
     <t>Preston</t>
   </si>
   <si>
     <t>Preston - Gadget</t>
-  </si>
-  <si>
-    <t>Ian</t>
   </si>
   <si>
     <t>Artist - Moo</t>
@@ -561,7 +567,16 @@
     <t>Lost 3-4</t>
   </si>
   <si>
+    <t>Ryan</t>
+  </si>
+  <si>
     <t>Artist</t>
+  </si>
+  <si>
+    <t>Banksy - Father Ted</t>
+  </si>
+  <si>
+    <t>Drew 2-2</t>
   </si>
   <si>
     <t>S Rob</t>
@@ -577,7 +592,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -633,11 +648,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -790,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -924,9 +934,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,24 +1628,22 @@
       <c r="C5" s="16">
         <v>1.0</v>
       </c>
-      <c r="D5" s="16">
-        <v>-3.0</v>
-      </c>
-      <c r="E5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
+        <v>0.0</v>
+      </c>
       <c r="F5" s="16">
         <v>2.0</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="16">
         <v>-3.0</v>
       </c>
-      <c r="H5" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="I5" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="J5" s="17">
-        <v>2.0</v>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16">
+        <v>-2.0</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="16">
@@ -1651,13 +1656,17 @@
         <v>2.0</v>
       </c>
       <c r="O5" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="P5" s="16">
         <v>1.0</v>
       </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
+      <c r="P5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="R5" s="16">
+        <v>0.0</v>
+      </c>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
@@ -1695,7 +1704,7 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
@@ -1703,23 +1712,23 @@
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC40" si="4">COUNTIF($B5:$AX5, "&lt;0")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BF5" s="20">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.75</v>
+        <v>0.7435897436</v>
       </c>
       <c r="BG5" s="20"/>
     </row>
@@ -1731,22 +1740,24 @@
       <c r="C6" s="23">
         <v>1.0</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23">
-        <v>0.0</v>
-      </c>
+      <c r="D6" s="23">
+        <v>-3.0</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="23">
         <v>2.0</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="23">
+        <v>-3.0</v>
+      </c>
+      <c r="H6" s="23">
         <v>3.0</v>
       </c>
-      <c r="H6" s="23">
-        <v>-3.0</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23">
-        <v>-2.0</v>
+      <c r="I6" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="J6" s="24">
+        <v>2.0</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="23">
@@ -1759,13 +1770,17 @@
         <v>2.0</v>
       </c>
       <c r="O6" s="23">
+        <v>-1.0</v>
+      </c>
+      <c r="P6" s="23">
         <v>1.0</v>
       </c>
-      <c r="P6" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+      <c r="Q6" s="23">
+        <v>-2.0</v>
+      </c>
+      <c r="R6" s="23">
+        <v>0.0</v>
+      </c>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
@@ -1803,11 +1818,11 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB6" s="5">
         <f t="shared" si="3"/>
@@ -1815,19 +1830,19 @@
       </c>
       <c r="BC6" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BF6" s="20">
         <f t="shared" si="7"/>
-        <v>0.7575757576</v>
+        <v>0.6666666667</v>
       </c>
       <c r="BG6" s="20"/>
     </row>
@@ -1872,8 +1887,12 @@
         <v>1.0</v>
       </c>
       <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
+      <c r="Q7" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="R7" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S7" s="28"/>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
@@ -1911,15 +1930,15 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB7" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
@@ -1927,11 +1946,11 @@
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BF7" s="20">
         <f t="shared" si="7"/>
@@ -1945,7 +1964,7 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D8" s="16">
         <v>3.0</v>
@@ -1954,9 +1973,11 @@
         <v>0.0</v>
       </c>
       <c r="F8" s="16">
-        <v>-2.0</v>
-      </c>
-      <c r="G8" s="16"/>
+        <v>2.0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>3.0</v>
+      </c>
       <c r="H8" s="16">
         <v>-3.0</v>
       </c>
@@ -1964,24 +1985,28 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="16">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="16">
         <v>3.0</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="16"/>
+      <c r="N8" s="16">
+        <v>-2.0</v>
+      </c>
+      <c r="O8" s="16">
         <v>1.0</v>
       </c>
-      <c r="N8" s="16">
+      <c r="P8" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="Q8" s="16">
         <v>2.0</v>
       </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17">
-        <v>-1.0</v>
-      </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="R8" s="17">
+        <v>0.0</v>
+      </c>
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
@@ -2019,31 +2044,31 @@
       </c>
       <c r="AZ8" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BA8" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB8" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC8" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BF8" s="20">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.619047619</v>
       </c>
       <c r="BG8" s="20"/>
     </row>
@@ -2053,7 +2078,7 @@
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D9" s="34">
         <v>3.0</v>
@@ -2062,11 +2087,9 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="34">
-        <v>2.0</v>
-      </c>
-      <c r="G9" s="34">
-        <v>3.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="G9" s="34"/>
       <c r="H9" s="34">
         <v>-3.0</v>
       </c>
@@ -2074,24 +2097,28 @@
         <v>2.0</v>
       </c>
       <c r="J9" s="34">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K9" s="32"/>
       <c r="L9" s="34">
         <v>3.0</v>
       </c>
-      <c r="M9" s="34"/>
+      <c r="M9" s="34">
+        <v>1.0</v>
+      </c>
       <c r="N9" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="O9" s="34"/>
+      <c r="P9" s="33">
+        <v>-1.0</v>
+      </c>
+      <c r="Q9" s="34">
         <v>-2.0</v>
       </c>
-      <c r="O9" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="P9" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
+      <c r="R9" s="34">
+        <v>0.0</v>
+      </c>
       <c r="S9" s="34"/>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
@@ -2129,7 +2156,7 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
@@ -2137,7 +2164,7 @@
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
@@ -2145,15 +2172,15 @@
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BF9" s="20">
         <f t="shared" si="7"/>
-        <v>0.6111111111</v>
+        <v>0.5897435897</v>
       </c>
       <c r="BG9" s="20"/>
     </row>
@@ -2202,7 +2229,9 @@
       <c r="P10" s="28">
         <v>1.0</v>
       </c>
-      <c r="Q10" s="28"/>
+      <c r="Q10" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="R10" s="34"/>
       <c r="S10" s="34"/>
       <c r="T10" s="34"/>
@@ -2241,7 +2270,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2253,7 +2282,7 @@
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
@@ -2261,11 +2290,11 @@
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF10" s="20">
         <f t="shared" si="7"/>
-        <v>0.5641025641</v>
+        <v>0.5238095238</v>
       </c>
       <c r="BG10" s="20"/>
     </row>
@@ -2311,7 +2340,9 @@
         <v>-1.0</v>
       </c>
       <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
+      <c r="R11" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
       <c r="U11" s="28"/>
@@ -2349,7 +2380,7 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
@@ -2357,7 +2388,7 @@
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
@@ -2365,7 +2396,7 @@
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
@@ -2373,7 +2404,7 @@
       </c>
       <c r="BF11" s="20">
         <f t="shared" si="7"/>
-        <v>0.4848484848</v>
+        <v>0.4722222222</v>
       </c>
       <c r="BG11" s="20"/>
     </row>
@@ -2421,7 +2452,9 @@
         <v>-1.0</v>
       </c>
       <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
+      <c r="R12" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
@@ -2459,7 +2492,7 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
@@ -2467,7 +2500,7 @@
       </c>
       <c r="BB12" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC12" s="5">
         <f t="shared" si="4"/>
@@ -2475,7 +2508,7 @@
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
@@ -2483,7 +2516,7 @@
       </c>
       <c r="BF12" s="20">
         <f t="shared" si="7"/>
-        <v>0.4444444444</v>
+        <v>0.4358974359</v>
       </c>
       <c r="BG12" s="20"/>
     </row>
@@ -2493,41 +2526,51 @@
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D13" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="E13" s="28"/>
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0.0</v>
+      </c>
       <c r="F13" s="28">
         <v>-2.0</v>
       </c>
       <c r="G13" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="H13" s="28"/>
+        <v>-3.0</v>
+      </c>
+      <c r="H13" s="28">
+        <v>-3.0</v>
+      </c>
       <c r="I13" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J13" s="28">
         <v>2.0</v>
       </c>
       <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
+      <c r="L13" s="28">
+        <v>-3.0</v>
+      </c>
       <c r="M13" s="29">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="N13" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="O13" s="28">
         <v>-1.0</v>
       </c>
       <c r="P13" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
+        <v>-1.0</v>
+      </c>
+      <c r="Q13" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="R13" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
@@ -2565,7 +2608,7 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
@@ -2573,23 +2616,23 @@
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="BF13" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.3777777778</v>
       </c>
       <c r="BG13" s="20"/>
     </row>
@@ -2602,32 +2645,26 @@
         <v>-1.0</v>
       </c>
       <c r="D14" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="E14" s="28">
-        <v>0.0</v>
-      </c>
+        <v>-3.0</v>
+      </c>
+      <c r="E14" s="28"/>
       <c r="F14" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G14" s="28">
         <v>3.0</v>
       </c>
-      <c r="H14" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="H14" s="28"/>
       <c r="I14" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J14" s="29">
-        <v>-2.0</v>
+      <c r="J14" s="28">
+        <v>2.0</v>
       </c>
       <c r="K14" s="27"/>
-      <c r="L14" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="M14" s="28">
-        <v>-1.0</v>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29">
+        <v>1.0</v>
       </c>
       <c r="N14" s="28">
         <v>2.0</v>
@@ -2636,10 +2673,14 @@
         <v>-1.0</v>
       </c>
       <c r="P14" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
+        <v>1.0</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="R14" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S14" s="28"/>
       <c r="T14" s="28"/>
       <c r="U14" s="28"/>
@@ -2677,11 +2718,11 @@
       </c>
       <c r="AZ14" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
@@ -2689,19 +2730,19 @@
       </c>
       <c r="BC14" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="BF14" s="20">
         <f t="shared" si="7"/>
-        <v>0.3333333333</v>
+        <v>0.4444444444</v>
       </c>
       <c r="BG14" s="20"/>
     </row>
@@ -2711,38 +2752,38 @@
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="D15" s="29">
+        <v>-1.0</v>
+      </c>
+      <c r="D15" s="28">
         <v>3.0</v>
       </c>
       <c r="E15" s="28">
         <v>0.0</v>
       </c>
       <c r="F15" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G15" s="28">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="H15" s="28">
         <v>-3.0</v>
       </c>
       <c r="I15" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="J15" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
+      </c>
+      <c r="J15" s="29">
+        <v>-2.0</v>
       </c>
       <c r="K15" s="27"/>
       <c r="L15" s="28">
         <v>-3.0</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="28">
         <v>-1.0</v>
       </c>
       <c r="N15" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O15" s="28">
         <v>-1.0</v>
@@ -2750,7 +2791,9 @@
       <c r="P15" s="28">
         <v>-1.0</v>
       </c>
-      <c r="Q15" s="28"/>
+      <c r="Q15" s="28">
+        <v>2.0</v>
+      </c>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
       <c r="T15" s="28"/>
@@ -2789,11 +2832,11 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
@@ -2805,15 +2848,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="BF15" s="20">
         <f t="shared" si="7"/>
-        <v>0.3333333333</v>
+        <v>0.380952381</v>
       </c>
       <c r="BG15" s="20"/>
     </row>
@@ -2823,28 +2866,42 @@
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="28">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D16" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="28">
+      <c r="H16" s="29">
         <v>3.0</v>
       </c>
       <c r="I16" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="J16" s="28">
         <v>2.0</v>
       </c>
-      <c r="J16" s="28"/>
       <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
+      <c r="L16" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="M16" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="N16" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="O16" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="P16" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>2.0</v>
+      </c>
       <c r="R16" s="28"/>
       <c r="S16" s="28"/>
       <c r="T16" s="28"/>
@@ -2883,11 +2940,11 @@
       </c>
       <c r="AZ16" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="BA16" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
@@ -2895,19 +2952,19 @@
       </c>
       <c r="BC16" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="BF16" s="20">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.4545454545</v>
       </c>
       <c r="BG16" s="20"/>
     </row>
@@ -2916,32 +2973,42 @@
         <v>71</v>
       </c>
       <c r="B17" s="27"/>
-      <c r="C17" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="28"/>
       <c r="G17" s="28">
         <v>3.0</v>
       </c>
       <c r="H17" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I17" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="L17" s="29">
+        <v>-3.0</v>
+      </c>
+      <c r="M17" s="28">
+        <v>-1.0</v>
+      </c>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
+      <c r="P17" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="R17" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S17" s="28"/>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
@@ -2979,7 +3046,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -2987,23 +3054,23 @@
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BF17" s="20">
         <f t="shared" si="7"/>
-        <v>0.8</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BG17" s="20"/>
     </row>
@@ -3012,38 +3079,48 @@
         <v>72</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="C18" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="D18" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="G18" s="28"/>
+        <v>-2.0</v>
+      </c>
+      <c r="G18" s="28">
+        <v>-3.0</v>
+      </c>
       <c r="H18" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I18" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="J18" s="28">
         <v>-2.0</v>
       </c>
+      <c r="J18" s="28"/>
       <c r="K18" s="27"/>
       <c r="L18" s="28">
         <v>-3.0</v>
       </c>
-      <c r="M18" s="28"/>
-      <c r="N18" s="29">
-        <v>-2.0</v>
-      </c>
+      <c r="M18" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="N18" s="28"/>
       <c r="O18" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="P18" s="28">
         <v>-1.0</v>
       </c>
-      <c r="P18" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
+      <c r="Q18" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="R18" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
       <c r="U18" s="28"/>
@@ -3081,7 +3158,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3089,23 +3166,23 @@
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="BF18" s="20">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.358974359</v>
       </c>
       <c r="BG18" s="20"/>
     </row>
@@ -3114,42 +3191,42 @@
         <v>73</v>
       </c>
       <c r="B19" s="27"/>
-      <c r="C19" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D19" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="F19" s="28">
+        <v>2.0</v>
+      </c>
       <c r="G19" s="28"/>
-      <c r="H19" s="29">
+      <c r="H19" s="28">
         <v>3.0</v>
       </c>
       <c r="I19" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="J19" s="28">
         <v>-2.0</v>
-      </c>
-      <c r="J19" s="28">
-        <v>2.0</v>
       </c>
       <c r="K19" s="27"/>
       <c r="L19" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="M19" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="M19" s="28"/>
+      <c r="N19" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O19" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N19" s="28">
+      <c r="P19" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q19" s="28">
         <v>-2.0</v>
       </c>
-      <c r="O19" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P19" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
+      <c r="R19" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S19" s="28"/>
       <c r="T19" s="28"/>
       <c r="U19" s="28"/>
@@ -3195,23 +3272,23 @@
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="BF19" s="20">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.4333333333</v>
       </c>
       <c r="BG19" s="20"/>
     </row>
@@ -3220,9 +3297,11 @@
         <v>74</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
+      <c r="C20" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D20" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="E20" s="28">
         <v>0.0</v>
@@ -3234,12 +3313,14 @@
       <c r="H20" s="28">
         <v>-3.0</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="J20" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J20" s="28"/>
       <c r="K20" s="27"/>
-      <c r="L20" s="29">
+      <c r="L20" s="28">
         <v>-3.0</v>
       </c>
       <c r="M20" s="28">
@@ -3247,10 +3328,10 @@
       </c>
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
-      <c r="P20" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="29">
+        <v>2.0</v>
+      </c>
       <c r="R20" s="28"/>
       <c r="S20" s="28"/>
       <c r="T20" s="28"/>
@@ -3289,11 +3370,11 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
@@ -3301,19 +3382,19 @@
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="BF20" s="20">
         <f t="shared" si="7"/>
-        <v>0.4166666667</v>
+        <v>0.4333333333</v>
       </c>
       <c r="BG20" s="20"/>
     </row>
@@ -3326,31 +3407,21 @@
         <v>1.0</v>
       </c>
       <c r="D21" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="E21" s="28">
-        <v>0.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="E21" s="28"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="28">
+      <c r="G21" s="28"/>
+      <c r="H21" s="28">
         <v>3.0</v>
       </c>
-      <c r="H21" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="I21" s="29">
+      <c r="I21" s="28">
         <v>2.0</v>
       </c>
-      <c r="J21" s="28">
-        <v>-2.0</v>
-      </c>
+      <c r="J21" s="28"/>
       <c r="K21" s="27"/>
-      <c r="L21" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="M21" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="28"/>
       <c r="O21" s="28"/>
       <c r="P21" s="28"/>
@@ -3393,31 +3464,31 @@
       </c>
       <c r="AZ21" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BA21" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BB21" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC21" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BD21" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BE21" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>9</v>
       </c>
       <c r="BF21" s="20">
         <f t="shared" si="7"/>
-        <v>0.3703703704</v>
+        <v>1</v>
       </c>
       <c r="BG21" s="20"/>
     </row>
@@ -3429,38 +3500,26 @@
       <c r="C22" s="28">
         <v>-1.0</v>
       </c>
-      <c r="D22" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="E22" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G22" s="28">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="H22" s="28">
         <v>3.0</v>
       </c>
-      <c r="I22" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="J22" s="28">
+      <c r="I22" s="28">
         <v>2.0</v>
       </c>
+      <c r="J22" s="28"/>
       <c r="K22" s="27"/>
       <c r="L22" s="28"/>
-      <c r="M22" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="N22" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="O22" s="28">
-        <v>-1.0</v>
-      </c>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="28"/>
@@ -3501,31 +3560,31 @@
       </c>
       <c r="AZ22" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="BA22" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BB22" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC22" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BD22" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="BE22" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>9</v>
       </c>
       <c r="BF22" s="20">
         <f t="shared" si="7"/>
-        <v>0.303030303</v>
+        <v>0.8</v>
       </c>
       <c r="BG22" s="20"/>
     </row>
@@ -3538,9 +3597,9 @@
         <v>-1.0</v>
       </c>
       <c r="D23" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="E23" s="29">
+        <v>-3.0</v>
+      </c>
+      <c r="E23" s="28">
         <v>0.0</v>
       </c>
       <c r="F23" s="28">
@@ -3550,28 +3609,32 @@
         <v>-3.0</v>
       </c>
       <c r="H23" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="I23" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="I23" s="29">
         <v>-2.0</v>
       </c>
-      <c r="J23" s="28"/>
+      <c r="J23" s="28">
+        <v>2.0</v>
+      </c>
       <c r="K23" s="27"/>
-      <c r="L23" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="L23" s="28"/>
       <c r="M23" s="28">
         <v>1.0</v>
       </c>
-      <c r="N23" s="28"/>
+      <c r="N23" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="O23" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P23" s="28">
         <v>-1.0</v>
       </c>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="R23" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S23" s="28"/>
       <c r="T23" s="28"/>
       <c r="U23" s="28"/>
@@ -3609,7 +3672,7 @@
       </c>
       <c r="AZ23" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BA23" s="5">
         <f t="shared" si="2"/>
@@ -3617,15 +3680,15 @@
       </c>
       <c r="BB23" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC23" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BE23" s="5">
         <f t="shared" si="6"/>
@@ -3633,7 +3696,7 @@
       </c>
       <c r="BF23" s="20">
         <f t="shared" si="7"/>
-        <v>0.303030303</v>
+        <v>0.2820512821</v>
       </c>
       <c r="BG23" s="20"/>
     </row>
@@ -3678,8 +3741,12 @@
         <v>1.0</v>
       </c>
       <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
+      <c r="Q24" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="R24" s="29">
+        <v>0.0</v>
+      </c>
       <c r="S24" s="28"/>
       <c r="T24" s="28"/>
       <c r="U24" s="28"/>
@@ -3717,7 +3784,7 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
@@ -3725,23 +3792,23 @@
       </c>
       <c r="BB24" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="BF24" s="20">
         <f t="shared" si="7"/>
-        <v>0.303030303</v>
+        <v>0.2820512821</v>
       </c>
       <c r="BG24" s="20"/>
     </row>
@@ -3777,7 +3844,9 @@
       </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
+      <c r="R25" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S25" s="28"/>
       <c r="T25" s="28"/>
       <c r="U25" s="28"/>
@@ -3815,7 +3884,7 @@
       </c>
       <c r="AZ25" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
@@ -3823,7 +3892,7 @@
       </c>
       <c r="BB25" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
@@ -3831,7 +3900,7 @@
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
@@ -3839,7 +3908,7 @@
       </c>
       <c r="BF25" s="20">
         <f t="shared" si="7"/>
-        <v>0.3888888889</v>
+        <v>0.380952381</v>
       </c>
       <c r="BG25" s="20"/>
     </row>
@@ -3866,7 +3935,9 @@
       <c r="P26" s="28">
         <v>1.0</v>
       </c>
-      <c r="Q26" s="28"/>
+      <c r="Q26" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="R26" s="28"/>
       <c r="S26" s="28"/>
       <c r="T26" s="28"/>
@@ -3905,7 +3976,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -3917,7 +3988,7 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
@@ -3925,11 +3996,11 @@
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF26" s="20">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.6666666667</v>
       </c>
       <c r="BG26" s="20"/>
     </row>
@@ -4035,9 +4106,7 @@
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
-      <c r="D28" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -4048,10 +4117,16 @@
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
+      <c r="O28" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
+      <c r="Q28" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="R28" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S28" s="28"/>
       <c r="T28" s="28"/>
       <c r="U28" s="28"/>
@@ -4089,7 +4164,7 @@
       </c>
       <c r="AZ28" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BA28" s="5">
         <f t="shared" si="2"/>
@@ -4097,23 +4172,23 @@
       </c>
       <c r="BB28" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC28" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD28" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BE28" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="BF28" s="20">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.4444444444</v>
       </c>
       <c r="BG28" s="20"/>
     </row>
@@ -4123,14 +4198,14 @@
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="D29" s="28">
+        <v>3.0</v>
+      </c>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
-      <c r="I29" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="I29" s="28"/>
       <c r="J29" s="28"/>
       <c r="K29" s="27"/>
       <c r="L29" s="28"/>
@@ -4197,7 +4272,7 @@
       </c>
       <c r="BE29" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BF29" s="20">
         <f t="shared" si="7"/>
@@ -4388,7 +4463,9 @@
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
+      <c r="I32" s="28">
+        <v>2.0</v>
+      </c>
       <c r="J32" s="28"/>
       <c r="K32" s="27"/>
       <c r="L32" s="28"/>
@@ -4435,11 +4512,11 @@
       </c>
       <c r="AZ32" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA32" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB32" s="5">
         <f t="shared" si="3"/>
@@ -4451,15 +4528,15 @@
       </c>
       <c r="BD32" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE32" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BF32" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="BF32" s="20">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="BG32" s="20"/>
     </row>
@@ -5235,7 +5312,7 @@
       </c>
       <c r="O41" s="34">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P41" s="34">
         <f t="shared" si="8"/>
@@ -5243,11 +5320,11 @@
       </c>
       <c r="Q41" s="34">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R41" s="34">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S41" s="34">
         <f t="shared" si="8"/>
@@ -5428,8 +5505,12 @@
       <c r="P42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
+      <c r="Q42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="S42" s="40"/>
       <c r="T42" s="40"/>
       <c r="U42" s="40"/>
@@ -25832,33 +25913,33 @@
         <v>1</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>56</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="45">
         <v>2.0</v>
@@ -25882,13 +25963,13 @@
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B4" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" s="44">
         <v>0.0</v>
@@ -25897,18 +25978,18 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="44">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G4" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I4" s="44">
         <v>18.0</v>
       </c>
       <c r="J4" s="46">
         <f t="shared" ref="J4:J8" si="2">I4/B4</f>
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -25916,13 +25997,13 @@
         <v>79</v>
       </c>
       <c r="B5" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C5" s="44">
         <v>1.0</v>
       </c>
       <c r="D5" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E5" s="44">
         <v>0.0</v>
@@ -25932,19 +26013,19 @@
       </c>
       <c r="G5" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="44">
         <v>24.0</v>
       </c>
       <c r="J5" s="46">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B6" s="44">
         <v>1.0</v>
@@ -25959,7 +26040,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" s="44">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G6" s="44">
         <f t="shared" si="1"/>
@@ -25975,7 +26056,7 @@
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B7" s="45">
         <v>1.0</v>
@@ -26006,7 +26087,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="44">
         <v>1.0</v>
@@ -26062,7 +26143,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="44">
         <v>2.0</v>
@@ -26087,7 +26168,7 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="44">
         <v>1.0</v>
@@ -26113,7 +26194,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="44">
         <v>2.0</v>
@@ -26201,7 +26282,7 @@
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B15" s="44">
         <v>1.0</v>
@@ -26232,38 +26313,38 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B16" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16" s="44">
         <v>0.0</v>
       </c>
       <c r="D16" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E16" s="44">
         <v>1.0</v>
       </c>
       <c r="F16" s="44">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="G16" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="44">
         <v>12.0</v>
       </c>
       <c r="J16" s="46">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="B17" s="44">
         <v>1.0</v>
@@ -26278,7 +26359,7 @@
         <v>1.0</v>
       </c>
       <c r="F17" s="44">
-        <v>-2.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
@@ -26294,7 +26375,7 @@
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B18" s="44">
         <v>1.0</v>
@@ -26325,7 +26406,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19" s="44">
         <v>1.0</v>
@@ -26356,7 +26437,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B20" s="44">
         <v>1.0</v>
@@ -26387,7 +26468,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B21" s="44">
         <v>1.0</v>
@@ -26418,10 +26499,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B22" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C22" s="44">
         <v>0.0</v>
@@ -26430,10 +26511,10 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F22" s="44">
-        <v>-3.0</v>
+        <v>-4.0</v>
       </c>
       <c r="G22" s="44">
         <f t="shared" si="1"/>
@@ -26444,7 +26525,7 @@
       </c>
       <c r="J22" s="46">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -26528,7 +26609,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G27" s="44">
         <f t="shared" si="1"/>
@@ -26568,7 +26649,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G30" s="44">
         <f t="shared" si="1"/>
@@ -26592,7 +26673,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G32" s="44">
         <f t="shared" si="1"/>
@@ -26604,7 +26685,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="G33" s="44">
         <f t="shared" si="1"/>
@@ -26631,7 +26712,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="36" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G36" s="44">
         <f t="shared" si="1"/>
@@ -27786,17 +27867,17 @@
         <v>50</v>
       </c>
       <c r="AY1" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
@@ -27884,7 +27965,7 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28">
@@ -27962,7 +28043,7 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -28032,7 +28113,7 @@
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="28">
@@ -28108,7 +28189,7 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
@@ -28132,7 +28213,9 @@
         <v>1.0</v>
       </c>
       <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="P6" s="28">
+        <v>1.0</v>
+      </c>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
@@ -28171,7 +28254,7 @@
       <c r="AZ6" s="6"/>
       <c r="BA6" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB6" s="5"/>
       <c r="BC6" s="5">
@@ -28180,29 +28263,29 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="28"/>
+        <v>116</v>
+      </c>
+      <c r="B7" s="27"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
-      <c r="G7" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
+      <c r="I7" s="28">
+        <v>1.0</v>
+      </c>
       <c r="J7" s="28"/>
       <c r="K7" s="27"/>
-      <c r="L7" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="L7" s="28"/>
       <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P7" s="28"/>
+      <c r="N7" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28">
+        <v>2.0</v>
+      </c>
       <c r="Q7" s="28"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28"/>
@@ -28241,38 +28324,36 @@
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="BB7" s="5">
+        <v>7</v>
+      </c>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28">
-        <v>1.0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="G8" s="28">
+        <v>2.0</v>
+      </c>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="J8" s="28"/>
       <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
+      <c r="L8" s="28">
+        <v>3.0</v>
+      </c>
       <c r="M8" s="28"/>
-      <c r="N8" s="28">
+      <c r="N8" s="28"/>
+      <c r="O8" s="28">
         <v>1.0</v>
-      </c>
-      <c r="O8" s="28">
-        <v>2.0</v>
       </c>
       <c r="P8" s="28"/>
       <c r="Q8" s="28"/>
@@ -28322,31 +28403,29 @@
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
+      <c r="C9" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D9" s="28"/>
-      <c r="E9" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="H9" s="28"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K9" s="27"/>
       <c r="L9" s="28"/>
-      <c r="M9" s="28">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="O9" s="28">
         <v>2.0</v>
-      </c>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28">
-        <v>1.0</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -28389,41 +28468,43 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="BB9" s="5"/>
-      <c r="BC9" s="5">
+      <c r="BB9" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="C10" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="28"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="28">
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28">
         <v>1.0</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
+      <c r="J10" s="28">
+        <v>1.0</v>
+      </c>
       <c r="K10" s="27"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
-      <c r="N10" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="N10" s="28"/>
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
+      <c r="Q10" s="28">
+        <v>3.0</v>
+      </c>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
-      <c r="U10" s="50"/>
+      <c r="U10" s="28"/>
       <c r="V10" s="28"/>
       <c r="W10" s="28"/>
       <c r="X10" s="28"/>
@@ -28457,37 +28538,41 @@
       <c r="AZ10" s="6"/>
       <c r="BA10" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="BB10" s="5"/>
-      <c r="BC10" s="5">
+        <v>6</v>
+      </c>
+      <c r="BB10" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+      <c r="E11" s="28">
+        <v>1.0</v>
+      </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="H11" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="J11" s="28">
+        <v>1.0</v>
+      </c>
       <c r="K11" s="27"/>
-      <c r="L11" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="L11" s="28"/>
       <c r="M11" s="28">
         <v>2.0</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="28"/>
+      <c r="O11" s="28">
         <v>1.0</v>
       </c>
-      <c r="O11" s="28"/>
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
@@ -28527,7 +28612,7 @@
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB11" s="5"/>
       <c r="BC11" s="5">
@@ -28536,24 +28621,26 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="D12" s="28">
+        <v>3.0</v>
+      </c>
       <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
+      <c r="F12" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
-      <c r="I12" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="27"/>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
       <c r="N12" s="28">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
@@ -28561,7 +28648,7 @@
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
+      <c r="U12" s="50"/>
       <c r="V12" s="28"/>
       <c r="W12" s="28"/>
       <c r="X12" s="28"/>
@@ -28598,30 +28685,34 @@
         <v>5</v>
       </c>
       <c r="BB12" s="5"/>
-      <c r="BC12" s="5"/>
+      <c r="BC12" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BF12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
-      <c r="E13" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="L13" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="M13" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N13" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="28"/>
@@ -28662,31 +28753,29 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="BB13" s="5">
-        <v>1.0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BB13" s="5"/>
       <c r="BC13" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="E14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28">
+        <v>2.0</v>
+      </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="H14" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="27"/>
       <c r="L14" s="28"/>
@@ -28698,7 +28787,7 @@
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
       <c r="T14" s="28"/>
-      <c r="U14" s="50"/>
+      <c r="U14" s="28"/>
       <c r="V14" s="28"/>
       <c r="W14" s="28"/>
       <c r="X14" s="28"/>
@@ -28734,27 +28823,25 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="BB14" s="5"/>
+      <c r="BB14" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC14" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="F15" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -28762,10 +28849,10 @@
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
-      <c r="O15" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28">
+        <v>2.0</v>
+      </c>
       <c r="Q15" s="28"/>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
@@ -28807,27 +28894,27 @@
         <v>4</v>
       </c>
       <c r="BB15" s="5"/>
-      <c r="BC15" s="5"/>
+      <c r="BC15" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B16" s="27"/>
-      <c r="C16" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="D16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28">
+        <v>3.0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="28">
+      <c r="H16" s="28"/>
+      <c r="I16" s="28">
         <v>1.0</v>
       </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="J16" s="28"/>
       <c r="K16" s="27"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -28838,7 +28925,7 @@
       <c r="R16" s="28"/>
       <c r="S16" s="28"/>
       <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
+      <c r="U16" s="50"/>
       <c r="V16" s="28"/>
       <c r="W16" s="28"/>
       <c r="X16" s="28"/>
@@ -28872,27 +28959,31 @@
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BB16" s="5"/>
-      <c r="BC16" s="5"/>
+      <c r="BC16" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
+      <c r="E17" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28">
         <v>1.0</v>
       </c>
-      <c r="I17" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="27"/>
       <c r="L17" s="28"/>
@@ -28940,31 +29031,35 @@
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
+      <c r="H18" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="I18" s="28">
+        <v>1.0</v>
+      </c>
       <c r="J18" s="28"/>
       <c r="K18" s="27"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
+      <c r="O18" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P18" s="28"/>
       <c r="Q18" s="28"/>
       <c r="R18" s="28"/>
@@ -29004,12 +29099,10 @@
       <c r="AZ18" s="6"/>
       <c r="BA18" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="5"/>
-      <c r="BC18" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BC18" s="5"/>
       <c r="BF18" s="6"/>
     </row>
     <row r="19">
@@ -29018,22 +29111,26 @@
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="D19" s="28">
+        <v>1.0</v>
+      </c>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="27"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
+      <c r="O19" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
+      <c r="Q19" s="28">
+        <v>1.0</v>
+      </c>
       <c r="R19" s="28"/>
       <c r="S19" s="28"/>
       <c r="T19" s="28"/>
@@ -29071,27 +29168,23 @@
       <c r="AZ19" s="6"/>
       <c r="BA19" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB19" s="5"/>
-      <c r="BC19" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BC19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
@@ -29142,28 +29235,30 @@
         <v>2</v>
       </c>
       <c r="BB20" s="5"/>
-      <c r="BC20" s="5"/>
+      <c r="BC20" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
+      <c r="C21" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D21" s="28"/>
-      <c r="E21" s="28">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28">
         <v>1.0</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
       <c r="K21" s="27"/>
       <c r="L21" s="28"/>
-      <c r="M21" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="M21" s="28"/>
       <c r="N21" s="28"/>
       <c r="O21" s="28"/>
       <c r="P21" s="28"/>
@@ -29212,14 +29307,14 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
-      <c r="D22" s="28">
+      <c r="D22" s="28"/>
+      <c r="E22" s="28">
         <v>1.0</v>
       </c>
-      <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -29227,11 +29322,11 @@
       <c r="J22" s="28"/>
       <c r="K22" s="27"/>
       <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="M22" s="28">
+        <v>1.0</v>
+      </c>
       <c r="N22" s="28"/>
-      <c r="O22" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O22" s="28"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="28"/>
@@ -29278,7 +29373,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -29287,16 +29382,18 @@
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
+      <c r="I23" s="28">
+        <v>1.0</v>
+      </c>
       <c r="J23" s="28"/>
       <c r="K23" s="27"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
       <c r="N23" s="28"/>
-      <c r="O23" s="28">
+      <c r="O23" s="28"/>
+      <c r="P23" s="28">
         <v>1.0</v>
       </c>
-      <c r="P23" s="28"/>
       <c r="Q23" s="28"/>
       <c r="R23" s="28"/>
       <c r="S23" s="28"/>
@@ -29335,22 +29432,18 @@
       <c r="AZ23" s="6"/>
       <c r="BA23" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BB23" s="5">
-        <v>1.0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
-      <c r="D24" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -29361,7 +29454,9 @@
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
       <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
+      <c r="O24" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
       <c r="R24" s="28"/>
@@ -29403,19 +29498,21 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="BB24" s="5"/>
+      <c r="BB24" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28">
+      <c r="D25" s="28">
         <v>1.0</v>
       </c>
+      <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
@@ -29472,15 +29569,15 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28">
+      <c r="E26" s="28">
         <v>1.0</v>
       </c>
+      <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
@@ -29536,18 +29633,18 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="I27" s="28"/>
       <c r="J27" s="28"/>
       <c r="K27" s="27"/>
       <c r="L27" s="28"/>
@@ -29664,7 +29761,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
@@ -29681,7 +29778,9 @@
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
       <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
+      <c r="Q29" s="28">
+        <v>1.0</v>
+      </c>
       <c r="R29" s="28"/>
       <c r="S29" s="28"/>
       <c r="T29" s="28"/>
@@ -29719,14 +29818,14 @@
       <c r="AZ29" s="6"/>
       <c r="BA29" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB29" s="5"/>
       <c r="BC29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
@@ -29788,7 +29887,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
@@ -29912,7 +30011,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="28"/>
@@ -29974,7 +30073,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
@@ -30305,7 +30404,7 @@
       </c>
       <c r="O39" s="44">
         <f>'League Table'!O41</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P39" s="44">
         <f>'League Table'!P41</f>
@@ -30313,11 +30412,11 @@
       </c>
       <c r="Q39" s="44">
         <f>'League Table'!Q41</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R39" s="44">
         <f>'League Table'!R41</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S39" s="44">
         <f>'League Table'!S41</f>
@@ -30481,7 +30580,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="44" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B41" s="44">
         <f t="shared" ref="B41:AV41" si="2">SUM(B3:B37)</f>
@@ -30541,11 +30640,11 @@
       </c>
       <c r="P41" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q41" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R41" s="44">
         <f t="shared" si="2"/>
@@ -61399,7 +61498,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="2"/>
@@ -61564,10 +61663,10 @@
         <v>50</v>
       </c>
       <c r="AY3" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="BA3" s="53" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
@@ -61626,38 +61725,40 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16">
         <v>1.0</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="E5" s="16"/>
-      <c r="F5" s="16">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="H5" s="16">
         <v>1.0</v>
       </c>
-      <c r="G5" s="16">
+      <c r="I5" s="16"/>
+      <c r="J5" s="16">
         <v>1.0</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="J5" s="16">
-        <v>5.0</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="16">
+      <c r="M5" s="16"/>
+      <c r="N5" s="16">
         <v>1.0</v>
       </c>
-      <c r="N5" s="16"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16">
         <v>2.0</v>
       </c>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -61694,44 +61795,46 @@
       <c r="AY5" s="16"/>
       <c r="BA5" s="44">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54">
         <v>1.0</v>
       </c>
-      <c r="D6" s="54">
-        <v>2.0</v>
-      </c>
+      <c r="D6" s="54"/>
       <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
+      <c r="F6" s="54">
+        <v>1.0</v>
+      </c>
       <c r="G6" s="54">
-        <v>4.0</v>
-      </c>
-      <c r="H6" s="54">
         <v>1.0</v>
       </c>
-      <c r="I6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54">
+        <v>1.0</v>
+      </c>
       <c r="J6" s="54">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="K6" s="55"/>
       <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34">
+      <c r="M6" s="34">
         <v>1.0</v>
       </c>
+      <c r="N6" s="34"/>
       <c r="O6" s="34"/>
       <c r="P6" s="34">
         <v>2.0</v>
       </c>
       <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
+      <c r="R6" s="34">
+        <v>1.0</v>
+      </c>
       <c r="S6" s="34"/>
       <c r="T6" s="34"/>
       <c r="U6" s="34"/>
@@ -61767,25 +61870,25 @@
       <c r="AY6" s="34"/>
       <c r="BA6" s="44">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="E7" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="28"/>
       <c r="G7" s="28"/>
-      <c r="H7" s="28">
+      <c r="H7" s="28"/>
+      <c r="I7" s="28">
         <v>1.0</v>
       </c>
-      <c r="I7" s="28"/>
       <c r="J7" s="28">
         <v>1.0</v>
       </c>
@@ -61793,14 +61896,20 @@
       <c r="L7" s="28">
         <v>1.0</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="28"/>
+      <c r="N7" s="28">
         <v>1.0</v>
       </c>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
+      <c r="O7" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
+      <c r="Q7" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="R7" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S7" s="28"/>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
@@ -61836,25 +61945,25 @@
       <c r="AY7" s="28"/>
       <c r="BA7" s="44">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="16">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
         <v>1.0</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="I8" s="16"/>
       <c r="J8" s="16">
         <v>1.0</v>
       </c>
@@ -61862,16 +61971,16 @@
       <c r="L8" s="16">
         <v>1.0</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16">
+      <c r="M8" s="16">
         <v>1.0</v>
       </c>
-      <c r="O8" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="R8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
@@ -61907,12 +62016,12 @@
       <c r="AY8" s="16"/>
       <c r="BA8" s="44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34">
@@ -62046,7 +62155,7 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -62113,7 +62222,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -62137,7 +62246,9 @@
         <v>1.0</v>
       </c>
       <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
+      <c r="R12" s="34">
+        <v>1.0</v>
+      </c>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
       <c r="U12" s="34"/>
@@ -62173,12 +62284,12 @@
       <c r="AY12" s="34"/>
       <c r="BA12" s="44">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="28">
@@ -62363,7 +62474,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -62424,7 +62535,7 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -62432,9 +62543,7 @@
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="H17" s="28"/>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
@@ -62442,7 +62551,9 @@
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
+      <c r="P17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
       <c r="S17" s="28"/>
@@ -62485,7 +62596,7 @@
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -62493,11 +62604,11 @@
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="H18" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I18" s="28"/>
-      <c r="J18" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="J18" s="28"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -62546,19 +62657,19 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="J19" s="28">
+        <v>1.0</v>
+      </c>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
@@ -62607,16 +62718,16 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="28">
+      <c r="F20" s="28"/>
+      <c r="G20" s="28">
         <v>1.0</v>
       </c>
-      <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
@@ -62674,7 +62785,9 @@
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
@@ -62722,12 +62835,12 @@
       <c r="AY21" s="28"/>
       <c r="BA21" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -62786,7 +62899,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -62845,7 +62958,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -62904,7 +63017,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
@@ -62963,7 +63076,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -63022,7 +63135,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -63081,7 +63194,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
@@ -63140,7 +63253,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -63199,7 +63312,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -63258,7 +63371,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="36" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -63274,9 +63387,7 @@
       <c r="M31" s="28"/>
       <c r="N31" s="28"/>
       <c r="O31" s="28"/>
-      <c r="P31" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="P31" s="28"/>
       <c r="Q31" s="28"/>
       <c r="R31" s="28"/>
       <c r="S31" s="28"/>
@@ -63314,7 +63425,7 @@
       <c r="AY31" s="28"/>
       <c r="BA31" s="44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -63378,7 +63489,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -63437,7 +63548,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
@@ -63832,7 +63943,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" ref="B41:AY41" si="2">SUM(B5:B39)</f>
@@ -63896,11 +64007,11 @@
       </c>
       <c r="Q41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S41" s="5">
         <f t="shared" si="2"/>
@@ -64036,7 +64147,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -65023,19 +65134,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="44" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -65051,16 +65162,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G3" s="49"/>
       <c r="H3" s="5"/>
@@ -65072,10 +65183,10 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
@@ -65089,16 +65200,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="5"/>
@@ -65110,16 +65221,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="5"/>
@@ -65131,27 +65242,27 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I7" s="5"/>
       <c r="K7" s="44" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -65160,16 +65271,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G8" s="49"/>
       <c r="H8" s="5"/>
@@ -65181,32 +65292,32 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G9" s="49"/>
       <c r="H9" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I9" s="5">
         <v>3.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="L9" s="5">
         <v>2.0</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N9" s="5">
         <v>3.0</v>
@@ -65217,30 +65328,32 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="49" t="s">
         <v>159</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>157</v>
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I10" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" s="5">
         <v>2.0</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="L10" s="5"/>
       <c r="M10" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="N10" s="5">
         <v>3.0</v>
@@ -65251,30 +65364,30 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I11" s="5">
         <v>2.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N11" s="5">
         <v>3.0</v>
@@ -65285,30 +65398,30 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I12" s="5">
         <v>2.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="N12" s="5">
         <v>3.0</v>
@@ -65319,31 +65432,31 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
       <c r="H13" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I13" s="5">
         <v>2.0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="N13" s="5">
         <v>3.0</v>
@@ -65354,30 +65467,30 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I14" s="5">
         <v>2.0</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="N14" s="5">
         <v>3.0</v>
@@ -65388,33 +65501,33 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="49" t="s">
         <v>173</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" s="49" t="s">
-        <v>170</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I15" s="5">
         <v>2.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N15" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="16">
@@ -65422,33 +65535,33 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G16" s="49"/>
       <c r="H16" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="I16" s="5">
         <v>2.0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="N16" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="17">
@@ -65456,28 +65569,28 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I17" s="5"/>
       <c r="K17" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N17" s="5">
         <v>2.0</v>
@@ -65487,21 +65600,29 @@
       <c r="A18" s="49">
         <v>16.0</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="B18" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>141</v>
+      </c>
       <c r="G18" s="49"/>
       <c r="H18" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I18" s="5"/>
       <c r="K18" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="N18" s="5">
         <v>2.0</v>
@@ -65511,21 +65632,29 @@
       <c r="A19" s="49">
         <v>17.0</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
+      <c r="B19" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>136</v>
+      </c>
       <c r="G19" s="49"/>
       <c r="H19" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N19" s="5">
         <v>2.0</v>
@@ -65541,13 +65670,13 @@
       <c r="E20" s="49"/>
       <c r="G20" s="49"/>
       <c r="H20" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="N20" s="59">
         <v>1.0</v>
@@ -65563,13 +65692,13 @@
       <c r="E21" s="49"/>
       <c r="G21" s="49"/>
       <c r="H21" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="N21" s="59">
         <v>1.0</v>
@@ -65585,13 +65714,13 @@
       <c r="E22" s="49"/>
       <c r="G22" s="49"/>
       <c r="H22" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N22" s="59">
         <v>1.0</v>
@@ -65607,13 +65736,13 @@
       <c r="E23" s="49"/>
       <c r="G23" s="49"/>
       <c r="H23" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N23" s="59">
         <v>1.0</v>
@@ -65628,12 +65757,14 @@
       <c r="D24" s="49"/>
       <c r="E24" s="49"/>
       <c r="G24" s="49"/>
-      <c r="H24" s="60"/>
+      <c r="H24" s="5" t="s">
+        <v>181</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="N24" s="59">
         <v>1.0</v>
@@ -65653,7 +65784,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="N25" s="59">
         <v>1.0</v>
@@ -65673,7 +65804,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="N26" s="59">
         <v>1.0</v>
@@ -65692,7 +65823,7 @@
       <c r="I27" s="5"/>
       <c r="K27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="N27" s="59">
         <v>1.0</v>
@@ -65710,8 +65841,12 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
+      <c r="M28" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="N28" s="59">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="49">

</xml_diff>

<commit_message>
063 Game week 18 update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="6gNUf0hGLVgnOgh7+iO1a49nYPtIhHgVVQWqCdorvyA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="FqOX//pNsjCv6g2IFLN0FKhbvWJmRAzSKTWgJfdfp+o="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="188">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -210,10 +210,10 @@
     <t>KERMIT</t>
   </si>
   <si>
-    <t xml:space="preserve">MAMAS </t>
+    <t>CAPTAIN KIRK</t>
   </si>
   <si>
-    <t>CAPTAIN KIRK</t>
+    <t xml:space="preserve">MAMAS </t>
   </si>
   <si>
     <t>BRUCE</t>
@@ -225,28 +225,28 @@
     <t>CARLOS</t>
   </si>
   <si>
+    <t>INSPECTOR GADGET</t>
+  </si>
+  <si>
+    <t>DWARF</t>
+  </si>
+  <si>
     <t>PRESTON</t>
   </si>
   <si>
-    <t>INSPECTOR GADGET</t>
+    <t>ARTIST</t>
+  </si>
+  <si>
+    <t>FLO</t>
   </si>
   <si>
     <t>DUNCAN</t>
-  </si>
-  <si>
-    <t>DWARF</t>
   </si>
   <si>
     <t>KRYTON</t>
   </si>
   <si>
     <t>ZIGZAG</t>
-  </si>
-  <si>
-    <t>ARTIST</t>
-  </si>
-  <si>
-    <t>FLO</t>
   </si>
   <si>
     <t>TUNDE</t>
@@ -584,6 +584,9 @@
   <si>
     <t>Captain Kirk</t>
   </si>
+  <si>
+    <t>ZigZag - Wilson</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -931,6 +934,9 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -1667,7 +1673,9 @@
       <c r="R5" s="16">
         <v>0.0</v>
       </c>
-      <c r="S5" s="16"/>
+      <c r="S5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
       <c r="V5" s="16"/>
@@ -1704,11 +1712,11 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
@@ -1720,15 +1728,15 @@
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="BF5" s="20">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.7435897436</v>
+        <v>0.7619047619</v>
       </c>
       <c r="BG5" s="20"/>
     </row>
@@ -1893,7 +1901,9 @@
       <c r="R7" s="28">
         <v>0.0</v>
       </c>
-      <c r="S7" s="28"/>
+      <c r="S7" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
       <c r="V7" s="28"/>
@@ -1930,7 +1940,7 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
@@ -1942,7 +1952,7 @@
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
@@ -1950,11 +1960,11 @@
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BF7" s="20">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.619047619</v>
       </c>
       <c r="BG7" s="20"/>
     </row>
@@ -1964,7 +1974,7 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D8" s="16">
         <v>3.0</v>
@@ -1973,11 +1983,9 @@
         <v>0.0</v>
       </c>
       <c r="F8" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="G8" s="16">
-        <v>3.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="G8" s="16"/>
       <c r="H8" s="16">
         <v>-3.0</v>
       </c>
@@ -1985,29 +1993,31 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="16">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="16">
         <v>3.0</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="M8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="N8" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17">
+        <v>-1.0</v>
+      </c>
+      <c r="Q8" s="16">
         <v>-2.0</v>
       </c>
-      <c r="O8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="P8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="Q8" s="16">
+      <c r="R8" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="16">
         <v>2.0</v>
       </c>
-      <c r="R8" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
@@ -2064,7 +2074,7 @@
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BF8" s="20">
         <f t="shared" si="7"/>
@@ -2078,7 +2088,7 @@
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D9" s="34">
         <v>3.0</v>
@@ -2087,9 +2097,11 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="34">
-        <v>-2.0</v>
-      </c>
-      <c r="G9" s="34"/>
+        <v>2.0</v>
+      </c>
+      <c r="G9" s="34">
+        <v>3.0</v>
+      </c>
       <c r="H9" s="34">
         <v>-3.0</v>
       </c>
@@ -2097,29 +2109,31 @@
         <v>2.0</v>
       </c>
       <c r="J9" s="34">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K9" s="32"/>
       <c r="L9" s="34">
         <v>3.0</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="34"/>
+      <c r="N9" s="34">
+        <v>-2.0</v>
+      </c>
+      <c r="O9" s="34">
         <v>1.0</v>
       </c>
-      <c r="N9" s="34">
+      <c r="P9" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Q9" s="34">
         <v>2.0</v>
-      </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="33">
-        <v>-1.0</v>
-      </c>
-      <c r="Q9" s="34">
-        <v>-2.0</v>
       </c>
       <c r="R9" s="34">
         <v>0.0</v>
       </c>
-      <c r="S9" s="34"/>
+      <c r="S9" s="34">
+        <v>-2.0</v>
+      </c>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
       <c r="V9" s="34"/>
@@ -2156,11 +2170,11 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
@@ -2168,19 +2182,19 @@
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF9" s="20">
         <f t="shared" si="7"/>
-        <v>0.5897435897</v>
+        <v>0.5777777778</v>
       </c>
       <c r="BG9" s="20"/>
     </row>
@@ -2233,7 +2247,9 @@
         <v>-2.0</v>
       </c>
       <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
+      <c r="S10" s="34">
+        <v>-2.0</v>
+      </c>
       <c r="T10" s="34"/>
       <c r="U10" s="34"/>
       <c r="V10" s="34"/>
@@ -2270,7 +2286,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2282,7 +2298,7 @@
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
@@ -2290,11 +2306,11 @@
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF10" s="20">
         <f t="shared" si="7"/>
-        <v>0.5238095238</v>
+        <v>0.4888888889</v>
       </c>
       <c r="BG10" s="20"/>
     </row>
@@ -2343,7 +2359,9 @@
       <c r="R11" s="28">
         <v>0.0</v>
       </c>
-      <c r="S11" s="28"/>
+      <c r="S11" s="29">
+        <v>2.0</v>
+      </c>
       <c r="T11" s="28"/>
       <c r="U11" s="28"/>
       <c r="V11" s="28"/>
@@ -2380,11 +2398,11 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="3"/>
@@ -2396,15 +2414,15 @@
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF11" s="20">
         <f t="shared" si="7"/>
-        <v>0.4722222222</v>
+        <v>0.5128205128</v>
       </c>
       <c r="BG11" s="20"/>
     </row>
@@ -2455,7 +2473,9 @@
       <c r="R12" s="28">
         <v>0.0</v>
       </c>
-      <c r="S12" s="28"/>
+      <c r="S12" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
@@ -2492,11 +2512,11 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB12" s="5">
         <f t="shared" si="3"/>
@@ -2508,15 +2528,15 @@
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="BF12" s="20">
         <f t="shared" si="7"/>
-        <v>0.4358974359</v>
+        <v>0.4761904762</v>
       </c>
       <c r="BG12" s="20"/>
     </row>
@@ -2526,52 +2546,48 @@
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="E13" s="28">
-        <v>0.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="E13" s="28"/>
       <c r="F13" s="28">
         <v>-2.0</v>
       </c>
       <c r="G13" s="28">
-        <v>-3.0</v>
-      </c>
-      <c r="H13" s="28">
-        <v>-3.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="28"/>
       <c r="I13" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J13" s="28">
         <v>2.0</v>
       </c>
       <c r="K13" s="27"/>
-      <c r="L13" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="L13" s="28"/>
       <c r="M13" s="29">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N13" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O13" s="28">
         <v>-1.0</v>
       </c>
       <c r="P13" s="28">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q13" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="R13" s="28">
         <v>0.0</v>
       </c>
-      <c r="S13" s="28"/>
+      <c r="S13" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
       <c r="V13" s="28"/>
@@ -2608,31 +2624,31 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="20">
         <f t="shared" si="7"/>
-        <v>0.3777777778</v>
+        <v>0.4871794872</v>
       </c>
       <c r="BG13" s="20"/>
     </row>
@@ -2648,13 +2664,11 @@
         <v>-3.0</v>
       </c>
       <c r="E14" s="28"/>
-      <c r="F14" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="G14" s="28">
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29">
         <v>3.0</v>
       </c>
-      <c r="H14" s="28"/>
       <c r="I14" s="28">
         <v>-2.0</v>
       </c>
@@ -2662,26 +2676,28 @@
         <v>2.0</v>
       </c>
       <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29">
+      <c r="L14" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="M14" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="N14" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="O14" s="28">
         <v>1.0</v>
       </c>
-      <c r="N14" s="28">
+      <c r="P14" s="28">
+        <v>-1.0</v>
+      </c>
+      <c r="Q14" s="28">
         <v>2.0</v>
       </c>
-      <c r="O14" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="P14" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q14" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="R14" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="S14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T14" s="28"/>
       <c r="U14" s="28"/>
       <c r="V14" s="28"/>
@@ -2722,11 +2738,11 @@
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="5">
         <f t="shared" si="4"/>
@@ -2734,15 +2750,15 @@
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="BF14" s="20">
         <f t="shared" si="7"/>
-        <v>0.4444444444</v>
+        <v>0.5</v>
       </c>
       <c r="BG14" s="20"/>
     </row>
@@ -2752,38 +2768,38 @@
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D15" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="29">
         <v>3.0</v>
       </c>
       <c r="E15" s="28">
         <v>0.0</v>
       </c>
       <c r="F15" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G15" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H15" s="28">
         <v>-3.0</v>
       </c>
       <c r="I15" s="28">
-        <v>-2.0</v>
-      </c>
-      <c r="J15" s="29">
-        <v>-2.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="J15" s="28">
+        <v>2.0</v>
       </c>
       <c r="K15" s="27"/>
       <c r="L15" s="28">
         <v>-3.0</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15" s="29">
         <v>-1.0</v>
       </c>
       <c r="N15" s="28">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="O15" s="28">
         <v>-1.0</v>
@@ -2794,7 +2810,9 @@
       <c r="Q15" s="28">
         <v>2.0</v>
       </c>
-      <c r="R15" s="28"/>
+      <c r="R15" s="28">
+        <v>0.0</v>
+      </c>
       <c r="S15" s="28"/>
       <c r="T15" s="28"/>
       <c r="U15" s="28"/>
@@ -2832,7 +2850,7 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
@@ -2840,7 +2858,7 @@
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC15" s="5">
         <f t="shared" si="4"/>
@@ -2848,15 +2866,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="BF15" s="20">
         <f t="shared" si="7"/>
-        <v>0.380952381</v>
+        <v>0.3777777778</v>
       </c>
       <c r="BG15" s="20"/>
     </row>
@@ -2865,45 +2883,45 @@
         <v>70</v>
       </c>
       <c r="B16" s="27"/>
-      <c r="C16" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="D16" s="28">
-        <v>-3.0</v>
-      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>2.0</v>
+      </c>
       <c r="G16" s="28"/>
-      <c r="H16" s="29">
+      <c r="H16" s="28">
         <v>3.0</v>
       </c>
       <c r="I16" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="J16" s="28">
         <v>-2.0</v>
-      </c>
-      <c r="J16" s="28">
-        <v>2.0</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="M16" s="28">
+        <v>-3.0</v>
+      </c>
+      <c r="M16" s="28"/>
+      <c r="N16" s="29">
+        <v>-2.0</v>
+      </c>
+      <c r="O16" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N16" s="28">
+      <c r="P16" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="Q16" s="28">
         <v>-2.0</v>
       </c>
-      <c r="O16" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P16" s="28">
-        <v>-1.0</v>
-      </c>
-      <c r="Q16" s="28">
+      <c r="R16" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="S16" s="28">
         <v>2.0</v>
       </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
       <c r="T16" s="28"/>
       <c r="U16" s="28"/>
       <c r="V16" s="28"/>
@@ -2948,23 +2966,23 @@
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC16" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF16" s="20">
         <f t="shared" si="7"/>
-        <v>0.4545454545</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG16" s="20"/>
     </row>
@@ -2973,9 +2991,11 @@
         <v>71</v>
       </c>
       <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D17" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="E17" s="28">
         <v>0.0</v>
@@ -2987,12 +3007,14 @@
       <c r="H17" s="28">
         <v>-3.0</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="J17" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J17" s="28"/>
       <c r="K17" s="27"/>
-      <c r="L17" s="29">
+      <c r="L17" s="28">
         <v>-3.0</v>
       </c>
       <c r="M17" s="28">
@@ -3000,16 +3022,14 @@
       </c>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
-      <c r="P17" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="Q17" s="28">
+      <c r="P17" s="28"/>
+      <c r="Q17" s="29">
         <v>2.0</v>
       </c>
-      <c r="R17" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="S17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28">
+        <v>2.0</v>
+      </c>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
@@ -3046,31 +3066,31 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="BF17" s="20">
         <f t="shared" si="7"/>
-        <v>0.4666666667</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG17" s="20"/>
     </row>
@@ -3085,14 +3105,14 @@
       <c r="D18" s="28">
         <v>3.0</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="28">
         <v>0.0</v>
       </c>
       <c r="F18" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G18" s="28">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="H18" s="28">
         <v>-3.0</v>
@@ -3100,17 +3120,21 @@
       <c r="I18" s="28">
         <v>-2.0</v>
       </c>
-      <c r="J18" s="28"/>
+      <c r="J18" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="K18" s="27"/>
       <c r="L18" s="28">
         <v>-3.0</v>
       </c>
       <c r="M18" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="N18" s="28"/>
+        <v>-1.0</v>
+      </c>
+      <c r="N18" s="28">
+        <v>2.0</v>
+      </c>
       <c r="O18" s="28">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="P18" s="28">
         <v>-1.0</v>
@@ -3118,9 +3142,7 @@
       <c r="Q18" s="28">
         <v>2.0</v>
       </c>
-      <c r="R18" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="R18" s="28"/>
       <c r="S18" s="28"/>
       <c r="T18" s="28"/>
       <c r="U18" s="28"/>
@@ -3158,31 +3180,31 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="BF18" s="20">
         <f t="shared" si="7"/>
-        <v>0.358974359</v>
+        <v>0.380952381</v>
       </c>
       <c r="BG18" s="20"/>
     </row>
@@ -3192,37 +3214,37 @@
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="G19" s="28"/>
+      <c r="D19" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28">
+        <v>3.0</v>
+      </c>
       <c r="H19" s="28">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I19" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="J19" s="28">
         <v>-2.0</v>
       </c>
+      <c r="J19" s="28"/>
       <c r="K19" s="27"/>
-      <c r="L19" s="28">
+      <c r="L19" s="29">
         <v>-3.0</v>
       </c>
-      <c r="M19" s="28"/>
-      <c r="N19" s="29">
-        <v>-2.0</v>
-      </c>
-      <c r="O19" s="28">
+      <c r="M19" s="28">
         <v>-1.0</v>
       </c>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
       <c r="P19" s="28">
         <v>1.0</v>
       </c>
       <c r="Q19" s="28">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="R19" s="28">
         <v>0.0</v>
@@ -3272,23 +3294,23 @@
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="BF19" s="20">
         <f t="shared" si="7"/>
-        <v>0.4333333333</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BG19" s="20"/>
     </row>
@@ -3298,42 +3320,50 @@
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="28">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D20" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="29">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="28">
+        <v>-2.0</v>
+      </c>
+      <c r="G20" s="28">
         <v>-3.0</v>
-      </c>
-      <c r="E20" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28">
-        <v>3.0</v>
       </c>
       <c r="H20" s="28">
         <v>-3.0</v>
       </c>
-      <c r="I20" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="J20" s="28">
+      <c r="I20" s="28">
         <v>-2.0</v>
       </c>
+      <c r="J20" s="28"/>
       <c r="K20" s="27"/>
       <c r="L20" s="28">
         <v>-3.0</v>
       </c>
       <c r="M20" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="P20" s="28">
         <v>-1.0</v>
       </c>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="29">
+      <c r="Q20" s="28">
         <v>2.0</v>
       </c>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
+      <c r="R20" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="S20" s="29">
+        <v>-2.0</v>
+      </c>
       <c r="T20" s="28"/>
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
@@ -3370,7 +3400,7 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
@@ -3378,23 +3408,23 @@
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="BF20" s="20">
         <f t="shared" si="7"/>
-        <v>0.4333333333</v>
+        <v>0.3333333333</v>
       </c>
       <c r="BG20" s="20"/>
     </row>
@@ -3635,7 +3665,9 @@
       <c r="R23" s="28">
         <v>0.0</v>
       </c>
-      <c r="S23" s="28"/>
+      <c r="S23" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T23" s="28"/>
       <c r="U23" s="28"/>
       <c r="V23" s="28"/>
@@ -3672,7 +3704,7 @@
       </c>
       <c r="AZ23" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA23" s="5">
         <f t="shared" si="2"/>
@@ -3684,7 +3716,7 @@
       </c>
       <c r="BC23" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD23" s="5">
         <f t="shared" si="5"/>
@@ -3692,11 +3724,11 @@
       </c>
       <c r="BE23" s="5">
         <f t="shared" si="6"/>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="BF23" s="20">
         <f t="shared" si="7"/>
-        <v>0.2820512821</v>
+        <v>0.2619047619</v>
       </c>
       <c r="BG23" s="20"/>
     </row>
@@ -3747,7 +3779,9 @@
       <c r="R24" s="29">
         <v>0.0</v>
       </c>
-      <c r="S24" s="28"/>
+      <c r="S24" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T24" s="28"/>
       <c r="U24" s="28"/>
       <c r="V24" s="28"/>
@@ -3784,7 +3818,7 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
@@ -3796,7 +3830,7 @@
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
@@ -3804,11 +3838,11 @@
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="BF24" s="20">
         <f t="shared" si="7"/>
-        <v>0.2820512821</v>
+        <v>0.2619047619</v>
       </c>
       <c r="BG24" s="20"/>
     </row>
@@ -3844,10 +3878,12 @@
       </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
-      <c r="R25" s="28">
+      <c r="R25" s="29">
         <v>0.0</v>
       </c>
-      <c r="S25" s="28"/>
+      <c r="S25" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T25" s="28"/>
       <c r="U25" s="28"/>
       <c r="V25" s="28"/>
@@ -3884,7 +3920,7 @@
       </c>
       <c r="AZ25" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
@@ -3896,7 +3932,7 @@
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
@@ -3904,11 +3940,11 @@
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="BF25" s="20">
         <f t="shared" si="7"/>
-        <v>0.380952381</v>
+        <v>0.3333333333</v>
       </c>
       <c r="BG25" s="20"/>
     </row>
@@ -3939,7 +3975,9 @@
         <v>-2.0</v>
       </c>
       <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
+      <c r="S26" s="28">
+        <v>-2.0</v>
+      </c>
       <c r="T26" s="28"/>
       <c r="U26" s="28"/>
       <c r="V26" s="28"/>
@@ -3976,7 +4014,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -3988,7 +4026,7 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
@@ -3996,11 +4034,11 @@
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="BF26" s="20">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.5</v>
       </c>
       <c r="BG26" s="20"/>
     </row>
@@ -5328,7 +5366,7 @@
       </c>
       <c r="S41" s="34">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T41" s="34">
         <f t="shared" si="8"/>
@@ -25963,7 +26001,7 @@
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="44">
         <v>2.0</v>
@@ -26056,7 +26094,7 @@
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" s="45">
         <v>1.0</v>
@@ -26143,7 +26181,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" s="44">
         <v>2.0</v>
@@ -26168,7 +26206,7 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="44">
         <v>1.0</v>
@@ -26194,7 +26232,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="44">
         <v>2.0</v>
@@ -26219,7 +26257,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="44">
         <v>2.0</v>
@@ -26234,7 +26272,7 @@
         <v>1.0</v>
       </c>
       <c r="F13" s="44">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G13" s="44">
         <f t="shared" si="1"/>
@@ -26250,26 +26288,26 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B14" s="44">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="44">
         <v>1.0</v>
       </c>
-      <c r="C14" s="44">
+      <c r="D14" s="44">
         <v>0.0</v>
       </c>
-      <c r="D14" s="44">
+      <c r="E14" s="44">
         <v>1.0</v>
       </c>
-      <c r="E14" s="44">
-        <v>0.0</v>
-      </c>
       <c r="F14" s="44">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G14" s="44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="44">
@@ -26277,12 +26315,12 @@
       </c>
       <c r="J14" s="46">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B15" s="44">
         <v>1.0</v>
@@ -26313,7 +26351,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" s="44">
         <v>2.0</v>
@@ -26328,7 +26366,7 @@
         <v>1.0</v>
       </c>
       <c r="F16" s="44">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G16" s="44">
         <f t="shared" si="1"/>
@@ -26344,38 +26382,38 @@
     </row>
     <row r="17">
       <c r="A17" s="36" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B17" s="44">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C17" s="44">
         <v>0.0</v>
       </c>
       <c r="D17" s="44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E17" s="44">
         <v>1.0</v>
       </c>
       <c r="F17" s="44">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="44">
         <v>23.0</v>
       </c>
       <c r="J17" s="46">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="B18" s="44">
         <v>1.0</v>
@@ -26390,7 +26428,7 @@
         <v>1.0</v>
       </c>
       <c r="F18" s="44">
-        <v>-2.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G18" s="44">
         <f t="shared" si="1"/>
@@ -26406,7 +26444,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B19" s="44">
         <v>1.0</v>
@@ -26437,7 +26475,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" s="44">
         <v>1.0</v>
@@ -26468,7 +26506,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="44">
         <v>1.0</v>
@@ -27932,14 +27970,51 @@
       <c r="R2" s="7">
         <v>45776.0</v>
       </c>
-      <c r="U2" s="49"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
+      <c r="S2" s="7">
+        <v>45783.0</v>
+      </c>
+      <c r="T2" s="7">
+        <v>45790.0</v>
+      </c>
+      <c r="U2" s="7">
+        <v>45797.0</v>
+      </c>
+      <c r="V2" s="7">
+        <v>45804.0</v>
+      </c>
+      <c r="W2" s="7">
+        <v>45811.0</v>
+      </c>
+      <c r="X2" s="7">
+        <v>45818.0</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>45825.0</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>45832.0</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>45839.0</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>45846.0</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>45853.0</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>45860.0</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>45867.0</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>45874.0</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>45881.0</v>
+      </c>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
@@ -28043,31 +28118,37 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="C4" s="28">
+        <v>2.0</v>
+      </c>
       <c r="D4" s="28">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
-      <c r="G4" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="28"/>
-      <c r="I4" s="28">
-        <v>7.0</v>
-      </c>
+      <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="27"/>
       <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="M4" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
+      <c r="P4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
+      <c r="R4" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S4" s="28"/>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
@@ -28104,41 +28185,35 @@
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="BB4" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="28"/>
-      <c r="C5" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="C5" s="28"/>
       <c r="D5" s="28">
         <v>1.0</v>
       </c>
       <c r="E5" s="28"/>
-      <c r="F5" s="28">
+      <c r="F5" s="28"/>
+      <c r="G5" s="28">
         <v>1.0</v>
       </c>
-      <c r="G5" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="H5" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="I5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28">
+        <v>7.0</v>
+      </c>
       <c r="J5" s="28"/>
       <c r="K5" s="27"/>
       <c r="L5" s="28"/>
-      <c r="M5" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="M5" s="28"/>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
@@ -28189,33 +28264,35 @@
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="28">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="27"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="N6" s="28">
         <v>1.0</v>
       </c>
+      <c r="N6" s="28"/>
       <c r="O6" s="28"/>
-      <c r="P6" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="P6" s="28"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
@@ -28256,10 +28333,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="BB6" s="5"/>
-      <c r="BC6" s="5">
-        <v>3.0</v>
-      </c>
+      <c r="BB6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="BC6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
@@ -28333,31 +28410,31 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="28"/>
+        <v>73</v>
+      </c>
+      <c r="B8" s="27"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="28">
+        <v>2.0</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="28">
+      <c r="G8" s="28"/>
+      <c r="H8" s="28">
         <v>2.0</v>
       </c>
-      <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="27"/>
-      <c r="L8" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O8" s="28"/>
       <c r="P8" s="28"/>
       <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
+      <c r="R8" s="28">
+        <v>2.0</v>
+      </c>
       <c r="S8" s="28"/>
       <c r="T8" s="28"/>
       <c r="U8" s="28"/>
@@ -28397,35 +28474,35 @@
         <v>6</v>
       </c>
       <c r="BB8" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="BC8" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28">
-        <v>1.0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="28">
+        <v>2.0</v>
+      </c>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="J9" s="28"/>
       <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
+      <c r="L9" s="28">
+        <v>3.0</v>
+      </c>
       <c r="M9" s="28"/>
-      <c r="N9" s="28">
+      <c r="N9" s="28"/>
+      <c r="O9" s="28">
         <v>1.0</v>
-      </c>
-      <c r="O9" s="28">
-        <v>2.0</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -28475,7 +28552,7 @@
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="28">
@@ -28485,22 +28562,22 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K10" s="27"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
+      <c r="N10" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="O10" s="28">
+        <v>2.0</v>
+      </c>
       <c r="P10" s="28"/>
-      <c r="Q10" s="28">
-        <v>3.0</v>
-      </c>
+      <c r="Q10" s="28"/>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
@@ -28547,14 +28624,14 @@
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="28">
+        <v>1.0</v>
+      </c>
       <c r="D11" s="28"/>
-      <c r="E11" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28">
@@ -28566,15 +28643,13 @@
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="M11" s="28"/>
       <c r="N11" s="28"/>
-      <c r="O11" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O11" s="28"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
+      <c r="Q11" s="28">
+        <v>3.0</v>
+      </c>
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
@@ -28614,41 +28689,45 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="BB11" s="5"/>
-      <c r="BC11" s="5">
+      <c r="BB11" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="28">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28">
         <v>1.0</v>
       </c>
+      <c r="F12" s="28"/>
       <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="H12" s="28">
+        <v>1.0</v>
+      </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="J12" s="28">
+        <v>1.0</v>
+      </c>
       <c r="K12" s="27"/>
       <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28">
+      <c r="M12" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28">
         <v>1.0</v>
       </c>
-      <c r="O12" s="28"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
-      <c r="U12" s="50"/>
+      <c r="U12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="28"/>
       <c r="X12" s="28"/>
@@ -28682,7 +28761,7 @@
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BB12" s="5"/>
       <c r="BC12" s="5">
@@ -28692,7 +28771,7 @@
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
@@ -28700,23 +28779,23 @@
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="H13" s="28">
+        <v>2.0</v>
+      </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="28">
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28">
         <v>2.0</v>
       </c>
-      <c r="M13" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="N13" s="28">
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28">
         <v>1.0</v>
       </c>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
@@ -28757,37 +28836,39 @@
       </c>
       <c r="BB13" s="5"/>
       <c r="BC13" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="F14" s="28"/>
+      <c r="D14" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G14" s="28"/>
-      <c r="H14" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="27"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="N14" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
       <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
+      <c r="U14" s="50"/>
       <c r="V14" s="28"/>
       <c r="W14" s="28"/>
       <c r="X14" s="28"/>
@@ -28821,18 +28902,16 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="BB14" s="5">
-        <v>1.0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BB14" s="5"/>
       <c r="BC14" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
@@ -28840,19 +28919,21 @@
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="H15" s="28"/>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
       <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="L15" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="M15" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="N15" s="28">
+        <v>1.0</v>
+      </c>
       <c r="O15" s="28"/>
-      <c r="P15" s="28">
-        <v>2.0</v>
-      </c>
+      <c r="P15" s="28"/>
       <c r="Q15" s="28"/>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
@@ -28891,11 +28972,11 @@
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB15" s="5"/>
       <c r="BC15" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -28922,7 +29003,9 @@
       <c r="O16" s="28"/>
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
+      <c r="R16" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S16" s="28"/>
       <c r="T16" s="28"/>
       <c r="U16" s="50"/>
@@ -28959,7 +29042,7 @@
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB16" s="5"/>
       <c r="BC16" s="5">
@@ -28994,7 +29077,9 @@
       </c>
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
+      <c r="R17" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S17" s="28"/>
       <c r="T17" s="28"/>
       <c r="U17" s="28"/>
@@ -29031,7 +29116,7 @@
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
@@ -29107,7 +29192,7 @@
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
@@ -29307,7 +29392,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
@@ -29439,7 +29524,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -29454,12 +29539,14 @@
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
       <c r="N24" s="28"/>
-      <c r="O24" s="28">
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28">
         <v>1.0</v>
       </c>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
+      <c r="R24" s="28">
+        <v>1.0</v>
+      </c>
       <c r="S24" s="28"/>
       <c r="T24" s="28"/>
       <c r="U24" s="28"/>
@@ -29496,22 +29583,18 @@
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BB24" s="5">
-        <v>1.0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="BB24" s="5"/>
       <c r="BC24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
-      <c r="D25" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -29522,7 +29605,9 @@
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
+      <c r="O25" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
@@ -29564,19 +29649,21 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="BB25" s="5"/>
+      <c r="BB25" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28">
+      <c r="D26" s="28">
         <v>1.0</v>
       </c>
+      <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
@@ -29633,15 +29720,15 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28">
+      <c r="E27" s="28">
         <v>1.0</v>
       </c>
+      <c r="F27" s="28"/>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
@@ -29697,13 +29784,15 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="36" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="28">
+        <v>1.0</v>
+      </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -29712,9 +29801,7 @@
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
-      <c r="O28" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="O28" s="28"/>
       <c r="P28" s="28"/>
       <c r="Q28" s="28"/>
       <c r="R28" s="28"/>
@@ -29761,7 +29848,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
@@ -29776,11 +29863,11 @@
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
       <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
+      <c r="O29" s="28">
+        <v>1.0</v>
+      </c>
       <c r="P29" s="28"/>
-      <c r="Q29" s="28">
-        <v>1.0</v>
-      </c>
+      <c r="Q29" s="28"/>
       <c r="R29" s="28"/>
       <c r="S29" s="28"/>
       <c r="T29" s="28"/>
@@ -30073,7 +30160,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
@@ -30420,7 +30507,7 @@
       </c>
       <c r="S39" s="44">
         <f>'League Table'!S41</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T39" s="44">
         <f>'League Table'!T41</f>
@@ -30648,7 +30735,7 @@
       </c>
       <c r="R41" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S41" s="44">
         <f t="shared" si="2"/>
@@ -61725,7 +61812,7 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16">
@@ -62021,7 +62108,7 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34">
@@ -62047,8 +62134,12 @@
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
+      <c r="R9" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="S9" s="59">
+        <v>2.0</v>
+      </c>
       <c r="T9" s="34"/>
       <c r="U9" s="34"/>
       <c r="V9" s="34"/>
@@ -62083,7 +62174,7 @@
       <c r="AY9" s="34"/>
       <c r="BA9" s="44">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -62222,7 +62313,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -62474,7 +62565,7 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -62779,7 +62870,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -62840,7 +62931,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -62958,7 +63049,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -63253,7 +63344,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -63489,7 +63580,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -64011,11 +64102,11 @@
       </c>
       <c r="R41" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T41" s="5">
         <f t="shared" si="2"/>
@@ -64147,7 +64238,7 @@
       </c>
       <c r="BA41" s="44">
         <f>SUM(B41:AZ41)</f>
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -65319,8 +65410,8 @@
       <c r="M9" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="N9" s="5">
-        <v>3.0</v>
+      <c r="N9" s="60">
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
@@ -65356,7 +65447,7 @@
         <v>159</v>
       </c>
       <c r="N10" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
@@ -65664,8 +65755,12 @@
       <c r="A20" s="49">
         <v>18.0</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>162</v>
+      </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
       <c r="G20" s="49"/>
@@ -65673,13 +65768,15 @@
         <v>157</v>
       </c>
       <c r="I20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N20" s="59">
-        <v>1.0</v>
+        <v>172</v>
+      </c>
+      <c r="N20" s="60">
+        <v>2.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -65698,9 +65795,9 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="N21" s="59">
+        <v>185</v>
+      </c>
+      <c r="N21" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65722,7 +65819,7 @@
       <c r="M22" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="N22" s="59">
+      <c r="N22" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65744,7 +65841,7 @@
       <c r="M23" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="N23" s="59">
+      <c r="N23" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65766,7 +65863,7 @@
       <c r="M24" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N24" s="59">
+      <c r="N24" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65786,7 +65883,7 @@
       <c r="M25" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="N25" s="59">
+      <c r="N25" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65806,7 +65903,7 @@
       <c r="M26" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="N26" s="59">
+      <c r="N26" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65825,7 +65922,7 @@
       <c r="M27" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="N27" s="59">
+      <c r="N27" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65844,7 +65941,7 @@
       <c r="M28" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="N28" s="59">
+      <c r="N28" s="60">
         <v>1.0</v>
       </c>
     </row>
@@ -65859,8 +65956,6 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="49">
@@ -65979,6 +66074,7 @@
       <c r="E38" s="49"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
+      <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -70883,6 +70979,11 @@
       <c r="H1000" s="5"/>
       <c r="I1000" s="5"/>
       <c r="N1000" s="5"/>
+    </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="H1001" s="5"/>
+      <c r="I1001" s="5"/>
+      <c r="N1001" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$F$47"/>

</xml_diff>

<commit_message>
077 Game week 32 update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="2F6KVHz8FecYWasJzwnEivH5MSBjWz01hG6YqOG4NuE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oSTkFgWt7aUQ3XhcajXrZz4WuFO30v9b7CdS+AzNPMs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="217">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -671,6 +671,9 @@
   <si>
     <t xml:space="preserve">Khen </t>
   </si>
+  <si>
+    <t>Duncan - Wilson</t>
+  </si>
 </sst>
 </file>
 
@@ -1779,7 +1782,9 @@
       <c r="AF5" s="16">
         <v>1.0</v>
       </c>
-      <c r="AG5" s="16"/>
+      <c r="AG5" s="16">
+        <v>0.0</v>
+      </c>
       <c r="AH5" s="16"/>
       <c r="AI5" s="16"/>
       <c r="AJ5" s="16"/>
@@ -1802,7 +1807,7 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
@@ -1810,7 +1815,7 @@
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC40" si="4">COUNTIF($B5:$AX5, "&lt;0")</f>
@@ -1818,7 +1823,7 @@
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
@@ -1826,7 +1831,7 @@
       </c>
       <c r="BF5" s="19">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.5897435897</v>
+        <v>0.5802469136</v>
       </c>
       <c r="BG5" s="19"/>
     </row>
@@ -1911,7 +1916,9 @@
       <c r="AF6" s="22">
         <v>1.0</v>
       </c>
-      <c r="AG6" s="22"/>
+      <c r="AG6" s="22">
+        <v>0.0</v>
+      </c>
       <c r="AH6" s="22"/>
       <c r="AI6" s="22"/>
       <c r="AJ6" s="22"/>
@@ -1934,7 +1941,7 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
@@ -1942,7 +1949,7 @@
       </c>
       <c r="BB6" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BC6" s="5">
         <f t="shared" si="4"/>
@@ -1950,7 +1957,7 @@
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
@@ -1958,7 +1965,7 @@
       </c>
       <c r="BF6" s="19">
         <f t="shared" si="7"/>
-        <v>0.6086956522</v>
+        <v>0.5972222222</v>
       </c>
       <c r="BG6" s="19"/>
     </row>
@@ -2047,7 +2054,9 @@
       <c r="AF7" s="26">
         <v>1.0</v>
       </c>
-      <c r="AG7" s="26"/>
+      <c r="AG7" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AH7" s="26"/>
       <c r="AI7" s="26"/>
       <c r="AJ7" s="26"/>
@@ -2070,7 +2079,7 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
@@ -2078,7 +2087,7 @@
       </c>
       <c r="BB7" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
@@ -2086,7 +2095,7 @@
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
@@ -2094,7 +2103,7 @@
       </c>
       <c r="BF7" s="19">
         <f t="shared" si="7"/>
-        <v>0.52</v>
+        <v>0.5128205128</v>
       </c>
       <c r="BG7" s="19"/>
     </row>
@@ -2185,7 +2194,9 @@
       <c r="AF8" s="16">
         <v>1.0</v>
       </c>
-      <c r="AG8" s="16"/>
+      <c r="AG8" s="16">
+        <v>0.0</v>
+      </c>
       <c r="AH8" s="16"/>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
@@ -2208,7 +2219,7 @@
       </c>
       <c r="AZ8" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA8" s="5">
         <f t="shared" si="2"/>
@@ -2216,7 +2227,7 @@
       </c>
       <c r="BB8" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BC8" s="5">
         <f t="shared" si="4"/>
@@ -2224,7 +2235,7 @@
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
@@ -2232,7 +2243,7 @@
       </c>
       <c r="BF8" s="19">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4938271605</v>
       </c>
       <c r="BG8" s="19"/>
     </row>
@@ -2449,7 +2460,9 @@
       <c r="AF10" s="30">
         <v>-1.0</v>
       </c>
-      <c r="AG10" s="30"/>
+      <c r="AG10" s="30">
+        <v>0.0</v>
+      </c>
       <c r="AH10" s="30"/>
       <c r="AI10" s="30"/>
       <c r="AJ10" s="30"/>
@@ -2472,7 +2485,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2480,7 +2493,7 @@
       </c>
       <c r="BB10" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
@@ -2488,7 +2501,7 @@
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
@@ -2496,7 +2509,7 @@
       </c>
       <c r="BF10" s="19">
         <f t="shared" si="7"/>
-        <v>0.5303030303</v>
+        <v>0.5217391304</v>
       </c>
       <c r="BG10" s="19"/>
     </row>
@@ -2579,13 +2592,15 @@
       <c r="AD11" s="26">
         <v>-5.0</v>
       </c>
-      <c r="AE11" s="26">
+      <c r="AE11" s="27">
         <v>0.0</v>
       </c>
       <c r="AF11" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG11" s="26"/>
+      <c r="AG11" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH11" s="26"/>
       <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
@@ -2608,7 +2623,7 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
@@ -2616,7 +2631,7 @@
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
@@ -2624,7 +2639,7 @@
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
@@ -2632,7 +2647,7 @@
       </c>
       <c r="BF11" s="19">
         <f t="shared" si="7"/>
-        <v>0.4533333333</v>
+        <v>0.4487179487</v>
       </c>
       <c r="BG11" s="19"/>
     </row>
@@ -2723,7 +2738,9 @@
       <c r="AF12" s="26">
         <v>1.0</v>
       </c>
-      <c r="AG12" s="26"/>
+      <c r="AG12" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH12" s="26"/>
       <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
@@ -2746,7 +2763,7 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
@@ -2754,7 +2771,7 @@
       </c>
       <c r="BB12" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC12" s="5">
         <f t="shared" si="4"/>
@@ -2762,7 +2779,7 @@
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
@@ -2770,7 +2787,7 @@
       </c>
       <c r="BF12" s="19">
         <f t="shared" si="7"/>
-        <v>0.4358974359</v>
+        <v>0.4320987654</v>
       </c>
       <c r="BG12" s="19"/>
     </row>
@@ -2847,11 +2864,13 @@
       <c r="AD13" s="26">
         <v>5.0</v>
       </c>
-      <c r="AE13" s="27">
+      <c r="AE13" s="26">
         <v>0.0</v>
       </c>
       <c r="AF13" s="26"/>
-      <c r="AG13" s="26"/>
+      <c r="AG13" s="27">
+        <v>0.0</v>
+      </c>
       <c r="AH13" s="26"/>
       <c r="AI13" s="26"/>
       <c r="AJ13" s="26"/>
@@ -2874,7 +2893,7 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
@@ -2882,7 +2901,7 @@
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
@@ -2890,7 +2909,7 @@
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
@@ -2898,7 +2917,7 @@
       </c>
       <c r="BF13" s="19">
         <f t="shared" si="7"/>
-        <v>0.4920634921</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG13" s="19"/>
     </row>
@@ -3109,7 +3128,9 @@
       <c r="AF15" s="27">
         <v>1.0</v>
       </c>
-      <c r="AG15" s="26"/>
+      <c r="AG15" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH15" s="26"/>
       <c r="AI15" s="26"/>
       <c r="AJ15" s="26"/>
@@ -3132,7 +3153,7 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
@@ -3140,7 +3161,7 @@
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BC15" s="5">
         <f t="shared" si="4"/>
@@ -3148,7 +3169,7 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
@@ -3156,7 +3177,7 @@
       </c>
       <c r="BF15" s="19">
         <f t="shared" si="7"/>
-        <v>0.4545454545</v>
+        <v>0.4492753623</v>
       </c>
       <c r="BG15" s="19"/>
     </row>
@@ -3359,7 +3380,9 @@
       <c r="AF17" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG17" s="26"/>
+      <c r="AG17" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH17" s="26"/>
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
@@ -3382,7 +3405,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -3390,7 +3413,7 @@
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
@@ -3398,7 +3421,7 @@
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
@@ -3406,7 +3429,7 @@
       </c>
       <c r="BF17" s="19">
         <f t="shared" si="7"/>
-        <v>0.4202898551</v>
+        <v>0.4166666667</v>
       </c>
       <c r="BG17" s="19"/>
     </row>
@@ -3491,7 +3514,9 @@
       <c r="AF18" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG18" s="26"/>
+      <c r="AG18" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH18" s="26"/>
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
@@ -3514,7 +3539,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3522,7 +3547,7 @@
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
@@ -3530,7 +3555,7 @@
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
@@ -3538,7 +3563,7 @@
       </c>
       <c r="BF18" s="19">
         <f t="shared" si="7"/>
-        <v>0.4202898551</v>
+        <v>0.4166666667</v>
       </c>
       <c r="BG18" s="19"/>
     </row>
@@ -3749,7 +3774,9 @@
       <c r="AF20" s="26">
         <v>1.0</v>
       </c>
-      <c r="AG20" s="26"/>
+      <c r="AG20" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH20" s="26"/>
       <c r="AI20" s="26"/>
       <c r="AJ20" s="26"/>
@@ -3772,7 +3799,7 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
@@ -3780,7 +3807,7 @@
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
@@ -3788,7 +3815,7 @@
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
@@ -3796,7 +3823,7 @@
       </c>
       <c r="BF20" s="19">
         <f t="shared" si="7"/>
-        <v>0.3888888889</v>
+        <v>0.3866666667</v>
       </c>
       <c r="BG20" s="19"/>
     </row>
@@ -4385,7 +4412,9 @@
       </c>
       <c r="AE26" s="26"/>
       <c r="AF26" s="26"/>
-      <c r="AG26" s="26"/>
+      <c r="AG26" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH26" s="26"/>
       <c r="AI26" s="26"/>
       <c r="AJ26" s="26"/>
@@ -4408,7 +4437,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -4416,7 +4445,7 @@
       </c>
       <c r="BB26" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
@@ -4424,7 +4453,7 @@
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
@@ -4432,7 +4461,7 @@
       </c>
       <c r="BF26" s="19">
         <f t="shared" si="7"/>
-        <v>0.4444444444</v>
+        <v>0.4333333333</v>
       </c>
       <c r="BG26" s="19"/>
     </row>
@@ -4595,7 +4624,9 @@
         <v>0.0</v>
       </c>
       <c r="AF28" s="26"/>
-      <c r="AG28" s="26"/>
+      <c r="AG28" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH28" s="26"/>
       <c r="AI28" s="26"/>
       <c r="AJ28" s="26"/>
@@ -4618,7 +4649,7 @@
       </c>
       <c r="AZ28" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA28" s="5">
         <f t="shared" si="2"/>
@@ -4626,7 +4657,7 @@
       </c>
       <c r="BB28" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC28" s="5">
         <f t="shared" si="4"/>
@@ -4634,7 +4665,7 @@
       </c>
       <c r="BD28" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BE28" s="5">
         <f t="shared" si="6"/>
@@ -4642,7 +4673,7 @@
       </c>
       <c r="BF28" s="19">
         <f t="shared" si="7"/>
-        <v>0.7777777778</v>
+        <v>0.6666666667</v>
       </c>
       <c r="BG28" s="19"/>
     </row>
@@ -5872,7 +5903,7 @@
       </c>
       <c r="AG41" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AH41" s="30">
         <f t="shared" si="8"/>
@@ -6039,7 +6070,9 @@
       <c r="AF42" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="AG42" s="5"/>
+      <c r="AG42" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="AH42" s="36"/>
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
@@ -26556,57 +26589,57 @@
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B11" s="39">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C11" s="39">
         <v>1.0</v>
       </c>
       <c r="D11" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="F11" s="39">
         <v>0.0</v>
-      </c>
-      <c r="E11" s="39">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="39">
-        <v>5.0</v>
       </c>
       <c r="G11" s="39">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="42"/>
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B12" s="39">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C12" s="39">
         <v>1.0</v>
       </c>
       <c r="D12" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="39">
         <v>0.0</v>
-      </c>
-      <c r="E12" s="39">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="39">
-        <v>3.0</v>
       </c>
       <c r="G12" s="39">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J12" s="42"/>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="39">
         <v>1.0</v>
@@ -26621,7 +26654,7 @@
         <v>0.0</v>
       </c>
       <c r="F13" s="39">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G13" s="39">
         <f t="shared" si="1"/>
@@ -26632,7 +26665,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="39">
         <v>1.0</v>
@@ -26647,7 +26680,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" s="39">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G14" s="39">
         <f t="shared" si="1"/>
@@ -26657,7 +26690,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="B15" s="39">
         <v>1.0</v>
@@ -26672,7 +26705,7 @@
         <v>0.0</v>
       </c>
       <c r="F15" s="39">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G15" s="39">
         <f t="shared" si="1"/>
@@ -26688,10 +26721,10 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B16" s="39">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C16" s="39">
         <v>1.0</v>
@@ -26700,10 +26733,10 @@
         <v>0.0</v>
       </c>
       <c r="E16" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F16" s="39">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G16" s="39">
         <f t="shared" si="1"/>
@@ -26715,15 +26748,15 @@
       </c>
       <c r="J16" s="42">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="B17" s="39">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C17" s="39">
         <v>1.0</v>
@@ -26732,10 +26765,10 @@
         <v>0.0</v>
       </c>
       <c r="E17" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F17" s="39">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G17" s="39">
         <f t="shared" si="1"/>
@@ -26746,12 +26779,12 @@
       </c>
       <c r="J17" s="42">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="32" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B18" s="39">
         <v>2.0</v>
@@ -28637,49 +28670,57 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="26"/>
+        <v>66</v>
+      </c>
+      <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="26">
+      <c r="D7" s="26"/>
+      <c r="E7" s="26">
         <v>1.0</v>
       </c>
-      <c r="E7" s="26"/>
       <c r="F7" s="26"/>
-      <c r="G7" s="26">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26">
         <v>1.0</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="J7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26">
+        <v>1.0</v>
+      </c>
       <c r="K7" s="25"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
+      <c r="M7" s="26">
+        <v>2.0</v>
+      </c>
       <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
+      <c r="O7" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
+      <c r="T7" s="26">
+        <v>1.0</v>
+      </c>
       <c r="U7" s="26"/>
       <c r="V7" s="26"/>
       <c r="W7" s="25"/>
       <c r="X7" s="26"/>
       <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
+      <c r="AA7" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AB7" s="26"/>
-      <c r="AC7" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AC7" s="26"/>
       <c r="AD7" s="26"/>
       <c r="AE7" s="26">
         <v>1.0</v>
       </c>
-      <c r="AF7" s="26"/>
+      <c r="AF7" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AG7" s="26"/>
       <c r="AH7" s="26"/>
       <c r="AI7" s="26"/>
@@ -28702,51 +28743,43 @@
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="BB7" s="5">
+        <v>12</v>
+      </c>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="25"/>
+        <v>74</v>
+      </c>
+      <c r="B8" s="26"/>
       <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26">
+      <c r="D8" s="26">
         <v>1.0</v>
       </c>
-      <c r="F8" s="26">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26">
         <v>1.0</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26">
+        <v>7.0</v>
+      </c>
       <c r="J8" s="26"/>
       <c r="K8" s="25"/>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
-      <c r="O8" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O8" s="26"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
-      <c r="R8" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="R8" s="26"/>
       <c r="S8" s="26"/>
-      <c r="T8" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="U8" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
       <c r="V8" s="26"/>
       <c r="W8" s="25"/>
       <c r="X8" s="26"/>
@@ -28754,7 +28787,9 @@
       <c r="Z8" s="26"/>
       <c r="AA8" s="26"/>
       <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
+      <c r="AC8" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AD8" s="26"/>
       <c r="AE8" s="26">
         <v>1.0</v>
@@ -28782,7 +28817,7 @@
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB8" s="5">
         <v>1.0</v>
@@ -28791,7 +28826,7 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="26"/>
@@ -28799,40 +28834,40 @@
       <c r="E9" s="26">
         <v>1.0</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="26">
+        <v>1.0</v>
+      </c>
       <c r="G9" s="26"/>
       <c r="H9" s="26">
         <v>1.0</v>
       </c>
       <c r="I9" s="26"/>
-      <c r="J9" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="J9" s="26"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
-      <c r="M9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="M9" s="26"/>
       <c r="N9" s="26"/>
       <c r="O9" s="26">
         <v>1.0</v>
       </c>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
+      <c r="R9" s="26">
+        <v>1.0</v>
+      </c>
       <c r="S9" s="26"/>
       <c r="T9" s="26">
         <v>1.0</v>
       </c>
-      <c r="U9" s="26"/>
+      <c r="U9" s="26">
+        <v>3.0</v>
+      </c>
       <c r="V9" s="26"/>
       <c r="W9" s="25"/>
       <c r="X9" s="26"/>
       <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
-      <c r="AA9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AA9" s="26"/>
       <c r="AB9" s="26"/>
       <c r="AC9" s="26"/>
       <c r="AD9" s="26"/>
@@ -28864,10 +28899,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="BB9" s="5"/>
-      <c r="BC9" s="5">
+      <c r="BB9" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
@@ -29685,7 +29720,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="26"/>
@@ -29693,9 +29728,7 @@
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="H21" s="26"/>
       <c r="I21" s="26">
         <v>1.0</v>
       </c>
@@ -29704,30 +29737,30 @@
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
-      <c r="O21" s="26">
+      <c r="O21" s="26"/>
+      <c r="P21" s="26">
         <v>1.0</v>
       </c>
-      <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
-      <c r="U21" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="25"/>
-      <c r="X21" s="26"/>
+      <c r="X21" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
       <c r="AA21" s="26"/>
-      <c r="AB21" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AB21" s="26"/>
       <c r="AC21" s="26"/>
       <c r="AD21" s="26"/>
       <c r="AE21" s="26"/>
-      <c r="AF21" s="26"/>
+      <c r="AF21" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AG21" s="26"/>
       <c r="AH21" s="26"/>
       <c r="AI21" s="26"/>
@@ -29753,50 +29786,54 @@
         <v>6</v>
       </c>
       <c r="BB21" s="5"/>
-      <c r="BC21" s="5"/>
+      <c r="BC21" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
-      <c r="G22" s="26">
+      <c r="G22" s="26"/>
+      <c r="H22" s="26">
         <v>1.0</v>
       </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="I22" s="26">
+        <v>1.0</v>
+      </c>
       <c r="J22" s="26"/>
       <c r="K22" s="25"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
+      <c r="O22" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
       <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
+      <c r="U22" s="26">
+        <v>1.0</v>
+      </c>
       <c r="V22" s="26"/>
       <c r="W22" s="25"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
-      <c r="Z22" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Z22" s="26"/>
       <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
+      <c r="AB22" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AC22" s="26"/>
       <c r="AD22" s="26"/>
-      <c r="AE22" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AE22" s="26"/>
       <c r="AF22" s="26"/>
       <c r="AG22" s="26"/>
       <c r="AH22" s="26"/>
@@ -29820,36 +29857,32 @@
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="BB22" s="5">
-        <v>1.0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="BB22" s="5"/>
       <c r="BC22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="C23" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="26">
+        <v>1.0</v>
+      </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
       <c r="K23" s="25"/>
-      <c r="L23" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="M23" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="N23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
@@ -29861,12 +29894,16 @@
       <c r="W23" s="25"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
+      <c r="Z23" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AA23" s="26"/>
       <c r="AB23" s="26"/>
       <c r="AC23" s="26"/>
       <c r="AD23" s="26"/>
-      <c r="AE23" s="26"/>
+      <c r="AE23" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AF23" s="26"/>
       <c r="AG23" s="26"/>
       <c r="AH23" s="26"/>
@@ -29892,41 +29929,41 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="BB23" s="5"/>
-      <c r="BC23" s="5">
+      <c r="BB23" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
-      <c r="D24" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
-      <c r="I24" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="I24" s="26"/>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
+      <c r="L24" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="M24" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="N24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="O24" s="26"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
-      <c r="R24" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="R24" s="26"/>
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
-      <c r="U24" s="46"/>
+      <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
       <c r="X24" s="26"/>
@@ -29969,16 +30006,20 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="D25" s="26">
+        <v>3.0</v>
+      </c>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="I25" s="26">
+        <v>1.0</v>
+      </c>
       <c r="J25" s="26"/>
       <c r="K25" s="25"/>
       <c r="L25" s="26"/>
@@ -29987,28 +30028,22 @@
       <c r="O25" s="26"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+      <c r="R25" s="26">
+        <v>1.0</v>
+      </c>
       <c r="S25" s="26"/>
       <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
+      <c r="U25" s="46"/>
       <c r="V25" s="26"/>
       <c r="W25" s="25"/>
       <c r="X25" s="26"/>
-      <c r="Y25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
-      <c r="AA25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AA25" s="26"/>
       <c r="AB25" s="26"/>
       <c r="AC25" s="26"/>
-      <c r="AD25" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AE25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AD25" s="26"/>
+      <c r="AE25" s="26"/>
       <c r="AF25" s="26"/>
       <c r="AG25" s="26"/>
       <c r="AH25" s="26"/>
@@ -30035,11 +30070,13 @@
         <v>5</v>
       </c>
       <c r="BB25" s="5"/>
-      <c r="BC25" s="5"/>
+      <c r="BC25" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
@@ -30066,14 +30103,16 @@
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
+      <c r="AA26" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AB26" s="26"/>
-      <c r="AC26" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AC26" s="26"/>
       <c r="AD26" s="26"/>
       <c r="AE26" s="26"/>
-      <c r="AF26" s="26"/>
+      <c r="AF26" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AG26" s="26"/>
       <c r="AH26" s="26"/>
       <c r="AI26" s="26"/>
@@ -30096,16 +30135,16 @@
       <c r="AZ26" s="6"/>
       <c r="BA26" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="BB26" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="32" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="26"/>
@@ -30120,9 +30159,7 @@
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
-      <c r="O27" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O27" s="26"/>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
       <c r="R27" s="26"/>
@@ -30133,14 +30170,20 @@
       <c r="W27" s="25"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
+      <c r="AA27" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AB27" s="26"/>
       <c r="AC27" s="26"/>
-      <c r="AD27" s="26"/>
-      <c r="AE27" s="26"/>
+      <c r="AD27" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AE27" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF27" s="26"/>
       <c r="AG27" s="26"/>
       <c r="AH27" s="26"/>
@@ -30164,16 +30207,14 @@
       <c r="AZ27" s="6"/>
       <c r="BA27" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BB27" s="5"/>
-      <c r="BC27" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BC27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="26"/>
@@ -30182,18 +30223,14 @@
       <c r="F28" s="26"/>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
-      <c r="I28" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="I28" s="26"/>
       <c r="J28" s="26"/>
       <c r="K28" s="25"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
-      <c r="P28" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
       <c r="R28" s="26"/>
       <c r="S28" s="26"/>
@@ -30201,14 +30238,14 @@
       <c r="U28" s="26"/>
       <c r="V28" s="26"/>
       <c r="W28" s="25"/>
-      <c r="X28" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
       <c r="Z28" s="26"/>
       <c r="AA28" s="26"/>
       <c r="AB28" s="26"/>
-      <c r="AC28" s="26"/>
+      <c r="AC28" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AD28" s="26"/>
       <c r="AE28" s="26"/>
       <c r="AF28" s="26"/>
@@ -30236,20 +30273,20 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="BB28" s="5"/>
+      <c r="BB28" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BC28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
-      <c r="F29" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="F29" s="26"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
@@ -30258,19 +30295,21 @@
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
+      <c r="O29" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
       <c r="S29" s="26"/>
       <c r="T29" s="26"/>
       <c r="U29" s="26"/>
-      <c r="V29" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="V29" s="26"/>
       <c r="W29" s="25"/>
       <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
+      <c r="Y29" s="26">
+        <v>2.0</v>
+      </c>
       <c r="Z29" s="26"/>
       <c r="AA29" s="26"/>
       <c r="AB29" s="26"/>
@@ -30300,22 +30339,24 @@
       <c r="AZ29" s="6"/>
       <c r="BA29" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB29" s="5"/>
-      <c r="BC29" s="5"/>
+      <c r="BC29" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="32" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="26">
+      <c r="E30" s="26"/>
+      <c r="F30" s="26">
         <v>1.0</v>
       </c>
-      <c r="F30" s="26"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -30331,14 +30372,14 @@
       <c r="S30" s="26"/>
       <c r="T30" s="26"/>
       <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
+      <c r="V30" s="26">
+        <v>1.0</v>
+      </c>
       <c r="W30" s="25"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
       <c r="Z30" s="26"/>
-      <c r="AA30" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AA30" s="26"/>
       <c r="AB30" s="26"/>
       <c r="AC30" s="26"/>
       <c r="AD30" s="26"/>
@@ -30373,12 +30414,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
+      <c r="E31" s="26">
+        <v>1.0</v>
+      </c>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
@@ -30401,7 +30444,7 @@
       <c r="Y31" s="26"/>
       <c r="Z31" s="26"/>
       <c r="AA31" s="26">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="AB31" s="26"/>
       <c r="AC31" s="26"/>
@@ -31089,7 +31132,7 @@
       </c>
       <c r="AG40" s="5">
         <f>'League Table'!AG41</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AH40" s="5">
         <f>'League Table'!AH41</f>
@@ -31317,7 +31360,7 @@
       </c>
       <c r="AF42" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG42" s="18">
         <f t="shared" si="2"/>
@@ -62373,7 +62416,9 @@
       <c r="AF5" s="16">
         <v>1.0</v>
       </c>
-      <c r="AG5" s="16"/>
+      <c r="AG5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AH5" s="16"/>
       <c r="AI5" s="16"/>
       <c r="AJ5" s="16"/>
@@ -62394,7 +62439,7 @@
       <c r="AY5" s="16"/>
       <c r="BA5" s="39">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -62464,7 +62509,9 @@
       <c r="AF6" s="30">
         <v>1.0</v>
       </c>
-      <c r="AG6" s="30"/>
+      <c r="AG6" s="30">
+        <v>1.0</v>
+      </c>
       <c r="AH6" s="30"/>
       <c r="AI6" s="30"/>
       <c r="AJ6" s="30"/>
@@ -62485,7 +62532,7 @@
       <c r="AY6" s="30"/>
       <c r="BA6" s="39">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -62912,7 +62959,9 @@
       <c r="AD12" s="30"/>
       <c r="AE12" s="30"/>
       <c r="AF12" s="30"/>
-      <c r="AG12" s="30"/>
+      <c r="AG12" s="30">
+        <v>1.0</v>
+      </c>
       <c r="AH12" s="30"/>
       <c r="AI12" s="30"/>
       <c r="AJ12" s="30"/>
@@ -62933,7 +62982,7 @@
       <c r="AY12" s="30"/>
       <c r="BA12" s="39">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -63044,7 +63093,9 @@
       <c r="AD14" s="26"/>
       <c r="AE14" s="26"/>
       <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
+      <c r="AG14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AH14" s="26"/>
       <c r="AI14" s="26"/>
       <c r="AJ14" s="26"/>
@@ -63065,7 +63116,7 @@
       <c r="AY14" s="26"/>
       <c r="BA14" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -64738,7 +64789,7 @@
       </c>
       <c r="AG41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH41" s="5">
         <f t="shared" si="2"/>
@@ -64814,7 +64865,7 @@
       </c>
       <c r="BA41" s="39">
         <f>SUM(B41:AZ41)</f>
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66756,10 +66807,18 @@
       <c r="A34" s="45">
         <v>32.0</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
+      <c r="B34" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>143</v>
+      </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="M34" s="5"/>

</xml_diff>

<commit_message>
078 Game week 33 update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oSTkFgWt7aUQ3XhcajXrZz4WuFO30v9b7CdS+AzNPMs="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="E2Ox0McbiBIfVGcGmfGy5CQRYFVKURrzWQrj4UT6cys="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="218">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -219,13 +219,16 @@
     <t>DOM</t>
   </si>
   <si>
+    <t>WILSON</t>
+  </si>
+  <si>
     <t>KERMIT</t>
   </si>
   <si>
     <t>IAN</t>
   </si>
   <si>
-    <t>WILSON</t>
+    <t>CARLOS</t>
   </si>
   <si>
     <t xml:space="preserve">MAMAS </t>
@@ -234,19 +237,16 @@
     <t>ARTIST</t>
   </si>
   <si>
+    <t>INSPECTOR GADGET</t>
+  </si>
+  <si>
     <t>CAPTAIN KIRK</t>
   </si>
   <si>
-    <t>CARLOS</t>
-  </si>
-  <si>
-    <t>INSPECTOR GADGET</t>
+    <t>PRESTON</t>
   </si>
   <si>
     <t>DWARF</t>
-  </si>
-  <si>
-    <t>PRESTON</t>
   </si>
   <si>
     <t>FLO</t>
@@ -258,13 +258,13 @@
     <t>TOY BOY</t>
   </si>
   <si>
+    <t>SONES</t>
+  </si>
+  <si>
     <t>KRYTON</t>
   </si>
   <si>
     <t>TUNDE</t>
-  </si>
-  <si>
-    <t>SONES</t>
   </si>
   <si>
     <t>BANKSY</t>
@@ -273,13 +273,13 @@
     <t>PHANTOM</t>
   </si>
   <si>
-    <t xml:space="preserve">STRAIGHT ROB </t>
+    <t>CHRIS B</t>
   </si>
   <si>
     <t>ELBOW</t>
   </si>
   <si>
-    <t>FRED</t>
+    <t xml:space="preserve">STRAIGHT ROB </t>
   </si>
   <si>
     <t>MOO</t>
@@ -291,7 +291,7 @@
     <t>CARZOLA</t>
   </si>
   <si>
-    <t>CHRIS B</t>
+    <t>CHARLIE</t>
   </si>
   <si>
     <t>DOGGER</t>
@@ -618,13 +618,13 @@
     <t>Dom - Kermit</t>
   </si>
   <si>
-    <t>S Rob</t>
-  </si>
-  <si>
     <t>Gadget - Mamas</t>
   </si>
   <si>
     <t>Lost 5-6</t>
+  </si>
+  <si>
+    <t>S Rob</t>
   </si>
   <si>
     <t>Banksy</t>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>Duncan - Wilson</t>
+  </si>
+  <si>
+    <t>Dom - Posh</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1788,9 @@
       <c r="AG5" s="16">
         <v>0.0</v>
       </c>
-      <c r="AH5" s="16"/>
+      <c r="AH5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AI5" s="16"/>
       <c r="AJ5" s="16"/>
       <c r="AK5" s="16"/>
@@ -1807,11 +1812,11 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
@@ -1823,15 +1828,15 @@
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BF5" s="19">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.5802469136</v>
+        <v>0.5952380952</v>
       </c>
       <c r="BG5" s="19"/>
     </row>
@@ -1919,7 +1924,9 @@
       <c r="AG6" s="22">
         <v>0.0</v>
       </c>
-      <c r="AH6" s="22"/>
+      <c r="AH6" s="23">
+        <v>2.0</v>
+      </c>
       <c r="AI6" s="22"/>
       <c r="AJ6" s="22"/>
       <c r="AK6" s="22"/>
@@ -1941,11 +1948,11 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB6" s="5">
         <f t="shared" si="3"/>
@@ -1957,15 +1964,15 @@
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BF6" s="19">
         <f t="shared" si="7"/>
-        <v>0.5972222222</v>
+        <v>0.6133333333</v>
       </c>
       <c r="BG6" s="19"/>
     </row>
@@ -2057,7 +2064,9 @@
       <c r="AG7" s="27">
         <v>0.0</v>
       </c>
-      <c r="AH7" s="26"/>
+      <c r="AH7" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI7" s="26"/>
       <c r="AJ7" s="26"/>
       <c r="AK7" s="26"/>
@@ -2079,11 +2088,11 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BB7" s="5">
         <f t="shared" si="3"/>
@@ -2095,15 +2104,15 @@
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BF7" s="19">
         <f t="shared" si="7"/>
-        <v>0.5128205128</v>
+        <v>0.5308641975</v>
       </c>
       <c r="BG7" s="19"/>
     </row>
@@ -2331,7 +2340,9 @@
         <v>1.0</v>
       </c>
       <c r="AG9" s="30"/>
-      <c r="AH9" s="30"/>
+      <c r="AH9" s="30">
+        <v>2.0</v>
+      </c>
       <c r="AI9" s="30"/>
       <c r="AJ9" s="30"/>
       <c r="AK9" s="30"/>
@@ -2353,11 +2364,11 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
@@ -2369,15 +2380,15 @@
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="BF9" s="19">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="BG9" s="19"/>
     </row>
@@ -2463,7 +2474,9 @@
       <c r="AG10" s="30">
         <v>0.0</v>
       </c>
-      <c r="AH10" s="30"/>
+      <c r="AH10" s="31">
+        <v>-2.0</v>
+      </c>
       <c r="AI10" s="30"/>
       <c r="AJ10" s="30"/>
       <c r="AK10" s="30"/>
@@ -2485,7 +2498,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2497,7 +2510,7 @@
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
@@ -2505,11 +2518,11 @@
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BF10" s="19">
         <f t="shared" si="7"/>
-        <v>0.5217391304</v>
+        <v>0.5</v>
       </c>
       <c r="BG10" s="19"/>
     </row>
@@ -2522,24 +2535,24 @@
         <v>1.0</v>
       </c>
       <c r="D11" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="E11" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G11" s="26">
         <v>3.0</v>
       </c>
-      <c r="E11" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="H11" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="I11" s="26">
         <v>-2.0</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="I11" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="J11" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="J11" s="26"/>
       <c r="K11" s="25"/>
       <c r="L11" s="26">
         <v>3.0</v>
@@ -2547,26 +2560,24 @@
       <c r="M11" s="26">
         <v>-1.0</v>
       </c>
-      <c r="N11" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="N11" s="26"/>
       <c r="O11" s="26">
         <v>1.0</v>
       </c>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="P11" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Q11" s="26"/>
       <c r="R11" s="26">
         <v>0.0</v>
       </c>
-      <c r="S11" s="26">
-        <v>-2.0</v>
+      <c r="S11" s="27">
+        <v>2.0</v>
       </c>
       <c r="T11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U11" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="U11" s="26">
         <v>0.0</v>
       </c>
       <c r="V11" s="26">
@@ -2574,34 +2585,30 @@
       </c>
       <c r="W11" s="25"/>
       <c r="X11" s="26"/>
-      <c r="Y11" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="Y11" s="26"/>
       <c r="Z11" s="26">
         <v>-2.0</v>
       </c>
       <c r="AA11" s="26">
         <v>3.0</v>
       </c>
-      <c r="AB11" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="AB11" s="26"/>
       <c r="AC11" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AD11" s="26">
-        <v>-5.0</v>
-      </c>
-      <c r="AE11" s="27">
+        <v>5.0</v>
+      </c>
+      <c r="AE11" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF11" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AG11" s="26">
+      <c r="AF11" s="26"/>
+      <c r="AG11" s="27">
         <v>0.0</v>
       </c>
-      <c r="AH11" s="26"/>
+      <c r="AH11" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
       <c r="AK11" s="26"/>
@@ -2623,7 +2630,7 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
@@ -2635,7 +2642,7 @@
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
@@ -2643,11 +2650,11 @@
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="BF11" s="19">
         <f t="shared" si="7"/>
-        <v>0.4487179487</v>
+        <v>0.5072463768</v>
       </c>
       <c r="BG11" s="19"/>
     </row>
@@ -2657,43 +2664,43 @@
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="D12" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="E12" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="27">
         <v>0.0</v>
       </c>
       <c r="F12" s="26">
         <v>-2.0</v>
       </c>
-      <c r="G12" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="G12" s="26"/>
       <c r="H12" s="26">
         <v>3.0</v>
       </c>
-      <c r="I12" s="27">
-        <v>-2.0</v>
+      <c r="I12" s="26">
+        <v>2.0</v>
       </c>
       <c r="J12" s="26">
         <v>2.0</v>
       </c>
       <c r="K12" s="25"/>
-      <c r="L12" s="26"/>
+      <c r="L12" s="26">
+        <v>3.0</v>
+      </c>
       <c r="M12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="N12" s="26">
         <v>-2.0</v>
       </c>
       <c r="O12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="P12" s="26"/>
-      <c r="Q12" s="27">
-        <v>-2.0</v>
+      <c r="Q12" s="26">
+        <v>2.0</v>
       </c>
       <c r="R12" s="26">
         <v>0.0</v>
@@ -2704,23 +2711,21 @@
       <c r="T12" s="26">
         <v>3.0</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="27">
         <v>0.0</v>
       </c>
       <c r="V12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="W12" s="25"/>
-      <c r="X12" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="X12" s="26"/>
       <c r="Y12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="Z12" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AA12" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="AA12" s="26">
         <v>3.0</v>
       </c>
       <c r="AB12" s="26">
@@ -2732,16 +2737,18 @@
       <c r="AD12" s="26">
         <v>-5.0</v>
       </c>
-      <c r="AE12" s="26">
+      <c r="AE12" s="27">
         <v>0.0</v>
       </c>
       <c r="AF12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AG12" s="26">
         <v>0.0</v>
       </c>
-      <c r="AH12" s="26"/>
+      <c r="AH12" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
       <c r="AK12" s="26"/>
@@ -2783,7 +2790,7 @@
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="BF12" s="19">
         <f t="shared" si="7"/>
@@ -2797,7 +2804,7 @@
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D13" s="26">
         <v>-3.0</v>
@@ -2806,69 +2813,79 @@
         <v>0.0</v>
       </c>
       <c r="F13" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="G13" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="H13" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="I13" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="J13" s="26">
         <v>2.0</v>
       </c>
-      <c r="G13" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="H13" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="I13" s="26">
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="N13" s="26">
         <v>-2.0</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M13" s="26">
+      <c r="O13" s="26">
         <v>-1.0</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="P13" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Q13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="R13" s="26">
         <v>0.0</v>
       </c>
-      <c r="S13" s="27">
-        <v>2.0</v>
+      <c r="S13" s="26">
+        <v>-2.0</v>
       </c>
       <c r="T13" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="U13" s="26">
         <v>0.0</v>
       </c>
       <c r="V13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="W13" s="25"/>
+      <c r="X13" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="Y13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Z13" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AA13" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AB13" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AC13" s="26">
         <v>-1.0</v>
       </c>
-      <c r="W13" s="25"/>
-      <c r="X13" s="26"/>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA13" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="26">
-        <v>1.0</v>
-      </c>
       <c r="AD13" s="26">
-        <v>5.0</v>
+        <v>-5.0</v>
       </c>
       <c r="AE13" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF13" s="26"/>
-      <c r="AG13" s="27">
+      <c r="AF13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AG13" s="26">
         <v>0.0</v>
       </c>
       <c r="AH13" s="26"/>
@@ -2893,11 +2910,11 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
@@ -2905,19 +2922,19 @@
       </c>
       <c r="BC13" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>-8</v>
       </c>
       <c r="BF13" s="19">
         <f t="shared" si="7"/>
-        <v>0.4848484848</v>
+        <v>0.4320987654</v>
       </c>
       <c r="BG13" s="19"/>
     </row>
@@ -2926,8 +2943,8 @@
         <v>68</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="27">
-        <v>-1.0</v>
+      <c r="C14" s="26">
+        <v>1.0</v>
       </c>
       <c r="D14" s="26">
         <v>3.0</v>
@@ -2935,11 +2952,11 @@
       <c r="E14" s="26">
         <v>0.0</v>
       </c>
-      <c r="F14" s="26">
-        <v>2.0</v>
+      <c r="F14" s="27">
+        <v>-2.0</v>
       </c>
       <c r="G14" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H14" s="26">
         <v>-3.0</v>
@@ -2951,55 +2968,63 @@
         <v>-2.0</v>
       </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="N14" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="O14" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="O14" s="27">
         <v>1.0</v>
       </c>
       <c r="P14" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q14" s="26">
-        <v>2.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="Q14" s="26"/>
       <c r="R14" s="26">
         <v>0.0</v>
       </c>
       <c r="S14" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="T14" s="26">
         <v>-3.0</v>
       </c>
-      <c r="U14" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V14" s="27">
-        <v>1.0</v>
-      </c>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
       <c r="W14" s="25"/>
       <c r="X14" s="26">
         <v>-2.0</v>
       </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26">
+      <c r="Y14" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Z14" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AA14" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="AB14" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AC14" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AD14" s="26">
+        <v>5.0</v>
+      </c>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AG14" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF14" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
+      <c r="AH14" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI14" s="26"/>
       <c r="AJ14" s="26"/>
       <c r="AK14" s="26"/>
@@ -3021,31 +3046,31 @@
       </c>
       <c r="AZ14" s="5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BC14" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="BF14" s="19">
         <f t="shared" si="7"/>
-        <v>0.4920634921</v>
+        <v>0.44</v>
       </c>
       <c r="BG14" s="19"/>
     </row>
@@ -3054,15 +3079,23 @@
         <v>69</v>
       </c>
       <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="C15" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="D15" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E15" s="26">
+        <v>0.0</v>
+      </c>
       <c r="F15" s="26">
         <v>2.0</v>
       </c>
-      <c r="G15" s="26"/>
+      <c r="G15" s="26">
+        <v>3.0</v>
+      </c>
       <c r="H15" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I15" s="26">
         <v>2.0</v>
@@ -3072,66 +3105,56 @@
       </c>
       <c r="K15" s="25"/>
       <c r="L15" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="M15" s="26"/>
-      <c r="N15" s="27">
+      <c r="N15" s="26">
         <v>-2.0</v>
       </c>
       <c r="O15" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" s="26">
         <v>1.0</v>
       </c>
       <c r="Q15" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="R15" s="26">
         <v>0.0</v>
       </c>
       <c r="S15" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="T15" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="U15" s="26">
         <v>0.0</v>
       </c>
-      <c r="V15" s="26">
+      <c r="V15" s="27">
         <v>1.0</v>
       </c>
       <c r="W15" s="25"/>
-      <c r="X15" s="27">
+      <c r="X15" s="26">
         <v>-2.0</v>
       </c>
       <c r="Y15" s="26"/>
-      <c r="Z15" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA15" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="AB15" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AC15" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AD15" s="26">
-        <v>-5.0</v>
-      </c>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
       <c r="AE15" s="26">
         <v>0.0</v>
       </c>
       <c r="AF15" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AG15" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="AH15" s="26"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI15" s="26"/>
       <c r="AJ15" s="26"/>
       <c r="AK15" s="26"/>
@@ -3153,7 +3176,7 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
@@ -3165,7 +3188,7 @@
       </c>
       <c r="BC15" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
@@ -3173,11 +3196,11 @@
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="BF15" s="19">
         <f t="shared" si="7"/>
-        <v>0.4492753623</v>
+        <v>0.4696969697</v>
       </c>
       <c r="BG15" s="19"/>
     </row>
@@ -3186,41 +3209,35 @@
         <v>70</v>
       </c>
       <c r="B16" s="25"/>
-      <c r="C16" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="D16" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E16" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="I16" s="26">
         <v>2.0</v>
       </c>
       <c r="J16" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M16" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="M16" s="26"/>
+      <c r="N16" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="O16" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="P16" s="26">
         <v>1.0</v>
-      </c>
-      <c r="N16" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="27">
-        <v>-1.0</v>
       </c>
       <c r="Q16" s="26">
         <v>-2.0</v>
@@ -3231,25 +3248,47 @@
       <c r="S16" s="26">
         <v>2.0</v>
       </c>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
+      <c r="T16" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="U16" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="V16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="W16" s="25"/>
-      <c r="X16" s="26"/>
+      <c r="X16" s="27">
+        <v>-2.0</v>
+      </c>
       <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
+      <c r="Z16" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AA16" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AB16" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AC16" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AD16" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AE16" s="26"/>
-      <c r="AF16" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AG16" s="26"/>
-      <c r="AH16" s="26"/>
+        <v>-5.0</v>
+      </c>
+      <c r="AE16" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AF16" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AG16" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AH16" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI16" s="26"/>
       <c r="AJ16" s="26"/>
       <c r="AK16" s="26"/>
@@ -3271,7 +3310,7 @@
       </c>
       <c r="AZ16" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="BA16" s="5">
         <f t="shared" si="2"/>
@@ -3279,23 +3318,23 @@
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BC16" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>-7</v>
       </c>
       <c r="BF16" s="19">
         <f t="shared" si="7"/>
-        <v>0.6041666667</v>
+        <v>0.4305555556</v>
       </c>
       <c r="BG16" s="19"/>
     </row>
@@ -3305,44 +3344,42 @@
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D17" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="G17" s="26">
         <v>3.0</v>
       </c>
-      <c r="E17" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="27">
+      <c r="H17" s="26"/>
+      <c r="I17" s="26">
         <v>-2.0</v>
       </c>
-      <c r="G17" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="H17" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="I17" s="26">
+      <c r="J17" s="26">
         <v>2.0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>-2.0</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="26"/>
-      <c r="M17" s="26">
-        <v>-1.0</v>
+      <c r="M17" s="27">
+        <v>1.0</v>
       </c>
       <c r="N17" s="26">
         <v>2.0</v>
       </c>
-      <c r="O17" s="27">
+      <c r="O17" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="P17" s="26">
         <v>1.0</v>
       </c>
-      <c r="P17" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Q17" s="26"/>
+      <c r="Q17" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="R17" s="26">
         <v>0.0</v>
       </c>
@@ -3350,32 +3387,34 @@
         <v>2.0</v>
       </c>
       <c r="T17" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
+        <v>3.0</v>
+      </c>
+      <c r="U17" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="V17" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="W17" s="25"/>
       <c r="X17" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y17" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="Z17" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AA17" s="27">
+      <c r="AA17" s="26">
         <v>-3.0</v>
       </c>
-      <c r="AB17" s="26">
-        <v>3.0</v>
+      <c r="AB17" s="27">
+        <v>-3.0</v>
       </c>
       <c r="AC17" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AD17" s="26">
-        <v>5.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="AD17" s="26"/>
       <c r="AE17" s="26"/>
       <c r="AF17" s="26">
         <v>-1.0</v>
@@ -3383,7 +3422,9 @@
       <c r="AG17" s="26">
         <v>0.0</v>
       </c>
-      <c r="AH17" s="26"/>
+      <c r="AH17" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
       <c r="AK17" s="26"/>
@@ -3405,7 +3446,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -3417,7 +3458,7 @@
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
@@ -3425,11 +3466,11 @@
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="BF17" s="19">
         <f t="shared" si="7"/>
-        <v>0.4166666667</v>
+        <v>0.4</v>
       </c>
       <c r="BG17" s="19"/>
     </row>
@@ -3438,39 +3479,41 @@
         <v>72</v>
       </c>
       <c r="B18" s="25"/>
-      <c r="C18" s="26">
-        <v>-1.0</v>
+      <c r="C18" s="27">
+        <v>1.0</v>
       </c>
       <c r="D18" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="E18" s="26"/>
+        <v>3.0</v>
+      </c>
+      <c r="E18" s="26">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="26">
         <v>-2.0</v>
       </c>
-      <c r="G18" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="H18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26">
+        <v>-3.0</v>
+      </c>
       <c r="I18" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J18" s="26">
         <v>2.0</v>
       </c>
       <c r="K18" s="25"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="27">
+      <c r="L18" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="M18" s="26">
         <v>1.0</v>
       </c>
       <c r="N18" s="26">
         <v>2.0</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="26"/>
+      <c r="P18" s="27">
         <v>-1.0</v>
-      </c>
-      <c r="P18" s="26">
-        <v>1.0</v>
       </c>
       <c r="Q18" s="26">
         <v>-2.0</v>
@@ -3481,42 +3524,24 @@
       <c r="S18" s="26">
         <v>2.0</v>
       </c>
-      <c r="T18" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U18" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V18" s="27">
-        <v>-1.0</v>
-      </c>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
       <c r="W18" s="25"/>
-      <c r="X18" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="Y18" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Z18" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA18" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="AB18" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AC18" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AD18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="26">
+        <v>5.0</v>
+      </c>
       <c r="AE18" s="26"/>
       <c r="AF18" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG18" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AG18" s="26"/>
       <c r="AH18" s="26"/>
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
@@ -3539,7 +3564,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3547,23 +3572,23 @@
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>12</v>
       </c>
       <c r="BF18" s="19">
         <f t="shared" si="7"/>
-        <v>0.4166666667</v>
+        <v>0.6041666667</v>
       </c>
       <c r="BG18" s="19"/>
     </row>
@@ -3573,35 +3598,41 @@
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="D19" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F19" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="G19" s="26">
         <v>-3.0</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27">
-        <v>3.0</v>
+      <c r="H19" s="26">
+        <v>-3.0</v>
       </c>
       <c r="I19" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J19" s="26">
         <v>2.0</v>
       </c>
       <c r="K19" s="25"/>
       <c r="L19" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M19" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="M19" s="27">
         <v>-1.0</v>
       </c>
       <c r="N19" s="26">
         <v>-2.0</v>
       </c>
       <c r="O19" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="P19" s="26">
         <v>-1.0</v>
@@ -3609,39 +3640,47 @@
       <c r="Q19" s="26">
         <v>2.0</v>
       </c>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="R19" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="S19" s="26"/>
       <c r="T19" s="26">
         <v>-3.0</v>
       </c>
-      <c r="U19" s="26"/>
+      <c r="U19" s="26">
+        <v>0.0</v>
+      </c>
       <c r="V19" s="26">
         <v>-1.0</v>
       </c>
       <c r="W19" s="25"/>
       <c r="X19" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="Y19" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="27">
         <v>1.0</v>
       </c>
-      <c r="Z19" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AA19" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="26"/>
+      <c r="AD19" s="26">
+        <v>5.0</v>
+      </c>
       <c r="AE19" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF19" s="26"/>
-      <c r="AG19" s="26"/>
-      <c r="AH19" s="26"/>
+      <c r="AF19" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AG19" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AH19" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI19" s="26"/>
       <c r="AJ19" s="26"/>
       <c r="AK19" s="26"/>
@@ -3663,31 +3702,31 @@
       </c>
       <c r="AZ19" s="5">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="BA19" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-9</v>
       </c>
       <c r="BF19" s="19">
         <f t="shared" si="7"/>
-        <v>0.4912280702</v>
+        <v>0.3717948718</v>
       </c>
       <c r="BG19" s="19"/>
     </row>
@@ -3697,41 +3736,35 @@
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27">
         <v>3.0</v>
       </c>
-      <c r="E20" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="26">
+      <c r="I20" s="26">
         <v>-2.0</v>
-      </c>
-      <c r="G20" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="H20" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="I20" s="26">
-        <v>2.0</v>
       </c>
       <c r="J20" s="26">
         <v>2.0</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="M20" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="M20" s="26">
         <v>-1.0</v>
       </c>
       <c r="N20" s="26">
         <v>-2.0</v>
       </c>
       <c r="O20" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="P20" s="26">
         <v>-1.0</v>
@@ -3739,44 +3772,38 @@
       <c r="Q20" s="26">
         <v>2.0</v>
       </c>
-      <c r="R20" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="S20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26">
+        <v>2.0</v>
+      </c>
       <c r="T20" s="26">
         <v>-3.0</v>
       </c>
-      <c r="U20" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="U20" s="26"/>
       <c r="V20" s="26">
         <v>-1.0</v>
       </c>
       <c r="W20" s="25"/>
       <c r="X20" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="Y20" s="26"/>
+        <v>2.0</v>
+      </c>
+      <c r="Y20" s="27">
+        <v>1.0</v>
+      </c>
       <c r="Z20" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA20" s="26"/>
+        <v>2.0</v>
+      </c>
+      <c r="AA20" s="26">
+        <v>-3.0</v>
+      </c>
       <c r="AB20" s="26"/>
-      <c r="AC20" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="AD20" s="26">
-        <v>5.0</v>
-      </c>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="26"/>
       <c r="AE20" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AG20" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="26"/>
       <c r="AH20" s="26"/>
       <c r="AI20" s="26"/>
       <c r="AJ20" s="26"/>
@@ -3799,31 +3826,31 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-7</v>
+        <v>1</v>
       </c>
       <c r="BF20" s="19">
         <f t="shared" si="7"/>
-        <v>0.3866666667</v>
+        <v>0.4912280702</v>
       </c>
       <c r="BG20" s="19"/>
     </row>
@@ -4009,7 +4036,9 @@
         <v>1.0</v>
       </c>
       <c r="AG22" s="26"/>
-      <c r="AH22" s="26"/>
+      <c r="AH22" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI22" s="26"/>
       <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
@@ -4031,7 +4060,7 @@
       </c>
       <c r="AZ22" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BA22" s="5">
         <f t="shared" si="2"/>
@@ -4043,7 +4072,7 @@
       </c>
       <c r="BC22" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BD22" s="5">
         <f t="shared" si="5"/>
@@ -4051,11 +4080,11 @@
       </c>
       <c r="BE22" s="5">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BF22" s="19">
         <f t="shared" si="7"/>
-        <v>0.5666666667</v>
+        <v>0.5151515152</v>
       </c>
       <c r="BG22" s="19"/>
     </row>
@@ -4165,57 +4194,59 @@
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
-      <c r="D24" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E24" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="26"/>
-      <c r="G24" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="H24" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="I24" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="M24" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
       <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
+      <c r="O24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P24" s="26">
         <v>1.0</v>
       </c>
       <c r="Q24" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="R24" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="S24" s="26"/>
+        <v>-2.0</v>
+      </c>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
       <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
+      <c r="Y24" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Z24" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AA24" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AB24" s="26">
+        <v>-3.0</v>
+      </c>
       <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
+      <c r="AD24" s="26">
+        <v>-5.0</v>
+      </c>
       <c r="AE24" s="26"/>
       <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
-      <c r="AH24" s="26"/>
+      <c r="AG24" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AH24" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
       <c r="AK24" s="26"/>
@@ -4237,31 +4268,31 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB24" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="BF24" s="19">
         <f t="shared" si="7"/>
-        <v>0.4666666667</v>
+        <v>0.4848484848</v>
       </c>
       <c r="BG24" s="19"/>
     </row>
@@ -4270,30 +4301,42 @@
         <v>79</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="C25" s="26"/>
       <c r="D25" s="26">
         <v>3.0</v>
       </c>
-      <c r="E25" s="26"/>
+      <c r="E25" s="26">
+        <v>0.0</v>
+      </c>
       <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="G25" s="26">
+        <v>3.0</v>
+      </c>
       <c r="H25" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I25" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J25" s="26"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
+      <c r="L25" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="M25" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="N25" s="26"/>
       <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+      <c r="P25" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Q25" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="R25" s="26">
+        <v>0.0</v>
+      </c>
       <c r="S25" s="26"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
@@ -4331,7 +4374,7 @@
       </c>
       <c r="AZ25" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
@@ -4339,23 +4382,23 @@
       </c>
       <c r="BB25" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BF25" s="19">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.4666666667</v>
       </c>
       <c r="BG25" s="19"/>
     </row>
@@ -4364,57 +4407,45 @@
         <v>80</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="C26" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="26">
+        <v>3.0</v>
+      </c>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
+      <c r="H26" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="I26" s="26">
+        <v>2.0</v>
+      </c>
       <c r="J26" s="26"/>
       <c r="K26" s="25"/>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
-      <c r="O26" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="P26" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q26" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
       <c r="R26" s="26"/>
-      <c r="S26" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="S26" s="26"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
       <c r="V26" s="26"/>
       <c r="W26" s="25"/>
       <c r="X26" s="26"/>
-      <c r="Y26" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Z26" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="AA26" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AB26" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
       <c r="AC26" s="26"/>
-      <c r="AD26" s="26">
-        <v>-5.0</v>
-      </c>
+      <c r="AD26" s="26"/>
       <c r="AE26" s="26"/>
       <c r="AF26" s="26"/>
-      <c r="AG26" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AG26" s="26"/>
       <c r="AH26" s="26"/>
       <c r="AI26" s="26"/>
       <c r="AJ26" s="26"/>
@@ -4437,7 +4468,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -4445,23 +4476,23 @@
       </c>
       <c r="BB26" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>9</v>
       </c>
       <c r="BF26" s="19">
         <f t="shared" si="7"/>
-        <v>0.4333333333</v>
+        <v>1</v>
       </c>
       <c r="BG26" s="19"/>
     </row>
@@ -4533,7 +4564,9 @@
         <v>-1.0</v>
       </c>
       <c r="AG27" s="26"/>
-      <c r="AH27" s="26"/>
+      <c r="AH27" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI27" s="26"/>
       <c r="AJ27" s="26"/>
       <c r="AK27" s="26"/>
@@ -4555,7 +4588,7 @@
       </c>
       <c r="AZ27" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BA27" s="5">
         <f t="shared" si="2"/>
@@ -4567,7 +4600,7 @@
       </c>
       <c r="BC27" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BD27" s="5">
         <f t="shared" si="5"/>
@@ -4575,11 +4608,11 @@
       </c>
       <c r="BE27" s="5">
         <f t="shared" si="6"/>
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="BF27" s="19">
         <f t="shared" si="7"/>
-        <v>0.2083333333</v>
+        <v>0.1960784314</v>
       </c>
       <c r="BG27" s="19"/>
     </row>
@@ -4682,28 +4715,18 @@
         <v>83</v>
       </c>
       <c r="B29" s="25"/>
-      <c r="C29" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
-      <c r="G29" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="26"/>
       <c r="K29" s="25"/>
-      <c r="L29" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="M29" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="N29" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
       <c r="O29" s="26"/>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
@@ -4714,16 +4737,28 @@
       <c r="V29" s="26"/>
       <c r="W29" s="25"/>
       <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
+      <c r="Y29" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
+      <c r="AA29" s="26">
+        <v>-3.0</v>
+      </c>
       <c r="AB29" s="26"/>
-      <c r="AC29" s="26"/>
-      <c r="AD29" s="26"/>
-      <c r="AE29" s="26"/>
+      <c r="AC29" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AD29" s="27">
+        <v>-5.0</v>
+      </c>
+      <c r="AE29" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AF29" s="26"/>
       <c r="AG29" s="26"/>
-      <c r="AH29" s="26"/>
+      <c r="AH29" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI29" s="26"/>
       <c r="AJ29" s="26"/>
       <c r="AK29" s="26"/>
@@ -4745,7 +4780,7 @@
       </c>
       <c r="AZ29" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BA29" s="5">
         <f t="shared" si="2"/>
@@ -4753,7 +4788,7 @@
       </c>
       <c r="BB29" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC29" s="5">
         <f t="shared" si="4"/>
@@ -4761,15 +4796,15 @@
       </c>
       <c r="BD29" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE29" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="BF29" s="19">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.3888888889</v>
       </c>
       <c r="BG29" s="19"/>
     </row>
@@ -4864,18 +4899,28 @@
         <v>85</v>
       </c>
       <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
+      <c r="C31" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="26">
+        <v>-3.0</v>
+      </c>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
+      <c r="L31" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="M31" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="N31" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="O31" s="26"/>
       <c r="P31" s="26"/>
       <c r="Q31" s="26"/>
@@ -4913,15 +4958,15 @@
       <c r="AW31" s="26"/>
       <c r="AX31" s="26"/>
       <c r="AY31" s="18">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="AZ31" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA31" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB31" s="5">
         <f t="shared" si="3"/>
@@ -4929,19 +4974,19 @@
       </c>
       <c r="BC31" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD31" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BE31" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BF31" s="19" t="str">
+        <v>-2</v>
+      </c>
+      <c r="BF31" s="19">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="BG31" s="19"/>
     </row>
@@ -5015,7 +5060,7 @@
       <c r="AW32" s="26"/>
       <c r="AX32" s="26"/>
       <c r="AY32" s="18">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="AZ32" s="5">
         <f t="shared" si="1"/>
@@ -5197,7 +5242,7 @@
       <c r="AW34" s="26"/>
       <c r="AX34" s="26"/>
       <c r="AY34" s="18">
-        <v>30.0</v>
+        <v>28.0</v>
       </c>
       <c r="AZ34" s="5">
         <f t="shared" si="1"/>
@@ -5256,26 +5301,18 @@
       <c r="V35" s="26"/>
       <c r="W35" s="25"/>
       <c r="X35" s="26"/>
-      <c r="Y35" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Y35" s="26"/>
       <c r="Z35" s="26"/>
-      <c r="AA35" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="AA35" s="26"/>
       <c r="AB35" s="26"/>
-      <c r="AC35" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AD35" s="27">
-        <v>-5.0</v>
-      </c>
-      <c r="AE35" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AC35" s="26"/>
+      <c r="AD35" s="26"/>
+      <c r="AE35" s="26"/>
       <c r="AF35" s="26"/>
       <c r="AG35" s="26"/>
-      <c r="AH35" s="26"/>
+      <c r="AH35" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AI35" s="26"/>
       <c r="AJ35" s="26"/>
       <c r="AK35" s="26"/>
@@ -5293,11 +5330,11 @@
       <c r="AW35" s="26"/>
       <c r="AX35" s="26"/>
       <c r="AY35" s="18">
-        <v>31.0</v>
+        <v>29.0</v>
       </c>
       <c r="AZ35" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BA35" s="5">
         <f t="shared" si="2"/>
@@ -5305,23 +5342,23 @@
       </c>
       <c r="BB35" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC35" s="5">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BD35" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BE35" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="BF35" s="19">
         <f t="shared" si="7"/>
-        <v>0.2666666667</v>
+        <v>1</v>
       </c>
       <c r="BG35" s="19"/>
     </row>
@@ -5381,7 +5418,7 @@
       <c r="AW36" s="26"/>
       <c r="AX36" s="26"/>
       <c r="AY36" s="18">
-        <v>32.0</v>
+        <v>30.3214285714286</v>
       </c>
       <c r="AZ36" s="5">
         <f t="shared" si="1"/>
@@ -5471,7 +5508,7 @@
       <c r="AW37" s="26"/>
       <c r="AX37" s="26"/>
       <c r="AY37" s="18">
-        <v>33.0</v>
+        <v>31.1071428571429</v>
       </c>
       <c r="AZ37" s="5">
         <f t="shared" si="1"/>
@@ -5561,7 +5598,7 @@
       <c r="AW38" s="26"/>
       <c r="AX38" s="26"/>
       <c r="AY38" s="18">
-        <v>34.0</v>
+        <v>31.8928571428571</v>
       </c>
       <c r="AZ38" s="5">
         <f t="shared" si="1"/>
@@ -5651,7 +5688,7 @@
       <c r="AW39" s="26"/>
       <c r="AX39" s="26"/>
       <c r="AY39" s="18">
-        <v>35.0</v>
+        <v>32.6785714285714</v>
       </c>
       <c r="AZ39" s="5">
         <f t="shared" si="1"/>
@@ -5723,7 +5760,9 @@
         <v>-1.0</v>
       </c>
       <c r="AG40" s="26"/>
-      <c r="AH40" s="26"/>
+      <c r="AH40" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AI40" s="26"/>
       <c r="AJ40" s="26"/>
       <c r="AK40" s="26"/>
@@ -5741,11 +5780,11 @@
       <c r="AW40" s="26"/>
       <c r="AX40" s="26"/>
       <c r="AY40" s="18">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="AZ40" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA40" s="5">
         <f t="shared" si="2"/>
@@ -5757,7 +5796,7 @@
       </c>
       <c r="BC40" s="5">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD40" s="5">
         <f t="shared" si="5"/>
@@ -5765,7 +5804,7 @@
       </c>
       <c r="BE40" s="5">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="BF40" s="19">
         <f t="shared" si="7"/>
@@ -5907,7 +5946,7 @@
       </c>
       <c r="AH41" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AI41" s="30">
         <f t="shared" si="8"/>
@@ -6073,7 +6112,9 @@
       <c r="AG42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AH42" s="36"/>
+      <c r="AH42" s="36" t="s">
+        <v>103</v>
+      </c>
       <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
       <c r="AK42" s="5"/>
@@ -26386,31 +26427,31 @@
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B4" s="41">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C4" s="41">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" s="41">
         <v>0.0</v>
       </c>
       <c r="E4" s="41">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" s="41">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G4" s="41">
         <f t="shared" ref="G4:G29" si="1">SUM(C4*3)+D4</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" s="39">
         <v>2.0</v>
@@ -26425,7 +26466,7 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="39">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G5" s="39">
         <f t="shared" si="1"/>
@@ -26434,10 +26475,10 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B6" s="39">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C6" s="39">
         <v>2.0</v>
@@ -26446,7 +26487,7 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" s="39">
         <v>3.0</v>
@@ -26460,12 +26501,13 @@
       </c>
       <c r="J6" s="42">
         <f t="shared" ref="J6:J10" si="2">I6/B6</f>
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="M6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="39">
         <v>3.0</v>
@@ -26493,13 +26535,14 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="M7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B8" s="39">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C8" s="39">
         <v>1.0</v>
@@ -26508,10 +26551,10 @@
         <v>1.0</v>
       </c>
       <c r="E8" s="39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F8" s="39">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" s="39">
         <f t="shared" si="1"/>
@@ -26522,12 +26565,12 @@
       </c>
       <c r="J8" s="42">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="14" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B9" s="41">
         <v>3.0</v>
@@ -26542,7 +26585,7 @@
         <v>1.0</v>
       </c>
       <c r="F9" s="41">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G9" s="41">
         <f t="shared" si="1"/>
@@ -26555,6 +26598,7 @@
         <f t="shared" si="2"/>
         <v>6.333333333</v>
       </c>
+      <c r="M9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
@@ -26586,10 +26630,11 @@
         <f t="shared" si="2"/>
         <v>6.333333333</v>
       </c>
+      <c r="M10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="39">
         <v>3.0</v>
@@ -26611,6 +26656,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="42"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
@@ -26636,6 +26682,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="42"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
@@ -26665,7 +26712,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" s="39">
         <v>1.0</v>
@@ -26784,7 +26831,7 @@
     </row>
     <row r="18">
       <c r="A18" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B18" s="39">
         <v>2.0</v>
@@ -26815,7 +26862,7 @@
     </row>
     <row r="19">
       <c r="A19" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="39">
         <v>3.0</v>
@@ -26846,7 +26893,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B20" s="39">
         <v>3.0</v>
@@ -26874,6 +26921,7 @@
         <f t="shared" si="3"/>
         <v>6.333333333</v>
       </c>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
@@ -26908,7 +26956,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="39">
         <v>3.0</v>
@@ -26936,10 +26984,11 @@
         <f t="shared" si="3"/>
         <v>4.666666667</v>
       </c>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="39">
         <v>3.0</v>
@@ -26967,10 +27016,11 @@
         <f t="shared" si="3"/>
         <v>8.333333333</v>
       </c>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" s="39">
         <v>3.0</v>
@@ -26998,6 +27048,7 @@
         <f t="shared" si="3"/>
         <v>1.666666667</v>
       </c>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
@@ -27029,10 +27080,11 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="39">
         <v>1.0</v>
@@ -27094,7 +27146,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B28" s="39">
         <v>1.0</v>
@@ -28428,7 +28480,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="30">
@@ -28590,56 +28642,60 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="D6" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E6" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26">
+        <v>1.0</v>
+      </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="H6" s="26">
+        <v>1.0</v>
+      </c>
       <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="J6" s="26">
+        <v>1.0</v>
+      </c>
       <c r="K6" s="25"/>
       <c r="L6" s="26"/>
       <c r="M6" s="26">
         <v>2.0</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="26"/>
+      <c r="O6" s="26">
         <v>1.0</v>
       </c>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26">
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26">
         <v>1.0</v>
       </c>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="S6" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="T6" s="26"/>
       <c r="U6" s="26"/>
       <c r="V6" s="26"/>
       <c r="W6" s="25"/>
       <c r="X6" s="26"/>
       <c r="Y6" s="26"/>
       <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
+      <c r="AA6" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AB6" s="26"/>
       <c r="AC6" s="26"/>
-      <c r="AD6" s="26">
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26">
         <v>1.0</v>
       </c>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
+      <c r="AF6" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AG6" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AH6" s="26"/>
       <c r="AI6" s="26"/>
       <c r="AJ6" s="26"/>
@@ -28661,66 +28717,64 @@
       <c r="AZ6" s="6"/>
       <c r="BA6" s="6">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB6" s="5"/>
       <c r="BC6" s="5">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26">
-        <v>1.0</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="26"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="H7" s="26"/>
       <c r="I7" s="26"/>
-      <c r="J7" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="J7" s="26"/>
       <c r="K7" s="25"/>
       <c r="L7" s="26"/>
       <c r="M7" s="26">
         <v>2.0</v>
       </c>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26">
+      <c r="N7" s="26">
         <v>1.0</v>
       </c>
-      <c r="P7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26">
+      <c r="R7" s="26">
         <v>1.0</v>
       </c>
+      <c r="S7" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T7" s="26"/>
       <c r="U7" s="26"/>
       <c r="V7" s="26"/>
       <c r="W7" s="25"/>
       <c r="X7" s="26"/>
       <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AA7" s="26"/>
       <c r="AB7" s="26"/>
       <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="26">
+      <c r="AD7" s="26">
         <v>1.0</v>
       </c>
-      <c r="AF7" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
       <c r="AG7" s="26"/>
       <c r="AH7" s="26"/>
       <c r="AI7" s="26"/>
@@ -28743,16 +28797,16 @@
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BB7" s="5"/>
       <c r="BC7" s="5">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -28906,7 +28960,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="26">
@@ -29058,54 +29112,52 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="E12" s="26"/>
       <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="G12" s="26">
+        <v>2.0</v>
+      </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26">
+      <c r="L12" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26">
         <v>1.0</v>
       </c>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
-      <c r="S12" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="S12" s="26"/>
       <c r="T12" s="26"/>
       <c r="U12" s="26"/>
       <c r="V12" s="26"/>
       <c r="W12" s="25"/>
-      <c r="X12" s="26">
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26">
         <v>1.0</v>
       </c>
-      <c r="Y12" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AB12" s="26"/>
       <c r="AC12" s="26"/>
       <c r="AD12" s="26"/>
       <c r="AE12" s="26">
         <v>1.0</v>
       </c>
       <c r="AF12" s="26"/>
-      <c r="AG12" s="26"/>
+      <c r="AG12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AH12" s="26"/>
       <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
@@ -29129,14 +29181,14 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="BB12" s="5"/>
-      <c r="BC12" s="5">
-        <v>2.0</v>
-      </c>
+      <c r="BB12" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="BC12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="26"/>
@@ -29144,38 +29196,44 @@
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
+      <c r="H13" s="26">
+        <v>2.0</v>
+      </c>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="25"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
-      <c r="O13" s="26">
+      <c r="O13" s="26"/>
+      <c r="P13" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26">
         <v>1.0</v>
       </c>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U13" s="26"/>
+      <c r="S13" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="V13" s="26"/>
       <c r="W13" s="25"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
       <c r="Z13" s="26"/>
-      <c r="AA13" s="26">
-        <v>4.0</v>
-      </c>
+      <c r="AA13" s="26"/>
       <c r="AB13" s="26"/>
       <c r="AC13" s="26"/>
       <c r="AD13" s="26"/>
       <c r="AE13" s="26"/>
       <c r="AF13" s="26"/>
-      <c r="AG13" s="26"/>
+      <c r="AG13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AH13" s="26"/>
       <c r="AI13" s="26"/>
       <c r="AJ13" s="26"/>
@@ -29197,55 +29255,57 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="BB13" s="5">
-        <v>2.0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="BB13" s="5"/>
       <c r="BC13" s="5">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="BF13" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="B14" s="25"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="E14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="F14" s="26"/>
-      <c r="G14" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="N14" s="26"/>
-      <c r="O14" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O14" s="26"/>
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
+      <c r="S14" s="26">
+        <v>2.0</v>
+      </c>
       <c r="T14" s="26"/>
       <c r="U14" s="26"/>
       <c r="V14" s="26"/>
       <c r="W14" s="25"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
+      <c r="X14" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Y14" s="26">
+        <v>2.0</v>
+      </c>
       <c r="Z14" s="26"/>
-      <c r="AA14" s="26">
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26">
         <v>1.0</v>
       </c>
-      <c r="AB14" s="26"/>
       <c r="AC14" s="26"/>
       <c r="AD14" s="26"/>
       <c r="AE14" s="26">
@@ -29274,16 +29334,16 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="BB14" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC14" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="BB14" s="5"/>
+      <c r="BC14" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="26"/>
@@ -29291,36 +29351,32 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="H15" s="26"/>
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
       <c r="K15" s="25"/>
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="O15" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
-      <c r="R15" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="S15" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="U15" s="26"/>
       <c r="V15" s="26"/>
       <c r="W15" s="25"/>
       <c r="X15" s="26"/>
       <c r="Y15" s="26"/>
       <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
+      <c r="AA15" s="26">
+        <v>4.0</v>
+      </c>
       <c r="AB15" s="26"/>
       <c r="AC15" s="26"/>
       <c r="AD15" s="26"/>
@@ -29350,9 +29406,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="BB15" s="5"/>
+      <c r="BB15" s="5">
+        <v>2.0</v>
+      </c>
       <c r="BC15" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -29648,7 +29706,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -29864,7 +29922,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="26">
@@ -29936,7 +29994,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
@@ -29948,16 +30006,12 @@
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="M24" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="N24" s="26">
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26">
         <v>1.0</v>
       </c>
-      <c r="O24" s="26"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
       <c r="R24" s="26"/>
@@ -29967,7 +30021,9 @@
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
       <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
+      <c r="Y24" s="26">
+        <v>2.0</v>
+      </c>
       <c r="Z24" s="26"/>
       <c r="AA24" s="26"/>
       <c r="AB24" s="26"/>
@@ -29975,7 +30031,9 @@
       <c r="AD24" s="26"/>
       <c r="AE24" s="26"/>
       <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
+      <c r="AG24" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AH24" s="26"/>
       <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
@@ -30001,39 +30059,39 @@
       </c>
       <c r="BB24" s="5"/>
       <c r="BC24" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="26"/>
-      <c r="D25" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
-      <c r="I25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="I25" s="26"/>
       <c r="J25" s="26"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
+      <c r="L25" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="M25" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="N25" s="26">
+        <v>1.0</v>
+      </c>
       <c r="O25" s="26"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="R25" s="26"/>
       <c r="S25" s="26"/>
       <c r="T25" s="26"/>
-      <c r="U25" s="46"/>
+      <c r="U25" s="26"/>
       <c r="V25" s="26"/>
       <c r="W25" s="25"/>
       <c r="X25" s="26"/>
@@ -30076,16 +30134,20 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="26">
+        <v>3.0</v>
+      </c>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
+      <c r="I26" s="26">
+        <v>1.0</v>
+      </c>
       <c r="J26" s="26"/>
       <c r="K26" s="25"/>
       <c r="L26" s="26"/>
@@ -30094,25 +30156,23 @@
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>
       <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
+      <c r="R26" s="26">
+        <v>1.0</v>
+      </c>
       <c r="S26" s="26"/>
       <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
+      <c r="U26" s="46"/>
       <c r="V26" s="26"/>
       <c r="W26" s="25"/>
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
-      <c r="AA26" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AA26" s="26"/>
       <c r="AB26" s="26"/>
       <c r="AC26" s="26"/>
       <c r="AD26" s="26"/>
       <c r="AE26" s="26"/>
-      <c r="AF26" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AF26" s="26"/>
       <c r="AG26" s="26"/>
       <c r="AH26" s="26"/>
       <c r="AI26" s="26"/>
@@ -30144,7 +30204,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="32" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="26"/>
@@ -30169,22 +30229,18 @@
       <c r="V27" s="26"/>
       <c r="W27" s="25"/>
       <c r="X27" s="26"/>
-      <c r="Y27" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
       <c r="AA27" s="26">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="AB27" s="26"/>
       <c r="AC27" s="26"/>
-      <c r="AD27" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AE27" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AF27" s="26"/>
+      <c r="AD27" s="26"/>
+      <c r="AE27" s="26"/>
+      <c r="AF27" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AG27" s="26"/>
       <c r="AH27" s="26"/>
       <c r="AI27" s="26"/>
@@ -30210,11 +30266,13 @@
         <v>5</v>
       </c>
       <c r="BB27" s="5"/>
-      <c r="BC27" s="5"/>
+      <c r="BC27" s="5">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="26"/>
@@ -30239,15 +30297,21 @@
       <c r="V28" s="26"/>
       <c r="W28" s="25"/>
       <c r="X28" s="26"/>
-      <c r="Y28" s="26"/>
+      <c r="Y28" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Z28" s="26"/>
-      <c r="AA28" s="26"/>
+      <c r="AA28" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AB28" s="26"/>
-      <c r="AC28" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AD28" s="26"/>
-      <c r="AE28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AE28" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF28" s="26"/>
       <c r="AG28" s="26"/>
       <c r="AH28" s="26"/>
@@ -30271,16 +30335,14 @@
       <c r="AZ28" s="6"/>
       <c r="BA28" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="BB28" s="5">
-        <v>1.0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BB28" s="5"/>
       <c r="BC28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -30295,9 +30357,7 @@
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
-      <c r="O29" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O29" s="26"/>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
@@ -30307,13 +30367,13 @@
       <c r="V29" s="26"/>
       <c r="W29" s="25"/>
       <c r="X29" s="26"/>
-      <c r="Y29" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="Y29" s="26"/>
       <c r="Z29" s="26"/>
       <c r="AA29" s="26"/>
       <c r="AB29" s="26"/>
-      <c r="AC29" s="26"/>
+      <c r="AC29" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AD29" s="26"/>
       <c r="AE29" s="26"/>
       <c r="AF29" s="26"/>
@@ -30341,10 +30401,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="BB29" s="5"/>
-      <c r="BC29" s="5">
+      <c r="BB29" s="5">
         <v>1.0</v>
       </c>
+      <c r="BC29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="32" t="s">
@@ -30544,7 +30604,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="26"/>
@@ -30890,9 +30950,15 @@
       <c r="AG37" s="48">
         <v>45881.0</v>
       </c>
-      <c r="AH37" s="49"/>
-      <c r="AI37" s="49"/>
-      <c r="AJ37" s="49"/>
+      <c r="AH37" s="48">
+        <v>45888.0</v>
+      </c>
+      <c r="AI37" s="48">
+        <v>45895.0</v>
+      </c>
+      <c r="AJ37" s="48">
+        <v>45902.0</v>
+      </c>
       <c r="AK37" s="49"/>
       <c r="AL37" s="49"/>
       <c r="AM37" s="49"/>
@@ -31136,7 +31202,7 @@
       </c>
       <c r="AH40" s="5">
         <f>'League Table'!AH41</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AI40" s="5">
         <f>'League Table'!AI41</f>
@@ -31239,7 +31305,7 @@
         <v>131</v>
       </c>
       <c r="B42" s="18">
-        <f t="shared" ref="B42:AG42" si="2">SUM(B3:B36)</f>
+        <f t="shared" ref="B42:AJ42" si="2">SUM(B3:B36)</f>
         <v>0</v>
       </c>
       <c r="C42" s="18">
@@ -31364,22 +31430,22 @@
       </c>
       <c r="AG42" s="18">
         <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AH42" s="18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH42" s="6">
-        <f t="shared" ref="AH42:AV42" si="3">SUM(AH4:AH38)</f>
+      <c r="AI42" s="18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI42" s="6">
-        <f t="shared" si="3"/>
+      <c r="AJ42" s="18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ42" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="AK42" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AK42:AV42" si="3">SUM(AK4:AK38)</f>
         <v>0</v>
       </c>
       <c r="AL42" s="6">
@@ -62444,7 +62510,7 @@
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -62841,7 +62907,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -62914,7 +62980,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -62987,7 +63053,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -63031,7 +63097,9 @@
       <c r="AE13" s="26"/>
       <c r="AF13" s="26"/>
       <c r="AG13" s="26"/>
-      <c r="AH13" s="26"/>
+      <c r="AH13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AI13" s="26"/>
       <c r="AJ13" s="26"/>
       <c r="AK13" s="26"/>
@@ -63051,7 +63119,7 @@
       <c r="AY13" s="26"/>
       <c r="BA13" s="39">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -63184,19 +63252,15 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B16" s="26"/>
-      <c r="C16" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="H16" s="26"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
@@ -63218,11 +63282,15 @@
       <c r="AA16" s="26"/>
       <c r="AB16" s="26"/>
       <c r="AC16" s="26"/>
-      <c r="AD16" s="26"/>
+      <c r="AD16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AE16" s="26"/>
       <c r="AF16" s="26"/>
       <c r="AG16" s="26"/>
-      <c r="AH16" s="26"/>
+      <c r="AH16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AI16" s="26"/>
       <c r="AJ16" s="26"/>
       <c r="AK16" s="26"/>
@@ -63247,21 +63315,23 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+      <c r="C17" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
+      <c r="H17" s="26">
+        <v>1.0</v>
+      </c>
       <c r="I17" s="26"/>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
-      <c r="L17" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
@@ -63303,12 +63373,12 @@
       <c r="AY17" s="26"/>
       <c r="BA17" s="39">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="32" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -63369,7 +63439,7 @@
     </row>
     <row r="19">
       <c r="A19" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -63381,7 +63451,9 @@
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+      <c r="L19" s="26">
+        <v>1.0</v>
+      </c>
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
@@ -63399,9 +63471,7 @@
       <c r="AA19" s="26"/>
       <c r="AB19" s="26"/>
       <c r="AC19" s="26"/>
-      <c r="AD19" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AD19" s="26"/>
       <c r="AE19" s="26"/>
       <c r="AF19" s="26"/>
       <c r="AG19" s="26"/>
@@ -63430,7 +63500,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -63674,7 +63744,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -63735,7 +63805,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -63853,7 +63923,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -64089,7 +64159,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
@@ -64266,7 +64336,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -64443,7 +64513,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
@@ -64793,7 +64863,7 @@
       </c>
       <c r="AH41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI41" s="5">
         <f t="shared" si="2"/>
@@ -64865,7 +64935,7 @@
       </c>
       <c r="BA41" s="39">
         <f>SUM(B41:AZ41)</f>
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66095,10 +66165,10 @@
       </c>
       <c r="G11" s="45"/>
       <c r="H11" s="5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="I11" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>176</v>
@@ -66110,7 +66180,7 @@
         <v>148</v>
       </c>
       <c r="N11" s="5">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="12">
@@ -66131,7 +66201,7 @@
       </c>
       <c r="G12" s="45"/>
       <c r="H12" s="5" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="I12" s="5">
         <v>4.0</v>
@@ -66216,10 +66286,10 @@
         <v>2.0</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="N14" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15">
@@ -66250,7 +66320,7 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N15" s="5">
         <v>4.0</v>
@@ -66284,7 +66354,7 @@
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="N16" s="5">
         <v>4.0</v>
@@ -66318,7 +66388,7 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="N17" s="5">
         <v>4.0</v>
@@ -66352,7 +66422,7 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="N18" s="5">
         <v>4.0</v>
@@ -66444,9 +66514,11 @@
       </c>
       <c r="G21" s="45"/>
       <c r="H21" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I21" s="5"/>
+        <v>189</v>
+      </c>
+      <c r="I21" s="5">
+        <v>2.0</v>
+      </c>
       <c r="K21" s="5" t="s">
         <v>171</v>
       </c>
@@ -66476,7 +66548,7 @@
       </c>
       <c r="G22" s="45"/>
       <c r="H22" s="5" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
       <c r="I22" s="5"/>
       <c r="K22" s="5" t="s">
@@ -66495,10 +66567,10 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>199</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>200</v>
       </c>
       <c r="D23" s="45" t="s">
         <v>180</v>
@@ -66508,7 +66580,7 @@
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="5" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="I23" s="5"/>
       <c r="K23" s="5" t="s">
@@ -66540,7 +66612,7 @@
       </c>
       <c r="G24" s="45"/>
       <c r="H24" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I24" s="5"/>
       <c r="K24" s="5" t="s">
@@ -66572,7 +66644,7 @@
       </c>
       <c r="G25" s="45"/>
       <c r="H25" s="5" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="I25" s="5"/>
       <c r="K25" s="5" t="s">
@@ -66607,7 +66679,9 @@
         <v>196</v>
       </c>
       <c r="I26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="K26" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
         <v>203</v>
@@ -66639,10 +66713,10 @@
       <c r="I27" s="5"/>
       <c r="K27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="N27" s="57">
-        <v>1.0</v>
+        <v>189</v>
+      </c>
+      <c r="N27" s="5">
+        <v>2.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -66668,7 +66742,7 @@
       <c r="I28" s="5"/>
       <c r="K28" s="5"/>
       <c r="M28" s="5" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="N28" s="57">
         <v>1.0</v>
@@ -66694,7 +66768,7 @@
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="N29" s="57">
         <v>1.0</v>
@@ -66720,7 +66794,7 @@
       <c r="I30" s="5"/>
       <c r="K30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="N30" s="57">
         <v>1.0</v>
@@ -66828,10 +66902,18 @@
       <c r="A35" s="45">
         <v>33.0</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
+      <c r="B35" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>154</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="M35" s="5"/>

</xml_diff>

<commit_message>
083 Game week 38 update
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="/Pp+ozo03evYlou6yoD5gsDlZNBRXeQ/1Lr+yorJtuk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="EEodVdc5IGuKlN969ht/aakT3X6mHD8ZL0qnZqerYBs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="228">
   <si>
     <t>MARLOW DUKES 2025</t>
   </si>
@@ -201,16 +201,19 @@
     <t>%</t>
   </si>
   <si>
-    <t>ZIGZAG</t>
+    <t>POSH CHRIS</t>
   </si>
   <si>
-    <t>POSH CHRIS</t>
+    <t>ZIGZAG</t>
   </si>
   <si>
     <t>BRUCE</t>
   </si>
   <si>
     <t>DUNCAN</t>
+  </si>
+  <si>
+    <t>FATHER TED</t>
   </si>
   <si>
     <t>IAN</t>
@@ -220,9 +223,6 @@
   </si>
   <si>
     <t>CARLOS</t>
-  </si>
-  <si>
-    <t>FATHER TED</t>
   </si>
   <si>
     <t>KERMIT</t>
@@ -237,16 +237,16 @@
     <t>WILSON</t>
   </si>
   <si>
+    <t xml:space="preserve">MAMAS </t>
+  </si>
+  <si>
+    <t>PRESTON</t>
+  </si>
+  <si>
     <t>DWARF</t>
   </si>
   <si>
-    <t xml:space="preserve">MAMAS </t>
-  </si>
-  <si>
     <t>INSPECTOR GADGET</t>
-  </si>
-  <si>
-    <t>PRESTON</t>
   </si>
   <si>
     <t>CAPTAIN KIRK</t>
@@ -258,13 +258,13 @@
     <t>SONES</t>
   </si>
   <si>
+    <t>KRYTON</t>
+  </si>
+  <si>
     <t>TOY BOY</t>
   </si>
   <si>
     <t>PHANTOM</t>
-  </si>
-  <si>
-    <t>KRYTON</t>
   </si>
   <si>
     <t>BANKSY</t>
@@ -543,10 +543,10 @@
     <t>ZigZag</t>
   </si>
   <si>
-    <t>Preston</t>
+    <t>Carlos</t>
   </si>
   <si>
-    <t>Carlos</t>
+    <t>Preston</t>
   </si>
   <si>
     <t>Duncan - Dom</t>
@@ -663,6 +663,9 @@
     <t>Gadget - Father Ted</t>
   </si>
   <si>
+    <t>Phantom</t>
+  </si>
+  <si>
     <t>Banksy - Preston</t>
   </si>
   <si>
@@ -700,6 +703,9 @@
   </si>
   <si>
     <t>Tango - Bruce</t>
+  </si>
+  <si>
+    <t>Ian - Father Ted</t>
   </si>
 </sst>
 </file>
@@ -1729,40 +1735,40 @@
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16">
-        <v>-1.0</v>
-      </c>
-      <c r="D5" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="G5" s="17">
         <v>3.0</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="16">
-        <v>-2.0</v>
-      </c>
-      <c r="G5" s="16">
-        <v>-3.0</v>
       </c>
       <c r="H5" s="16">
         <v>-3.0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="16"/>
+      <c r="J5" s="16">
         <v>-2.0</v>
       </c>
-      <c r="J5" s="16"/>
       <c r="K5" s="15"/>
       <c r="L5" s="16">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="M5" s="16">
         <v>1.0</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="O5" s="16">
         <v>1.0</v>
       </c>
-      <c r="P5" s="16">
-        <v>-1.0</v>
+      <c r="P5" s="17">
+        <v>1.0</v>
       </c>
       <c r="Q5" s="16">
         <v>2.0</v>
@@ -1770,41 +1776,35 @@
       <c r="R5" s="16">
         <v>0.0</v>
       </c>
-      <c r="S5" s="17">
-        <v>-2.0</v>
+      <c r="S5" s="16">
+        <v>2.0</v>
       </c>
       <c r="T5" s="16">
         <v>3.0</v>
       </c>
-      <c r="U5" s="16">
-        <v>0.0</v>
-      </c>
+      <c r="U5" s="16"/>
       <c r="V5" s="16">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="W5" s="15"/>
-      <c r="X5" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="Y5" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="Z5" s="16">
-        <v>2.0</v>
-      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="17">
+        <v>-1.0</v>
+      </c>
+      <c r="Z5" s="16"/>
       <c r="AA5" s="16">
         <v>3.0</v>
       </c>
       <c r="AB5" s="16">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AC5" s="16">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AD5" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="AE5" s="17">
+        <v>-5.0</v>
+      </c>
+      <c r="AE5" s="16">
         <v>0.0</v>
       </c>
       <c r="AF5" s="16">
@@ -1813,22 +1813,22 @@
       <c r="AG5" s="16">
         <v>0.0</v>
       </c>
-      <c r="AH5" s="16">
+      <c r="AH5" s="17">
         <v>2.0</v>
       </c>
       <c r="AI5" s="16">
         <v>3.0</v>
       </c>
-      <c r="AJ5" s="16">
-        <v>-3.0</v>
-      </c>
+      <c r="AJ5" s="16"/>
       <c r="AK5" s="16">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AL5" s="16">
         <v>-1.0</v>
       </c>
-      <c r="AM5" s="16"/>
+      <c r="AM5" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16"/>
@@ -1845,31 +1845,31 @@
       </c>
       <c r="AZ5" s="5">
         <f t="shared" ref="AZ5:AZ40" si="1">COUNT(B5:AX5)</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="BA5" s="5">
         <f t="shared" ref="BA5:BA40" si="2">COUNTIF($B5:$AX5, "&gt;=1")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BB5" s="5">
         <f t="shared" ref="BB5:BB40" si="3">COUNTIF($B5:$AX5, "0")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC5" s="5">
         <f t="shared" ref="BC5:BC40" si="4">COUNTIF($B5:$AX5, "&lt;0")</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BD5" s="5">
         <f t="shared" ref="BD5:BD40" si="5">SUM(BA5*3)+BB5</f>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="BE5" s="5">
         <f t="shared" ref="BE5:BE40" si="6">SUM(B5:AX5)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BF5" s="19">
         <f t="shared" ref="BF5:BF40" si="7">SUM(BA5*3+BB5*1)/SUM(AZ5*3)</f>
-        <v>0.5520833333</v>
+        <v>0.632183908</v>
       </c>
       <c r="BG5" s="19"/>
     </row>
@@ -1879,40 +1879,40 @@
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+        <v>-1.0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="23">
         <v>0.0</v>
       </c>
       <c r="F6" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="G6" s="23">
-        <v>3.0</v>
+        <v>-2.0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>-3.0</v>
       </c>
       <c r="H6" s="22">
         <v>-3.0</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22">
+      <c r="I6" s="22">
         <v>-2.0</v>
       </c>
+      <c r="J6" s="22"/>
       <c r="K6" s="21"/>
       <c r="L6" s="22">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="M6" s="22">
         <v>1.0</v>
       </c>
-      <c r="N6" s="22">
-        <v>2.0</v>
-      </c>
+      <c r="N6" s="22"/>
       <c r="O6" s="22">
         <v>1.0</v>
       </c>
-      <c r="P6" s="23">
-        <v>1.0</v>
+      <c r="P6" s="22">
+        <v>-1.0</v>
       </c>
       <c r="Q6" s="22">
         <v>2.0</v>
@@ -1920,35 +1920,41 @@
       <c r="R6" s="22">
         <v>0.0</v>
       </c>
-      <c r="S6" s="22">
-        <v>2.0</v>
+      <c r="S6" s="23">
+        <v>-2.0</v>
       </c>
       <c r="T6" s="22">
         <v>3.0</v>
       </c>
-      <c r="U6" s="22"/>
+      <c r="U6" s="22">
+        <v>0.0</v>
+      </c>
       <c r="V6" s="22">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="W6" s="21"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="23">
-        <v>-1.0</v>
-      </c>
-      <c r="Z6" s="22"/>
+      <c r="X6" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>2.0</v>
+      </c>
       <c r="AA6" s="22">
         <v>3.0</v>
       </c>
       <c r="AB6" s="22">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="AC6" s="22">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AD6" s="22">
-        <v>-5.0</v>
-      </c>
-      <c r="AE6" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="AE6" s="23">
         <v>0.0</v>
       </c>
       <c r="AF6" s="22">
@@ -1957,20 +1963,24 @@
       <c r="AG6" s="22">
         <v>0.0</v>
       </c>
-      <c r="AH6" s="23">
+      <c r="AH6" s="22">
         <v>2.0</v>
       </c>
       <c r="AI6" s="22">
         <v>3.0</v>
       </c>
-      <c r="AJ6" s="22"/>
+      <c r="AJ6" s="22">
+        <v>-3.0</v>
+      </c>
       <c r="AK6" s="22">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AL6" s="22">
         <v>-1.0</v>
       </c>
-      <c r="AM6" s="22"/>
+      <c r="AM6" s="22">
+        <v>-1.0</v>
+      </c>
       <c r="AN6" s="22"/>
       <c r="AO6" s="22"/>
       <c r="AP6" s="22"/>
@@ -1987,7 +1997,7 @@
       </c>
       <c r="AZ6" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="BA6" s="5">
         <f t="shared" si="2"/>
@@ -1995,23 +2005,23 @@
       </c>
       <c r="BB6" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC6" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BD6" s="5">
         <f t="shared" si="5"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BE6" s="5">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BF6" s="19">
         <f t="shared" si="7"/>
-        <v>0.619047619</v>
+        <v>0.5353535354</v>
       </c>
       <c r="BG6" s="19"/>
     </row>
@@ -2118,7 +2128,9 @@
       <c r="AL7" s="27">
         <v>1.0</v>
       </c>
-      <c r="AM7" s="26"/>
+      <c r="AM7" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN7" s="26"/>
       <c r="AO7" s="26"/>
       <c r="AP7" s="26"/>
@@ -2135,7 +2147,7 @@
       </c>
       <c r="AZ7" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA7" s="5">
         <f t="shared" si="2"/>
@@ -2147,7 +2159,7 @@
       </c>
       <c r="BC7" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD7" s="5">
         <f t="shared" si="5"/>
@@ -2155,11 +2167,11 @@
       </c>
       <c r="BE7" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="19">
         <f t="shared" si="7"/>
-        <v>0.5268817204</v>
+        <v>0.5104166667</v>
       </c>
       <c r="BG7" s="19"/>
     </row>
@@ -2266,7 +2278,9 @@
       <c r="AL8" s="16">
         <v>-1.0</v>
       </c>
-      <c r="AM8" s="16"/>
+      <c r="AM8" s="16">
+        <v>-1.0</v>
+      </c>
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
@@ -2283,7 +2297,7 @@
       </c>
       <c r="AZ8" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BA8" s="5">
         <f t="shared" si="2"/>
@@ -2295,7 +2309,7 @@
       </c>
       <c r="BC8" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BD8" s="5">
         <f t="shared" si="5"/>
@@ -2303,11 +2317,11 @@
       </c>
       <c r="BE8" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF8" s="19">
         <f t="shared" si="7"/>
-        <v>0.4946236559</v>
+        <v>0.4791666667</v>
       </c>
       <c r="BG8" s="19"/>
     </row>
@@ -2316,9 +2330,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="29"/>
-      <c r="C9" s="30">
-        <v>-1.0</v>
-      </c>
+      <c r="C9" s="30"/>
       <c r="D9" s="30">
         <v>-3.0</v>
       </c>
@@ -2328,20 +2340,22 @@
       <c r="F9" s="30">
         <v>-2.0</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="31">
         <v>-3.0</v>
       </c>
       <c r="H9" s="30">
         <v>3.0</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <v>-2.0</v>
       </c>
       <c r="J9" s="30">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K9" s="29"/>
-      <c r="L9" s="30"/>
+      <c r="L9" s="30">
+        <v>-3.0</v>
+      </c>
       <c r="M9" s="30">
         <v>1.0</v>
       </c>
@@ -2349,13 +2363,13 @@
         <v>-2.0</v>
       </c>
       <c r="O9" s="30">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="P9" s="30"/>
-      <c r="Q9" s="31">
+      <c r="Q9" s="30">
         <v>-2.0</v>
       </c>
-      <c r="R9" s="30">
+      <c r="R9" s="31">
         <v>0.0</v>
       </c>
       <c r="S9" s="30">
@@ -2377,44 +2391,40 @@
       <c r="Y9" s="30">
         <v>1.0</v>
       </c>
-      <c r="Z9" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AA9" s="31">
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30">
         <v>3.0</v>
       </c>
-      <c r="AB9" s="30">
-        <v>-3.0</v>
+      <c r="AB9" s="31">
+        <v>3.0</v>
       </c>
       <c r="AC9" s="30">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AD9" s="30">
         <v>-5.0</v>
       </c>
-      <c r="AE9" s="30">
-        <v>0.0</v>
-      </c>
+      <c r="AE9" s="30"/>
       <c r="AF9" s="30">
         <v>1.0</v>
       </c>
-      <c r="AG9" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="AI9" s="30"/>
       <c r="AJ9" s="30">
         <v>3.0</v>
       </c>
       <c r="AK9" s="30">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AL9" s="30">
         <v>-1.0</v>
       </c>
-      <c r="AM9" s="30"/>
+      <c r="AM9" s="31">
+        <v>1.0</v>
+      </c>
       <c r="AN9" s="30"/>
       <c r="AO9" s="30"/>
       <c r="AP9" s="30"/>
@@ -2431,23 +2441,23 @@
       </c>
       <c r="AZ9" s="5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="BA9" s="5">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BB9" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BC9" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BD9" s="5">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="BE9" s="5">
         <f t="shared" si="6"/>
@@ -2455,7 +2465,7 @@
       </c>
       <c r="BF9" s="19">
         <f t="shared" si="7"/>
-        <v>0.4731182796</v>
+        <v>0.5172413793</v>
       </c>
       <c r="BG9" s="19"/>
     </row>
@@ -2465,14 +2475,16 @@
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="30">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D10" s="30">
         <v>-3.0</v>
       </c>
-      <c r="E10" s="30"/>
+      <c r="E10" s="30">
+        <v>0.0</v>
+      </c>
       <c r="F10" s="30">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G10" s="30">
         <v>-3.0</v>
@@ -2480,79 +2492,89 @@
       <c r="H10" s="30">
         <v>3.0</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="31">
+        <v>-2.0</v>
+      </c>
+      <c r="J10" s="30">
         <v>2.0</v>
       </c>
-      <c r="J10" s="31">
-        <v>2.0</v>
-      </c>
       <c r="K10" s="29"/>
-      <c r="L10" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="L10" s="30"/>
       <c r="M10" s="30">
         <v>1.0</v>
       </c>
       <c r="N10" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="O10" s="26">
         <v>-1.0</v>
       </c>
-      <c r="P10" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q10" s="26">
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27">
         <v>-2.0</v>
       </c>
       <c r="R10" s="30">
         <v>0.0</v>
       </c>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="31">
+      <c r="S10" s="30">
+        <v>-2.0</v>
+      </c>
+      <c r="T10" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="U10" s="30">
         <v>0.0</v>
       </c>
-      <c r="V10" s="30"/>
+      <c r="V10" s="30">
+        <v>1.0</v>
+      </c>
       <c r="W10" s="29"/>
       <c r="X10" s="30">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y10" s="30">
-        <v>-1.0</v>
-      </c>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30">
-        <v>-3.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="Z10" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="AA10" s="31">
+        <v>3.0</v>
       </c>
       <c r="AB10" s="30">
         <v>-3.0</v>
       </c>
       <c r="AC10" s="30">
+        <v>-1.0</v>
+      </c>
+      <c r="AD10" s="30">
+        <v>-5.0</v>
+      </c>
+      <c r="AE10" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="AF10" s="30">
         <v>1.0</v>
-      </c>
-      <c r="AD10" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30">
-        <v>-1.0</v>
       </c>
       <c r="AG10" s="30">
         <v>0.0</v>
       </c>
-      <c r="AH10" s="31">
-        <v>-2.0</v>
-      </c>
+      <c r="AH10" s="30"/>
       <c r="AI10" s="30">
         <v>3.0</v>
       </c>
       <c r="AJ10" s="30">
         <v>3.0</v>
       </c>
-      <c r="AK10" s="30"/>
-      <c r="AL10" s="30"/>
-      <c r="AM10" s="30"/>
+      <c r="AK10" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AL10" s="30">
+        <v>-1.0</v>
+      </c>
+      <c r="AM10" s="31">
+        <v>-1.0</v>
+      </c>
       <c r="AN10" s="30"/>
       <c r="AO10" s="30"/>
       <c r="AP10" s="30"/>
@@ -2569,7 +2591,7 @@
       </c>
       <c r="AZ10" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BA10" s="5">
         <f t="shared" si="2"/>
@@ -2577,23 +2599,23 @@
       </c>
       <c r="BB10" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BC10" s="5">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BD10" s="5">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BE10" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="BF10" s="19">
         <f t="shared" si="7"/>
-        <v>0.5384615385</v>
+        <v>0.4583333333</v>
       </c>
       <c r="BG10" s="19"/>
     </row>
@@ -2606,70 +2628,68 @@
         <v>1.0</v>
       </c>
       <c r="D11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E11" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="27">
-        <v>-2.0</v>
+        <v>-3.0</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26">
+        <v>2.0</v>
       </c>
       <c r="G11" s="26">
         <v>-3.0</v>
       </c>
       <c r="H11" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="I11" s="26">
         <v>2.0</v>
       </c>
-      <c r="J11" s="26">
-        <v>-2.0</v>
+      <c r="J11" s="27">
+        <v>2.0</v>
       </c>
       <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="L11" s="26">
+        <v>3.0</v>
+      </c>
       <c r="M11" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N11" s="26">
         <v>2.0</v>
       </c>
-      <c r="O11" s="27">
+      <c r="O11" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="P11" s="26">
         <v>1.0</v>
       </c>
-      <c r="P11" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="Q11" s="26"/>
+      <c r="Q11" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="R11" s="26">
         <v>0.0</v>
       </c>
-      <c r="S11" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="T11" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="U11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="27">
+        <v>0.0</v>
+      </c>
       <c r="V11" s="26"/>
       <c r="W11" s="25"/>
       <c r="X11" s="26">
         <v>-2.0</v>
       </c>
       <c r="Y11" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AB11" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AC11" s="26">
         <v>1.0</v>
-      </c>
-      <c r="Z11" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AA11" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AB11" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AC11" s="26">
-        <v>-1.0</v>
       </c>
       <c r="AD11" s="26">
         <v>5.0</v>
@@ -2681,21 +2701,17 @@
       <c r="AG11" s="26">
         <v>0.0</v>
       </c>
-      <c r="AH11" s="26">
-        <v>2.0</v>
+      <c r="AH11" s="27">
+        <v>-2.0</v>
       </c>
       <c r="AI11" s="26">
         <v>3.0</v>
       </c>
-      <c r="AJ11" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AK11" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AL11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ11" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="26"/>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
@@ -2713,7 +2729,7 @@
       </c>
       <c r="AZ11" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="BA11" s="5">
         <f t="shared" si="2"/>
@@ -2725,7 +2741,7 @@
       </c>
       <c r="BC11" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BD11" s="5">
         <f t="shared" si="5"/>
@@ -2733,11 +2749,11 @@
       </c>
       <c r="BE11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BF11" s="19">
         <f t="shared" si="7"/>
-        <v>0.4827586207</v>
+        <v>0.5384615385</v>
       </c>
       <c r="BG11" s="19"/>
     </row>
@@ -2746,97 +2762,99 @@
         <v>66</v>
       </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D12" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="E12" s="26">
         <v>0.0</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="27">
         <v>-2.0</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>-3.0</v>
       </c>
       <c r="H12" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I12" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="J12" s="26">
         <v>-2.0</v>
       </c>
       <c r="K12" s="25"/>
-      <c r="L12" s="26">
+      <c r="L12" s="26"/>
+      <c r="M12" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="N12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="O12" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="P12" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="S12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T12" s="26">
         <v>-3.0</v>
       </c>
-      <c r="M12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="N12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="O12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="R12" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="S12" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="T12" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U12" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
       <c r="W12" s="25"/>
       <c r="X12" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="Y12" s="26">
         <v>1.0</v>
       </c>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26">
+      <c r="Z12" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AA12" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="AB12" s="26">
         <v>3.0</v>
       </c>
-      <c r="AB12" s="27">
-        <v>3.0</v>
-      </c>
       <c r="AC12" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AD12" s="26">
-        <v>-5.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE12" s="26"/>
       <c r="AF12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AG12" s="26"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AG12" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH12" s="26">
         <v>2.0</v>
       </c>
-      <c r="AI12" s="26"/>
-      <c r="AJ12" s="26">
+      <c r="AI12" s="26">
         <v>3.0</v>
       </c>
+      <c r="AJ12" s="27">
+        <v>-3.0</v>
+      </c>
       <c r="AK12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AL12" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="AM12" s="26"/>
       <c r="AN12" s="26"/>
@@ -2855,7 +2873,7 @@
       </c>
       <c r="AZ12" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="BA12" s="5">
         <f t="shared" si="2"/>
@@ -2867,7 +2885,7 @@
       </c>
       <c r="BC12" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD12" s="5">
         <f t="shared" si="5"/>
@@ -2875,11 +2893,11 @@
       </c>
       <c r="BE12" s="5">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="BF12" s="19">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4827586207</v>
       </c>
       <c r="BG12" s="19"/>
     </row>
@@ -2982,7 +3000,9 @@
       </c>
       <c r="AK13" s="26"/>
       <c r="AL13" s="26"/>
-      <c r="AM13" s="26"/>
+      <c r="AM13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN13" s="26"/>
       <c r="AO13" s="26"/>
       <c r="AP13" s="26"/>
@@ -2999,11 +3019,11 @@
       </c>
       <c r="AZ13" s="5">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BA13" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB13" s="5">
         <f t="shared" si="3"/>
@@ -3015,15 +3035,15 @@
       </c>
       <c r="BD13" s="5">
         <f t="shared" si="5"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="BE13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="19">
         <f t="shared" si="7"/>
-        <v>0.4367816092</v>
+        <v>0.4555555556</v>
       </c>
       <c r="BG13" s="19"/>
     </row>
@@ -3120,7 +3140,9 @@
       </c>
       <c r="AK14" s="26"/>
       <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
+      <c r="AM14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN14" s="26"/>
       <c r="AO14" s="26"/>
       <c r="AP14" s="26"/>
@@ -3137,11 +3159,11 @@
       </c>
       <c r="AZ14" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA14" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB14" s="5">
         <f t="shared" si="3"/>
@@ -3153,15 +3175,15 @@
       </c>
       <c r="BD14" s="5">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="BE14" s="5">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="19">
         <f t="shared" si="7"/>
-        <v>0.4743589744</v>
+        <v>0.4938271605</v>
       </c>
       <c r="BG14" s="19"/>
     </row>
@@ -3252,7 +3274,9 @@
       <c r="AL15" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM15" s="26"/>
+      <c r="AM15" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN15" s="26"/>
       <c r="AO15" s="26"/>
       <c r="AP15" s="26"/>
@@ -3269,11 +3293,11 @@
       </c>
       <c r="AZ15" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BA15" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB15" s="5">
         <f t="shared" si="3"/>
@@ -3285,15 +3309,15 @@
       </c>
       <c r="BD15" s="5">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="BE15" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BF15" s="19">
         <f t="shared" si="7"/>
-        <v>0.5217391304</v>
+        <v>0.5416666667</v>
       </c>
       <c r="BG15" s="19"/>
     </row>
@@ -3390,7 +3414,9 @@
         <v>-1.0</v>
       </c>
       <c r="AL16" s="26"/>
-      <c r="AM16" s="26"/>
+      <c r="AM16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN16" s="26"/>
       <c r="AO16" s="26"/>
       <c r="AP16" s="26"/>
@@ -3407,11 +3433,11 @@
       </c>
       <c r="AZ16" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BA16" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB16" s="5">
         <f t="shared" si="3"/>
@@ -3423,15 +3449,15 @@
       </c>
       <c r="BD16" s="5">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="BE16" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF16" s="19">
         <f t="shared" si="7"/>
-        <v>0.4487179487</v>
+        <v>0.4691358025</v>
       </c>
       <c r="BG16" s="19"/>
     </row>
@@ -3440,31 +3466,35 @@
         <v>71</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="26">
+      <c r="C17" s="27">
         <v>-1.0</v>
       </c>
       <c r="D17" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G17" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="26">
         <v>-3.0</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27">
-        <v>3.0</v>
-      </c>
       <c r="I17" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="J17" s="26">
         <v>-2.0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>2.0</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="26">
         <v>3.0</v>
       </c>
-      <c r="M17" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="M17" s="26"/>
       <c r="N17" s="26">
         <v>-2.0</v>
       </c>
@@ -3472,53 +3502,61 @@
         <v>1.0</v>
       </c>
       <c r="P17" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q17" s="26">
         <v>2.0</v>
       </c>
-      <c r="R17" s="26"/>
+      <c r="R17" s="26">
+        <v>0.0</v>
+      </c>
       <c r="S17" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="T17" s="26">
         <v>-3.0</v>
       </c>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26">
-        <v>-1.0</v>
+      <c r="U17" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="V17" s="27">
+        <v>1.0</v>
       </c>
       <c r="W17" s="25"/>
       <c r="X17" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="Y17" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="Z17" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AA17" s="26">
-        <v>-3.0</v>
-      </c>
+        <v>-2.0</v>
+      </c>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
       <c r="AD17" s="26"/>
       <c r="AE17" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF17" s="26"/>
+      <c r="AF17" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="AG17" s="26"/>
-      <c r="AH17" s="26"/>
-      <c r="AI17" s="27">
+      <c r="AH17" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="AI17" s="26">
         <v>3.0</v>
       </c>
-      <c r="AJ17" s="26"/>
-      <c r="AK17" s="26"/>
+      <c r="AJ17" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AK17" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AL17" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AM17" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM17" s="26"/>
       <c r="AN17" s="26"/>
       <c r="AO17" s="26"/>
       <c r="AP17" s="26"/>
@@ -3535,7 +3573,7 @@
       </c>
       <c r="AZ17" s="5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="BA17" s="5">
         <f t="shared" si="2"/>
@@ -3543,23 +3581,23 @@
       </c>
       <c r="BB17" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BC17" s="5">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BD17" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="BE17" s="5">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="BF17" s="19">
         <f t="shared" si="7"/>
-        <v>0.5396825397</v>
+        <v>0.4567901235</v>
       </c>
       <c r="BG17" s="19"/>
     </row>
@@ -3568,20 +3606,20 @@
         <v>72</v>
       </c>
       <c r="B18" s="25"/>
-      <c r="C18" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="C18" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="27">
         <v>3.0</v>
       </c>
       <c r="E18" s="26">
         <v>0.0</v>
       </c>
       <c r="F18" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G18" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H18" s="26">
         <v>-3.0</v>
@@ -3590,21 +3628,23 @@
         <v>2.0</v>
       </c>
       <c r="J18" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="M18" s="26"/>
+        <v>-3.0</v>
+      </c>
+      <c r="M18" s="27">
+        <v>-1.0</v>
+      </c>
       <c r="N18" s="26">
         <v>-2.0</v>
       </c>
       <c r="O18" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="P18" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="Q18" s="26">
         <v>2.0</v>
@@ -3612,40 +3652,46 @@
       <c r="R18" s="26">
         <v>0.0</v>
       </c>
-      <c r="S18" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="S18" s="26"/>
       <c r="T18" s="26">
         <v>-3.0</v>
       </c>
       <c r="U18" s="26">
         <v>0.0</v>
       </c>
-      <c r="V18" s="27">
-        <v>1.0</v>
+      <c r="V18" s="26">
+        <v>-1.0</v>
       </c>
       <c r="W18" s="25"/>
       <c r="X18" s="26">
         <v>-2.0</v>
       </c>
       <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
+      <c r="Z18" s="26">
+        <v>-2.0</v>
+      </c>
       <c r="AA18" s="26"/>
       <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="26"/>
+      <c r="AC18" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="AD18" s="26">
+        <v>5.0</v>
+      </c>
       <c r="AE18" s="26">
         <v>0.0</v>
       </c>
-      <c r="AF18" s="27">
-        <v>-1.0</v>
-      </c>
-      <c r="AG18" s="26"/>
+      <c r="AF18" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AG18" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH18" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AI18" s="26">
-        <v>3.0</v>
+      <c r="AI18" s="27">
+        <v>-3.0</v>
       </c>
       <c r="AJ18" s="26">
         <v>-3.0</v>
@@ -3654,9 +3700,11 @@
         <v>-1.0</v>
       </c>
       <c r="AL18" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM18" s="26"/>
+        <v>1.0</v>
+      </c>
+      <c r="AM18" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN18" s="26"/>
       <c r="AO18" s="26"/>
       <c r="AP18" s="26"/>
@@ -3673,7 +3721,7 @@
       </c>
       <c r="AZ18" s="5">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="BA18" s="5">
         <f t="shared" si="2"/>
@@ -3681,23 +3729,23 @@
       </c>
       <c r="BB18" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BC18" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="BD18" s="5">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="BE18" s="5">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-14</v>
       </c>
       <c r="BF18" s="19">
         <f t="shared" si="7"/>
-        <v>0.4358974359</v>
+        <v>0.376344086</v>
       </c>
       <c r="BG18" s="19"/>
     </row>
@@ -3713,13 +3761,11 @@
         <v>-3.0</v>
       </c>
       <c r="E19" s="26"/>
-      <c r="F19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="G19" s="26">
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27">
         <v>3.0</v>
       </c>
-      <c r="H19" s="26"/>
       <c r="I19" s="26">
         <v>-2.0</v>
       </c>
@@ -3727,78 +3773,68 @@
         <v>2.0</v>
       </c>
       <c r="K19" s="25"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27">
+      <c r="L19" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="M19" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="N19" s="26">
+        <v>-2.0</v>
+      </c>
+      <c r="O19" s="26">
         <v>1.0</v>
       </c>
-      <c r="N19" s="26">
+      <c r="P19" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="Q19" s="26">
         <v>2.0</v>
       </c>
-      <c r="O19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="R19" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="R19" s="26"/>
       <c r="S19" s="26">
         <v>2.0</v>
       </c>
       <c r="T19" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U19" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="V19" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26">
         <v>-1.0</v>
       </c>
       <c r="W19" s="25"/>
       <c r="X19" s="26">
         <v>2.0</v>
       </c>
-      <c r="Y19" s="26">
-        <v>-1.0</v>
+      <c r="Y19" s="27">
+        <v>1.0</v>
       </c>
       <c r="Z19" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="AA19" s="26">
         <v>-3.0</v>
       </c>
-      <c r="AB19" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="AC19" s="26">
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26">
         <v>1.0</v>
       </c>
-      <c r="AD19" s="26"/>
-      <c r="AE19" s="26"/>
-      <c r="AF19" s="26">
+      <c r="AM19" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AG19" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="AH19" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AK19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AL19" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM19" s="26"/>
       <c r="AN19" s="26"/>
       <c r="AO19" s="26"/>
       <c r="AP19" s="26"/>
@@ -3815,31 +3851,31 @@
       </c>
       <c r="AZ19" s="5">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="BA19" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB19" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BC19" s="5">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="BD19" s="5">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BE19" s="5">
         <f t="shared" si="6"/>
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="BF19" s="19">
         <f t="shared" si="7"/>
-        <v>0.3928571429</v>
+        <v>0.5151515152</v>
       </c>
       <c r="BG19" s="19"/>
     </row>
@@ -3849,82 +3885,80 @@
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="E20" s="26">
-        <v>0.0</v>
-      </c>
+        <v>-1.0</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="E20" s="26"/>
       <c r="F20" s="26">
         <v>-2.0</v>
       </c>
       <c r="G20" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="H20" s="26">
-        <v>-3.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="H20" s="26"/>
       <c r="I20" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J20" s="26">
         <v>2.0</v>
       </c>
       <c r="K20" s="25"/>
-      <c r="L20" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="L20" s="26"/>
       <c r="M20" s="27">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="N20" s="26">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="O20" s="26">
         <v>-1.0</v>
       </c>
       <c r="P20" s="26">
-        <v>-1.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q20" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="R20" s="26">
         <v>0.0</v>
       </c>
-      <c r="S20" s="26"/>
+      <c r="S20" s="26">
+        <v>2.0</v>
+      </c>
       <c r="T20" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="U20" s="26">
         <v>0.0</v>
       </c>
-      <c r="V20" s="26">
+      <c r="V20" s="27">
         <v>-1.0</v>
       </c>
       <c r="W20" s="25"/>
       <c r="X20" s="26">
-        <v>-2.0</v>
-      </c>
-      <c r="Y20" s="26"/>
+        <v>2.0</v>
+      </c>
+      <c r="Y20" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="Z20" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="27">
+      <c r="AA20" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AB20" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="AC20" s="26">
         <v>1.0</v>
       </c>
-      <c r="AD20" s="26">
-        <v>5.0</v>
-      </c>
-      <c r="AE20" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="26"/>
       <c r="AF20" s="26">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AG20" s="26">
         <v>0.0</v>
@@ -3932,19 +3966,19 @@
       <c r="AH20" s="26">
         <v>-2.0</v>
       </c>
-      <c r="AI20" s="27">
-        <v>-3.0</v>
-      </c>
+      <c r="AI20" s="26"/>
       <c r="AJ20" s="26">
-        <v>-3.0</v>
+        <v>3.0</v>
       </c>
       <c r="AK20" s="26">
         <v>-1.0</v>
       </c>
       <c r="AL20" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AM20" s="26"/>
+        <v>-1.0</v>
+      </c>
+      <c r="AM20" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN20" s="26"/>
       <c r="AO20" s="26"/>
       <c r="AP20" s="26"/>
@@ -3961,15 +3995,15 @@
       </c>
       <c r="AZ20" s="5">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BA20" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BB20" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" si="4"/>
@@ -3977,15 +4011,15 @@
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="6"/>
-        <v>-15</v>
+        <v>-7</v>
       </c>
       <c r="BF20" s="19">
         <f t="shared" si="7"/>
-        <v>0.3555555556</v>
+        <v>0.3793103448</v>
       </c>
       <c r="BG20" s="19"/>
     </row>
@@ -4176,7 +4210,9 @@
       <c r="AL22" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM22" s="26"/>
+      <c r="AM22" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN22" s="26"/>
       <c r="AO22" s="26"/>
       <c r="AP22" s="26"/>
@@ -4193,7 +4229,7 @@
       </c>
       <c r="AZ22" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BA22" s="5">
         <f t="shared" si="2"/>
@@ -4205,7 +4241,7 @@
       </c>
       <c r="BC22" s="5">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BD22" s="5">
         <f t="shared" si="5"/>
@@ -4213,11 +4249,11 @@
       </c>
       <c r="BE22" s="5">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BF22" s="19">
         <f t="shared" si="7"/>
-        <v>0.5897435897</v>
+        <v>0.5476190476</v>
       </c>
       <c r="BG22" s="19"/>
     </row>
@@ -4336,39 +4372,45 @@
         <v>78</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="E24" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="F24" s="26"/>
       <c r="G24" s="26">
         <v>3.0</v>
       </c>
       <c r="H24" s="26">
-        <v>3.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I24" s="26">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
+      <c r="L24" s="27">
+        <v>-3.0</v>
+      </c>
+      <c r="M24" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
+      <c r="P24" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Q24" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="R24" s="26">
+        <v>0.0</v>
+      </c>
       <c r="S24" s="26"/>
-      <c r="T24" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="U24" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
       <c r="X24" s="26"/>
@@ -4382,11 +4424,21 @@
       <c r="AF24" s="26"/>
       <c r="AG24" s="26"/>
       <c r="AH24" s="26"/>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="26"/>
-      <c r="AM24" s="26"/>
+      <c r="AI24" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AJ24" s="26">
+        <v>-3.0</v>
+      </c>
+      <c r="AK24" s="27">
+        <v>-1.0</v>
+      </c>
+      <c r="AL24" s="26">
+        <v>-1.0</v>
+      </c>
+      <c r="AM24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN24" s="26"/>
       <c r="AO24" s="26"/>
       <c r="AP24" s="26"/>
@@ -4403,7 +4455,7 @@
       </c>
       <c r="AZ24" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BA24" s="5">
         <f t="shared" si="2"/>
@@ -4411,23 +4463,23 @@
       </c>
       <c r="BB24" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC24" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="BD24" s="5">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BE24" s="5">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>-7</v>
       </c>
       <c r="BF24" s="19">
         <f t="shared" si="7"/>
-        <v>0.7619047619</v>
+        <v>0.3777777778</v>
       </c>
       <c r="BG24" s="19"/>
     </row>
@@ -4436,13 +4488,23 @@
         <v>79</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="C25" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="F25" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="G25" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="H25" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="I25" s="26">
+        <v>2.0</v>
+      </c>
       <c r="J25" s="26"/>
       <c r="K25" s="25"/>
       <c r="L25" s="26"/>
@@ -4453,39 +4515,29 @@
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
+      <c r="T25" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="U25" s="26">
+        <v>0.0</v>
+      </c>
       <c r="V25" s="26"/>
       <c r="W25" s="25"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
       <c r="AA25" s="26"/>
-      <c r="AB25" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="AC25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26"/>
       <c r="AD25" s="26"/>
-      <c r="AE25" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AE25" s="26"/>
       <c r="AF25" s="26"/>
-      <c r="AG25" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="AG25" s="26"/>
       <c r="AH25" s="26"/>
       <c r="AI25" s="26"/>
-      <c r="AJ25" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="AK25" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AL25" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ25" s="26"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
       <c r="AM25" s="26"/>
       <c r="AN25" s="26"/>
       <c r="AO25" s="26"/>
@@ -4507,11 +4559,11 @@
       </c>
       <c r="BA25" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BB25" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC25" s="5">
         <f t="shared" si="4"/>
@@ -4519,15 +4571,15 @@
       </c>
       <c r="BD25" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BE25" s="5">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="BF25" s="19">
         <f t="shared" si="7"/>
-        <v>0.6666666667</v>
+        <v>0.7619047619</v>
       </c>
       <c r="BG25" s="19"/>
     </row>
@@ -4537,41 +4589,21 @@
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
-      <c r="D26" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="E26" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="26"/>
-      <c r="G26" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="H26" s="26">
-        <v>-3.0</v>
-      </c>
-      <c r="I26" s="26">
-        <v>-2.0</v>
-      </c>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="26"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="27">
-        <v>-3.0</v>
-      </c>
-      <c r="M26" s="26">
-        <v>-1.0</v>
-      </c>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
-      <c r="P26" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Q26" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="R26" s="26">
-        <v>0.0</v>
-      </c>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
       <c r="S26" s="26"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
@@ -4581,26 +4613,34 @@
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="26"/>
+      <c r="AB26" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="AC26" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AD26" s="26"/>
-      <c r="AE26" s="26"/>
+      <c r="AE26" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AF26" s="26"/>
-      <c r="AG26" s="26"/>
+      <c r="AG26" s="26">
+        <v>0.0</v>
+      </c>
       <c r="AH26" s="26"/>
-      <c r="AI26" s="26">
-        <v>-3.0</v>
-      </c>
+      <c r="AI26" s="26"/>
       <c r="AJ26" s="26">
         <v>-3.0</v>
       </c>
-      <c r="AK26" s="27">
+      <c r="AK26" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AL26" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AM26" s="26">
         <v>-1.0</v>
       </c>
-      <c r="AL26" s="26">
-        <v>-1.0</v>
-      </c>
-      <c r="AM26" s="26"/>
       <c r="AN26" s="26"/>
       <c r="AO26" s="26"/>
       <c r="AP26" s="26"/>
@@ -4617,7 +4657,7 @@
       </c>
       <c r="AZ26" s="5">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="BA26" s="5">
         <f t="shared" si="2"/>
@@ -4629,7 +4669,7 @@
       </c>
       <c r="BC26" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="BD26" s="5">
         <f t="shared" si="5"/>
@@ -4637,11 +4677,11 @@
       </c>
       <c r="BE26" s="5">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="BF26" s="19">
         <f t="shared" si="7"/>
-        <v>0.3333333333</v>
+        <v>0.5833333333</v>
       </c>
       <c r="BG26" s="19"/>
     </row>
@@ -4726,7 +4766,9 @@
       <c r="AL27" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM27" s="26"/>
+      <c r="AM27" s="26">
+        <v>-1.0</v>
+      </c>
       <c r="AN27" s="26"/>
       <c r="AO27" s="26"/>
       <c r="AP27" s="26"/>
@@ -4743,7 +4785,7 @@
       </c>
       <c r="AZ27" s="5">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="BA27" s="5">
         <f t="shared" si="2"/>
@@ -4755,7 +4797,7 @@
       </c>
       <c r="BC27" s="5">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BD27" s="5">
         <f t="shared" si="5"/>
@@ -4763,11 +4805,11 @@
       </c>
       <c r="BE27" s="5">
         <f t="shared" si="6"/>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="BF27" s="19">
         <f t="shared" si="7"/>
-        <v>0.2166666667</v>
+        <v>0.2063492063</v>
       </c>
       <c r="BG27" s="19"/>
     </row>
@@ -6137,7 +6179,7 @@
       </c>
       <c r="AM41" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AN41" s="30">
         <f t="shared" si="8"/>
@@ -6298,7 +6340,9 @@
       <c r="AL42" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AM42" s="5"/>
+      <c r="AM42" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="AN42" s="5"/>
       <c r="AO42" s="5"/>
       <c r="AP42" s="5"/>
@@ -26603,7 +26647,7 @@
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="41">
         <v>3.0</v>
@@ -26651,7 +26695,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="39">
         <v>4.0</v>
@@ -26675,33 +26719,33 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B6" s="39">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C6" s="39">
         <v>2.0</v>
       </c>
       <c r="D6" s="39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="39">
         <v>1.0</v>
       </c>
       <c r="F6" s="39">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" s="39">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6" s="39">
         <v>18.0</v>
       </c>
       <c r="J6" s="42">
         <f t="shared" ref="J6:J10" si="2">I6/B6</f>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="43"/>
@@ -26709,26 +26753,26 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B7" s="39">
         <v>3.0</v>
       </c>
       <c r="C7" s="39">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" s="39">
         <v>1.0</v>
       </c>
       <c r="F7" s="39">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G7" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I7" s="39">
         <v>24.0</v>
@@ -26741,7 +26785,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B8" s="39">
         <v>3.0</v>
@@ -26756,7 +26800,7 @@
         <v>1.0</v>
       </c>
       <c r="F8" s="39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" s="39">
         <f t="shared" si="1"/>
@@ -26772,7 +26816,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="39">
         <v>3.0</v>
@@ -26914,7 +26958,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="39">
         <v>1.0</v>
@@ -27066,19 +27110,19 @@
     </row>
     <row r="19">
       <c r="A19" s="32" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B19" s="39">
         <v>3.0</v>
       </c>
       <c r="C19" s="39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19" s="39">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="39">
         <v>0.0</v>
-      </c>
-      <c r="E19" s="39">
-        <v>2.0</v>
       </c>
       <c r="F19" s="39">
         <v>0.0</v>
@@ -27097,22 +27141,22 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="B20" s="39">
         <v>3.0</v>
       </c>
       <c r="C20" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="39">
         <v>0.0</v>
       </c>
-      <c r="D20" s="39">
-        <v>3.0</v>
-      </c>
       <c r="E20" s="39">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="F20" s="39">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G20" s="39">
         <f t="shared" si="1"/>
@@ -27129,10 +27173,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="B21" s="39">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C21" s="39">
         <v>1.0</v>
@@ -27141,7 +27185,7 @@
         <v>0.0</v>
       </c>
       <c r="E21" s="39">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F21" s="39">
         <v>-1.0</v>
@@ -27155,12 +27199,12 @@
       </c>
       <c r="J21" s="42">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="39">
         <v>3.0</v>
@@ -27256,7 +27300,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="39">
         <v>4.0</v>
@@ -27288,7 +27332,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B26" s="39">
         <v>3.0</v>
@@ -27374,7 +27418,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B29" s="39">
         <v>2.0</v>
@@ -28625,69 +28669,63 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="B3" s="15"/>
       <c r="C3" s="16">
         <v>1.0</v>
       </c>
-      <c r="D3" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="16">
-        <v>4.0</v>
-      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="16">
         <v>1.0</v>
       </c>
       <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="J3" s="16">
+        <v>1.0</v>
+      </c>
       <c r="K3" s="15"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
+      <c r="Q3" s="16">
+        <v>3.0</v>
+      </c>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
       <c r="U3" s="16"/>
-      <c r="V3" s="16">
+      <c r="V3" s="16"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="16">
+        <v>6.0</v>
+      </c>
+      <c r="Y3" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="Z3" s="16">
         <v>2.0</v>
       </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16">
-        <v>1.0</v>
-      </c>
       <c r="AA3" s="16"/>
-      <c r="AB3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AC3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AD3" s="16">
-        <v>3.0</v>
-      </c>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
       <c r="AE3" s="16"/>
       <c r="AF3" s="16"/>
       <c r="AG3" s="16"/>
-      <c r="AH3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="AI3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AJ3" s="16"/>
       <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
+      <c r="AL3" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AM3" s="16"/>
       <c r="AN3" s="16"/>
       <c r="AO3" s="16"/>
@@ -28704,67 +28742,77 @@
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6">
         <f t="shared" ref="BA3:BA36" si="1">SUM(B3:AY3)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BB3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC3" s="5"/>
+        <v>2.0</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="29"/>
+        <v>62</v>
+      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="30">
         <v>1.0</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="30">
+        <v>1.0</v>
+      </c>
       <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>4.0</v>
+      </c>
       <c r="H4" s="30">
         <v>1.0</v>
       </c>
       <c r="I4" s="30"/>
-      <c r="J4" s="30">
-        <v>1.0</v>
-      </c>
+      <c r="J4" s="30"/>
       <c r="K4" s="29"/>
       <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+      <c r="M4" s="30">
+        <v>1.0</v>
+      </c>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
-      <c r="Q4" s="30">
-        <v>3.0</v>
-      </c>
+      <c r="Q4" s="30"/>
       <c r="R4" s="30"/>
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
+      <c r="V4" s="30">
+        <v>2.0</v>
+      </c>
       <c r="W4" s="29"/>
-      <c r="X4" s="30">
-        <v>6.0</v>
-      </c>
-      <c r="Y4" s="30">
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30">
         <v>1.0</v>
       </c>
-      <c r="Z4" s="30">
-        <v>2.0</v>
-      </c>
       <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
+      <c r="AB4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>3.0</v>
+      </c>
       <c r="AE4" s="30"/>
       <c r="AF4" s="30"/>
       <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30">
-        <v>2.0</v>
-      </c>
+      <c r="AH4" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="AI4" s="30"/>
       <c r="AJ4" s="30"/>
       <c r="AK4" s="30"/>
       <c r="AL4" s="30"/>
@@ -28784,18 +28832,16 @@
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BB4" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="BC4" s="5">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="BC4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26">
@@ -28879,7 +28925,7 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -29121,61 +29167,57 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
+      <c r="C9" s="26">
+        <v>1.0</v>
+      </c>
       <c r="D9" s="26"/>
-      <c r="E9" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="26">
+        <v>2.0</v>
+      </c>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
-      <c r="M9" s="26">
+      <c r="M9" s="26"/>
+      <c r="N9" s="26">
         <v>1.0</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
+      <c r="O9" s="26">
+        <v>2.0</v>
+      </c>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
-      <c r="S9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="S9" s="26"/>
       <c r="T9" s="26"/>
       <c r="U9" s="26"/>
       <c r="V9" s="26"/>
       <c r="W9" s="25"/>
-      <c r="X9" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="Y9" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
       <c r="AA9" s="26"/>
       <c r="AB9" s="26">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="AC9" s="26"/>
       <c r="AD9" s="26"/>
-      <c r="AE9" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AE9" s="26"/>
       <c r="AF9" s="26"/>
       <c r="AG9" s="26"/>
       <c r="AH9" s="26"/>
       <c r="AI9" s="26"/>
       <c r="AJ9" s="26"/>
-      <c r="AK9" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="AL9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AM9" s="26"/>
       <c r="AN9" s="26"/>
       <c r="AO9" s="26"/>
@@ -29192,72 +29234,66 @@
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="BC9" s="5">
-        <v>2.0</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="BC9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="25"/>
+        <v>72</v>
+      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26">
         <v>1.0</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="26">
+        <v>7.0</v>
+      </c>
       <c r="J10" s="26"/>
       <c r="K10" s="25"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
-      <c r="O10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O10" s="26"/>
       <c r="P10" s="26"/>
-      <c r="Q10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
-      <c r="U10" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="V10" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
       <c r="W10" s="25"/>
       <c r="X10" s="26"/>
       <c r="Y10" s="26"/>
-      <c r="Z10" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="Z10" s="26"/>
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="26">
+      <c r="AC10" s="26">
         <v>1.0</v>
       </c>
-      <c r="AE10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF10" s="26"/>
       <c r="AG10" s="26"/>
       <c r="AH10" s="26"/>
-      <c r="AI10" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AI10" s="26"/>
       <c r="AJ10" s="26"/>
       <c r="AK10" s="26"/>
-      <c r="AL10" s="26"/>
+      <c r="AL10" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM10" s="26"/>
       <c r="AN10" s="26"/>
       <c r="AO10" s="26"/>
@@ -29274,39 +29310,37 @@
       <c r="AZ10" s="6"/>
       <c r="BA10" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB10" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC10" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="BC10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="D11" s="26"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" s="26"/>
-      <c r="I11" s="26">
-        <v>7.0</v>
-      </c>
+      <c r="I11" s="26"/>
       <c r="J11" s="26"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="L11" s="26">
+        <v>3.0</v>
+      </c>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
+      <c r="O11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
@@ -29318,22 +29352,30 @@
       <c r="X11" s="26"/>
       <c r="Y11" s="26"/>
       <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
+      <c r="AA11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AB11" s="26"/>
-      <c r="AC11" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AC11" s="26"/>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26">
         <v>1.0</v>
       </c>
       <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
+      <c r="AG11" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AH11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
-      <c r="AK11" s="26"/>
-      <c r="AL11" s="26"/>
+      <c r="AK11" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="AL11" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
@@ -29350,7 +29392,7 @@
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BB11" s="5">
         <v>1.0</v>
@@ -29359,7 +29401,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
@@ -29367,41 +29409,39 @@
       <c r="E12" s="26">
         <v>1.0</v>
       </c>
-      <c r="F12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
       <c r="K12" s="25"/>
       <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="M12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="N12" s="26"/>
-      <c r="O12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
-      <c r="R12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="U12" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
       <c r="V12" s="26"/>
       <c r="W12" s="25"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
+      <c r="X12" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="Y12" s="26">
+        <v>2.0</v>
+      </c>
       <c r="Z12" s="26"/>
       <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
+      <c r="AB12" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AC12" s="26"/>
       <c r="AD12" s="26"/>
       <c r="AE12" s="26">
@@ -29410,11 +29450,11 @@
       <c r="AF12" s="26"/>
       <c r="AG12" s="26"/>
       <c r="AH12" s="26"/>
-      <c r="AI12" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
-      <c r="AK12" s="26"/>
+      <c r="AK12" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AL12" s="26"/>
       <c r="AM12" s="26"/>
       <c r="AN12" s="26"/>
@@ -29437,64 +29477,66 @@
       <c r="BB12" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC12" s="5"/>
+      <c r="BC12" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="D13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="G13" s="26"/>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26">
         <v>1.0</v>
       </c>
       <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
+      <c r="Q13" s="26">
+        <v>1.0</v>
+      </c>
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
       <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
+      <c r="U13" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="V13" s="26">
+        <v>3.0</v>
+      </c>
       <c r="W13" s="25"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26">
+      <c r="Z13" s="26">
         <v>1.0</v>
       </c>
+      <c r="AA13" s="26"/>
       <c r="AB13" s="26"/>
       <c r="AC13" s="26"/>
-      <c r="AD13" s="26"/>
-      <c r="AE13" s="26">
+      <c r="AD13" s="26">
         <v>1.0</v>
       </c>
+      <c r="AE13" s="26"/>
       <c r="AF13" s="26"/>
-      <c r="AG13" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AH13" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="AI13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AJ13" s="26"/>
-      <c r="AK13" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AK13" s="26"/>
       <c r="AL13" s="26"/>
       <c r="AM13" s="26"/>
       <c r="AN13" s="26"/>
@@ -29517,57 +29559,67 @@
       <c r="BB13" s="5">
         <v>1.0</v>
       </c>
-      <c r="BC13" s="5"/>
+      <c r="BC13" s="5">
+        <v>1.0</v>
+      </c>
       <c r="BF13" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="26">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26">
         <v>1.0</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
+      <c r="H14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="I14" s="26"/>
-      <c r="J14" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="J14" s="26"/>
       <c r="K14" s="25"/>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
-      <c r="N14" s="26">
+      <c r="N14" s="26"/>
+      <c r="O14" s="26">
         <v>1.0</v>
-      </c>
-      <c r="O14" s="26">
-        <v>2.0</v>
       </c>
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
+      <c r="R14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
+      <c r="T14" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="U14" s="26">
+        <v>3.0</v>
+      </c>
       <c r="V14" s="26"/>
       <c r="W14" s="25"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
       <c r="AA14" s="26"/>
-      <c r="AB14" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AB14" s="26"/>
       <c r="AC14" s="26"/>
       <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
+      <c r="AE14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AF14" s="26"/>
       <c r="AG14" s="26"/>
       <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
+      <c r="AI14" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AJ14" s="26"/>
       <c r="AK14" s="26"/>
       <c r="AL14" s="26"/>
@@ -29587,10 +29639,10 @@
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BB14" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="BC14" s="5"/>
     </row>
@@ -29975,7 +30027,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -30054,14 +30106,16 @@
         <v>78</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="C21" s="26">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26">
         <v>2.0</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
+      <c r="H21" s="26">
+        <v>2.0</v>
+      </c>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
       <c r="K21" s="25"/>
@@ -30071,14 +30125,12 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
+      <c r="R21" s="26">
+        <v>2.0</v>
+      </c>
       <c r="S21" s="26"/>
-      <c r="T21" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="U21" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="25"/>
       <c r="X21" s="26"/>
@@ -30095,7 +30147,9 @@
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
       <c r="AK21" s="26"/>
-      <c r="AL21" s="26"/>
+      <c r="AL21" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AM21" s="26"/>
       <c r="AN21" s="26"/>
       <c r="AO21" s="26"/>
@@ -30114,17 +30168,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="BB21" s="5"/>
+      <c r="BB21" s="5">
+        <v>2.0</v>
+      </c>
       <c r="BC21" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="C22" s="26">
+        <v>2.0</v>
+      </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
@@ -30141,29 +30199,27 @@
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
+      <c r="T22" s="26">
+        <v>3.0</v>
+      </c>
+      <c r="U22" s="26">
+        <v>2.0</v>
+      </c>
       <c r="V22" s="26"/>
       <c r="W22" s="25"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
-      <c r="AA22" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
       <c r="AC22" s="26"/>
       <c r="AD22" s="26"/>
       <c r="AE22" s="26"/>
-      <c r="AF22" s="26">
-        <v>3.0</v>
-      </c>
+      <c r="AF22" s="26"/>
       <c r="AG22" s="26"/>
       <c r="AH22" s="26"/>
       <c r="AI22" s="26"/>
-      <c r="AJ22" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
       <c r="AL22" s="26"/>
       <c r="AM22" s="26"/>
@@ -30186,12 +30242,12 @@
       </c>
       <c r="BB22" s="5"/>
       <c r="BC22" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
@@ -30200,18 +30256,14 @@
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
-      <c r="I23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="I23" s="26"/>
       <c r="J23" s="26"/>
       <c r="K23" s="25"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
-      <c r="P23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
       <c r="S23" s="26"/>
@@ -30219,12 +30271,12 @@
       <c r="U23" s="26"/>
       <c r="V23" s="26"/>
       <c r="W23" s="25"/>
-      <c r="X23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
+      <c r="AA23" s="26">
+        <v>2.0</v>
+      </c>
       <c r="AB23" s="26"/>
       <c r="AC23" s="26"/>
       <c r="AD23" s="26"/>
@@ -30235,10 +30287,10 @@
       <c r="AG23" s="26"/>
       <c r="AH23" s="26"/>
       <c r="AI23" s="26"/>
-      <c r="AJ23" s="26"/>
-      <c r="AK23" s="26">
-        <v>1.0</v>
-      </c>
+      <c r="AJ23" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="AK23" s="26"/>
       <c r="AL23" s="26"/>
       <c r="AM23" s="26"/>
       <c r="AN23" s="26"/>
@@ -30265,37 +30317,37 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
-      <c r="E24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="E24" s="26"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
-      <c r="H24" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="I24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="J24" s="26"/>
       <c r="K24" s="25"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="P24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Q24" s="26"/>
-      <c r="R24" s="26">
-        <v>2.0</v>
-      </c>
+      <c r="R24" s="26"/>
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="25"/>
-      <c r="X24" s="26"/>
+      <c r="X24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="Y24" s="26"/>
       <c r="Z24" s="26"/>
       <c r="AA24" s="26"/>
@@ -30303,12 +30355,16 @@
       <c r="AC24" s="26"/>
       <c r="AD24" s="26"/>
       <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
+      <c r="AF24" s="26">
+        <v>3.0</v>
+      </c>
       <c r="AG24" s="26"/>
       <c r="AH24" s="26"/>
       <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
+      <c r="AK24" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AL24" s="26"/>
       <c r="AM24" s="26"/>
       <c r="AN24" s="26"/>
@@ -30326,11 +30382,9 @@
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="BB24" s="5">
-        <v>2.0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="BB24" s="5"/>
       <c r="BC24" s="5">
         <v>1.0</v>
       </c>
@@ -30621,7 +30675,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
@@ -30951,7 +31005,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="26"/>
@@ -31507,7 +31561,7 @@
       </c>
       <c r="AM40" s="5">
         <f>'League Table'!AM41</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AN40" s="5">
         <f>'League Table'!AN41</f>
@@ -31735,7 +31789,7 @@
       </c>
       <c r="AL42" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM42" s="6">
         <f t="shared" si="3"/>
@@ -62779,7 +62833,9 @@
       <c r="AL5" s="16">
         <v>1.0</v>
       </c>
-      <c r="AM5" s="16"/>
+      <c r="AM5" s="16">
+        <v>2.0</v>
+      </c>
       <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16"/>
@@ -62794,7 +62850,7 @@
       <c r="AY5" s="16"/>
       <c r="BA5" s="39">
         <f t="shared" ref="BA5:BA37" si="1">SUM(B5:AY5)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -62894,7 +62950,7 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26">
@@ -63036,7 +63092,9 @@
       <c r="AL8" s="16">
         <v>1.0</v>
       </c>
-      <c r="AM8" s="16"/>
+      <c r="AM8" s="16">
+        <v>1.0</v>
+      </c>
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
@@ -63051,7 +63109,7 @@
       <c r="AY8" s="16"/>
       <c r="BA8" s="39">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -63109,7 +63167,9 @@
       <c r="AJ9" s="30"/>
       <c r="AK9" s="30"/>
       <c r="AL9" s="30"/>
-      <c r="AM9" s="30"/>
+      <c r="AM9" s="30">
+        <v>1.0</v>
+      </c>
       <c r="AN9" s="30"/>
       <c r="AO9" s="30"/>
       <c r="AP9" s="30"/>
@@ -63124,12 +63184,12 @@
       <c r="AY9" s="30"/>
       <c r="BA9" s="39">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -63204,7 +63264,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -63279,7 +63339,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -63352,7 +63412,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -63425,7 +63485,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -63602,7 +63662,9 @@
       <c r="AL16" s="26">
         <v>1.0</v>
       </c>
-      <c r="AM16" s="26"/>
+      <c r="AM16" s="26">
+        <v>1.0</v>
+      </c>
       <c r="AN16" s="26"/>
       <c r="AO16" s="26"/>
       <c r="AP16" s="26"/>
@@ -63617,12 +63679,12 @@
       <c r="AY16" s="26"/>
       <c r="BA16" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26">
@@ -63807,7 +63869,7 @@
     </row>
     <row r="20">
       <c r="A20" s="32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -63929,7 +63991,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -64409,7 +64471,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -64527,7 +64589,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -64704,7 +64766,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
@@ -65192,7 +65254,7 @@
       </c>
       <c r="AM41" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN41" s="5">
         <f t="shared" si="2"/>
@@ -65244,7 +65306,7 @@
       </c>
       <c r="BA41" s="39">
         <f>SUM(B41:AZ41)</f>
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -66417,7 +66479,7 @@
         <v>168</v>
       </c>
       <c r="N9" s="5">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
@@ -66438,19 +66500,19 @@
       </c>
       <c r="G10" s="46"/>
       <c r="H10" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="L10" s="5">
         <v>3.0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N10" s="5">
         <v>7.0</v>
@@ -66467,14 +66529,14 @@
         <v>176</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>167</v>
       </c>
       <c r="G11" s="46"/>
       <c r="H11" s="5" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="I11" s="5">
         <v>5.0</v>
@@ -66483,7 +66545,7 @@
         <v>177</v>
       </c>
       <c r="L11" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>150</v>
@@ -66510,7 +66572,7 @@
       </c>
       <c r="G12" s="46"/>
       <c r="H12" s="5" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="I12" s="5">
         <v>5.0</v>
@@ -66615,7 +66677,7 @@
         <v>177</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G15" s="46"/>
       <c r="H15" s="5" t="s">
@@ -66625,7 +66687,7 @@
         <v>4.0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L15" s="5">
         <v>2.0</v>
@@ -66651,7 +66713,7 @@
         <v>184</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G16" s="46"/>
       <c r="H16" s="5" t="s">
@@ -66687,7 +66749,7 @@
         <v>157</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17" s="46"/>
       <c r="H17" s="5" t="s">
@@ -66701,7 +66763,7 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N17" s="5">
         <v>5.0</v>
@@ -66772,7 +66834,7 @@
         <v>177</v>
       </c>
       <c r="N19" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
@@ -66793,7 +66855,7 @@
       </c>
       <c r="G20" s="46"/>
       <c r="H20" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I20" s="5">
         <v>2.0</v>
@@ -66891,7 +66953,7 @@
         <v>181</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G23" s="46"/>
       <c r="H23" s="5" t="s">
@@ -66955,7 +67017,7 @@
         <v>150</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G25" s="46"/>
       <c r="H25" s="5" t="s">
@@ -67019,7 +67081,7 @@
         <v>182</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G27" s="46"/>
       <c r="H27" s="5" t="s">
@@ -67081,7 +67143,9 @@
       <c r="E29" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>213</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="K29" s="5"/>
       <c r="M29" s="5" t="s">
@@ -67096,7 +67160,7 @@
         <v>28.0</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" s="46" t="s">
         <v>190</v>
@@ -67122,10 +67186,10 @@
         <v>29.0</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D31" s="46" t="s">
         <v>156</v>
@@ -67151,7 +67215,7 @@
         <v>152</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D32" s="46" t="s">
         <v>145</v>
@@ -67174,7 +67238,7 @@
         <v>31.0</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C33" s="46" t="s">
         <v>187</v>
@@ -67188,7 +67252,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N33" s="58">
         <v>1.0</v>
@@ -67199,7 +67263,7 @@
         <v>32.0</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C34" s="46" t="s">
         <v>194</v>
@@ -67224,7 +67288,7 @@
         <v>33.0</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C35" s="46" t="s">
         <v>170</v>
@@ -67237,15 +67301,19 @@
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="N35" s="58">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="46">
         <v>34.0</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C36" s="46" t="s">
         <v>149</v>
@@ -67266,7 +67334,7 @@
         <v>35.0</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C37" s="46" t="s">
         <v>161</v>
@@ -67287,10 +67355,10 @@
         <v>36.0</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D38" s="46" t="s">
         <v>199</v>
@@ -67307,7 +67375,7 @@
         <v>37.0</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C39" s="46" t="s">
         <v>187</v>
@@ -67326,10 +67394,18 @@
       <c r="A40" s="46">
         <v>38.0</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
+      <c r="B40" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>168</v>
+      </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="N40" s="5"/>

</xml_diff>